<commit_message>
Custom datapage selection enabled
Compartments, characteristics and parameters can now seemingly be placed onto their own pages, as was done in Optima TB.
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9E595C-27FF-49FB-ACE4-774D69D3353F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815FEF56-A265-450C-ACCB-25945B983BA9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Custom Databook Pages" sheetId="7" r:id="rId1"/>
@@ -209,22 +209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column currently denotes whether a databook should request
-values from the user for the historical size of this compartment.
-A value of '-1' suppresses it from appearing in the databook.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -249,6 +234,40 @@
 Framework file parsing should also warn the user about a compartment
 with nonzero setup weight that is suppressed in the databook, i.e.
 has a databook order of '-1'.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{36495753-86C4-4D54-89E3-C16AFFF3861C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column optionally marks whether a data-input section should
+appear for this compartment in a custom databook sheet, if allowed
+to appear at all according to 'databook order'.
+Each value should be a code name for a desired page defined in
+the 'custom databook pages' worksheet page.
+If a cell is left empty, the enabled data-input section should appear
+in a default databook page dedicated to state variables.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{B326D675-59B6-4C74-8331-BE959611E5E2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column currently denotes whether a databook should request
+values from the user for the historical size of this compartment.
+A value of '-1' suppresses it from appearing in the databook.</t>
         </r>
       </text>
     </comment>
@@ -583,7 +602,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="525">
   <si>
     <t>Code Name</t>
   </si>
@@ -2155,6 +2174,9 @@
   </si>
   <si>
     <t>Active TB Death Rates</t>
+  </si>
+  <si>
+    <t>Databook Page</t>
   </si>
 </sst>
 </file>
@@ -2577,8 +2599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{337CD50C-13A1-4CF6-8BA4-65F2738C29EE}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2683,24 +2705,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.06640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.9296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2717,13 +2740,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>429</v>
       </c>
@@ -2739,12 +2765,15 @@
       <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>431</v>
       </c>
@@ -2760,12 +2789,11 @@
       <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>433</v>
       </c>
@@ -2781,12 +2809,11 @@
       <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>434</v>
       </c>
@@ -2802,12 +2829,11 @@
       <c r="E5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>435</v>
       </c>
@@ -2823,12 +2849,11 @@
       <c r="E6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>436</v>
       </c>
@@ -2844,12 +2869,11 @@
       <c r="E7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>437</v>
       </c>
@@ -2865,12 +2889,11 @@
       <c r="E8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>438</v>
       </c>
@@ -2886,12 +2909,11 @@
       <c r="E9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>439</v>
       </c>
@@ -2907,12 +2929,11 @@
       <c r="E10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>440</v>
       </c>
@@ -2928,12 +2949,11 @@
       <c r="E11" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>441</v>
       </c>
@@ -2949,12 +2969,11 @@
       <c r="E12" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>442</v>
       </c>
@@ -2970,12 +2989,11 @@
       <c r="E13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>443</v>
       </c>
@@ -2991,12 +3009,11 @@
       <c r="E14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>444</v>
       </c>
@@ -3012,12 +3029,11 @@
       <c r="E15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>445</v>
       </c>
@@ -3033,12 +3049,11 @@
       <c r="E16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>446</v>
       </c>
@@ -3054,12 +3069,11 @@
       <c r="E17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>447</v>
       </c>
@@ -3075,12 +3089,11 @@
       <c r="E18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>448</v>
       </c>
@@ -3096,12 +3109,11 @@
       <c r="E19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>449</v>
       </c>
@@ -3117,12 +3129,11 @@
       <c r="E20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>450</v>
       </c>
@@ -3138,12 +3149,11 @@
       <c r="E21" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>451</v>
       </c>
@@ -3159,12 +3169,11 @@
       <c r="E22" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
         <v>452</v>
       </c>
@@ -3180,12 +3189,11 @@
       <c r="E23" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>453</v>
       </c>
@@ -3201,12 +3209,11 @@
       <c r="E24" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="6" t="s">
         <v>454</v>
       </c>
@@ -3222,12 +3229,11 @@
       <c r="E25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="6" t="s">
         <v>455</v>
       </c>
@@ -3243,12 +3249,11 @@
       <c r="E26" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="6" t="s">
         <v>456</v>
       </c>
@@ -3264,12 +3269,11 @@
       <c r="E27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="6" t="s">
         <v>457</v>
       </c>
@@ -3285,12 +3289,11 @@
       <c r="E28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
         <v>458</v>
       </c>
@@ -3306,12 +3309,11 @@
       <c r="E29" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="6" t="s">
         <v>459</v>
       </c>
@@ -3327,12 +3329,11 @@
       <c r="E30" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="6" t="s">
         <v>460</v>
       </c>
@@ -3348,12 +3349,11 @@
       <c r="E31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="6" t="s">
         <v>461</v>
       </c>
@@ -3369,12 +3369,11 @@
       <c r="E32" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="6" t="s">
         <v>464</v>
       </c>
@@ -3391,13 +3390,13 @@
         <v>7</v>
       </c>
       <c r="F33" s="4">
+        <v>0</v>
+      </c>
+      <c r="H33" s="7">
         <v>-1</v>
       </c>
-      <c r="G33" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="34" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
         <v>495</v>
       </c>
@@ -3414,13 +3413,13 @@
         <v>7</v>
       </c>
       <c r="F34" s="4">
+        <v>0</v>
+      </c>
+      <c r="H34" s="7">
         <v>-1</v>
       </c>
-      <c r="G34" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="6" t="s">
         <v>462</v>
       </c>
@@ -3437,13 +3436,13 @@
         <v>7</v>
       </c>
       <c r="F35" s="4">
+        <v>0</v>
+      </c>
+      <c r="H35" s="7">
         <v>-1</v>
       </c>
-      <c r="G35" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="6" t="s">
         <v>463</v>
       </c>
@@ -3460,13 +3459,13 @@
         <v>7</v>
       </c>
       <c r="F36" s="4">
+        <v>0</v>
+      </c>
+      <c r="H36" s="7">
         <v>-1</v>
       </c>
-      <c r="G36" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="37" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A37" s="6" t="s">
         <v>497</v>
       </c>
@@ -3483,10 +3482,10 @@
         <v>7</v>
       </c>
       <c r="F37" s="4">
+        <v>0</v>
+      </c>
+      <c r="H37" s="7">
         <v>-1</v>
-      </c>
-      <c r="G37" s="4">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3505,7 +3504,7 @@
   <dimension ref="A1:AO41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AI14" sqref="AI14"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Restricted multiple links for parameter with source comp
Because of ambiguity in how to disaggregate flows between transitions when one of them is an infinite-basin source compartment, a parameter that is associated with such a transition can have no others.
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB85650-426A-4B63-A82E-C58E71D56190}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68124BBB-F46B-4AEB-AC5B-DA8B45A5B0B8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -640,7 +640,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="598">
   <si>
     <t>Code Name</t>
   </si>
@@ -3871,8 +3871,8 @@
   <dimension ref="A1:AO41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AK34" sqref="AK34"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4650,96 +4650,36 @@
       <c r="B34" s="10" t="s">
         <v>544</v>
       </c>
-      <c r="C34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="H34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="I34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="J34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="K34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="L34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="M34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="N34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="O34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="P34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="Q34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="R34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="S34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="T34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="U34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="V34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="W34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="X34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="Y34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="Z34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="AA34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="AB34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="AC34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="AD34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="AE34" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="AF34" s="10" t="s">
-        <v>544</v>
-      </c>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="10"/>
+      <c r="S34" s="10"/>
+      <c r="T34" s="10"/>
+      <c r="U34" s="10"/>
+      <c r="V34" s="10"/>
+      <c r="W34" s="10"/>
+      <c r="X34" s="10"/>
+      <c r="Y34" s="10"/>
+      <c r="Z34" s="10"/>
+      <c r="AA34" s="10"/>
+      <c r="AB34" s="10"/>
+      <c r="AC34" s="10"/>
+      <c r="AD34" s="10"/>
+      <c r="AE34" s="10"/>
+      <c r="AF34" s="10"/>
     </row>
     <row r="35" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">

</xml_diff>

<commit_message>
Set up proportion format and continue with cascade
More validations are in this commit to verify that junctions only have outflow transitions in proportion format, while a parameter that is associated with such a transition cannot be related to any others.
The parameter page of the TB framework continues to be developed.
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86BAEC3-6403-4932-A5E5-ED2167EAAFD0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4333B03-4EBA-47F3-A0F9-830A6424E3D9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Custom Databook Pages" sheetId="7" r:id="rId1"/>
@@ -640,7 +640,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="476">
   <si>
     <t>Code Name</t>
   </si>
@@ -1903,6 +1903,171 @@
   </si>
   <si>
     <t>XDR-SN death rate (treated)</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>l_treat</t>
+  </si>
+  <si>
+    <t>l_fail</t>
+  </si>
+  <si>
+    <t>l_succ</t>
+  </si>
+  <si>
+    <t>LTBI treatment uptake rate</t>
+  </si>
+  <si>
+    <t>LTBI treatment abandonment rate</t>
+  </si>
+  <si>
+    <t>LTBI treatment success rate</t>
+  </si>
+  <si>
+    <t>probability</t>
+  </si>
+  <si>
+    <t>e_dep</t>
+  </si>
+  <si>
+    <t>l_dep</t>
+  </si>
+  <si>
+    <t>Early latency departure rate</t>
+  </si>
+  <si>
+    <t>Late latency departure rate</t>
+  </si>
+  <si>
+    <t>p_branch</t>
+  </si>
+  <si>
+    <t>Probability of activation versus early-late progression</t>
+  </si>
+  <si>
+    <t>(1-p_branch)*e_dep</t>
+  </si>
+  <si>
+    <t>p_branch*e_dep</t>
+  </si>
+  <si>
+    <t>spd_infxness</t>
+  </si>
+  <si>
+    <t>spm_infxness</t>
+  </si>
+  <si>
+    <t>spx_infxness</t>
+  </si>
+  <si>
+    <t>snd_infxness</t>
+  </si>
+  <si>
+    <t>snm_infxness</t>
+  </si>
+  <si>
+    <t>snx_infxness</t>
+  </si>
+  <si>
+    <t>vac_fac</t>
+  </si>
+  <si>
+    <t>lat_fac</t>
+  </si>
+  <si>
+    <t>sn_fac</t>
+  </si>
+  <si>
+    <t>mdr_fac</t>
+  </si>
+  <si>
+    <t>xdr_fac</t>
+  </si>
+  <si>
+    <t>foi</t>
+  </si>
+  <si>
+    <t>Infection vulnerability factor (vaccinated versus susceptible)</t>
+  </si>
+  <si>
+    <t>Infection vulnerability factor (treated latent versus susceptible)</t>
+  </si>
+  <si>
+    <t>DS-SP infectiousness</t>
+  </si>
+  <si>
+    <t>Relative infectiousness (SN versus SP)</t>
+  </si>
+  <si>
+    <t>Relative infectiousness (MDR versus DS)</t>
+  </si>
+  <si>
+    <t>Relative infectiousness (XDR versus DS)</t>
+  </si>
+  <si>
+    <t>MDR-SP infectiousness</t>
+  </si>
+  <si>
+    <t>XDR-SP infectiousness</t>
+  </si>
+  <si>
+    <t>DS-SN infectiousness</t>
+  </si>
+  <si>
+    <t>MDR-SN infectiousness</t>
+  </si>
+  <si>
+    <t>XDR-SN infectiousness</t>
+  </si>
+  <si>
+    <t>Force of infection</t>
+  </si>
+  <si>
+    <t>foi*lat_fac</t>
+  </si>
+  <si>
+    <t>foi*vac_fac</t>
+  </si>
+  <si>
+    <t>foi_p</t>
+  </si>
+  <si>
+    <t>foi_n</t>
+  </si>
+  <si>
+    <t>Force of infection from SP prevalence</t>
+  </si>
+  <si>
+    <t>Force of infection from SN prevalence</t>
+  </si>
+  <si>
+    <t>spd_infxness*spd_prevx+spm_infxness*spm_prevx+spx_infxness*spx_prevx</t>
+  </si>
+  <si>
+    <t>snd_infxness*snd_prevx+snm_infxness*snm_prevx+snx_infxness*snx_prevx</t>
+  </si>
+  <si>
+    <t>foi_p+foi_n</t>
+  </si>
+  <si>
+    <t>spd_infxness*mdr_fac</t>
+  </si>
+  <si>
+    <t>spd_infxness*xdr_fac</t>
+  </si>
+  <si>
+    <t>sn_fac*spd_infxness*xdr_fac</t>
+  </si>
+  <si>
+    <t>sn_fac*spd_infxness*mdr_fac</t>
+  </si>
+  <si>
+    <t>sn_fac*spd_infxness</t>
+  </si>
+  <si>
+    <t>proportion</t>
   </si>
 </sst>
 </file>
@@ -1965,7 +2130,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2008,6 +2173,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3315,9 +3483,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AO41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AJ22" sqref="AJ22:AK22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3674,12 +3842,6 @@
       <c r="V11" s="11" t="s">
         <v>294</v>
       </c>
-      <c r="AJ11" s="11" t="s">
-        <v>274</v>
-      </c>
-      <c r="AK11" s="11" t="s">
-        <v>273</v>
-      </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A12" s="12" t="str">
@@ -3695,12 +3857,6 @@
       <c r="S12" s="11" t="s">
         <v>297</v>
       </c>
-      <c r="AJ12" s="11" t="s">
-        <v>274</v>
-      </c>
-      <c r="AK12" s="11" t="s">
-        <v>273</v>
-      </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A13" s="12" t="str">
@@ -3910,12 +4066,6 @@
       </c>
       <c r="AC22" s="11" t="s">
         <v>300</v>
-      </c>
-      <c r="AJ22" s="11" t="s">
-        <v>274</v>
-      </c>
-      <c r="AK22" s="11" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.45">
@@ -5601,19 +5751,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FC8421-05BA-4BE1-A1F1-3F12A4E7E369}">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A10" sqref="A10"/>
+      <selection pane="topRight" activeCell="C43" sqref="C43:C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.1328125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.53125" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.9296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.265625" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.73046875" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.796875" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" style="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.86328125" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.06640625" style="10"/>
@@ -5649,10 +5801,14 @@
       <c r="B2" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="11" t="s">
+        <v>421</v>
+      </c>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="F2" s="11" t="s">
+        <v>92</v>
+      </c>
       <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -5665,7 +5821,9 @@
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
+      <c r="F3" s="11" t="s">
+        <v>92</v>
+      </c>
       <c r="G3" s="11"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
@@ -5675,10 +5833,14 @@
       <c r="B4" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="11" t="s">
+        <v>421</v>
+      </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
+      <c r="F4" s="11" t="s">
+        <v>92</v>
+      </c>
       <c r="G4" s="11"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
@@ -5691,7 +5853,9 @@
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
+      <c r="F5" s="11" t="s">
+        <v>92</v>
+      </c>
       <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
@@ -5704,587 +5868,771 @@
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
+      <c r="F6" s="13" t="s">
+        <v>102</v>
+      </c>
       <c r="G6" s="11"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
-        <v>281</v>
+        <v>422</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>349</v>
+        <v>425</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
+      <c r="F7" s="13" t="s">
+        <v>102</v>
+      </c>
       <c r="G7" s="11"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
-        <v>283</v>
+        <v>423</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>350</v>
+        <v>426</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
+      <c r="F8" s="13" t="s">
+        <v>102</v>
+      </c>
       <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
-        <v>284</v>
+        <v>424</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>351</v>
+        <v>427</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="F9" s="13" t="s">
+        <v>102</v>
+      </c>
       <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>352</v>
-      </c>
-      <c r="C10" s="11"/>
+        <v>349</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>428</v>
+      </c>
       <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="E10" s="11" t="s">
+        <v>422</v>
+      </c>
       <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
+      <c r="G10" s="11">
+        <v>-1</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="11" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>353</v>
-      </c>
-      <c r="C11" s="11"/>
+        <v>350</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>428</v>
+      </c>
       <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
+      <c r="E11" s="11" t="s">
+        <v>423</v>
+      </c>
       <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
+      <c r="G11" s="11">
+        <v>-1</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>428</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11" t="s">
+        <v>424</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>428</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11" t="s">
+        <v>422</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>428</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11" t="s">
+        <v>423</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B15" s="14" t="s">
         <v>354</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" s="13" t="s">
-        <v>282</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>356</v>
-      </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>357</v>
-      </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>358</v>
-      </c>
-      <c r="C15" s="11"/>
+      <c r="C15" s="11" t="s">
+        <v>428</v>
+      </c>
       <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
+      <c r="E15" s="11" t="s">
+        <v>424</v>
+      </c>
       <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
+      <c r="G15" s="11">
+        <v>-1</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A16" s="13" t="s">
-        <v>291</v>
+      <c r="A16" s="11" t="s">
+        <v>429</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>359</v>
+        <v>431</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
+      <c r="F16" s="13" t="s">
+        <v>104</v>
+      </c>
       <c r="G16" s="11"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" s="13" t="s">
-        <v>290</v>
+      <c r="A17" s="11" t="s">
+        <v>430</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>360</v>
+        <v>432</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
+      <c r="F17" s="13" t="s">
+        <v>104</v>
+      </c>
       <c r="G17" s="11"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="13" t="s">
-        <v>292</v>
+      <c r="A18" s="11" t="s">
+        <v>433</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>361</v>
+        <v>434</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
+      <c r="F18" s="13" t="s">
+        <v>104</v>
+      </c>
       <c r="G18" s="11"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="C19" s="11"/>
+      <c r="A19" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>428</v>
+      </c>
       <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
+      <c r="E19" s="11" t="s">
+        <v>435</v>
+      </c>
       <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
+      <c r="G19" s="11">
+        <v>-1</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A20" s="11" t="s">
-        <v>355</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="C20" s="11"/>
+      <c r="A20" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>428</v>
+      </c>
       <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
+      <c r="E20" s="11" t="s">
+        <v>435</v>
+      </c>
       <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
+      <c r="G20" s="11">
+        <v>-1</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21" s="11" t="s">
-        <v>362</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>365</v>
-      </c>
-      <c r="C21" s="11"/>
+      <c r="A21" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>358</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>428</v>
+      </c>
       <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
+      <c r="E21" s="11" t="s">
+        <v>436</v>
+      </c>
       <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
+      <c r="G21" s="11">
+        <v>-1</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" s="11" t="s">
-        <v>323</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>366</v>
-      </c>
-      <c r="C22" s="11"/>
+      <c r="A22" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>428</v>
+      </c>
       <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
+      <c r="E22" s="11" t="s">
+        <v>436</v>
+      </c>
       <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
+      <c r="G22" s="11">
+        <v>-1</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="13" t="s">
-        <v>293</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>367</v>
-      </c>
-      <c r="C23" s="11"/>
+        <v>290</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>428</v>
+      </c>
       <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
+      <c r="E23" s="11" t="s">
+        <v>430</v>
+      </c>
       <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
+      <c r="G23" s="11">
+        <v>-1</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>368</v>
-      </c>
-      <c r="C24" s="11"/>
+        <v>292</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>361</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>428</v>
+      </c>
       <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
+      <c r="E24" s="11" t="s">
+        <v>430</v>
+      </c>
       <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
+      <c r="G24" s="11">
+        <v>-1</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="13" t="s">
-        <v>295</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>369</v>
+        <v>443</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>449</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
+      <c r="F25" s="11" t="s">
+        <v>100</v>
+      </c>
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="13" t="s">
-        <v>296</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>370</v>
+        <v>444</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>450</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
+      <c r="F26" s="11" t="s">
+        <v>100</v>
+      </c>
       <c r="G26" s="11"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="13" t="s">
-        <v>297</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>371</v>
+        <v>437</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>451</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
+      <c r="F27" s="11" t="s">
+        <v>100</v>
+      </c>
       <c r="G27" s="11"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="13" t="s">
-        <v>298</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>372</v>
+        <v>445</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>452</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
+      <c r="F28" s="11" t="s">
+        <v>100</v>
+      </c>
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A29" s="13" t="s">
-        <v>299</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>373</v>
+      <c r="A29" s="17" t="s">
+        <v>446</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>453</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
+      <c r="F29" s="11" t="s">
+        <v>100</v>
+      </c>
       <c r="G29" s="11"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A30" s="13" t="s">
-        <v>300</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>374</v>
+      <c r="A30" s="17" t="s">
+        <v>447</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>454</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
+      <c r="F30" s="11" t="s">
+        <v>100</v>
+      </c>
       <c r="G30" s="11"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="13" t="s">
-        <v>301</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>375</v>
+        <v>438</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>455</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
+      <c r="E31" s="13" t="s">
+        <v>470</v>
+      </c>
       <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
+      <c r="G31" s="11">
+        <v>-1</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="13" t="s">
-        <v>302</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>376</v>
+        <v>439</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>456</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
+      <c r="E32" s="13" t="s">
+        <v>471</v>
+      </c>
       <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
+      <c r="G32" s="11">
+        <v>-1</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="13" t="s">
-        <v>308</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>377</v>
+        <v>440</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>457</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
+      <c r="E33" s="11" t="s">
+        <v>474</v>
+      </c>
       <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
+      <c r="G33" s="11">
+        <v>-1</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="13" t="s">
-        <v>325</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>378</v>
+        <v>441</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>458</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
+      <c r="E34" s="13" t="s">
+        <v>473</v>
+      </c>
       <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
+      <c r="G34" s="11">
+        <v>-1</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>379</v>
+        <v>442</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>459</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
+      <c r="E35" s="13" t="s">
+        <v>472</v>
+      </c>
       <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
+      <c r="G35" s="11">
+        <v>-1</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="13" t="s">
-        <v>303</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>380</v>
+        <v>463</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>465</v>
       </c>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
+      <c r="E36" s="11" t="s">
+        <v>467</v>
+      </c>
       <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
+      <c r="G36" s="11">
+        <v>-1</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="13" t="s">
-        <v>311</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>381</v>
+        <v>464</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>466</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
+      <c r="E37" s="11" t="s">
+        <v>468</v>
+      </c>
       <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
+      <c r="G37" s="11">
+        <v>-1</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="13" t="s">
-        <v>327</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>382</v>
+        <v>448</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>460</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
+      <c r="E38" s="13" t="s">
+        <v>469</v>
+      </c>
       <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
+      <c r="G38" s="11">
+        <v>-1</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A39" s="13" t="s">
-        <v>313</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>383</v>
-      </c>
-      <c r="C39" s="11"/>
+      <c r="A39" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>428</v>
+      </c>
       <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
+      <c r="E39" s="11" t="s">
+        <v>448</v>
+      </c>
       <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
+      <c r="G39" s="11">
+        <v>-1</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A40" s="13" t="s">
-        <v>304</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>384</v>
-      </c>
-      <c r="C40" s="11"/>
+      <c r="A40" s="11" t="s">
+        <v>355</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>428</v>
+      </c>
       <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
+      <c r="E40" s="11" t="s">
+        <v>462</v>
+      </c>
       <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
+      <c r="G40" s="11">
+        <v>-1</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A41" s="13" t="s">
-        <v>314</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>385</v>
-      </c>
-      <c r="C41" s="11"/>
+      <c r="A41" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>428</v>
+      </c>
       <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
+      <c r="E41" s="11" t="s">
+        <v>461</v>
+      </c>
       <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
+      <c r="G41" s="11">
+        <v>-1</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A42" s="13" t="s">
-        <v>329</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>386</v>
-      </c>
-      <c r="C42" s="11"/>
+      <c r="A42" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>428</v>
+      </c>
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
+      <c r="F42" s="11" t="s">
+        <v>100</v>
+      </c>
       <c r="G42" s="11"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="13" t="s">
-        <v>315</v>
+        <v>293</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>387</v>
-      </c>
-      <c r="C43" s="11"/>
+        <v>367</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>475</v>
+      </c>
       <c r="D43" s="11"/>
       <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
+      <c r="F43" s="11" t="s">
+        <v>98</v>
+      </c>
       <c r="G43" s="11"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="13" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>388</v>
-      </c>
-      <c r="C44" s="11"/>
+        <v>368</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>475</v>
+      </c>
       <c r="D44" s="11"/>
       <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
+      <c r="F44" s="11" t="s">
+        <v>98</v>
+      </c>
       <c r="G44" s="11"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" s="13" t="s">
-        <v>316</v>
+        <v>295</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>389</v>
-      </c>
-      <c r="C45" s="11"/>
+        <v>369</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>475</v>
+      </c>
       <c r="D45" s="11"/>
       <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
+      <c r="F45" s="11" t="s">
+        <v>98</v>
+      </c>
       <c r="G45" s="11"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="13" t="s">
-        <v>331</v>
+        <v>296</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>390</v>
-      </c>
-      <c r="C46" s="11"/>
+        <v>370</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>475</v>
+      </c>
       <c r="D46" s="11"/>
       <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
+      <c r="F46" s="11" t="s">
+        <v>98</v>
+      </c>
       <c r="G46" s="11"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="13" t="s">
-        <v>318</v>
+        <v>297</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>391</v>
-      </c>
-      <c r="C47" s="11"/>
+        <v>371</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>475</v>
+      </c>
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
+      <c r="F47" s="11" t="s">
+        <v>98</v>
+      </c>
       <c r="G47" s="11"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="13" t="s">
-        <v>306</v>
-      </c>
-      <c r="B48" s="15" t="s">
-        <v>392</v>
-      </c>
-      <c r="C48" s="11"/>
+        <v>298</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>372</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>475</v>
+      </c>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
+      <c r="F48" s="11" t="s">
+        <v>98</v>
+      </c>
       <c r="G48" s="11"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="13" t="s">
-        <v>319</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>393</v>
-      </c>
-      <c r="C49" s="11"/>
+        <v>299</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>373</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>475</v>
+      </c>
       <c r="D49" s="11"/>
       <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
+      <c r="F49" s="11" t="s">
+        <v>98</v>
+      </c>
       <c r="G49" s="11"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="13" t="s">
-        <v>333</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>394</v>
-      </c>
-      <c r="C50" s="11"/>
+        <v>300</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>374</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>475</v>
+      </c>
       <c r="D50" s="11"/>
       <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
+      <c r="F50" s="11" t="s">
+        <v>98</v>
+      </c>
       <c r="G50" s="11"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="13" t="s">
-        <v>321</v>
+        <v>301</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>395</v>
+        <v>375</v>
       </c>
       <c r="C51" s="11"/>
       <c r="D51" s="11"/>
@@ -6294,10 +6642,10 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" s="13" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>396</v>
+        <v>376</v>
       </c>
       <c r="C52" s="11"/>
       <c r="D52" s="11"/>
@@ -6307,10 +6655,10 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="13" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="C53" s="11"/>
       <c r="D53" s="11"/>
@@ -6320,10 +6668,10 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="13" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>398</v>
+        <v>378</v>
       </c>
       <c r="C54" s="11"/>
       <c r="D54" s="11"/>
@@ -6333,10 +6681,10 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="13" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
       <c r="C55" s="11"/>
       <c r="D55" s="11"/>
@@ -6346,10 +6694,10 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="13" t="s">
-        <v>326</v>
+        <v>303</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>400</v>
+        <v>380</v>
       </c>
       <c r="C56" s="11"/>
       <c r="D56" s="11"/>
@@ -6359,10 +6707,10 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="13" t="s">
-        <v>328</v>
+        <v>311</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>401</v>
+        <v>381</v>
       </c>
       <c r="C57" s="11"/>
       <c r="D57" s="11"/>
@@ -6372,10 +6720,10 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="13" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="C58" s="11"/>
       <c r="D58" s="11"/>
@@ -6385,10 +6733,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="13" t="s">
-        <v>332</v>
+        <v>313</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
       <c r="C59" s="11"/>
       <c r="D59" s="11"/>
@@ -6398,10 +6746,10 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="13" t="s">
-        <v>334</v>
+        <v>304</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
       <c r="C60" s="11"/>
       <c r="D60" s="11"/>
@@ -6411,10 +6759,10 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="13" t="s">
-        <v>317</v>
-      </c>
-      <c r="B61" s="16" t="s">
-        <v>405</v>
+        <v>314</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>385</v>
       </c>
       <c r="C61" s="11"/>
       <c r="D61" s="11"/>
@@ -6424,10 +6772,10 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="13" t="s">
-        <v>320</v>
-      </c>
-      <c r="B62" s="16" t="s">
-        <v>406</v>
+        <v>329</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>386</v>
       </c>
       <c r="C62" s="11"/>
       <c r="D62" s="11"/>
@@ -6437,10 +6785,10 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="13" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>407</v>
+        <v>387</v>
       </c>
       <c r="C63" s="11"/>
       <c r="D63" s="11"/>
@@ -6450,10 +6798,10 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="13" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>408</v>
+        <v>388</v>
       </c>
       <c r="C64" s="11"/>
       <c r="D64" s="11"/>
@@ -6463,10 +6811,10 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A65" s="13" t="s">
-        <v>336</v>
-      </c>
-      <c r="B65" s="16" t="s">
-        <v>409</v>
+        <v>316</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>389</v>
       </c>
       <c r="C65" s="11"/>
       <c r="D65" s="11"/>
@@ -6476,10 +6824,10 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A66" s="13" t="s">
-        <v>338</v>
-      </c>
-      <c r="B66" s="16" t="s">
-        <v>410</v>
+        <v>331</v>
+      </c>
+      <c r="B66" s="15" t="s">
+        <v>390</v>
       </c>
       <c r="C66" s="11"/>
       <c r="D66" s="11"/>
@@ -6489,10 +6837,10 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="B67" s="16" t="s">
-        <v>411</v>
+        <v>318</v>
+      </c>
+      <c r="B67" s="15" t="s">
+        <v>391</v>
       </c>
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
@@ -6502,10 +6850,10 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68" s="13" t="s">
-        <v>337</v>
-      </c>
-      <c r="B68" s="16" t="s">
-        <v>412</v>
+        <v>306</v>
+      </c>
+      <c r="B68" s="15" t="s">
+        <v>392</v>
       </c>
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
@@ -6515,10 +6863,10 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A69" s="13" t="s">
-        <v>339</v>
-      </c>
-      <c r="B69" s="16" t="s">
-        <v>413</v>
+        <v>319</v>
+      </c>
+      <c r="B69" s="15" t="s">
+        <v>393</v>
       </c>
       <c r="C69" s="11"/>
       <c r="D69" s="11"/>
@@ -6528,10 +6876,10 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A70" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="B70" s="16" t="s">
-        <v>414</v>
+        <v>333</v>
+      </c>
+      <c r="B70" s="15" t="s">
+        <v>394</v>
       </c>
       <c r="C70" s="11"/>
       <c r="D70" s="11"/>
@@ -6541,10 +6889,10 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71" s="13" t="s">
-        <v>342</v>
-      </c>
-      <c r="B71" s="16" t="s">
-        <v>415</v>
+        <v>321</v>
+      </c>
+      <c r="B71" s="15" t="s">
+        <v>395</v>
       </c>
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
@@ -6554,10 +6902,10 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="B72" s="16" t="s">
-        <v>416</v>
+        <v>307</v>
+      </c>
+      <c r="B72" s="15" t="s">
+        <v>396</v>
       </c>
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
@@ -6567,10 +6915,10 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73" s="13" t="s">
-        <v>346</v>
-      </c>
-      <c r="B73" s="16" t="s">
-        <v>417</v>
+        <v>322</v>
+      </c>
+      <c r="B73" s="15" t="s">
+        <v>397</v>
       </c>
       <c r="C73" s="11"/>
       <c r="D73" s="11"/>
@@ -6580,10 +6928,10 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74" s="13" t="s">
-        <v>343</v>
-      </c>
-      <c r="B74" s="16" t="s">
-        <v>418</v>
+        <v>335</v>
+      </c>
+      <c r="B74" s="15" t="s">
+        <v>398</v>
       </c>
       <c r="C74" s="11"/>
       <c r="D74" s="11"/>
@@ -6593,10 +6941,10 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A75" s="13" t="s">
-        <v>345</v>
-      </c>
-      <c r="B75" s="16" t="s">
-        <v>419</v>
+        <v>324</v>
+      </c>
+      <c r="B75" s="15" t="s">
+        <v>399</v>
       </c>
       <c r="C75" s="11"/>
       <c r="D75" s="11"/>
@@ -6606,16 +6954,276 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A76" s="13" t="s">
-        <v>347</v>
-      </c>
-      <c r="B76" s="16" t="s">
-        <v>420</v>
+        <v>326</v>
+      </c>
+      <c r="B76" s="15" t="s">
+        <v>400</v>
       </c>
       <c r="C76" s="11"/>
       <c r="D76" s="11"/>
       <c r="E76" s="11"/>
       <c r="F76" s="11"/>
       <c r="G76" s="11"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A77" s="13" t="s">
+        <v>328</v>
+      </c>
+      <c r="B77" s="15" t="s">
+        <v>401</v>
+      </c>
+      <c r="C77" s="11"/>
+      <c r="D77" s="11"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A78" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="B78" s="15" t="s">
+        <v>402</v>
+      </c>
+      <c r="C78" s="11"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+      <c r="G78" s="11"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A79" s="13" t="s">
+        <v>332</v>
+      </c>
+      <c r="B79" s="15" t="s">
+        <v>403</v>
+      </c>
+      <c r="C79" s="11"/>
+      <c r="D79" s="11"/>
+      <c r="E79" s="11"/>
+      <c r="F79" s="11"/>
+      <c r="G79" s="11"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A80" s="13" t="s">
+        <v>334</v>
+      </c>
+      <c r="B80" s="15" t="s">
+        <v>404</v>
+      </c>
+      <c r="C80" s="11"/>
+      <c r="D80" s="11"/>
+      <c r="E80" s="11"/>
+      <c r="F80" s="11"/>
+      <c r="G80" s="11"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A81" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="B81" s="16" t="s">
+        <v>405</v>
+      </c>
+      <c r="C81" s="11"/>
+      <c r="D81" s="11"/>
+      <c r="E81" s="11"/>
+      <c r="F81" s="11"/>
+      <c r="G81" s="11"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A82" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="B82" s="16" t="s">
+        <v>406</v>
+      </c>
+      <c r="C82" s="11"/>
+      <c r="D82" s="11"/>
+      <c r="E82" s="11"/>
+      <c r="F82" s="11"/>
+      <c r="G82" s="11"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A83" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="B83" s="15" t="s">
+        <v>407</v>
+      </c>
+      <c r="C83" s="11"/>
+      <c r="D83" s="11"/>
+      <c r="E83" s="11"/>
+      <c r="F83" s="11"/>
+      <c r="G83" s="11"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A84" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="B84" s="15" t="s">
+        <v>408</v>
+      </c>
+      <c r="C84" s="11"/>
+      <c r="D84" s="11"/>
+      <c r="E84" s="11"/>
+      <c r="F84" s="11"/>
+      <c r="G84" s="11"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A85" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="B85" s="16" t="s">
+        <v>409</v>
+      </c>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
+      <c r="E85" s="11"/>
+      <c r="F85" s="11"/>
+      <c r="G85" s="11"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A86" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="B86" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="C86" s="11"/>
+      <c r="D86" s="11"/>
+      <c r="E86" s="11"/>
+      <c r="F86" s="11"/>
+      <c r="G86" s="11"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A87" s="13" t="s">
+        <v>340</v>
+      </c>
+      <c r="B87" s="16" t="s">
+        <v>411</v>
+      </c>
+      <c r="C87" s="11"/>
+      <c r="D87" s="11"/>
+      <c r="E87" s="11"/>
+      <c r="F87" s="11"/>
+      <c r="G87" s="11"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A88" s="13" t="s">
+        <v>337</v>
+      </c>
+      <c r="B88" s="16" t="s">
+        <v>412</v>
+      </c>
+      <c r="C88" s="11"/>
+      <c r="D88" s="11"/>
+      <c r="E88" s="11"/>
+      <c r="F88" s="11"/>
+      <c r="G88" s="11"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A89" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="B89" s="16" t="s">
+        <v>413</v>
+      </c>
+      <c r="C89" s="11"/>
+      <c r="D89" s="11"/>
+      <c r="E89" s="11"/>
+      <c r="F89" s="11"/>
+      <c r="G89" s="11"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A90" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="B90" s="16" t="s">
+        <v>414</v>
+      </c>
+      <c r="C90" s="11"/>
+      <c r="D90" s="11"/>
+      <c r="E90" s="11"/>
+      <c r="F90" s="11"/>
+      <c r="G90" s="11"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A91" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="B91" s="16" t="s">
+        <v>415</v>
+      </c>
+      <c r="C91" s="11"/>
+      <c r="D91" s="11"/>
+      <c r="E91" s="11"/>
+      <c r="F91" s="11"/>
+      <c r="G91" s="11"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A92" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="B92" s="16" t="s">
+        <v>416</v>
+      </c>
+      <c r="C92" s="11"/>
+      <c r="D92" s="11"/>
+      <c r="E92" s="11"/>
+      <c r="F92" s="11"/>
+      <c r="G92" s="11"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A93" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="B93" s="16" t="s">
+        <v>417</v>
+      </c>
+      <c r="C93" s="11"/>
+      <c r="D93" s="11"/>
+      <c r="E93" s="11"/>
+      <c r="F93" s="11"/>
+      <c r="G93" s="11"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A94" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="B94" s="16" t="s">
+        <v>418</v>
+      </c>
+      <c r="C94" s="11"/>
+      <c r="D94" s="11"/>
+      <c r="E94" s="11"/>
+      <c r="F94" s="11"/>
+      <c r="G94" s="11"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A95" s="13" t="s">
+        <v>345</v>
+      </c>
+      <c r="B95" s="16" t="s">
+        <v>419</v>
+      </c>
+      <c r="C95" s="11"/>
+      <c r="D95" s="11"/>
+      <c r="E95" s="11"/>
+      <c r="F95" s="11"/>
+      <c r="G95" s="11"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A96" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="B96" s="16" t="s">
+        <v>420</v>
+      </c>
+      <c r="C96" s="11"/>
+      <c r="D96" s="11"/>
+      <c r="E96" s="11"/>
+      <c r="F96" s="11"/>
+      <c r="G96" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Time vector extraction hack
Extracting a data time range from a 'parameters' page in a databook no longer works if that page ceases to exist, i.e. because all parameters have been associated with custom data pages.
However, establishing a temporary hack for this allows the TB code to run with all parameters defined in the framework file.
Any of the following would be useful to work on for future commits; set up a hidden metadata databook page to store values like the year range, flesh out the TB databook to run an epi model, reinstall junction functionality, set up interpopulation dynamics.
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4333B03-4EBA-47F3-A0F9-830A6424E3D9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1275155F-C1F3-4FE4-9F9B-5687C174B3C0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Custom Databook Pages" sheetId="7" r:id="rId1"/>
@@ -640,7 +640,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="476">
   <si>
     <t>Code Name</t>
   </si>
@@ -2519,7 +2519,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3483,8 +3483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AO41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AJ22" sqref="AJ22:AK22"/>
     </sheetView>
   </sheetViews>
@@ -5753,10 +5753,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FC8421-05BA-4BE1-A1F1-3F12A4E7E369}">
   <dimension ref="A1:G96"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="C43" sqref="C43:C50"/>
+      <selection pane="topRight" activeCell="F75" sqref="F75:F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6637,7 +6637,9 @@
       <c r="C51" s="11"/>
       <c r="D51" s="11"/>
       <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
+      <c r="F51" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.45">
@@ -6650,7 +6652,9 @@
       <c r="C52" s="11"/>
       <c r="D52" s="11"/>
       <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
+      <c r="F52" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G52" s="11"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.45">
@@ -6663,7 +6667,9 @@
       <c r="C53" s="11"/>
       <c r="D53" s="11"/>
       <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
+      <c r="F53" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G53" s="11"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.45">
@@ -6676,7 +6682,9 @@
       <c r="C54" s="11"/>
       <c r="D54" s="11"/>
       <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
+      <c r="F54" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G54" s="11"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.45">
@@ -6689,7 +6697,9 @@
       <c r="C55" s="11"/>
       <c r="D55" s="11"/>
       <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
+      <c r="F55" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G55" s="11"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.45">
@@ -6702,7 +6712,9 @@
       <c r="C56" s="11"/>
       <c r="D56" s="11"/>
       <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
+      <c r="F56" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G56" s="11"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.45">
@@ -6715,7 +6727,9 @@
       <c r="C57" s="11"/>
       <c r="D57" s="11"/>
       <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
+      <c r="F57" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G57" s="11"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.45">
@@ -6728,7 +6742,9 @@
       <c r="C58" s="11"/>
       <c r="D58" s="11"/>
       <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
+      <c r="F58" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G58" s="11"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.45">
@@ -6741,7 +6757,9 @@
       <c r="C59" s="11"/>
       <c r="D59" s="11"/>
       <c r="E59" s="11"/>
-      <c r="F59" s="11"/>
+      <c r="F59" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G59" s="11"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.45">
@@ -6754,7 +6772,9 @@
       <c r="C60" s="11"/>
       <c r="D60" s="11"/>
       <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
+      <c r="F60" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.45">
@@ -6767,7 +6787,9 @@
       <c r="C61" s="11"/>
       <c r="D61" s="11"/>
       <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
+      <c r="F61" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G61" s="11"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.45">
@@ -6780,7 +6802,9 @@
       <c r="C62" s="11"/>
       <c r="D62" s="11"/>
       <c r="E62" s="11"/>
-      <c r="F62" s="11"/>
+      <c r="F62" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G62" s="11"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.45">
@@ -6793,7 +6817,9 @@
       <c r="C63" s="11"/>
       <c r="D63" s="11"/>
       <c r="E63" s="11"/>
-      <c r="F63" s="11"/>
+      <c r="F63" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G63" s="11"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.45">
@@ -6806,7 +6832,9 @@
       <c r="C64" s="11"/>
       <c r="D64" s="11"/>
       <c r="E64" s="11"/>
-      <c r="F64" s="11"/>
+      <c r="F64" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G64" s="11"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.45">
@@ -6819,7 +6847,9 @@
       <c r="C65" s="11"/>
       <c r="D65" s="11"/>
       <c r="E65" s="11"/>
-      <c r="F65" s="11"/>
+      <c r="F65" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G65" s="11"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.45">
@@ -6832,7 +6862,9 @@
       <c r="C66" s="11"/>
       <c r="D66" s="11"/>
       <c r="E66" s="11"/>
-      <c r="F66" s="11"/>
+      <c r="F66" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G66" s="11"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.45">
@@ -6845,7 +6877,9 @@
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
       <c r="E67" s="11"/>
-      <c r="F67" s="11"/>
+      <c r="F67" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G67" s="11"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.45">
@@ -6858,7 +6892,9 @@
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
       <c r="E68" s="11"/>
-      <c r="F68" s="11"/>
+      <c r="F68" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G68" s="11"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.45">
@@ -6871,7 +6907,9 @@
       <c r="C69" s="11"/>
       <c r="D69" s="11"/>
       <c r="E69" s="11"/>
-      <c r="F69" s="11"/>
+      <c r="F69" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G69" s="11"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.45">
@@ -6884,7 +6922,9 @@
       <c r="C70" s="11"/>
       <c r="D70" s="11"/>
       <c r="E70" s="11"/>
-      <c r="F70" s="11"/>
+      <c r="F70" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G70" s="11"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.45">
@@ -6897,7 +6937,9 @@
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
       <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
+      <c r="F71" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G71" s="11"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.45">
@@ -6910,7 +6952,9 @@
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
       <c r="E72" s="11"/>
-      <c r="F72" s="11"/>
+      <c r="F72" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G72" s="11"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.45">
@@ -6923,7 +6967,9 @@
       <c r="C73" s="11"/>
       <c r="D73" s="11"/>
       <c r="E73" s="11"/>
-      <c r="F73" s="11"/>
+      <c r="F73" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G73" s="11"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.45">
@@ -6936,7 +6982,9 @@
       <c r="C74" s="11"/>
       <c r="D74" s="11"/>
       <c r="E74" s="11"/>
-      <c r="F74" s="11"/>
+      <c r="F74" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="G74" s="11"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.45">
@@ -6949,7 +6997,9 @@
       <c r="C75" s="11"/>
       <c r="D75" s="11"/>
       <c r="E75" s="11"/>
-      <c r="F75" s="11"/>
+      <c r="F75" s="11" t="s">
+        <v>108</v>
+      </c>
       <c r="G75" s="11"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.45">
@@ -6962,7 +7012,9 @@
       <c r="C76" s="11"/>
       <c r="D76" s="11"/>
       <c r="E76" s="11"/>
-      <c r="F76" s="11"/>
+      <c r="F76" s="11" t="s">
+        <v>108</v>
+      </c>
       <c r="G76" s="11"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.45">
@@ -6975,7 +7027,9 @@
       <c r="C77" s="11"/>
       <c r="D77" s="11"/>
       <c r="E77" s="11"/>
-      <c r="F77" s="11"/>
+      <c r="F77" s="11" t="s">
+        <v>108</v>
+      </c>
       <c r="G77" s="11"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.45">
@@ -6988,7 +7042,9 @@
       <c r="C78" s="11"/>
       <c r="D78" s="11"/>
       <c r="E78" s="11"/>
-      <c r="F78" s="11"/>
+      <c r="F78" s="11" t="s">
+        <v>108</v>
+      </c>
       <c r="G78" s="11"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.45">
@@ -7001,7 +7057,9 @@
       <c r="C79" s="11"/>
       <c r="D79" s="11"/>
       <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
+      <c r="F79" s="11" t="s">
+        <v>108</v>
+      </c>
       <c r="G79" s="11"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.45">
@@ -7014,7 +7072,9 @@
       <c r="C80" s="11"/>
       <c r="D80" s="11"/>
       <c r="E80" s="11"/>
-      <c r="F80" s="11"/>
+      <c r="F80" s="11" t="s">
+        <v>108</v>
+      </c>
       <c r="G80" s="11"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.45">
@@ -7027,7 +7087,9 @@
       <c r="C81" s="11"/>
       <c r="D81" s="11"/>
       <c r="E81" s="11"/>
-      <c r="F81" s="11"/>
+      <c r="F81" s="11" t="s">
+        <v>108</v>
+      </c>
       <c r="G81" s="11"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.45">
@@ -7040,7 +7102,9 @@
       <c r="C82" s="11"/>
       <c r="D82" s="11"/>
       <c r="E82" s="11"/>
-      <c r="F82" s="11"/>
+      <c r="F82" s="11" t="s">
+        <v>108</v>
+      </c>
       <c r="G82" s="11"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.45">
@@ -7053,7 +7117,9 @@
       <c r="C83" s="11"/>
       <c r="D83" s="11"/>
       <c r="E83" s="11"/>
-      <c r="F83" s="11"/>
+      <c r="F83" s="11" t="s">
+        <v>108</v>
+      </c>
       <c r="G83" s="11"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.45">
@@ -7066,7 +7132,9 @@
       <c r="C84" s="11"/>
       <c r="D84" s="11"/>
       <c r="E84" s="11"/>
-      <c r="F84" s="11"/>
+      <c r="F84" s="11" t="s">
+        <v>108</v>
+      </c>
       <c r="G84" s="11"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.45">
@@ -7079,7 +7147,9 @@
       <c r="C85" s="11"/>
       <c r="D85" s="11"/>
       <c r="E85" s="11"/>
-      <c r="F85" s="11"/>
+      <c r="F85" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="G85" s="11"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.45">
@@ -7092,7 +7162,9 @@
       <c r="C86" s="11"/>
       <c r="D86" s="11"/>
       <c r="E86" s="11"/>
-      <c r="F86" s="11"/>
+      <c r="F86" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="G86" s="11"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.45">
@@ -7105,7 +7177,9 @@
       <c r="C87" s="11"/>
       <c r="D87" s="11"/>
       <c r="E87" s="11"/>
-      <c r="F87" s="11"/>
+      <c r="F87" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="G87" s="11"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.45">
@@ -7118,7 +7192,9 @@
       <c r="C88" s="11"/>
       <c r="D88" s="11"/>
       <c r="E88" s="11"/>
-      <c r="F88" s="11"/>
+      <c r="F88" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="G88" s="11"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.45">
@@ -7131,7 +7207,9 @@
       <c r="C89" s="11"/>
       <c r="D89" s="11"/>
       <c r="E89" s="11"/>
-      <c r="F89" s="11"/>
+      <c r="F89" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="G89" s="11"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.45">
@@ -7144,7 +7222,9 @@
       <c r="C90" s="11"/>
       <c r="D90" s="11"/>
       <c r="E90" s="11"/>
-      <c r="F90" s="11"/>
+      <c r="F90" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="G90" s="11"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.45">
@@ -7157,7 +7237,9 @@
       <c r="C91" s="11"/>
       <c r="D91" s="11"/>
       <c r="E91" s="11"/>
-      <c r="F91" s="11"/>
+      <c r="F91" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="G91" s="11"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.45">
@@ -7170,7 +7252,9 @@
       <c r="C92" s="11"/>
       <c r="D92" s="11"/>
       <c r="E92" s="11"/>
-      <c r="F92" s="11"/>
+      <c r="F92" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="G92" s="11"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.45">
@@ -7183,7 +7267,9 @@
       <c r="C93" s="11"/>
       <c r="D93" s="11"/>
       <c r="E93" s="11"/>
-      <c r="F93" s="11"/>
+      <c r="F93" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="G93" s="11"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.45">
@@ -7196,7 +7282,9 @@
       <c r="C94" s="11"/>
       <c r="D94" s="11"/>
       <c r="E94" s="11"/>
-      <c r="F94" s="11"/>
+      <c r="F94" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="G94" s="11"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.45">
@@ -7209,7 +7297,9 @@
       <c r="C95" s="11"/>
       <c r="D95" s="11"/>
       <c r="E95" s="11"/>
-      <c r="F95" s="11"/>
+      <c r="F95" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="G95" s="11"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.45">
@@ -7222,7 +7312,9 @@
       <c r="C96" s="11"/>
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
-      <c r="F96" s="11"/>
+      <c r="F96" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="G96" s="11"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TB databook given fake values from SA
Gauteng app values have been transferred across to the TB databook.
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1275155F-C1F3-4FE4-9F9B-5687C174B3C0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242F3167-4165-4EC9-BF22-04297819BDDA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1788,9 +1788,6 @@
     <t>MDR-SP treatment abandonment rate</t>
   </si>
   <si>
-    <t>MDR-SPtreatment success rate</t>
-  </si>
-  <si>
     <t>XDR-SP diagnosis rate</t>
   </si>
   <si>
@@ -2068,6 +2065,9 @@
   </si>
   <si>
     <t>proportion</t>
+  </si>
+  <si>
+    <t>MDR-SP treatment success rate</t>
   </si>
 </sst>
 </file>
@@ -2626,8 +2626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31:F32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2709,7 +2709,7 @@
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="11" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
@@ -2751,7 +2751,7 @@
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="11" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
@@ -2793,7 +2793,7 @@
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="11" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
@@ -2969,7 +2969,7 @@
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="11" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
@@ -3036,7 +3036,7 @@
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="11" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
@@ -3103,7 +3103,7 @@
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="11" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.45">
@@ -3193,7 +3193,7 @@
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="11" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.45">
@@ -3260,7 +3260,7 @@
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="11" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.45">
@@ -3327,7 +3327,7 @@
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="11" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.45">
@@ -3348,7 +3348,7 @@
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="11" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.45">
@@ -4331,7 +4331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D29B4020-084C-4F00-B628-93D126F8BCA7}">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -5753,10 +5753,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FC8421-05BA-4BE1-A1F1-3F12A4E7E369}">
   <dimension ref="A1:G96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="F75" sqref="F75:F84"/>
+      <selection pane="topRight" activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5802,7 +5802,7 @@
         <v>275</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
@@ -5834,7 +5834,7 @@
         <v>278</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
@@ -5875,10 +5875,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -5890,10 +5890,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
@@ -5905,10 +5905,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -5926,11 +5926,11 @@
         <v>349</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="11">
@@ -5945,11 +5945,11 @@
         <v>350</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="11" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="11">
@@ -5964,11 +5964,11 @@
         <v>351</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="11" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="11">
@@ -5983,11 +5983,11 @@
         <v>352</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="11">
@@ -6002,11 +6002,11 @@
         <v>353</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="11" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="11">
@@ -6021,11 +6021,11 @@
         <v>354</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="11" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="11">
@@ -6034,10 +6034,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -6049,10 +6049,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
@@ -6064,10 +6064,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="11" t="s">
+        <v>432</v>
+      </c>
+      <c r="B18" s="14" t="s">
         <v>433</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>434</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -6085,11 +6085,11 @@
         <v>356</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="11" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F19" s="11"/>
       <c r="G19" s="11">
@@ -6104,11 +6104,11 @@
         <v>357</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="11" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="11">
@@ -6123,11 +6123,11 @@
         <v>358</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="11" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="11">
@@ -6142,11 +6142,11 @@
         <v>359</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="11" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11">
@@ -6161,11 +6161,11 @@
         <v>360</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="11" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="11">
@@ -6180,11 +6180,11 @@
         <v>361</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="11" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F24" s="11"/>
       <c r="G24" s="11">
@@ -6193,10 +6193,10 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="13" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
@@ -6208,10 +6208,10 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="13" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
@@ -6223,10 +6223,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="13" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
@@ -6238,10 +6238,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="13" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
@@ -6253,10 +6253,10 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="17" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
@@ -6268,10 +6268,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="17" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
@@ -6283,15 +6283,15 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="13" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
       <c r="E31" s="13" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F31" s="11"/>
       <c r="G31" s="11">
@@ -6300,15 +6300,15 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="13" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
       <c r="E32" s="13" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F32" s="11"/>
       <c r="G32" s="11">
@@ -6317,15 +6317,15 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="13" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
       <c r="E33" s="11" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F33" s="11"/>
       <c r="G33" s="11">
@@ -6334,15 +6334,15 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="13" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
       <c r="E34" s="13" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F34" s="11"/>
       <c r="G34" s="11">
@@ -6351,15 +6351,15 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="13" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
       <c r="E35" s="13" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F35" s="11"/>
       <c r="G35" s="11">
@@ -6368,15 +6368,15 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="13" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
       <c r="E36" s="11" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F36" s="11"/>
       <c r="G36" s="11">
@@ -6385,15 +6385,15 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="13" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
       <c r="E37" s="11" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F37" s="11"/>
       <c r="G37" s="11">
@@ -6402,15 +6402,15 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="13" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
       <c r="E38" s="13" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F38" s="11"/>
       <c r="G38" s="11">
@@ -6425,11 +6425,11 @@
         <v>364</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D39" s="11"/>
       <c r="E39" s="11" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F39" s="11"/>
       <c r="G39" s="11">
@@ -6444,11 +6444,11 @@
         <v>363</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="11" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F40" s="11"/>
       <c r="G40" s="11">
@@ -6463,11 +6463,11 @@
         <v>365</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="11" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F41" s="11"/>
       <c r="G41" s="11">
@@ -6482,7 +6482,7 @@
         <v>366</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
@@ -6499,7 +6499,7 @@
         <v>367</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D43" s="11"/>
       <c r="E43" s="11"/>
@@ -6516,7 +6516,7 @@
         <v>368</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D44" s="11"/>
       <c r="E44" s="11"/>
@@ -6533,7 +6533,7 @@
         <v>369</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D45" s="11"/>
       <c r="E45" s="11"/>
@@ -6550,7 +6550,7 @@
         <v>370</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D46" s="11"/>
       <c r="E46" s="11"/>
@@ -6567,7 +6567,7 @@
         <v>371</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>
@@ -6584,7 +6584,7 @@
         <v>372</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
@@ -6601,7 +6601,7 @@
         <v>373</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D49" s="11"/>
       <c r="E49" s="11"/>
@@ -6618,7 +6618,7 @@
         <v>374</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D50" s="11"/>
       <c r="E50" s="11"/>
@@ -6737,7 +6737,7 @@
         <v>327</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>382</v>
+        <v>475</v>
       </c>
       <c r="C58" s="11"/>
       <c r="D58" s="11"/>
@@ -6752,7 +6752,7 @@
         <v>313</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C59" s="11"/>
       <c r="D59" s="11"/>
@@ -6767,7 +6767,7 @@
         <v>304</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C60" s="11"/>
       <c r="D60" s="11"/>
@@ -6782,7 +6782,7 @@
         <v>314</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C61" s="11"/>
       <c r="D61" s="11"/>
@@ -6797,7 +6797,7 @@
         <v>329</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C62" s="11"/>
       <c r="D62" s="11"/>
@@ -6812,7 +6812,7 @@
         <v>315</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C63" s="11"/>
       <c r="D63" s="11"/>
@@ -6827,7 +6827,7 @@
         <v>305</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C64" s="11"/>
       <c r="D64" s="11"/>
@@ -6842,7 +6842,7 @@
         <v>316</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C65" s="11"/>
       <c r="D65" s="11"/>
@@ -6857,7 +6857,7 @@
         <v>331</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C66" s="11"/>
       <c r="D66" s="11"/>
@@ -6872,7 +6872,7 @@
         <v>318</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
@@ -6887,7 +6887,7 @@
         <v>306</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
@@ -6902,7 +6902,7 @@
         <v>319</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C69" s="11"/>
       <c r="D69" s="11"/>
@@ -6917,7 +6917,7 @@
         <v>333</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C70" s="11"/>
       <c r="D70" s="11"/>
@@ -6932,7 +6932,7 @@
         <v>321</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
@@ -6947,7 +6947,7 @@
         <v>307</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
@@ -6962,7 +6962,7 @@
         <v>322</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C73" s="11"/>
       <c r="D73" s="11"/>
@@ -6977,7 +6977,7 @@
         <v>335</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C74" s="11"/>
       <c r="D74" s="11"/>
@@ -6992,7 +6992,7 @@
         <v>324</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C75" s="11"/>
       <c r="D75" s="11"/>
@@ -7007,7 +7007,7 @@
         <v>326</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C76" s="11"/>
       <c r="D76" s="11"/>
@@ -7022,7 +7022,7 @@
         <v>328</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C77" s="11"/>
       <c r="D77" s="11"/>
@@ -7037,7 +7037,7 @@
         <v>330</v>
       </c>
       <c r="B78" s="15" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C78" s="11"/>
       <c r="D78" s="11"/>
@@ -7052,7 +7052,7 @@
         <v>332</v>
       </c>
       <c r="B79" s="15" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C79" s="11"/>
       <c r="D79" s="11"/>
@@ -7067,7 +7067,7 @@
         <v>334</v>
       </c>
       <c r="B80" s="15" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C80" s="11"/>
       <c r="D80" s="11"/>
@@ -7082,7 +7082,7 @@
         <v>317</v>
       </c>
       <c r="B81" s="16" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C81" s="11"/>
       <c r="D81" s="11"/>
@@ -7097,7 +7097,7 @@
         <v>320</v>
       </c>
       <c r="B82" s="16" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C82" s="11"/>
       <c r="D82" s="11"/>
@@ -7112,7 +7112,7 @@
         <v>309</v>
       </c>
       <c r="B83" s="15" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C83" s="11"/>
       <c r="D83" s="11"/>
@@ -7127,7 +7127,7 @@
         <v>312</v>
       </c>
       <c r="B84" s="15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C84" s="11"/>
       <c r="D84" s="11"/>
@@ -7142,7 +7142,7 @@
         <v>336</v>
       </c>
       <c r="B85" s="16" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C85" s="11"/>
       <c r="D85" s="11"/>
@@ -7157,7 +7157,7 @@
         <v>338</v>
       </c>
       <c r="B86" s="16" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C86" s="11"/>
       <c r="D86" s="11"/>
@@ -7172,7 +7172,7 @@
         <v>340</v>
       </c>
       <c r="B87" s="16" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C87" s="11"/>
       <c r="D87" s="11"/>
@@ -7187,7 +7187,7 @@
         <v>337</v>
       </c>
       <c r="B88" s="16" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C88" s="11"/>
       <c r="D88" s="11"/>
@@ -7202,7 +7202,7 @@
         <v>339</v>
       </c>
       <c r="B89" s="16" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C89" s="11"/>
       <c r="D89" s="11"/>
@@ -7217,7 +7217,7 @@
         <v>341</v>
       </c>
       <c r="B90" s="16" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C90" s="11"/>
       <c r="D90" s="11"/>
@@ -7232,7 +7232,7 @@
         <v>342</v>
       </c>
       <c r="B91" s="16" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C91" s="11"/>
       <c r="D91" s="11"/>
@@ -7247,7 +7247,7 @@
         <v>344</v>
       </c>
       <c r="B92" s="16" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C92" s="11"/>
       <c r="D92" s="11"/>
@@ -7262,7 +7262,7 @@
         <v>346</v>
       </c>
       <c r="B93" s="16" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C93" s="11"/>
       <c r="D93" s="11"/>
@@ -7277,7 +7277,7 @@
         <v>343</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C94" s="11"/>
       <c r="D94" s="11"/>
@@ -7292,7 +7292,7 @@
         <v>345</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C95" s="11"/>
       <c r="D95" s="11"/>
@@ -7307,7 +7307,7 @@
         <v>347</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C96" s="11"/>
       <c r="D96" s="11"/>

</xml_diff>

<commit_message>
Create databook interactions page
A page for interactions is developed, where data can be provided via a connection matrix and TDVE table, just like with transfers.
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4A2F77-2A61-42B2-90CA-20866B40A710}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BDCCB8-DD77-4F1C-9A21-0D41B8AD9ECF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5680,10 +5680,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FC8421-05BA-4BE1-A1F1-3F12A4E7E369}">
   <dimension ref="A1:H98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="F41" sqref="F41"/>
+      <selection pane="topRight" activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6393,7 +6393,9 @@
         <v>464</v>
       </c>
       <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
+      <c r="D39" s="11">
+        <v>1</v>
+      </c>
       <c r="E39" s="13"/>
       <c r="F39" s="13" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
Framework interaction sheet set up
Interactions are now treated separately from parameters.
Also, although it may be a dangerous idea, configuration and workbook parsing warnings are now debug messages instead, treated as alerts to developers rather than user warnings.
This should reduce message spam upon import.
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BDCCB8-DD77-4F1C-9A21-0D41B8AD9ECF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F524D1-FAB5-4A51-9A96-CCAC2919B326}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Custom Databook Pages" sheetId="7" r:id="rId1"/>
     <sheet name="Compartments" sheetId="1" r:id="rId2"/>
     <sheet name="Transitions" sheetId="2" r:id="rId3"/>
     <sheet name="Characteristics" sheetId="8" r:id="rId4"/>
-    <sheet name="Parameters" sheetId="9" r:id="rId5"/>
+    <sheet name="Interactions" sheetId="10" r:id="rId5"/>
+    <sheet name="Parameters" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
@@ -454,6 +455,78 @@
     <author/>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{EB848832-138E-4807-B1A8-D7DF3DE2313D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column is for the 'code name' of a population interaction.
+These are special parameters that do not store values per population
+but per pairs of populations, specifically relating to how a source
+population interacts with a target population.
+Examples may include 'w_ctc', 'sex_partners', etc.
+The values that users provide for these matrix parameters, possibly
+time-dependent, can be propagated into population parameters by
+special functions such as 'srcpopavg'.
+Refer to documentation for more details.
+Note: A display name is a representative label that users interface
+with (e.g. in databooks and plots).
+It should be in title or sentence case.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{36D70CD2-777D-47CE-8B17-D057A2A5D8A6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column is for the 'display name' of a population interaction.
+These are special parameters that do not store values per population
+but per pairs of populations, specifically relating to how a source
+population interacts with a target population.
+Examples may include 'Contact weighting', 'Number of sex partners',
+etc.
+The values that users provide for these matrix parameters, possibly
+time-dependent, can be propagated into population parameters by
+special functions such as 'srcpopavg'.
+Refer to documentation for more details.
+Note: A display name is a representative label that users interface
+with (e.g. in databooks and plots).
+It should be in title or sentence case.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{5A3FB103-1D0A-4D71-88B5-B11FA384B5C6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column defines a 'default_value' attribute for a 'interpop' item.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{410F4B41-B661-437F-9D6C-2630D6921AC9}">
       <text>
         <r>
@@ -538,27 +611,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{C11C68D6-11FB-448A-8479-11977F3C8A42}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column is for tagging a parameter as an interaction.
-Interaction parameters are special; they store values not by
-population (i.e. in unary fashion) but by population pairs (i.e.
-in binary fashion).
-...
-Note: This tag is only enabled for a parameter by marking the
-corresponding cell 'y'.
-Anything else, including keeping the cell blank, disables the tag.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{727369DF-9454-4254-873C-A3C5C5E58366}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{727369DF-9454-4254-873C-A3C5C5E58366}">
       <text>
         <r>
           <rPr>
@@ -577,7 +630,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{3514B01A-966C-4E36-8CD8-B0E499FEDBF5}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{3514B01A-966C-4E36-8CD8-B0E499FEDBF5}">
       <text>
         <r>
           <rPr>
@@ -597,7 +650,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="465">
   <si>
     <t>Code Name</t>
   </si>
@@ -1985,16 +2038,13 @@
     <t>foi_in*lat_fac</t>
   </si>
   <si>
-    <t>srcpopsum(foi_out*alive*w_ctc)/srcpopsum(alive*w_ctc)</t>
-  </si>
-  <si>
     <t>w_ctc</t>
   </si>
   <si>
     <t>Preference weighting for one population interacting with another</t>
   </si>
   <si>
-    <t>Is Interaction</t>
+    <t>srcpopavg(foi_out,alive,w_ctc)</t>
   </si>
 </sst>
 </file>
@@ -5677,11 +5727,55 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6594BDD-62B5-4F98-B885-93E43B330298}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="10.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.9296875" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.06640625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>463</v>
+      </c>
+      <c r="C2" s="11">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FC8421-05BA-4BE1-A1F1-3F12A4E7E369}">
-  <dimension ref="A1:H98"/>
+  <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
       <selection pane="topRight" activeCell="E39" sqref="E39"/>
     </sheetView>
@@ -5693,13 +5787,12 @@
     <col min="3" max="3" width="9.265625" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.73046875" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="61" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.46484375" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.86328125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.06640625" style="10"/>
+    <col min="6" max="6" width="13" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.06640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -5716,16 +5809,13 @@
         <v>12</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>465</v>
+        <v>96</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="H1" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>255</v>
       </c>
@@ -5737,13 +5827,12 @@
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11" t="s">
+      <c r="F2" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="H2" s="11"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>258</v>
       </c>
@@ -5753,13 +5842,12 @@
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11" t="s">
+      <c r="F3" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="H3" s="11"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>256</v>
       </c>
@@ -5771,13 +5859,12 @@
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11" t="s">
+      <c r="F4" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="11"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>257</v>
       </c>
@@ -5787,13 +5874,12 @@
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11" t="s">
+      <c r="F5" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="H5" s="11"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
         <v>263</v>
       </c>
@@ -5803,13 +5889,12 @@
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="13" t="s">
+      <c r="F6" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="H6" s="11"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>405</v>
       </c>
@@ -5819,13 +5904,12 @@
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="13" t="s">
+      <c r="F7" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="H7" s="11"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
         <v>406</v>
       </c>
@@ -5835,13 +5919,12 @@
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="13" t="s">
+      <c r="F8" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="H8" s="11"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
         <v>407</v>
       </c>
@@ -5851,13 +5934,12 @@
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="13" t="s">
+      <c r="F9" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="H9" s="11"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
         <v>265</v>
       </c>
@@ -5872,12 +5954,11 @@
         <v>405</v>
       </c>
       <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G10" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="11" t="s">
         <v>267</v>
       </c>
@@ -5892,12 +5973,11 @@
         <v>406</v>
       </c>
       <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G11" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="11" t="s">
         <v>268</v>
       </c>
@@ -5912,12 +5992,11 @@
         <v>407</v>
       </c>
       <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G12" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="11" t="s">
         <v>270</v>
       </c>
@@ -5932,12 +6011,11 @@
         <v>405</v>
       </c>
       <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G13" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="11" t="s">
         <v>271</v>
       </c>
@@ -5952,12 +6030,11 @@
         <v>406</v>
       </c>
       <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G14" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="11" t="s">
         <v>272</v>
       </c>
@@ -5972,12 +6049,11 @@
         <v>407</v>
       </c>
       <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G15" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
         <v>412</v>
       </c>
@@ -5987,13 +6063,12 @@
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="13" t="s">
+      <c r="F16" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="H16" s="11"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
         <v>413</v>
       </c>
@@ -6003,13 +6078,12 @@
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="13" t="s">
+      <c r="F17" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="H17" s="11"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="11" t="s">
         <v>416</v>
       </c>
@@ -6019,13 +6093,12 @@
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="13" t="s">
+      <c r="F18" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="H18" s="11"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="13" t="s">
         <v>266</v>
       </c>
@@ -6040,12 +6113,11 @@
         <v>418</v>
       </c>
       <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G19" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="13" t="s">
         <v>273</v>
       </c>
@@ -6060,12 +6132,11 @@
         <v>418</v>
       </c>
       <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G20" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="13" t="s">
         <v>269</v>
       </c>
@@ -6080,12 +6151,11 @@
         <v>419</v>
       </c>
       <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G21" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="13" t="s">
         <v>275</v>
       </c>
@@ -6100,12 +6170,11 @@
         <v>419</v>
       </c>
       <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G22" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="13" t="s">
         <v>274</v>
       </c>
@@ -6120,12 +6189,11 @@
         <v>413</v>
       </c>
       <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G23" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="13" t="s">
         <v>276</v>
       </c>
@@ -6140,12 +6208,11 @@
         <v>413</v>
       </c>
       <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G24" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="13" t="s">
         <v>426</v>
       </c>
@@ -6155,13 +6222,12 @@
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11" t="s">
+      <c r="F25" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="H25" s="11"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G25" s="11"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="13" t="s">
         <v>427</v>
       </c>
@@ -6171,13 +6237,12 @@
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11" t="s">
+      <c r="F26" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="H26" s="11"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G26" s="11"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="13" t="s">
         <v>420</v>
       </c>
@@ -6187,13 +6252,12 @@
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11" t="s">
+      <c r="F27" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="H27" s="11"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G27" s="11"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="13" t="s">
         <v>428</v>
       </c>
@@ -6203,13 +6267,12 @@
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11" t="s">
+      <c r="F28" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="H28" s="11"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G28" s="11"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="17" t="s">
         <v>429</v>
       </c>
@@ -6219,13 +6282,12 @@
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11" t="s">
+      <c r="F29" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="H29" s="11"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G29" s="11"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="17" t="s">
         <v>430</v>
       </c>
@@ -6235,13 +6297,12 @@
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11" t="s">
+      <c r="F30" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="H30" s="11"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G30" s="11"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="13" t="s">
         <v>421</v>
       </c>
@@ -6253,13 +6314,12 @@
       <c r="E31" s="13" t="s">
         <v>449</v>
       </c>
-      <c r="F31" s="13"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F31" s="11"/>
+      <c r="G31" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="13" t="s">
         <v>422</v>
       </c>
@@ -6271,13 +6331,12 @@
       <c r="E32" s="13" t="s">
         <v>450</v>
       </c>
-      <c r="F32" s="13"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F32" s="11"/>
+      <c r="G32" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="13" t="s">
         <v>423</v>
       </c>
@@ -6290,12 +6349,11 @@
         <v>453</v>
       </c>
       <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G33" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="13" t="s">
         <v>424</v>
       </c>
@@ -6307,13 +6365,12 @@
       <c r="E34" s="13" t="s">
         <v>452</v>
       </c>
-      <c r="F34" s="13"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F34" s="11"/>
+      <c r="G34" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="13" t="s">
         <v>425</v>
       </c>
@@ -6325,13 +6382,12 @@
       <c r="E35" s="13" t="s">
         <v>451</v>
       </c>
-      <c r="F35" s="13"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F35" s="11"/>
+      <c r="G35" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="13" t="s">
         <v>442</v>
       </c>
@@ -6344,12 +6400,11 @@
         <v>446</v>
       </c>
       <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G36" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="13" t="s">
         <v>443</v>
       </c>
@@ -6362,12 +6417,11 @@
         <v>447</v>
       </c>
       <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G37" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="13" t="s">
         <v>456</v>
       </c>
@@ -6379,1005 +6433,927 @@
       <c r="E38" s="13" t="s">
         <v>448</v>
       </c>
-      <c r="F38" s="13"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F38" s="11"/>
+      <c r="G38" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="13" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="B39" s="14" t="s">
+        <v>459</v>
+      </c>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="13" t="s">
         <v>464</v>
       </c>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11">
-        <v>1</v>
-      </c>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A40" s="13" t="s">
+      <c r="F39" s="11"/>
+      <c r="G39" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A40" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>411</v>
+      </c>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11" t="s">
         <v>458</v>
       </c>
-      <c r="B40" s="14" t="s">
-        <v>459</v>
-      </c>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="13" t="s">
-        <v>462</v>
-      </c>
-      <c r="F40" s="13"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F40" s="11"/>
+      <c r="G40" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="11" t="s">
-        <v>264</v>
+        <v>339</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C41" s="11" t="s">
         <v>411</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="11" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G41" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="11" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C42" s="11" t="s">
         <v>411</v>
       </c>
       <c r="D42" s="11"/>
       <c r="E42" s="11" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G42" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="11" t="s">
-        <v>346</v>
+        <v>307</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C43" s="11" t="s">
         <v>411</v>
       </c>
       <c r="D43" s="11"/>
-      <c r="E43" s="11" t="s">
-        <v>461</v>
-      </c>
-      <c r="F43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11" t="s">
+        <v>84</v>
+      </c>
       <c r="G43" s="11"/>
-      <c r="H43" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A44" s="11" t="s">
-        <v>307</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>350</v>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A44" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>351</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>411</v>
+        <v>454</v>
       </c>
       <c r="D44" s="11"/>
       <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="H44" s="11"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F44" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="G44" s="11"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" s="13" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>454</v>
       </c>
       <c r="D45" s="11"/>
       <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11" t="s">
+      <c r="F45" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="H45" s="11"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G45" s="11"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="13" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>454</v>
       </c>
       <c r="D46" s="11"/>
       <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11" t="s">
+      <c r="F46" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="H46" s="11"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G46" s="11"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="13" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C47" s="11" t="s">
         <v>454</v>
       </c>
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11" t="s">
+      <c r="F47" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="H47" s="11"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G47" s="11"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="13" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C48" s="11" t="s">
         <v>454</v>
       </c>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11" t="s">
+      <c r="F48" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="H48" s="11"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G48" s="11"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="13" t="s">
-        <v>281</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>355</v>
+        <v>282</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>356</v>
       </c>
       <c r="C49" s="11" t="s">
         <v>454</v>
       </c>
       <c r="D49" s="11"/>
       <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11" t="s">
+      <c r="F49" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="H49" s="11"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G49" s="11"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="13" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C50" s="11" t="s">
         <v>454</v>
       </c>
       <c r="D50" s="11"/>
       <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11" t="s">
+      <c r="F50" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="H50" s="11"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G50" s="11"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="13" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C51" s="11" t="s">
         <v>454</v>
       </c>
       <c r="D51" s="11"/>
       <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11" t="s">
+      <c r="F51" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="H51" s="11"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G51" s="11"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="B52" s="16" t="s">
-        <v>358</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>454</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>359</v>
+      </c>
+      <c r="C52" s="11"/>
       <c r="D52" s="11"/>
       <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="H52" s="11"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F52" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="G52" s="11"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="13" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C53" s="11"/>
       <c r="D53" s="11"/>
       <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
-      <c r="G53" s="11" t="s">
+      <c r="F53" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H53" s="11"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G53" s="11"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="13" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C54" s="11"/>
       <c r="D54" s="11"/>
       <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11" t="s">
+      <c r="F54" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H54" s="11"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G54" s="11"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="13" t="s">
-        <v>292</v>
+        <v>309</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C55" s="11"/>
       <c r="D55" s="11"/>
       <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11" t="s">
+      <c r="F55" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H55" s="11"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G55" s="11"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="13" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C56" s="11"/>
       <c r="D56" s="11"/>
       <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
-      <c r="G56" s="11" t="s">
+      <c r="F56" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H56" s="11"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G56" s="11"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="13" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C57" s="11"/>
       <c r="D57" s="11"/>
       <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
-      <c r="G57" s="11" t="s">
+      <c r="F57" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H57" s="11"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G57" s="11"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="13" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C58" s="11"/>
       <c r="D58" s="11"/>
       <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
-      <c r="G58" s="11" t="s">
+      <c r="F58" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H58" s="11"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G58" s="11"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="13" t="s">
-        <v>295</v>
+        <v>311</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>365</v>
+        <v>455</v>
       </c>
       <c r="C59" s="11"/>
       <c r="D59" s="11"/>
       <c r="E59" s="11"/>
-      <c r="F59" s="11"/>
-      <c r="G59" s="11" t="s">
+      <c r="F59" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H59" s="11"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G59" s="11"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="13" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>455</v>
+        <v>366</v>
       </c>
       <c r="C60" s="11"/>
       <c r="D60" s="11"/>
       <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
-      <c r="G60" s="11" t="s">
+      <c r="F60" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H60" s="11"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G60" s="11"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="13" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C61" s="11"/>
       <c r="D61" s="11"/>
       <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11" t="s">
+      <c r="F61" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H61" s="11"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G61" s="11"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="13" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C62" s="11"/>
       <c r="D62" s="11"/>
       <c r="E62" s="11"/>
-      <c r="F62" s="11"/>
-      <c r="G62" s="11" t="s">
+      <c r="F62" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H62" s="11"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G62" s="11"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="13" t="s">
-        <v>298</v>
+        <v>313</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C63" s="11"/>
       <c r="D63" s="11"/>
       <c r="E63" s="11"/>
-      <c r="F63" s="11"/>
-      <c r="G63" s="11" t="s">
+      <c r="F63" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H63" s="11"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G63" s="11"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="13" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C64" s="11"/>
       <c r="D64" s="11"/>
       <c r="E64" s="11"/>
-      <c r="F64" s="11"/>
-      <c r="G64" s="11" t="s">
+      <c r="F64" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H64" s="11"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G64" s="11"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A65" s="13" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C65" s="11"/>
       <c r="D65" s="11"/>
       <c r="E65" s="11"/>
-      <c r="F65" s="11"/>
-      <c r="G65" s="11" t="s">
+      <c r="F65" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H65" s="11"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G65" s="11"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A66" s="13" t="s">
-        <v>289</v>
+        <v>300</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C66" s="11"/>
       <c r="D66" s="11"/>
       <c r="E66" s="11"/>
-      <c r="F66" s="11"/>
-      <c r="G66" s="11" t="s">
+      <c r="F66" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H66" s="11"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G66" s="11"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67" s="13" t="s">
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
       <c r="E67" s="11"/>
-      <c r="F67" s="11"/>
-      <c r="G67" s="11" t="s">
+      <c r="F67" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H67" s="11"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G67" s="11"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68" s="13" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
       <c r="E68" s="11"/>
-      <c r="F68" s="11"/>
-      <c r="G68" s="11" t="s">
+      <c r="F68" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H68" s="11"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G68" s="11"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A69" s="13" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C69" s="11"/>
       <c r="D69" s="11"/>
       <c r="E69" s="11"/>
-      <c r="F69" s="11"/>
-      <c r="G69" s="11" t="s">
+      <c r="F69" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H69" s="11"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G69" s="11"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A70" s="13" t="s">
-        <v>290</v>
+        <v>303</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C70" s="11"/>
       <c r="D70" s="11"/>
       <c r="E70" s="11"/>
-      <c r="F70" s="11"/>
-      <c r="G70" s="11" t="s">
+      <c r="F70" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H70" s="11"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G70" s="11"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71" s="13" t="s">
-        <v>303</v>
+        <v>317</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
       <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
-      <c r="G71" s="11" t="s">
+      <c r="F71" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H71" s="11"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G71" s="11"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" s="13" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
       <c r="E72" s="11"/>
-      <c r="F72" s="11"/>
-      <c r="G72" s="11" t="s">
+      <c r="F72" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H72" s="11"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G72" s="11"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73" s="13" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C73" s="11"/>
       <c r="D73" s="11"/>
       <c r="E73" s="11"/>
-      <c r="F73" s="11"/>
-      <c r="G73" s="11" t="s">
+      <c r="F73" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H73" s="11"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G73" s="11"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74" s="13" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C74" s="11"/>
       <c r="D74" s="11"/>
       <c r="E74" s="11"/>
-      <c r="F74" s="11"/>
-      <c r="G74" s="11" t="s">
+      <c r="F74" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H74" s="11"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G74" s="11"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A75" s="13" t="s">
-        <v>306</v>
+        <v>319</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C75" s="11"/>
       <c r="D75" s="11"/>
       <c r="E75" s="11"/>
-      <c r="F75" s="11"/>
-      <c r="G75" s="11" t="s">
+      <c r="F75" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="H75" s="11"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G75" s="11"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A76" s="13" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C76" s="11"/>
       <c r="D76" s="11"/>
       <c r="E76" s="11"/>
-      <c r="F76" s="11"/>
-      <c r="G76" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="H76" s="11"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F76" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G76" s="11"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A77" s="13" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C77" s="11"/>
       <c r="D77" s="11"/>
       <c r="E77" s="11"/>
-      <c r="F77" s="11"/>
-      <c r="G77" s="11" t="s">
+      <c r="F77" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="H77" s="11"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G77" s="11"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A78" s="13" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B78" s="15" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C78" s="11"/>
       <c r="D78" s="11"/>
       <c r="E78" s="11"/>
-      <c r="F78" s="11"/>
-      <c r="G78" s="11" t="s">
+      <c r="F78" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="H78" s="11"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G78" s="11"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A79" s="13" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B79" s="15" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C79" s="11"/>
       <c r="D79" s="11"/>
       <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
-      <c r="G79" s="11" t="s">
+      <c r="F79" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="H79" s="11"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G79" s="11"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A80" s="13" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B80" s="15" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C80" s="11"/>
       <c r="D80" s="11"/>
       <c r="E80" s="11"/>
-      <c r="F80" s="11"/>
-      <c r="G80" s="11" t="s">
+      <c r="F80" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="H80" s="11"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G80" s="11"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A81" s="13" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B81" s="15" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C81" s="11"/>
       <c r="D81" s="11"/>
       <c r="E81" s="11"/>
-      <c r="F81" s="11"/>
-      <c r="G81" s="11" t="s">
+      <c r="F81" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="H81" s="11"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G81" s="11"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A82" s="13" t="s">
-        <v>318</v>
-      </c>
-      <c r="B82" s="15" t="s">
-        <v>387</v>
+        <v>301</v>
+      </c>
+      <c r="B82" s="16" t="s">
+        <v>388</v>
       </c>
       <c r="C82" s="11"/>
       <c r="D82" s="11"/>
       <c r="E82" s="11"/>
-      <c r="F82" s="11"/>
-      <c r="G82" s="11" t="s">
+      <c r="F82" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="H82" s="11"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G82" s="11"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A83" s="13" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B83" s="16" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C83" s="11"/>
       <c r="D83" s="11"/>
       <c r="E83" s="11"/>
-      <c r="F83" s="11"/>
-      <c r="G83" s="11" t="s">
+      <c r="F83" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="H83" s="11"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G83" s="11"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A84" s="13" t="s">
-        <v>304</v>
-      </c>
-      <c r="B84" s="16" t="s">
-        <v>389</v>
+        <v>293</v>
+      </c>
+      <c r="B84" s="15" t="s">
+        <v>390</v>
       </c>
       <c r="C84" s="11"/>
       <c r="D84" s="11"/>
       <c r="E84" s="11"/>
-      <c r="F84" s="11"/>
-      <c r="G84" s="11" t="s">
+      <c r="F84" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="H84" s="11"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G84" s="11"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A85" s="13" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B85" s="15" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C85" s="11"/>
       <c r="D85" s="11"/>
       <c r="E85" s="11"/>
-      <c r="F85" s="11"/>
-      <c r="G85" s="11" t="s">
+      <c r="F85" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="H85" s="11"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G85" s="11"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A86" s="13" t="s">
-        <v>296</v>
-      </c>
-      <c r="B86" s="15" t="s">
-        <v>391</v>
+        <v>320</v>
+      </c>
+      <c r="B86" s="16" t="s">
+        <v>392</v>
       </c>
       <c r="C86" s="11"/>
       <c r="D86" s="11"/>
       <c r="E86" s="11"/>
-      <c r="F86" s="11"/>
-      <c r="G86" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="H86" s="11"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F86" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="G86" s="11"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A87" s="13" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B87" s="16" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C87" s="11"/>
       <c r="D87" s="11"/>
       <c r="E87" s="11"/>
-      <c r="F87" s="11"/>
-      <c r="G87" s="11" t="s">
+      <c r="F87" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="H87" s="11"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G87" s="11"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A88" s="13" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B88" s="16" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C88" s="11"/>
       <c r="D88" s="11"/>
       <c r="E88" s="11"/>
-      <c r="F88" s="11"/>
-      <c r="G88" s="11" t="s">
+      <c r="F88" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="H88" s="11"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G88" s="11"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A89" s="13" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B89" s="16" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C89" s="11"/>
       <c r="D89" s="11"/>
       <c r="E89" s="11"/>
-      <c r="F89" s="11"/>
-      <c r="G89" s="11" t="s">
+      <c r="F89" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="H89" s="11"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G89" s="11"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A90" s="13" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B90" s="16" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C90" s="11"/>
       <c r="D90" s="11"/>
       <c r="E90" s="11"/>
-      <c r="F90" s="11"/>
-      <c r="G90" s="11" t="s">
+      <c r="F90" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="H90" s="11"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G90" s="11"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A91" s="13" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B91" s="16" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C91" s="11"/>
       <c r="D91" s="11"/>
       <c r="E91" s="11"/>
-      <c r="F91" s="11"/>
-      <c r="G91" s="11" t="s">
+      <c r="F91" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="H91" s="11"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G91" s="11"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A92" s="13" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B92" s="16" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C92" s="11"/>
       <c r="D92" s="11"/>
       <c r="E92" s="11"/>
-      <c r="F92" s="11"/>
-      <c r="G92" s="11" t="s">
+      <c r="F92" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="H92" s="11"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G92" s="11"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A93" s="13" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B93" s="16" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C93" s="11"/>
       <c r="D93" s="11"/>
       <c r="E93" s="11"/>
-      <c r="F93" s="11"/>
-      <c r="G93" s="11" t="s">
+      <c r="F93" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="H93" s="11"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G93" s="11"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A94" s="13" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C94" s="11"/>
       <c r="D94" s="11"/>
       <c r="E94" s="11"/>
-      <c r="F94" s="11"/>
-      <c r="G94" s="11" t="s">
+      <c r="F94" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="H94" s="11"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G94" s="11"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A95" s="13" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C95" s="11"/>
       <c r="D95" s="11"/>
       <c r="E95" s="11"/>
-      <c r="F95" s="11"/>
-      <c r="G95" s="11" t="s">
+      <c r="F95" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="H95" s="11"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G95" s="11"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A96" s="13" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C96" s="11"/>
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
-      <c r="F96" s="11"/>
-      <c r="G96" s="11" t="s">
+      <c r="F96" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="H96" s="11"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G96" s="11"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A97" s="13" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B97" s="16" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C97" s="11"/>
       <c r="D97" s="11"/>
       <c r="E97" s="11"/>
-      <c r="F97" s="11"/>
-      <c r="G97" s="11" t="s">
+      <c r="F97" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="H97" s="11"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A98" s="13" t="s">
-        <v>331</v>
-      </c>
-      <c r="B98" s="16" t="s">
-        <v>403</v>
-      </c>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
-      <c r="E98" s="11"/>
-      <c r="F98" s="11"/>
-      <c r="G98" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="H98" s="11"/>
+      <c r="G97" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Reintroduce special rule in preliminary format
Needs proper testing on results, but this code appears to apply weighted averaging to parameters according to a characteristic and contact matrix.
Performance can certainly improve by preallocating time-dependent interaction arrays.
Nonetheless, this appears functional...
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F524D1-FAB5-4A51-9A96-CCAC2919B326}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40E3017-C866-4E8B-83C5-5119E8443240}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2044,7 +2044,7 @@
     <t>Preference weighting for one population interacting with another</t>
   </si>
   <si>
-    <t>srcpopavg(foi_out,alive,w_ctc)</t>
+    <t>SRC_POP_AVG(foi_out, alive, w_ctc)</t>
   </si>
 </sst>
 </file>
@@ -5731,7 +5731,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:XFD1048576"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5774,19 +5774,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FC8421-05BA-4BE1-A1F1-3F12A4E7E369}">
   <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="E39" sqref="E39"/>
+      <selection pane="topRight" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.265625" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.9296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.46484375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.59765625" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.265625" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.73046875" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62.06640625" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" style="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.86328125" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.06640625" style="10"/>

</xml_diff>

<commit_message>
Streamline performance of interactions
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\frameworks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40E3017-C866-4E8B-83C5-5119E8443240}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE85C0F0-486B-4703-8D15-FEAEF6BF2A8F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2044,7 +2044,7 @@
     <t>Preference weighting for one population interacting with another</t>
   </si>
   <si>
-    <t>SRC_POP_AVG(foi_out, alive, w_ctc)</t>
+    <t>SRC_POP_AVG(foi_out, w_ctc,alive)</t>
   </si>
 </sst>
 </file>
@@ -2499,13 +2499,13 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="25.73046875" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="9.06640625" style="3"/>
+    <col min="1" max="2" width="25.7109375" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>74</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>76</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>78</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>80</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>82</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>84</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>86</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>88</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>90</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>92</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>94</v>
       </c>
@@ -2607,19 +2607,19 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.06640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.9296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.86328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
@@ -2731,7 +2731,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>19</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>21</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>100</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>101</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>22</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>24</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>25</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>26</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>27</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>28</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>29</v>
       </c>
@@ -3016,7 +3016,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>30</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>31</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>32</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>33</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>34</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>35</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>36</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>37</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>38</v>
       </c>
@@ -3219,7 +3219,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>39</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>40</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>41</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>42</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>43</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>46</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>69</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>44</v>
       </c>
@@ -3398,7 +3398,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>45</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>71</v>
       </c>
@@ -3465,49 +3465,48 @@
       <selection pane="topRight" activeCell="AJ22" sqref="AJ22:AK22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.86328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.73046875" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.53125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.9296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.73046875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.46484375" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.3984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.19921875" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.59765625" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.46484375" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5" style="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6" style="11" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7" style="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.53125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.53125" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.53125" style="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.06640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.86328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.86328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.3984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8" style="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5" style="11" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="6" style="11" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7" style="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.53125" style="11" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.53125" style="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.53125" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.06640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.86328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.86328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.3984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.53125" style="11" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="2.9296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="4.86328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="3" style="11" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="4.85546875" style="11" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="8" style="11" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8.53125" style="11" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="5.796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="38" max="16384" width="9.06640625" style="11"/>
+    <col min="36" max="36" width="8.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="5.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="38" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="str">
         <f>Compartments!A2</f>
         <v>sus</v>
@@ -3652,7 +3651,7 @@
       <c r="AN1" s="12"/>
       <c r="AO1" s="12"/>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="str">
         <f>Compartments!A2</f>
         <v>sus</v>
@@ -3670,7 +3669,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="str">
         <f>Compartments!A3</f>
         <v>vac</v>
@@ -3685,7 +3684,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="str">
         <f>Compartments!A4</f>
         <v>lteu</v>
@@ -3706,7 +3705,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="str">
         <f>Compartments!A5</f>
         <v>ltet</v>
@@ -3724,7 +3723,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="str">
         <f>Compartments!A6</f>
         <v>ltlu</v>
@@ -3742,7 +3741,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="str">
         <f>Compartments!A7</f>
         <v>ltlt</v>
@@ -3760,7 +3759,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="str">
         <f>Compartments!A8</f>
         <v>ltr</v>
@@ -3775,7 +3774,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="str">
         <f>Compartments!A9</f>
         <v>ltex</v>
@@ -3793,7 +3792,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="str">
         <f>Compartments!A10</f>
         <v>ltlx</v>
@@ -3808,7 +3807,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="str">
         <f>Compartments!A11</f>
         <v>acj</v>
@@ -3820,7 +3819,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="str">
         <f>Compartments!A12</f>
         <v>spj</v>
@@ -3835,7 +3834,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="str">
         <f>Compartments!A13</f>
         <v>spdu</v>
@@ -3856,7 +3855,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="str">
         <f>Compartments!A14</f>
         <v>spdd</v>
@@ -3877,7 +3876,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="str">
         <f>Compartments!A15</f>
         <v>spdt</v>
@@ -3901,7 +3900,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="str">
         <f>Compartments!A16</f>
         <v>spmu</v>
@@ -3922,7 +3921,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="str">
         <f>Compartments!A17</f>
         <v>spmd</v>
@@ -3943,7 +3942,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="str">
         <f>Compartments!A18</f>
         <v>spmt</v>
@@ -3967,7 +3966,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="str">
         <f>Compartments!A19</f>
         <v>spxu</v>
@@ -3988,7 +3987,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="str">
         <f>Compartments!A20</f>
         <v>spxd</v>
@@ -4009,7 +4008,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="str">
         <f>Compartments!A21</f>
         <v>spxt</v>
@@ -4030,7 +4029,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="str">
         <f>Compartments!A22</f>
         <v>snj</v>
@@ -4045,7 +4044,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="str">
         <f>Compartments!A23</f>
         <v>sndu</v>
@@ -4066,7 +4065,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="str">
         <f>Compartments!A24</f>
         <v>sndd</v>
@@ -4087,7 +4086,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="str">
         <f>Compartments!A25</f>
         <v>sndt</v>
@@ -4111,7 +4110,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="str">
         <f>Compartments!A26</f>
         <v>snmu</v>
@@ -4132,7 +4131,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="str">
         <f>Compartments!A27</f>
         <v>snmd</v>
@@ -4153,7 +4152,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="str">
         <f>Compartments!A28</f>
         <v>snmt</v>
@@ -4177,7 +4176,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="str">
         <f>Compartments!A29</f>
         <v>snxu</v>
@@ -4198,7 +4197,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="str">
         <f>Compartments!A30</f>
         <v>snxd</v>
@@ -4219,7 +4218,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="str">
         <f>Compartments!A31</f>
         <v>snxt</v>
@@ -4240,7 +4239,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="str">
         <f>Compartments!A32</f>
         <v>acr</v>
@@ -4255,7 +4254,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>46</v>
       </c>
@@ -4263,7 +4262,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>69</v>
       </c>
@@ -4271,31 +4270,31 @@
         <v>256</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="12"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
     </row>
   </sheetData>
@@ -4312,21 +4311,21 @@
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.73046875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.9296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.19921875" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.53125" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.73046875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.86328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.06640625" style="3"/>
+    <col min="9" max="9" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4353,7 +4352,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>99</v>
       </c>
@@ -4372,7 +4371,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>102</v>
       </c>
@@ -4391,7 +4390,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>105</v>
       </c>
@@ -4410,7 +4409,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>106</v>
       </c>
@@ -4429,7 +4428,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>107</v>
       </c>
@@ -4448,7 +4447,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>116</v>
       </c>
@@ -4470,7 +4469,7 @@
       </c>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>117</v>
       </c>
@@ -4492,7 +4491,7 @@
       </c>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>118</v>
       </c>
@@ -4514,7 +4513,7 @@
       </c>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>119</v>
       </c>
@@ -4536,7 +4535,7 @@
       </c>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>120</v>
       </c>
@@ -4558,7 +4557,7 @@
       </c>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>121</v>
       </c>
@@ -4580,7 +4579,7 @@
       </c>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>248</v>
       </c>
@@ -4602,7 +4601,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>122</v>
       </c>
@@ -4624,7 +4623,7 @@
       </c>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>123</v>
       </c>
@@ -4646,7 +4645,7 @@
       </c>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>124</v>
       </c>
@@ -4668,7 +4667,7 @@
       </c>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>125</v>
       </c>
@@ -4690,7 +4689,7 @@
       </c>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>126</v>
       </c>
@@ -4712,7 +4711,7 @@
       </c>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>127</v>
       </c>
@@ -4734,7 +4733,7 @@
       </c>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>140</v>
       </c>
@@ -4756,7 +4755,7 @@
       </c>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>141</v>
       </c>
@@ -4778,7 +4777,7 @@
       </c>
       <c r="I21" s="11"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>147</v>
       </c>
@@ -4800,7 +4799,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>143</v>
       </c>
@@ -4822,7 +4821,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>144</v>
       </c>
@@ -4844,7 +4843,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>146</v>
       </c>
@@ -4863,7 +4862,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>142</v>
       </c>
@@ -4885,7 +4884,7 @@
       </c>
       <c r="I26" s="11"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>145</v>
       </c>
@@ -4907,7 +4906,7 @@
       </c>
       <c r="I27" s="7"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>157</v>
       </c>
@@ -4929,7 +4928,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>158</v>
       </c>
@@ -4951,7 +4950,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>159</v>
       </c>
@@ -4973,7 +4972,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>160</v>
       </c>
@@ -4995,7 +4994,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>161</v>
       </c>
@@ -5017,7 +5016,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>162</v>
       </c>
@@ -5039,7 +5038,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>169</v>
       </c>
@@ -5061,7 +5060,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>170</v>
       </c>
@@ -5083,7 +5082,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>171</v>
       </c>
@@ -5105,7 +5104,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>172</v>
       </c>
@@ -5127,7 +5126,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>173</v>
       </c>
@@ -5149,7 +5148,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>174</v>
       </c>
@@ -5171,7 +5170,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>181</v>
       </c>
@@ -5193,7 +5192,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>182</v>
       </c>
@@ -5215,7 +5214,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>183</v>
       </c>
@@ -5237,7 +5236,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>184</v>
       </c>
@@ -5259,7 +5258,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>185</v>
       </c>
@@ -5281,7 +5280,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>186</v>
       </c>
@@ -5303,7 +5302,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>187</v>
       </c>
@@ -5325,7 +5324,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>188</v>
       </c>
@@ -5347,7 +5346,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>189</v>
       </c>
@@ -5369,7 +5368,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>199</v>
       </c>
@@ -5391,7 +5390,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>200</v>
       </c>
@@ -5413,7 +5412,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>201</v>
       </c>
@@ -5435,7 +5434,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>202</v>
       </c>
@@ -5457,7 +5456,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>219</v>
       </c>
@@ -5479,7 +5478,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>220</v>
       </c>
@@ -5501,7 +5500,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>221</v>
       </c>
@@ -5523,7 +5522,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>222</v>
       </c>
@@ -5545,7 +5544,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>223</v>
       </c>
@@ -5567,7 +5566,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>224</v>
       </c>
@@ -5589,7 +5588,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>226</v>
       </c>
@@ -5611,7 +5610,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>227</v>
       </c>
@@ -5633,7 +5632,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>228</v>
       </c>
@@ -5655,7 +5654,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="62" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
         <v>252</v>
       </c>
@@ -5678,7 +5677,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>244</v>
       </c>
@@ -5700,7 +5699,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>245</v>
       </c>
@@ -5734,15 +5733,15 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1328125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.9296875" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.73046875" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.06640625" style="10"/>
+    <col min="1" max="1" width="10.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -5753,7 +5752,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>462</v>
       </c>
@@ -5777,22 +5776,22 @@
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="E38" sqref="E38"/>
+      <selection pane="topRight" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.46484375" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.59765625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.265625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.73046875" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="62.06640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.86328125" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.06640625" style="10"/>
+    <col min="7" max="7" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -5815,7 +5814,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>255</v>
       </c>
@@ -5832,7 +5831,7 @@
       </c>
       <c r="G2" s="11"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>258</v>
       </c>
@@ -5847,7 +5846,7 @@
       </c>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>256</v>
       </c>
@@ -5864,7 +5863,7 @@
       </c>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>257</v>
       </c>
@@ -5879,7 +5878,7 @@
       </c>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>263</v>
       </c>
@@ -5894,7 +5893,7 @@
       </c>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>405</v>
       </c>
@@ -5909,7 +5908,7 @@
       </c>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>406</v>
       </c>
@@ -5924,7 +5923,7 @@
       </c>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>407</v>
       </c>
@@ -5939,7 +5938,7 @@
       </c>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>265</v>
       </c>
@@ -5958,7 +5957,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>267</v>
       </c>
@@ -5977,7 +5976,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>268</v>
       </c>
@@ -5996,7 +5995,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>270</v>
       </c>
@@ -6015,7 +6014,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>271</v>
       </c>
@@ -6034,7 +6033,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>272</v>
       </c>
@@ -6053,7 +6052,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>412</v>
       </c>
@@ -6068,7 +6067,7 @@
       </c>
       <c r="G16" s="11"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>413</v>
       </c>
@@ -6083,7 +6082,7 @@
       </c>
       <c r="G17" s="11"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>416</v>
       </c>
@@ -6098,7 +6097,7 @@
       </c>
       <c r="G18" s="11"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>266</v>
       </c>
@@ -6117,7 +6116,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>273</v>
       </c>
@@ -6136,7 +6135,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>269</v>
       </c>
@@ -6155,7 +6154,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>275</v>
       </c>
@@ -6174,7 +6173,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>274</v>
       </c>
@@ -6193,7 +6192,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>276</v>
       </c>
@@ -6212,7 +6211,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>426</v>
       </c>
@@ -6227,7 +6226,7 @@
       </c>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>427</v>
       </c>
@@ -6242,7 +6241,7 @@
       </c>
       <c r="G26" s="11"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>420</v>
       </c>
@@ -6257,7 +6256,7 @@
       </c>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>428</v>
       </c>
@@ -6272,7 +6271,7 @@
       </c>
       <c r="G28" s="11"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>429</v>
       </c>
@@ -6287,7 +6286,7 @@
       </c>
       <c r="G29" s="11"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>430</v>
       </c>
@@ -6302,7 +6301,7 @@
       </c>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>421</v>
       </c>
@@ -6319,7 +6318,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>422</v>
       </c>
@@ -6336,7 +6335,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>423</v>
       </c>
@@ -6353,7 +6352,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>424</v>
       </c>
@@ -6370,7 +6369,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>425</v>
       </c>
@@ -6387,7 +6386,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>442</v>
       </c>
@@ -6404,7 +6403,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>443</v>
       </c>
@@ -6421,7 +6420,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>456</v>
       </c>
@@ -6438,7 +6437,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>458</v>
       </c>
@@ -6455,7 +6454,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>264</v>
       </c>
@@ -6474,7 +6473,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>339</v>
       </c>
@@ -6493,7 +6492,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>346</v>
       </c>
@@ -6512,7 +6511,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>307</v>
       </c>
@@ -6529,7 +6528,7 @@
       </c>
       <c r="G43" s="11"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>277</v>
       </c>
@@ -6546,7 +6545,7 @@
       </c>
       <c r="G44" s="11"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>278</v>
       </c>
@@ -6563,7 +6562,7 @@
       </c>
       <c r="G45" s="11"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>279</v>
       </c>
@@ -6580,7 +6579,7 @@
       </c>
       <c r="G46" s="11"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>280</v>
       </c>
@@ -6597,7 +6596,7 @@
       </c>
       <c r="G47" s="11"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>281</v>
       </c>
@@ -6614,7 +6613,7 @@
       </c>
       <c r="G48" s="11"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>282</v>
       </c>
@@ -6631,7 +6630,7 @@
       </c>
       <c r="G49" s="11"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>283</v>
       </c>
@@ -6648,7 +6647,7 @@
       </c>
       <c r="G50" s="11"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
         <v>284</v>
       </c>
@@ -6665,7 +6664,7 @@
       </c>
       <c r="G51" s="11"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
         <v>285</v>
       </c>
@@ -6680,7 +6679,7 @@
       </c>
       <c r="G52" s="11"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>286</v>
       </c>
@@ -6695,7 +6694,7 @@
       </c>
       <c r="G53" s="11"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
         <v>292</v>
       </c>
@@ -6710,7 +6709,7 @@
       </c>
       <c r="G54" s="11"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
         <v>309</v>
       </c>
@@ -6725,7 +6724,7 @@
       </c>
       <c r="G55" s="11"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
         <v>294</v>
       </c>
@@ -6740,7 +6739,7 @@
       </c>
       <c r="G56" s="11"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
         <v>287</v>
       </c>
@@ -6755,7 +6754,7 @@
       </c>
       <c r="G57" s="11"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
         <v>295</v>
       </c>
@@ -6770,7 +6769,7 @@
       </c>
       <c r="G58" s="11"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
         <v>311</v>
       </c>
@@ -6785,7 +6784,7 @@
       </c>
       <c r="G59" s="11"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
         <v>297</v>
       </c>
@@ -6800,7 +6799,7 @@
       </c>
       <c r="G60" s="11"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
         <v>288</v>
       </c>
@@ -6815,7 +6814,7 @@
       </c>
       <c r="G61" s="11"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
         <v>298</v>
       </c>
@@ -6830,7 +6829,7 @@
       </c>
       <c r="G62" s="11"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
         <v>313</v>
       </c>
@@ -6845,7 +6844,7 @@
       </c>
       <c r="G63" s="11"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
         <v>299</v>
       </c>
@@ -6860,7 +6859,7 @@
       </c>
       <c r="G64" s="11"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
         <v>289</v>
       </c>
@@ -6875,7 +6874,7 @@
       </c>
       <c r="G65" s="11"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
         <v>300</v>
       </c>
@@ -6890,7 +6889,7 @@
       </c>
       <c r="G66" s="11"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
         <v>315</v>
       </c>
@@ -6905,7 +6904,7 @@
       </c>
       <c r="G67" s="11"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
         <v>302</v>
       </c>
@@ -6920,7 +6919,7 @@
       </c>
       <c r="G68" s="11"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
         <v>290</v>
       </c>
@@ -6935,7 +6934,7 @@
       </c>
       <c r="G69" s="11"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
         <v>303</v>
       </c>
@@ -6950,7 +6949,7 @@
       </c>
       <c r="G70" s="11"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
         <v>317</v>
       </c>
@@ -6965,7 +6964,7 @@
       </c>
       <c r="G71" s="11"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
         <v>305</v>
       </c>
@@ -6980,7 +6979,7 @@
       </c>
       <c r="G72" s="11"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
         <v>291</v>
       </c>
@@ -6995,7 +6994,7 @@
       </c>
       <c r="G73" s="11"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="13" t="s">
         <v>306</v>
       </c>
@@ -7010,7 +7009,7 @@
       </c>
       <c r="G74" s="11"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
         <v>319</v>
       </c>
@@ -7025,7 +7024,7 @@
       </c>
       <c r="G75" s="11"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
         <v>308</v>
       </c>
@@ -7040,7 +7039,7 @@
       </c>
       <c r="G76" s="11"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
         <v>310</v>
       </c>
@@ -7055,7 +7054,7 @@
       </c>
       <c r="G77" s="11"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
         <v>312</v>
       </c>
@@ -7070,7 +7069,7 @@
       </c>
       <c r="G78" s="11"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
         <v>314</v>
       </c>
@@ -7085,7 +7084,7 @@
       </c>
       <c r="G79" s="11"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
         <v>316</v>
       </c>
@@ -7100,7 +7099,7 @@
       </c>
       <c r="G80" s="11"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
         <v>318</v>
       </c>
@@ -7115,7 +7114,7 @@
       </c>
       <c r="G81" s="11"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
         <v>301</v>
       </c>
@@ -7130,7 +7129,7 @@
       </c>
       <c r="G82" s="11"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
         <v>304</v>
       </c>
@@ -7145,7 +7144,7 @@
       </c>
       <c r="G83" s="11"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
         <v>293</v>
       </c>
@@ -7160,7 +7159,7 @@
       </c>
       <c r="G84" s="11"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
         <v>296</v>
       </c>
@@ -7175,7 +7174,7 @@
       </c>
       <c r="G85" s="11"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
         <v>320</v>
       </c>
@@ -7190,7 +7189,7 @@
       </c>
       <c r="G86" s="11"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
         <v>322</v>
       </c>
@@ -7205,7 +7204,7 @@
       </c>
       <c r="G87" s="11"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
         <v>324</v>
       </c>
@@ -7220,7 +7219,7 @@
       </c>
       <c r="G88" s="11"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
         <v>321</v>
       </c>
@@ -7235,7 +7234,7 @@
       </c>
       <c r="G89" s="11"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
         <v>323</v>
       </c>
@@ -7250,7 +7249,7 @@
       </c>
       <c r="G90" s="11"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
         <v>325</v>
       </c>
@@ -7265,7 +7264,7 @@
       </c>
       <c r="G91" s="11"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
         <v>326</v>
       </c>
@@ -7280,7 +7279,7 @@
       </c>
       <c r="G92" s="11"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
         <v>328</v>
       </c>
@@ -7295,7 +7294,7 @@
       </c>
       <c r="G93" s="11"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
         <v>330</v>
       </c>
@@ -7310,7 +7309,7 @@
       </c>
       <c r="G94" s="11"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
         <v>327</v>
       </c>
@@ -7325,7 +7324,7 @@
       </c>
       <c r="G95" s="11"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
         <v>329</v>
       </c>
@@ -7340,7 +7339,7 @@
       </c>
       <c r="G96" s="11"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
         <v>331</v>
       </c>

</xml_diff>

<commit_message>
Weighted averaging by target population
FOI experienced by a population is usually a contact-average of FOI produced by all other populations (i.e. preference for interaction times those doing the interacting).
In this case, SRC_POP_AVG(parameter, interaction, characteristic) is the appropriate syntax to use for such a parameter.
However, occasionally, it is not the target that contact-weights parameter values of sources, but a source that contact-weights parameter values across targets.
The TGT_POP_AVG function handles this and, as of this commit, appears to work properly.
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE85C0F0-486B-4703-8D15-FEAEF6BF2A8F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D15FA5-4B56-4660-8EA1-6B788D02D2B7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2044,7 +2044,7 @@
     <t>Preference weighting for one population interacting with another</t>
   </si>
   <si>
-    <t>SRC_POP_AVG(foi_out, w_ctc,alive)</t>
+    <t>TGT_POP_AVG(foi_out, w_ctc, alive)</t>
   </si>
 </sst>
 </file>
@@ -2499,13 +2499,13 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="25.7109375" style="3" customWidth="1"/>
+    <col min="1" max="2" width="25.73046875" style="3" customWidth="1"/>
     <col min="3" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>74</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="7" t="s">
         <v>76</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="7" t="s">
         <v>78</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
         <v>80</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="7" t="s">
         <v>82</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
         <v>84</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
         <v>86</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
         <v>88</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="7" t="s">
         <v>90</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="7" t="s">
         <v>92</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="7" t="s">
         <v>94</v>
       </c>
@@ -2607,19 +2607,19 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.73046875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.86328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.86328125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
@@ -2731,7 +2731,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>19</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>21</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>100</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>101</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>22</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>24</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>25</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>26</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>27</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>28</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>29</v>
       </c>
@@ -3016,7 +3016,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>30</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>31</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>32</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>33</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
         <v>34</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>35</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="6" t="s">
         <v>36</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="6" t="s">
         <v>37</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="6" t="s">
         <v>38</v>
       </c>
@@ -3219,7 +3219,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" s="6" t="s">
         <v>39</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
         <v>40</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="6" t="s">
         <v>41</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="6" t="s">
         <v>42</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="6" t="s">
         <v>43</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="6" t="s">
         <v>46</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
         <v>69</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="6" t="s">
         <v>44</v>
       </c>
@@ -3398,7 +3398,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="6" t="s">
         <v>45</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A37" s="6" t="s">
         <v>71</v>
       </c>
@@ -3465,48 +3465,48 @@
       <selection pane="topRight" activeCell="AJ22" sqref="AJ22:AK22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.86328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.73046875" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.59765625" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="6.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.73046875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6.3984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.1328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.59765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.3984375" style="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5" style="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6" style="11" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7" style="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.59765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.59765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.59765625" style="11" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8" style="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.86328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.86328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.3984375" style="11" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5" style="11" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="6" style="11" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7" style="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.59765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.59765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.59765625" style="11" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8" style="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.86328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.86328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.3984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.59765625" style="11" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="3" style="11" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="4.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="4.86328125" style="11" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="8" style="11" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="5.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.59765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="5.86328125" style="11" bestFit="1" customWidth="1"/>
     <col min="38" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.45">
       <c r="B1" s="12" t="str">
         <f>Compartments!A2</f>
         <v>sus</v>
@@ -3651,7 +3651,7 @@
       <c r="AN1" s="12"/>
       <c r="AO1" s="12"/>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="str">
         <f>Compartments!A2</f>
         <v>sus</v>
@@ -3669,7 +3669,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="str">
         <f>Compartments!A3</f>
         <v>vac</v>
@@ -3684,7 +3684,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="str">
         <f>Compartments!A4</f>
         <v>lteu</v>
@@ -3705,7 +3705,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="str">
         <f>Compartments!A5</f>
         <v>ltet</v>
@@ -3723,7 +3723,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="str">
         <f>Compartments!A6</f>
         <v>ltlu</v>
@@ -3741,7 +3741,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A7" s="12" t="str">
         <f>Compartments!A7</f>
         <v>ltlt</v>
@@ -3759,7 +3759,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A8" s="12" t="str">
         <f>Compartments!A8</f>
         <v>ltr</v>
@@ -3774,7 +3774,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="str">
         <f>Compartments!A9</f>
         <v>ltex</v>
@@ -3792,7 +3792,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A10" s="12" t="str">
         <f>Compartments!A10</f>
         <v>ltlx</v>
@@ -3807,7 +3807,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A11" s="12" t="str">
         <f>Compartments!A11</f>
         <v>acj</v>
@@ -3819,7 +3819,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A12" s="12" t="str">
         <f>Compartments!A12</f>
         <v>spj</v>
@@ -3834,7 +3834,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A13" s="12" t="str">
         <f>Compartments!A13</f>
         <v>spdu</v>
@@ -3855,7 +3855,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A14" s="12" t="str">
         <f>Compartments!A14</f>
         <v>spdd</v>
@@ -3876,7 +3876,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A15" s="12" t="str">
         <f>Compartments!A15</f>
         <v>spdt</v>
@@ -3900,7 +3900,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A16" s="12" t="str">
         <f>Compartments!A16</f>
         <v>spmu</v>
@@ -3921,7 +3921,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A17" s="12" t="str">
         <f>Compartments!A17</f>
         <v>spmd</v>
@@ -3942,7 +3942,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A18" s="12" t="str">
         <f>Compartments!A18</f>
         <v>spmt</v>
@@ -3966,7 +3966,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A19" s="12" t="str">
         <f>Compartments!A19</f>
         <v>spxu</v>
@@ -3987,7 +3987,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A20" s="12" t="str">
         <f>Compartments!A20</f>
         <v>spxd</v>
@@ -4008,7 +4008,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A21" s="12" t="str">
         <f>Compartments!A21</f>
         <v>spxt</v>
@@ -4029,7 +4029,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A22" s="12" t="str">
         <f>Compartments!A22</f>
         <v>snj</v>
@@ -4044,7 +4044,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A23" s="12" t="str">
         <f>Compartments!A23</f>
         <v>sndu</v>
@@ -4065,7 +4065,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A24" s="12" t="str">
         <f>Compartments!A24</f>
         <v>sndd</v>
@@ -4086,7 +4086,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A25" s="12" t="str">
         <f>Compartments!A25</f>
         <v>sndt</v>
@@ -4110,7 +4110,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A26" s="12" t="str">
         <f>Compartments!A26</f>
         <v>snmu</v>
@@ -4131,7 +4131,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A27" s="12" t="str">
         <f>Compartments!A27</f>
         <v>snmd</v>
@@ -4152,7 +4152,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A28" s="12" t="str">
         <f>Compartments!A28</f>
         <v>snmt</v>
@@ -4176,7 +4176,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A29" s="12" t="str">
         <f>Compartments!A29</f>
         <v>snxu</v>
@@ -4197,7 +4197,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A30" s="12" t="str">
         <f>Compartments!A30</f>
         <v>snxd</v>
@@ -4218,7 +4218,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A31" s="12" t="str">
         <f>Compartments!A31</f>
         <v>snxt</v>
@@ -4239,7 +4239,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A32" s="12" t="str">
         <f>Compartments!A32</f>
         <v>acr</v>
@@ -4254,7 +4254,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" s="12" t="s">
         <v>46</v>
       </c>
@@ -4262,7 +4262,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="12" t="s">
         <v>69</v>
       </c>
@@ -4270,31 +4270,31 @@
         <v>256</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" s="12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" s="12"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" s="12"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" s="12"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="12"/>
     </row>
   </sheetData>
@@ -4311,21 +4311,21 @@
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.73046875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.1328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.59765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.86328125" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.86328125" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4352,7 +4352,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
         <v>99</v>
       </c>
@@ -4371,7 +4371,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="8" t="s">
         <v>102</v>
       </c>
@@ -4390,7 +4390,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>105</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="8" t="s">
         <v>106</v>
       </c>
@@ -4428,7 +4428,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
         <v>107</v>
       </c>
@@ -4447,7 +4447,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>116</v>
       </c>
@@ -4469,7 +4469,7 @@
       </c>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>117</v>
       </c>
@@ -4491,7 +4491,7 @@
       </c>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>118</v>
       </c>
@@ -4513,7 +4513,7 @@
       </c>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>119</v>
       </c>
@@ -4535,7 +4535,7 @@
       </c>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>120</v>
       </c>
@@ -4557,7 +4557,7 @@
       </c>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>121</v>
       </c>
@@ -4579,7 +4579,7 @@
       </c>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
         <v>248</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="9" t="s">
         <v>122</v>
       </c>
@@ -4623,7 +4623,7 @@
       </c>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
         <v>123</v>
       </c>
@@ -4645,7 +4645,7 @@
       </c>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>124</v>
       </c>
@@ -4667,7 +4667,7 @@
       </c>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="9" t="s">
         <v>125</v>
       </c>
@@ -4689,7 +4689,7 @@
       </c>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>126</v>
       </c>
@@ -4711,7 +4711,7 @@
       </c>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>127</v>
       </c>
@@ -4733,7 +4733,7 @@
       </c>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>140</v>
       </c>
@@ -4755,7 +4755,7 @@
       </c>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
         <v>141</v>
       </c>
@@ -4777,7 +4777,7 @@
       </c>
       <c r="I21" s="11"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>147</v>
       </c>
@@ -4799,7 +4799,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="9" t="s">
         <v>143</v>
       </c>
@@ -4821,7 +4821,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="9" t="s">
         <v>144</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="9" t="s">
         <v>146</v>
       </c>
@@ -4862,7 +4862,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="9" t="s">
         <v>142</v>
       </c>
@@ -4884,7 +4884,7 @@
       </c>
       <c r="I26" s="11"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="9" t="s">
         <v>145</v>
       </c>
@@ -4906,7 +4906,7 @@
       </c>
       <c r="I27" s="7"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="9" t="s">
         <v>157</v>
       </c>
@@ -4928,7 +4928,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
         <v>158</v>
       </c>
@@ -4950,7 +4950,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>159</v>
       </c>
@@ -4972,7 +4972,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
         <v>160</v>
       </c>
@@ -4994,7 +4994,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="9" t="s">
         <v>161</v>
       </c>
@@ -5016,7 +5016,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="9" t="s">
         <v>162</v>
       </c>
@@ -5038,7 +5038,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
         <v>169</v>
       </c>
@@ -5060,7 +5060,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
         <v>170</v>
       </c>
@@ -5082,7 +5082,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
         <v>171</v>
       </c>
@@ -5104,7 +5104,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="9" t="s">
         <v>172</v>
       </c>
@@ -5126,7 +5126,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
         <v>173</v>
       </c>
@@ -5148,7 +5148,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>174</v>
       </c>
@@ -5170,7 +5170,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>181</v>
       </c>
@@ -5192,7 +5192,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>182</v>
       </c>
@@ -5214,7 +5214,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" s="9" t="s">
         <v>183</v>
       </c>
@@ -5236,7 +5236,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" s="9" t="s">
         <v>184</v>
       </c>
@@ -5258,7 +5258,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" s="9" t="s">
         <v>185</v>
       </c>
@@ -5280,7 +5280,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="9" t="s">
         <v>186</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" s="9" t="s">
         <v>187</v>
       </c>
@@ -5324,7 +5324,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" s="9" t="s">
         <v>188</v>
       </c>
@@ -5346,7 +5346,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="9" t="s">
         <v>189</v>
       </c>
@@ -5368,7 +5368,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="9" t="s">
         <v>199</v>
       </c>
@@ -5390,7 +5390,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="9" t="s">
         <v>200</v>
       </c>
@@ -5412,7 +5412,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="9" t="s">
         <v>201</v>
       </c>
@@ -5434,7 +5434,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="9" t="s">
         <v>202</v>
       </c>
@@ -5456,7 +5456,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" s="9" t="s">
         <v>219</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" s="9" t="s">
         <v>220</v>
       </c>
@@ -5500,7 +5500,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" s="9" t="s">
         <v>221</v>
       </c>
@@ -5522,7 +5522,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" s="9" t="s">
         <v>222</v>
       </c>
@@ -5544,7 +5544,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" s="9" t="s">
         <v>223</v>
       </c>
@@ -5566,7 +5566,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" s="9" t="s">
         <v>224</v>
       </c>
@@ -5588,7 +5588,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" s="9" t="s">
         <v>226</v>
       </c>
@@ -5610,7 +5610,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" s="9" t="s">
         <v>227</v>
       </c>
@@ -5632,7 +5632,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" s="9" t="s">
         <v>228</v>
       </c>
@@ -5654,7 +5654,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="62" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A62" s="14" t="s">
         <v>252</v>
       </c>
@@ -5677,7 +5677,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" s="8" t="s">
         <v>244</v>
       </c>
@@ -5699,7 +5699,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" s="9" t="s">
         <v>245</v>
       </c>
@@ -5733,15 +5733,15 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1328125" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.73046875" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -5752,7 +5752,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
         <v>462</v>
       </c>
@@ -5776,22 +5776,22 @@
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="E31" sqref="E31"/>
+      <selection pane="topRight" activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.59765625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.73046875" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="62" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.86328125" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -5814,7 +5814,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>255</v>
       </c>
@@ -5831,7 +5831,7 @@
       </c>
       <c r="G2" s="11"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>258</v>
       </c>
@@ -5846,7 +5846,7 @@
       </c>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>256</v>
       </c>
@@ -5863,7 +5863,7 @@
       </c>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>257</v>
       </c>
@@ -5878,7 +5878,7 @@
       </c>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
         <v>263</v>
       </c>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>405</v>
       </c>
@@ -5908,7 +5908,7 @@
       </c>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
         <v>406</v>
       </c>
@@ -5923,7 +5923,7 @@
       </c>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
         <v>407</v>
       </c>
@@ -5938,7 +5938,7 @@
       </c>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
         <v>265</v>
       </c>
@@ -5957,7 +5957,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="11" t="s">
         <v>267</v>
       </c>
@@ -5976,7 +5976,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="11" t="s">
         <v>268</v>
       </c>
@@ -5995,7 +5995,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="11" t="s">
         <v>270</v>
       </c>
@@ -6014,7 +6014,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="11" t="s">
         <v>271</v>
       </c>
@@ -6033,7 +6033,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="11" t="s">
         <v>272</v>
       </c>
@@ -6052,7 +6052,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
         <v>412</v>
       </c>
@@ -6067,7 +6067,7 @@
       </c>
       <c r="G16" s="11"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
         <v>413</v>
       </c>
@@ -6082,7 +6082,7 @@
       </c>
       <c r="G17" s="11"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="11" t="s">
         <v>416</v>
       </c>
@@ -6097,7 +6097,7 @@
       </c>
       <c r="G18" s="11"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="13" t="s">
         <v>266</v>
       </c>
@@ -6116,7 +6116,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="13" t="s">
         <v>273</v>
       </c>
@@ -6135,7 +6135,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="13" t="s">
         <v>269</v>
       </c>
@@ -6154,7 +6154,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="13" t="s">
         <v>275</v>
       </c>
@@ -6173,7 +6173,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="13" t="s">
         <v>274</v>
       </c>
@@ -6192,7 +6192,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="13" t="s">
         <v>276</v>
       </c>
@@ -6211,7 +6211,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="13" t="s">
         <v>426</v>
       </c>
@@ -6226,7 +6226,7 @@
       </c>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="13" t="s">
         <v>427</v>
       </c>
@@ -6241,7 +6241,7 @@
       </c>
       <c r="G26" s="11"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="13" t="s">
         <v>420</v>
       </c>
@@ -6256,7 +6256,7 @@
       </c>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="13" t="s">
         <v>428</v>
       </c>
@@ -6271,7 +6271,7 @@
       </c>
       <c r="G28" s="11"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="17" t="s">
         <v>429</v>
       </c>
@@ -6286,7 +6286,7 @@
       </c>
       <c r="G29" s="11"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="17" t="s">
         <v>430</v>
       </c>
@@ -6301,7 +6301,7 @@
       </c>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="13" t="s">
         <v>421</v>
       </c>
@@ -6318,7 +6318,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="13" t="s">
         <v>422</v>
       </c>
@@ -6335,7 +6335,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="13" t="s">
         <v>423</v>
       </c>
@@ -6352,7 +6352,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="13" t="s">
         <v>424</v>
       </c>
@@ -6369,7 +6369,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="13" t="s">
         <v>425</v>
       </c>
@@ -6386,7 +6386,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="13" t="s">
         <v>442</v>
       </c>
@@ -6403,7 +6403,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="13" t="s">
         <v>443</v>
       </c>
@@ -6420,7 +6420,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="13" t="s">
         <v>456</v>
       </c>
@@ -6437,7 +6437,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="13" t="s">
         <v>458</v>
       </c>
@@ -6454,7 +6454,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="11" t="s">
         <v>264</v>
       </c>
@@ -6473,7 +6473,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="11" t="s">
         <v>339</v>
       </c>
@@ -6492,7 +6492,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="11" t="s">
         <v>346</v>
       </c>
@@ -6511,7 +6511,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="11" t="s">
         <v>307</v>
       </c>
@@ -6528,7 +6528,7 @@
       </c>
       <c r="G43" s="11"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="13" t="s">
         <v>277</v>
       </c>
@@ -6545,7 +6545,7 @@
       </c>
       <c r="G44" s="11"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" s="13" t="s">
         <v>278</v>
       </c>
@@ -6562,7 +6562,7 @@
       </c>
       <c r="G45" s="11"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="13" t="s">
         <v>279</v>
       </c>
@@ -6579,7 +6579,7 @@
       </c>
       <c r="G46" s="11"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="13" t="s">
         <v>280</v>
       </c>
@@ -6596,7 +6596,7 @@
       </c>
       <c r="G47" s="11"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="13" t="s">
         <v>281</v>
       </c>
@@ -6613,7 +6613,7 @@
       </c>
       <c r="G48" s="11"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="13" t="s">
         <v>282</v>
       </c>
@@ -6630,7 +6630,7 @@
       </c>
       <c r="G49" s="11"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="13" t="s">
         <v>283</v>
       </c>
@@ -6647,7 +6647,7 @@
       </c>
       <c r="G50" s="11"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="13" t="s">
         <v>284</v>
       </c>
@@ -6664,7 +6664,7 @@
       </c>
       <c r="G51" s="11"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" s="13" t="s">
         <v>285</v>
       </c>
@@ -6679,7 +6679,7 @@
       </c>
       <c r="G52" s="11"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="13" t="s">
         <v>286</v>
       </c>
@@ -6694,7 +6694,7 @@
       </c>
       <c r="G53" s="11"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="13" t="s">
         <v>292</v>
       </c>
@@ -6709,7 +6709,7 @@
       </c>
       <c r="G54" s="11"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="13" t="s">
         <v>309</v>
       </c>
@@ -6724,7 +6724,7 @@
       </c>
       <c r="G55" s="11"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="13" t="s">
         <v>294</v>
       </c>
@@ -6739,7 +6739,7 @@
       </c>
       <c r="G56" s="11"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="13" t="s">
         <v>287</v>
       </c>
@@ -6754,7 +6754,7 @@
       </c>
       <c r="G57" s="11"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="13" t="s">
         <v>295</v>
       </c>
@@ -6769,7 +6769,7 @@
       </c>
       <c r="G58" s="11"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="13" t="s">
         <v>311</v>
       </c>
@@ -6784,7 +6784,7 @@
       </c>
       <c r="G59" s="11"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="13" t="s">
         <v>297</v>
       </c>
@@ -6799,7 +6799,7 @@
       </c>
       <c r="G60" s="11"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="13" t="s">
         <v>288</v>
       </c>
@@ -6814,7 +6814,7 @@
       </c>
       <c r="G61" s="11"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="13" t="s">
         <v>298</v>
       </c>
@@ -6829,7 +6829,7 @@
       </c>
       <c r="G62" s="11"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="13" t="s">
         <v>313</v>
       </c>
@@ -6844,7 +6844,7 @@
       </c>
       <c r="G63" s="11"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="13" t="s">
         <v>299</v>
       </c>
@@ -6859,7 +6859,7 @@
       </c>
       <c r="G64" s="11"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A65" s="13" t="s">
         <v>289</v>
       </c>
@@ -6874,7 +6874,7 @@
       </c>
       <c r="G65" s="11"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A66" s="13" t="s">
         <v>300</v>
       </c>
@@ -6889,7 +6889,7 @@
       </c>
       <c r="G66" s="11"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67" s="13" t="s">
         <v>315</v>
       </c>
@@ -6904,7 +6904,7 @@
       </c>
       <c r="G67" s="11"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68" s="13" t="s">
         <v>302</v>
       </c>
@@ -6919,7 +6919,7 @@
       </c>
       <c r="G68" s="11"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A69" s="13" t="s">
         <v>290</v>
       </c>
@@ -6934,7 +6934,7 @@
       </c>
       <c r="G69" s="11"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A70" s="13" t="s">
         <v>303</v>
       </c>
@@ -6949,7 +6949,7 @@
       </c>
       <c r="G70" s="11"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71" s="13" t="s">
         <v>317</v>
       </c>
@@ -6964,7 +6964,7 @@
       </c>
       <c r="G71" s="11"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" s="13" t="s">
         <v>305</v>
       </c>
@@ -6979,7 +6979,7 @@
       </c>
       <c r="G72" s="11"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73" s="13" t="s">
         <v>291</v>
       </c>
@@ -6994,7 +6994,7 @@
       </c>
       <c r="G73" s="11"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74" s="13" t="s">
         <v>306</v>
       </c>
@@ -7009,7 +7009,7 @@
       </c>
       <c r="G74" s="11"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A75" s="13" t="s">
         <v>319</v>
       </c>
@@ -7024,7 +7024,7 @@
       </c>
       <c r="G75" s="11"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A76" s="13" t="s">
         <v>308</v>
       </c>
@@ -7039,7 +7039,7 @@
       </c>
       <c r="G76" s="11"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A77" s="13" t="s">
         <v>310</v>
       </c>
@@ -7054,7 +7054,7 @@
       </c>
       <c r="G77" s="11"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A78" s="13" t="s">
         <v>312</v>
       </c>
@@ -7069,7 +7069,7 @@
       </c>
       <c r="G78" s="11"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A79" s="13" t="s">
         <v>314</v>
       </c>
@@ -7084,7 +7084,7 @@
       </c>
       <c r="G79" s="11"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A80" s="13" t="s">
         <v>316</v>
       </c>
@@ -7099,7 +7099,7 @@
       </c>
       <c r="G80" s="11"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A81" s="13" t="s">
         <v>318</v>
       </c>
@@ -7114,7 +7114,7 @@
       </c>
       <c r="G81" s="11"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A82" s="13" t="s">
         <v>301</v>
       </c>
@@ -7129,7 +7129,7 @@
       </c>
       <c r="G82" s="11"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A83" s="13" t="s">
         <v>304</v>
       </c>
@@ -7144,7 +7144,7 @@
       </c>
       <c r="G83" s="11"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A84" s="13" t="s">
         <v>293</v>
       </c>
@@ -7159,7 +7159,7 @@
       </c>
       <c r="G84" s="11"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A85" s="13" t="s">
         <v>296</v>
       </c>
@@ -7174,7 +7174,7 @@
       </c>
       <c r="G85" s="11"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A86" s="13" t="s">
         <v>320</v>
       </c>
@@ -7189,7 +7189,7 @@
       </c>
       <c r="G86" s="11"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A87" s="13" t="s">
         <v>322</v>
       </c>
@@ -7204,7 +7204,7 @@
       </c>
       <c r="G87" s="11"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A88" s="13" t="s">
         <v>324</v>
       </c>
@@ -7219,7 +7219,7 @@
       </c>
       <c r="G88" s="11"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A89" s="13" t="s">
         <v>321</v>
       </c>
@@ -7234,7 +7234,7 @@
       </c>
       <c r="G89" s="11"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A90" s="13" t="s">
         <v>323</v>
       </c>
@@ -7249,7 +7249,7 @@
       </c>
       <c r="G90" s="11"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A91" s="13" t="s">
         <v>325</v>
       </c>
@@ -7264,7 +7264,7 @@
       </c>
       <c r="G91" s="11"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A92" s="13" t="s">
         <v>326</v>
       </c>
@@ -7279,7 +7279,7 @@
       </c>
       <c r="G92" s="11"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A93" s="13" t="s">
         <v>328</v>
       </c>
@@ -7294,7 +7294,7 @@
       </c>
       <c r="G93" s="11"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A94" s="13" t="s">
         <v>330</v>
       </c>
@@ -7309,7 +7309,7 @@
       </c>
       <c r="G94" s="11"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A95" s="13" t="s">
         <v>327</v>
       </c>
@@ -7324,7 +7324,7 @@
       </c>
       <c r="G95" s="11"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A96" s="13" t="s">
         <v>329</v>
       </c>
@@ -7339,7 +7339,7 @@
       </c>
       <c r="G96" s="11"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A97" s="13" t="s">
         <v>331</v>
       </c>

</xml_diff>

<commit_message>
Tidy up print statements and logic
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\frameworks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D15FA5-4B56-4660-8EA1-6B788D02D2B7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB6C1D9-3962-4CC8-A13A-2A2D8F40257F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2044,7 +2044,7 @@
     <t>Preference weighting for one population interacting with another</t>
   </si>
   <si>
-    <t>TGT_POP_AVG(foi_out, w_ctc, alive)</t>
+    <t>SRC_POP_AVG(foi_out, w_ctc, alive)</t>
   </si>
 </sst>
 </file>
@@ -2499,13 +2499,13 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="25.73046875" style="3" customWidth="1"/>
+    <col min="1" max="2" width="25.7109375" style="3" customWidth="1"/>
     <col min="3" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>74</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>76</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>78</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>80</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>82</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>84</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>86</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>88</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>90</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>92</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>94</v>
       </c>
@@ -2607,19 +2607,19 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.86328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
@@ -2731,7 +2731,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>19</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>21</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>100</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>101</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>22</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>24</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>25</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>26</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>27</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>28</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>29</v>
       </c>
@@ -3016,7 +3016,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>30</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>31</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>32</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>33</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>34</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>35</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>36</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>37</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>38</v>
       </c>
@@ -3219,7 +3219,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>39</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>40</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>41</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>42</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>43</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>46</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>69</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>44</v>
       </c>
@@ -3398,7 +3398,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>45</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>71</v>
       </c>
@@ -3465,48 +3465,48 @@
       <selection pane="topRight" activeCell="AJ22" sqref="AJ22:AK22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.86328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.73046875" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.59765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.73046875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="6.3984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.1328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.59765625" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.3984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5" style="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6" style="11" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7" style="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.59765625" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.59765625" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.59765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.5703125" style="11" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8" style="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.86328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.86328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.3984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5" style="11" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="6" style="11" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7" style="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.59765625" style="11" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.59765625" style="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.59765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.5703125" style="11" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8" style="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.86328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.86328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.3984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.59765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.5703125" style="11" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="3" style="11" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="4.86328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="4.85546875" style="11" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="8" style="11" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8.59765625" style="11" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="5.86328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="5.85546875" style="11" bestFit="1" customWidth="1"/>
     <col min="38" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="B1" s="12" t="str">
         <f>Compartments!A2</f>
         <v>sus</v>
@@ -3651,7 +3651,7 @@
       <c r="AN1" s="12"/>
       <c r="AO1" s="12"/>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="str">
         <f>Compartments!A2</f>
         <v>sus</v>
@@ -3669,7 +3669,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="str">
         <f>Compartments!A3</f>
         <v>vac</v>
@@ -3684,7 +3684,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="str">
         <f>Compartments!A4</f>
         <v>lteu</v>
@@ -3705,7 +3705,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="str">
         <f>Compartments!A5</f>
         <v>ltet</v>
@@ -3723,7 +3723,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="str">
         <f>Compartments!A6</f>
         <v>ltlu</v>
@@ -3741,7 +3741,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="str">
         <f>Compartments!A7</f>
         <v>ltlt</v>
@@ -3759,7 +3759,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="str">
         <f>Compartments!A8</f>
         <v>ltr</v>
@@ -3774,7 +3774,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="str">
         <f>Compartments!A9</f>
         <v>ltex</v>
@@ -3792,7 +3792,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="str">
         <f>Compartments!A10</f>
         <v>ltlx</v>
@@ -3807,7 +3807,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="str">
         <f>Compartments!A11</f>
         <v>acj</v>
@@ -3819,7 +3819,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="str">
         <f>Compartments!A12</f>
         <v>spj</v>
@@ -3834,7 +3834,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="str">
         <f>Compartments!A13</f>
         <v>spdu</v>
@@ -3855,7 +3855,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="str">
         <f>Compartments!A14</f>
         <v>spdd</v>
@@ -3876,7 +3876,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="str">
         <f>Compartments!A15</f>
         <v>spdt</v>
@@ -3900,7 +3900,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="str">
         <f>Compartments!A16</f>
         <v>spmu</v>
@@ -3921,7 +3921,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="str">
         <f>Compartments!A17</f>
         <v>spmd</v>
@@ -3942,7 +3942,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="str">
         <f>Compartments!A18</f>
         <v>spmt</v>
@@ -3966,7 +3966,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="str">
         <f>Compartments!A19</f>
         <v>spxu</v>
@@ -3987,7 +3987,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="str">
         <f>Compartments!A20</f>
         <v>spxd</v>
@@ -4008,7 +4008,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="str">
         <f>Compartments!A21</f>
         <v>spxt</v>
@@ -4029,7 +4029,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="str">
         <f>Compartments!A22</f>
         <v>snj</v>
@@ -4044,7 +4044,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="str">
         <f>Compartments!A23</f>
         <v>sndu</v>
@@ -4065,7 +4065,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="str">
         <f>Compartments!A24</f>
         <v>sndd</v>
@@ -4086,7 +4086,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="str">
         <f>Compartments!A25</f>
         <v>sndt</v>
@@ -4110,7 +4110,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="str">
         <f>Compartments!A26</f>
         <v>snmu</v>
@@ -4131,7 +4131,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="str">
         <f>Compartments!A27</f>
         <v>snmd</v>
@@ -4152,7 +4152,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="str">
         <f>Compartments!A28</f>
         <v>snmt</v>
@@ -4176,7 +4176,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="str">
         <f>Compartments!A29</f>
         <v>snxu</v>
@@ -4197,7 +4197,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="str">
         <f>Compartments!A30</f>
         <v>snxd</v>
@@ -4218,7 +4218,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="str">
         <f>Compartments!A31</f>
         <v>snxt</v>
@@ -4239,7 +4239,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="str">
         <f>Compartments!A32</f>
         <v>acr</v>
@@ -4254,7 +4254,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>46</v>
       </c>
@@ -4262,7 +4262,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>69</v>
       </c>
@@ -4270,31 +4270,31 @@
         <v>256</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="12"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="12"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="12"/>
     </row>
   </sheetData>
@@ -4311,21 +4311,21 @@
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.1328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.59765625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.73046875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.86328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.86328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4352,7 +4352,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>99</v>
       </c>
@@ -4371,7 +4371,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>102</v>
       </c>
@@ -4390,7 +4390,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>105</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>106</v>
       </c>
@@ -4428,7 +4428,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>107</v>
       </c>
@@ -4447,7 +4447,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>116</v>
       </c>
@@ -4469,7 +4469,7 @@
       </c>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>117</v>
       </c>
@@ -4491,7 +4491,7 @@
       </c>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>118</v>
       </c>
@@ -4513,7 +4513,7 @@
       </c>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>119</v>
       </c>
@@ -4535,7 +4535,7 @@
       </c>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>120</v>
       </c>
@@ -4557,7 +4557,7 @@
       </c>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>121</v>
       </c>
@@ -4579,7 +4579,7 @@
       </c>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>248</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>122</v>
       </c>
@@ -4623,7 +4623,7 @@
       </c>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>123</v>
       </c>
@@ -4645,7 +4645,7 @@
       </c>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>124</v>
       </c>
@@ -4667,7 +4667,7 @@
       </c>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>125</v>
       </c>
@@ -4689,7 +4689,7 @@
       </c>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>126</v>
       </c>
@@ -4711,7 +4711,7 @@
       </c>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>127</v>
       </c>
@@ -4733,7 +4733,7 @@
       </c>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>140</v>
       </c>
@@ -4755,7 +4755,7 @@
       </c>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>141</v>
       </c>
@@ -4777,7 +4777,7 @@
       </c>
       <c r="I21" s="11"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>147</v>
       </c>
@@ -4799,7 +4799,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>143</v>
       </c>
@@ -4821,7 +4821,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>144</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>146</v>
       </c>
@@ -4862,7 +4862,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>142</v>
       </c>
@@ -4884,7 +4884,7 @@
       </c>
       <c r="I26" s="11"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>145</v>
       </c>
@@ -4906,7 +4906,7 @@
       </c>
       <c r="I27" s="7"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>157</v>
       </c>
@@ -4928,7 +4928,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>158</v>
       </c>
@@ -4950,7 +4950,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>159</v>
       </c>
@@ -4972,7 +4972,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>160</v>
       </c>
@@ -4994,7 +4994,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>161</v>
       </c>
@@ -5016,7 +5016,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>162</v>
       </c>
@@ -5038,7 +5038,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>169</v>
       </c>
@@ -5060,7 +5060,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>170</v>
       </c>
@@ -5082,7 +5082,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>171</v>
       </c>
@@ -5104,7 +5104,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>172</v>
       </c>
@@ -5126,7 +5126,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>173</v>
       </c>
@@ -5148,7 +5148,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>174</v>
       </c>
@@ -5170,7 +5170,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>181</v>
       </c>
@@ -5192,7 +5192,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>182</v>
       </c>
@@ -5214,7 +5214,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>183</v>
       </c>
@@ -5236,7 +5236,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>184</v>
       </c>
@@ -5258,7 +5258,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>185</v>
       </c>
@@ -5280,7 +5280,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>186</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>187</v>
       </c>
@@ -5324,7 +5324,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>188</v>
       </c>
@@ -5346,7 +5346,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>189</v>
       </c>
@@ -5368,7 +5368,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>199</v>
       </c>
@@ -5390,7 +5390,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>200</v>
       </c>
@@ -5412,7 +5412,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>201</v>
       </c>
@@ -5434,7 +5434,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>202</v>
       </c>
@@ -5456,7 +5456,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>219</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>220</v>
       </c>
@@ -5500,7 +5500,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>221</v>
       </c>
@@ -5522,7 +5522,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>222</v>
       </c>
@@ -5544,7 +5544,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>223</v>
       </c>
@@ -5566,7 +5566,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>224</v>
       </c>
@@ -5588,7 +5588,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>226</v>
       </c>
@@ -5610,7 +5610,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>227</v>
       </c>
@@ -5632,7 +5632,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>228</v>
       </c>
@@ -5654,7 +5654,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="62" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
         <v>252</v>
       </c>
@@ -5677,7 +5677,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>244</v>
       </c>
@@ -5699,7 +5699,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>245</v>
       </c>
@@ -5733,15 +5733,15 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -5752,7 +5752,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>462</v>
       </c>
@@ -5773,25 +5773,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FC8421-05BA-4BE1-A1F1-3F12A4E7E369}">
   <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="E39" sqref="E39"/>
+      <selection pane="topRight" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.3984375" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.59765625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.265625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="62" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -5814,7 +5814,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>255</v>
       </c>
@@ -5831,7 +5831,7 @@
       </c>
       <c r="G2" s="11"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>258</v>
       </c>
@@ -5846,7 +5846,7 @@
       </c>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>256</v>
       </c>
@@ -5863,7 +5863,7 @@
       </c>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>257</v>
       </c>
@@ -5878,7 +5878,7 @@
       </c>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>263</v>
       </c>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>405</v>
       </c>
@@ -5908,7 +5908,7 @@
       </c>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>406</v>
       </c>
@@ -5923,7 +5923,7 @@
       </c>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>407</v>
       </c>
@@ -5938,7 +5938,7 @@
       </c>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>265</v>
       </c>
@@ -5957,7 +5957,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>267</v>
       </c>
@@ -5976,7 +5976,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>268</v>
       </c>
@@ -5995,7 +5995,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>270</v>
       </c>
@@ -6014,7 +6014,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>271</v>
       </c>
@@ -6033,7 +6033,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>272</v>
       </c>
@@ -6052,7 +6052,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>412</v>
       </c>
@@ -6067,7 +6067,7 @@
       </c>
       <c r="G16" s="11"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>413</v>
       </c>
@@ -6082,7 +6082,7 @@
       </c>
       <c r="G17" s="11"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>416</v>
       </c>
@@ -6097,7 +6097,7 @@
       </c>
       <c r="G18" s="11"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>266</v>
       </c>
@@ -6116,7 +6116,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>273</v>
       </c>
@@ -6135,7 +6135,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>269</v>
       </c>
@@ -6154,7 +6154,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>275</v>
       </c>
@@ -6173,7 +6173,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>274</v>
       </c>
@@ -6192,7 +6192,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>276</v>
       </c>
@@ -6211,7 +6211,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>426</v>
       </c>
@@ -6226,7 +6226,7 @@
       </c>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>427</v>
       </c>
@@ -6241,7 +6241,7 @@
       </c>
       <c r="G26" s="11"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>420</v>
       </c>
@@ -6256,7 +6256,7 @@
       </c>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>428</v>
       </c>
@@ -6271,7 +6271,7 @@
       </c>
       <c r="G28" s="11"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>429</v>
       </c>
@@ -6286,7 +6286,7 @@
       </c>
       <c r="G29" s="11"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>430</v>
       </c>
@@ -6301,7 +6301,7 @@
       </c>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>421</v>
       </c>
@@ -6318,7 +6318,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>422</v>
       </c>
@@ -6335,7 +6335,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>423</v>
       </c>
@@ -6352,7 +6352,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>424</v>
       </c>
@@ -6369,7 +6369,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>425</v>
       </c>
@@ -6386,7 +6386,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>442</v>
       </c>
@@ -6403,7 +6403,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>443</v>
       </c>
@@ -6420,7 +6420,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>456</v>
       </c>
@@ -6437,7 +6437,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>458</v>
       </c>
@@ -6454,7 +6454,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>264</v>
       </c>
@@ -6473,7 +6473,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>339</v>
       </c>
@@ -6492,7 +6492,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>346</v>
       </c>
@@ -6511,7 +6511,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>307</v>
       </c>
@@ -6528,7 +6528,7 @@
       </c>
       <c r="G43" s="11"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>277</v>
       </c>
@@ -6545,7 +6545,7 @@
       </c>
       <c r="G44" s="11"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>278</v>
       </c>
@@ -6562,7 +6562,7 @@
       </c>
       <c r="G45" s="11"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>279</v>
       </c>
@@ -6579,7 +6579,7 @@
       </c>
       <c r="G46" s="11"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>280</v>
       </c>
@@ -6596,7 +6596,7 @@
       </c>
       <c r="G47" s="11"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>281</v>
       </c>
@@ -6613,7 +6613,7 @@
       </c>
       <c r="G48" s="11"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>282</v>
       </c>
@@ -6630,7 +6630,7 @@
       </c>
       <c r="G49" s="11"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>283</v>
       </c>
@@ -6647,7 +6647,7 @@
       </c>
       <c r="G50" s="11"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
         <v>284</v>
       </c>
@@ -6664,7 +6664,7 @@
       </c>
       <c r="G51" s="11"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
         <v>285</v>
       </c>
@@ -6679,7 +6679,7 @@
       </c>
       <c r="G52" s="11"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>286</v>
       </c>
@@ -6694,7 +6694,7 @@
       </c>
       <c r="G53" s="11"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
         <v>292</v>
       </c>
@@ -6709,7 +6709,7 @@
       </c>
       <c r="G54" s="11"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
         <v>309</v>
       </c>
@@ -6724,7 +6724,7 @@
       </c>
       <c r="G55" s="11"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
         <v>294</v>
       </c>
@@ -6739,7 +6739,7 @@
       </c>
       <c r="G56" s="11"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
         <v>287</v>
       </c>
@@ -6754,7 +6754,7 @@
       </c>
       <c r="G57" s="11"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
         <v>295</v>
       </c>
@@ -6769,7 +6769,7 @@
       </c>
       <c r="G58" s="11"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
         <v>311</v>
       </c>
@@ -6784,7 +6784,7 @@
       </c>
       <c r="G59" s="11"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
         <v>297</v>
       </c>
@@ -6799,7 +6799,7 @@
       </c>
       <c r="G60" s="11"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
         <v>288</v>
       </c>
@@ -6814,7 +6814,7 @@
       </c>
       <c r="G61" s="11"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
         <v>298</v>
       </c>
@@ -6829,7 +6829,7 @@
       </c>
       <c r="G62" s="11"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
         <v>313</v>
       </c>
@@ -6844,7 +6844,7 @@
       </c>
       <c r="G63" s="11"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
         <v>299</v>
       </c>
@@ -6859,7 +6859,7 @@
       </c>
       <c r="G64" s="11"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
         <v>289</v>
       </c>
@@ -6874,7 +6874,7 @@
       </c>
       <c r="G65" s="11"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
         <v>300</v>
       </c>
@@ -6889,7 +6889,7 @@
       </c>
       <c r="G66" s="11"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
         <v>315</v>
       </c>
@@ -6904,7 +6904,7 @@
       </c>
       <c r="G67" s="11"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
         <v>302</v>
       </c>
@@ -6919,7 +6919,7 @@
       </c>
       <c r="G68" s="11"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
         <v>290</v>
       </c>
@@ -6934,7 +6934,7 @@
       </c>
       <c r="G69" s="11"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
         <v>303</v>
       </c>
@@ -6949,7 +6949,7 @@
       </c>
       <c r="G70" s="11"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
         <v>317</v>
       </c>
@@ -6964,7 +6964,7 @@
       </c>
       <c r="G71" s="11"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
         <v>305</v>
       </c>
@@ -6979,7 +6979,7 @@
       </c>
       <c r="G72" s="11"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
         <v>291</v>
       </c>
@@ -6994,7 +6994,7 @@
       </c>
       <c r="G73" s="11"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="13" t="s">
         <v>306</v>
       </c>
@@ -7009,7 +7009,7 @@
       </c>
       <c r="G74" s="11"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
         <v>319</v>
       </c>
@@ -7024,7 +7024,7 @@
       </c>
       <c r="G75" s="11"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
         <v>308</v>
       </c>
@@ -7039,7 +7039,7 @@
       </c>
       <c r="G76" s="11"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
         <v>310</v>
       </c>
@@ -7054,7 +7054,7 @@
       </c>
       <c r="G77" s="11"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
         <v>312</v>
       </c>
@@ -7069,7 +7069,7 @@
       </c>
       <c r="G78" s="11"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
         <v>314</v>
       </c>
@@ -7084,7 +7084,7 @@
       </c>
       <c r="G79" s="11"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
         <v>316</v>
       </c>
@@ -7099,7 +7099,7 @@
       </c>
       <c r="G80" s="11"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
         <v>318</v>
       </c>
@@ -7114,7 +7114,7 @@
       </c>
       <c r="G81" s="11"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
         <v>301</v>
       </c>
@@ -7129,7 +7129,7 @@
       </c>
       <c r="G82" s="11"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
         <v>304</v>
       </c>
@@ -7144,7 +7144,7 @@
       </c>
       <c r="G83" s="11"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
         <v>293</v>
       </c>
@@ -7159,7 +7159,7 @@
       </c>
       <c r="G84" s="11"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
         <v>296</v>
       </c>
@@ -7174,7 +7174,7 @@
       </c>
       <c r="G85" s="11"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
         <v>320</v>
       </c>
@@ -7189,7 +7189,7 @@
       </c>
       <c r="G86" s="11"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
         <v>322</v>
       </c>
@@ -7204,7 +7204,7 @@
       </c>
       <c r="G87" s="11"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
         <v>324</v>
       </c>
@@ -7219,7 +7219,7 @@
       </c>
       <c r="G88" s="11"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
         <v>321</v>
       </c>
@@ -7234,7 +7234,7 @@
       </c>
       <c r="G89" s="11"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
         <v>323</v>
       </c>
@@ -7249,7 +7249,7 @@
       </c>
       <c r="G90" s="11"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
         <v>325</v>
       </c>
@@ -7264,7 +7264,7 @@
       </c>
       <c r="G91" s="11"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
         <v>326</v>
       </c>
@@ -7279,7 +7279,7 @@
       </c>
       <c r="G92" s="11"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
         <v>328</v>
       </c>
@@ -7294,7 +7294,7 @@
       </c>
       <c r="G93" s="11"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
         <v>330</v>
       </c>
@@ -7309,7 +7309,7 @@
       </c>
       <c r="G94" s="11"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
         <v>327</v>
       </c>
@@ -7324,7 +7324,7 @@
       </c>
       <c r="G95" s="11"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
         <v>329</v>
       </c>
@@ -7339,7 +7339,7 @@
       </c>
       <c r="G96" s="11"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
         <v>331</v>
       </c>

</xml_diff>

<commit_message>
Minor updates from SA original project
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB6C1D9-3962-4CC8-A13A-2A2D8F40257F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8EA89A-45C2-434C-848B-C51993A7BE08}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -598,7 +598,33 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{BAC0C8ED-DDB5-4067-82A2-58808108CB14}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{8566D7BB-D1CA-4A35-8F73-9A9D54D614CE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column defines a 'min' attribute for a 'par' item.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{D8CB5CD7-6C13-4D56-A891-23A4D6E3AE68}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column defines a 'max' attribute for a 'par' item.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{BAC0C8ED-DDB5-4067-82A2-58808108CB14}">
       <text>
         <r>
           <rPr>
@@ -611,7 +637,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{727369DF-9454-4254-873C-A3C5C5E58366}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{727369DF-9454-4254-873C-A3C5C5E58366}">
       <text>
         <r>
           <rPr>
@@ -630,7 +656,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{3514B01A-966C-4E36-8CD8-B0E499FEDBF5}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{3514B01A-966C-4E36-8CD8-B0E499FEDBF5}">
       <text>
         <r>
           <rPr>
@@ -650,7 +676,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="467">
   <si>
     <t>Code Name</t>
   </si>
@@ -2045,6 +2071,12 @@
   </si>
   <si>
     <t>SRC_POP_AVG(foi_out, w_ctc, alive)</t>
+  </si>
+  <si>
+    <t>Minimum Value</t>
+  </si>
+  <si>
+    <t>Maximum Value</t>
   </si>
 </sst>
 </file>
@@ -5771,12 +5803,12 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FC8421-05BA-4BE1-A1F1-3F12A4E7E369}">
-  <dimension ref="A1:G97"/>
+  <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="E41" sqref="E41"/>
+      <selection pane="topRight" activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5785,13 +5817,14 @@
     <col min="2" max="2" width="51.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="62" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="10"/>
+    <col min="5" max="6" width="20.7109375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="62" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -5805,16 +5838,22 @@
         <v>10</v>
       </c>
       <c r="E1" s="12" t="s">
+        <v>465</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>466</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>255</v>
       </c>
@@ -5826,12 +5865,14 @@
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>258</v>
       </c>
@@ -5841,12 +5882,14 @@
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="G3" s="11"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>256</v>
       </c>
@@ -5858,12 +5901,14 @@
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="11"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>257</v>
       </c>
@@ -5873,12 +5918,14 @@
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="11"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5" s="11"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>263</v>
       </c>
@@ -5888,12 +5935,14 @@
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>405</v>
       </c>
@@ -5903,12 +5952,14 @@
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>406</v>
       </c>
@@ -5918,12 +5969,14 @@
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="11"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8" s="11"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>407</v>
       </c>
@@ -5933,12 +5986,14 @@
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="11"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>265</v>
       </c>
@@ -5949,15 +6004,17 @@
         <v>411</v>
       </c>
       <c r="D10" s="11"/>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11" t="s">
         <v>405</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="11"/>
+      <c r="I10" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>267</v>
       </c>
@@ -5968,15 +6025,17 @@
         <v>411</v>
       </c>
       <c r="D11" s="11"/>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11" t="s">
         <v>406</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="11"/>
+      <c r="I11" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>268</v>
       </c>
@@ -5987,15 +6046,17 @@
         <v>411</v>
       </c>
       <c r="D12" s="11"/>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11" t="s">
         <v>407</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="11"/>
+      <c r="I12" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>270</v>
       </c>
@@ -6006,15 +6067,17 @@
         <v>411</v>
       </c>
       <c r="D13" s="11"/>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11" t="s">
         <v>405</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="11"/>
+      <c r="I13" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>271</v>
       </c>
@@ -6025,15 +6088,17 @@
         <v>411</v>
       </c>
       <c r="D14" s="11"/>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11" t="s">
         <v>406</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="11"/>
+      <c r="I14" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>272</v>
       </c>
@@ -6044,15 +6109,17 @@
         <v>411</v>
       </c>
       <c r="D15" s="11"/>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11" t="s">
         <v>407</v>
       </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="11"/>
+      <c r="I15" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>412</v>
       </c>
@@ -6062,12 +6129,14 @@
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="G16" s="11"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16" s="11"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>413</v>
       </c>
@@ -6077,12 +6146,14 @@
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="G17" s="11"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17" s="11"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>416</v>
       </c>
@@ -6092,12 +6163,14 @@
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="G18" s="11"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18" s="11"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>266</v>
       </c>
@@ -6108,15 +6181,17 @@
         <v>411</v>
       </c>
       <c r="D19" s="11"/>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11" t="s">
         <v>418</v>
       </c>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="11"/>
+      <c r="I19" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>273</v>
       </c>
@@ -6127,15 +6202,17 @@
         <v>411</v>
       </c>
       <c r="D20" s="11"/>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11" t="s">
         <v>418</v>
       </c>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="11"/>
+      <c r="I20" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>269</v>
       </c>
@@ -6146,15 +6223,17 @@
         <v>411</v>
       </c>
       <c r="D21" s="11"/>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11" t="s">
         <v>419</v>
       </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="11"/>
+      <c r="I21" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>275</v>
       </c>
@@ -6165,15 +6244,17 @@
         <v>411</v>
       </c>
       <c r="D22" s="11"/>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11" t="s">
         <v>419</v>
       </c>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="11"/>
+      <c r="I22" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>274</v>
       </c>
@@ -6184,15 +6265,17 @@
         <v>411</v>
       </c>
       <c r="D23" s="11"/>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11" t="s">
         <v>413</v>
       </c>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="11"/>
+      <c r="I23" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>276</v>
       </c>
@@ -6203,15 +6286,17 @@
         <v>411</v>
       </c>
       <c r="D24" s="11"/>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11" t="s">
         <v>413</v>
       </c>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="11"/>
+      <c r="I24" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>426</v>
       </c>
@@ -6221,12 +6306,14 @@
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
-      <c r="F25" s="11" t="s">
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="G25" s="11"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I25" s="11"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>427</v>
       </c>
@@ -6236,12 +6323,14 @@
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
-      <c r="F26" s="11" t="s">
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="G26" s="11"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I26" s="11"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>420</v>
       </c>
@@ -6251,12 +6340,14 @@
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
-      <c r="F27" s="11" t="s">
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="G27" s="11"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I27" s="11"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>428</v>
       </c>
@@ -6266,12 +6357,14 @@
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
-      <c r="F28" s="11" t="s">
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="G28" s="11"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I28" s="11"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>429</v>
       </c>
@@ -6281,12 +6374,14 @@
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="G29" s="11"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I29" s="11"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>430</v>
       </c>
@@ -6296,12 +6391,14 @@
       <c r="C30" s="11"/>
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
-      <c r="F30" s="11" t="s">
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="G30" s="11"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I30" s="11"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>421</v>
       </c>
@@ -6310,15 +6407,17 @@
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
-      <c r="E31" s="13" t="s">
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="13" t="s">
         <v>449</v>
       </c>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" s="11"/>
+      <c r="I31" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>422</v>
       </c>
@@ -6327,15 +6426,17 @@
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
-      <c r="E32" s="13" t="s">
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="13" t="s">
         <v>450</v>
       </c>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="11"/>
+      <c r="I32" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>423</v>
       </c>
@@ -6344,15 +6445,17 @@
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11" t="s">
         <v>453</v>
       </c>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="11"/>
+      <c r="I33" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>424</v>
       </c>
@@ -6361,15 +6464,17 @@
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
-      <c r="E34" s="13" t="s">
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="13" t="s">
         <v>452</v>
       </c>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="11"/>
+      <c r="I34" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>425</v>
       </c>
@@ -6378,15 +6483,17 @@
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
-      <c r="E35" s="13" t="s">
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="13" t="s">
         <v>451</v>
       </c>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="11"/>
+      <c r="I35" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>442</v>
       </c>
@@ -6395,15 +6502,17 @@
       </c>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
-      <c r="E36" s="11" t="s">
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11" t="s">
         <v>446</v>
       </c>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="11"/>
+      <c r="I36" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>443</v>
       </c>
@@ -6412,15 +6521,17 @@
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11" t="s">
         <v>447</v>
       </c>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" s="11"/>
+      <c r="I37" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>456</v>
       </c>
@@ -6429,15 +6540,17 @@
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
-      <c r="E38" s="13" t="s">
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="13" t="s">
         <v>448</v>
       </c>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38" s="11"/>
+      <c r="I38" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>458</v>
       </c>
@@ -6446,15 +6559,19 @@
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
-      <c r="E39" s="13" t="s">
+      <c r="E39" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="F39" s="11"/>
+      <c r="G39" s="13" t="s">
         <v>464</v>
       </c>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" s="11"/>
+      <c r="I39" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>264</v>
       </c>
@@ -6465,15 +6582,17 @@
         <v>411</v>
       </c>
       <c r="D40" s="11"/>
-      <c r="E40" s="11" t="s">
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11" t="s">
         <v>458</v>
       </c>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40" s="11"/>
+      <c r="I40" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>339</v>
       </c>
@@ -6484,15 +6603,17 @@
         <v>411</v>
       </c>
       <c r="D41" s="11"/>
-      <c r="E41" s="11" t="s">
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11" t="s">
         <v>460</v>
       </c>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41" s="11"/>
+      <c r="I41" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>346</v>
       </c>
@@ -6503,15 +6624,17 @@
         <v>411</v>
       </c>
       <c r="D42" s="11"/>
-      <c r="E42" s="11" t="s">
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11" t="s">
         <v>461</v>
       </c>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42" s="11"/>
+      <c r="I42" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>307</v>
       </c>
@@ -6523,12 +6646,14 @@
       </c>
       <c r="D43" s="11"/>
       <c r="E43" s="11"/>
-      <c r="F43" s="11" t="s">
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="G43" s="11"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I43" s="11"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>277</v>
       </c>
@@ -6540,12 +6665,14 @@
       </c>
       <c r="D44" s="11"/>
       <c r="E44" s="11"/>
-      <c r="F44" s="11" t="s">
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="G44" s="11"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I44" s="11"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>278</v>
       </c>
@@ -6557,12 +6684,14 @@
       </c>
       <c r="D45" s="11"/>
       <c r="E45" s="11"/>
-      <c r="F45" s="11" t="s">
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="G45" s="11"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I45" s="11"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>279</v>
       </c>
@@ -6574,12 +6703,14 @@
       </c>
       <c r="D46" s="11"/>
       <c r="E46" s="11"/>
-      <c r="F46" s="11" t="s">
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="G46" s="11"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I46" s="11"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>280</v>
       </c>
@@ -6591,12 +6722,14 @@
       </c>
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>
-      <c r="F47" s="11" t="s">
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="G47" s="11"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I47" s="11"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>281</v>
       </c>
@@ -6608,12 +6741,14 @@
       </c>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
-      <c r="F48" s="11" t="s">
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="G48" s="11"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I48" s="11"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>282</v>
       </c>
@@ -6625,12 +6760,14 @@
       </c>
       <c r="D49" s="11"/>
       <c r="E49" s="11"/>
-      <c r="F49" s="11" t="s">
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="G49" s="11"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I49" s="11"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>283</v>
       </c>
@@ -6642,12 +6779,14 @@
       </c>
       <c r="D50" s="11"/>
       <c r="E50" s="11"/>
-      <c r="F50" s="11" t="s">
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="G50" s="11"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I50" s="11"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
         <v>284</v>
       </c>
@@ -6659,12 +6798,14 @@
       </c>
       <c r="D51" s="11"/>
       <c r="E51" s="11"/>
-      <c r="F51" s="11" t="s">
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="G51" s="11"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I51" s="11"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
         <v>285</v>
       </c>
@@ -6674,12 +6815,14 @@
       <c r="C52" s="11"/>
       <c r="D52" s="11"/>
       <c r="E52" s="11"/>
-      <c r="F52" s="11" t="s">
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G52" s="11"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I52" s="11"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>286</v>
       </c>
@@ -6689,12 +6832,14 @@
       <c r="C53" s="11"/>
       <c r="D53" s="11"/>
       <c r="E53" s="11"/>
-      <c r="F53" s="11" t="s">
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G53" s="11"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I53" s="11"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
         <v>292</v>
       </c>
@@ -6704,12 +6849,14 @@
       <c r="C54" s="11"/>
       <c r="D54" s="11"/>
       <c r="E54" s="11"/>
-      <c r="F54" s="11" t="s">
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G54" s="11"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I54" s="11"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
         <v>309</v>
       </c>
@@ -6719,12 +6866,14 @@
       <c r="C55" s="11"/>
       <c r="D55" s="11"/>
       <c r="E55" s="11"/>
-      <c r="F55" s="11" t="s">
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G55" s="11"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I55" s="11"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
         <v>294</v>
       </c>
@@ -6734,12 +6883,14 @@
       <c r="C56" s="11"/>
       <c r="D56" s="11"/>
       <c r="E56" s="11"/>
-      <c r="F56" s="11" t="s">
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G56" s="11"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I56" s="11"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
         <v>287</v>
       </c>
@@ -6749,12 +6900,14 @@
       <c r="C57" s="11"/>
       <c r="D57" s="11"/>
       <c r="E57" s="11"/>
-      <c r="F57" s="11" t="s">
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G57" s="11"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I57" s="11"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
         <v>295</v>
       </c>
@@ -6764,12 +6917,14 @@
       <c r="C58" s="11"/>
       <c r="D58" s="11"/>
       <c r="E58" s="11"/>
-      <c r="F58" s="11" t="s">
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G58" s="11"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I58" s="11"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
         <v>311</v>
       </c>
@@ -6779,12 +6934,14 @@
       <c r="C59" s="11"/>
       <c r="D59" s="11"/>
       <c r="E59" s="11"/>
-      <c r="F59" s="11" t="s">
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G59" s="11"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I59" s="11"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
         <v>297</v>
       </c>
@@ -6794,12 +6951,14 @@
       <c r="C60" s="11"/>
       <c r="D60" s="11"/>
       <c r="E60" s="11"/>
-      <c r="F60" s="11" t="s">
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G60" s="11"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I60" s="11"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
         <v>288</v>
       </c>
@@ -6809,12 +6968,14 @@
       <c r="C61" s="11"/>
       <c r="D61" s="11"/>
       <c r="E61" s="11"/>
-      <c r="F61" s="11" t="s">
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G61" s="11"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I61" s="11"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
         <v>298</v>
       </c>
@@ -6824,12 +6985,14 @@
       <c r="C62" s="11"/>
       <c r="D62" s="11"/>
       <c r="E62" s="11"/>
-      <c r="F62" s="11" t="s">
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G62" s="11"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I62" s="11"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
         <v>313</v>
       </c>
@@ -6839,12 +7002,14 @@
       <c r="C63" s="11"/>
       <c r="D63" s="11"/>
       <c r="E63" s="11"/>
-      <c r="F63" s="11" t="s">
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G63" s="11"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I63" s="11"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
         <v>299</v>
       </c>
@@ -6854,12 +7019,14 @@
       <c r="C64" s="11"/>
       <c r="D64" s="11"/>
       <c r="E64" s="11"/>
-      <c r="F64" s="11" t="s">
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G64" s="11"/>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I64" s="11"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
         <v>289</v>
       </c>
@@ -6869,12 +7036,14 @@
       <c r="C65" s="11"/>
       <c r="D65" s="11"/>
       <c r="E65" s="11"/>
-      <c r="F65" s="11" t="s">
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G65" s="11"/>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I65" s="11"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
         <v>300</v>
       </c>
@@ -6884,12 +7053,14 @@
       <c r="C66" s="11"/>
       <c r="D66" s="11"/>
       <c r="E66" s="11"/>
-      <c r="F66" s="11" t="s">
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G66" s="11"/>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I66" s="11"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
         <v>315</v>
       </c>
@@ -6899,12 +7070,14 @@
       <c r="C67" s="11"/>
       <c r="D67" s="11"/>
       <c r="E67" s="11"/>
-      <c r="F67" s="11" t="s">
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G67" s="11"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I67" s="11"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
         <v>302</v>
       </c>
@@ -6914,12 +7087,14 @@
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
       <c r="E68" s="11"/>
-      <c r="F68" s="11" t="s">
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G68" s="11"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I68" s="11"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
         <v>290</v>
       </c>
@@ -6929,12 +7104,14 @@
       <c r="C69" s="11"/>
       <c r="D69" s="11"/>
       <c r="E69" s="11"/>
-      <c r="F69" s="11" t="s">
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G69" s="11"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I69" s="11"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
         <v>303</v>
       </c>
@@ -6944,12 +7121,14 @@
       <c r="C70" s="11"/>
       <c r="D70" s="11"/>
       <c r="E70" s="11"/>
-      <c r="F70" s="11" t="s">
+      <c r="F70" s="11"/>
+      <c r="G70" s="11"/>
+      <c r="H70" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G70" s="11"/>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I70" s="11"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
         <v>317</v>
       </c>
@@ -6959,12 +7138,14 @@
       <c r="C71" s="11"/>
       <c r="D71" s="11"/>
       <c r="E71" s="11"/>
-      <c r="F71" s="11" t="s">
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G71" s="11"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I71" s="11"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
         <v>305</v>
       </c>
@@ -6974,12 +7155,14 @@
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
       <c r="E72" s="11"/>
-      <c r="F72" s="11" t="s">
+      <c r="F72" s="11"/>
+      <c r="G72" s="11"/>
+      <c r="H72" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G72" s="11"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I72" s="11"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
         <v>291</v>
       </c>
@@ -6989,12 +7172,14 @@
       <c r="C73" s="11"/>
       <c r="D73" s="11"/>
       <c r="E73" s="11"/>
-      <c r="F73" s="11" t="s">
+      <c r="F73" s="11"/>
+      <c r="G73" s="11"/>
+      <c r="H73" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G73" s="11"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I73" s="11"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="13" t="s">
         <v>306</v>
       </c>
@@ -7004,12 +7189,14 @@
       <c r="C74" s="11"/>
       <c r="D74" s="11"/>
       <c r="E74" s="11"/>
-      <c r="F74" s="11" t="s">
+      <c r="F74" s="11"/>
+      <c r="G74" s="11"/>
+      <c r="H74" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G74" s="11"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I74" s="11"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
         <v>319</v>
       </c>
@@ -7019,12 +7206,14 @@
       <c r="C75" s="11"/>
       <c r="D75" s="11"/>
       <c r="E75" s="11"/>
-      <c r="F75" s="11" t="s">
+      <c r="F75" s="11"/>
+      <c r="G75" s="11"/>
+      <c r="H75" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G75" s="11"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I75" s="11"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
         <v>308</v>
       </c>
@@ -7034,12 +7223,14 @@
       <c r="C76" s="11"/>
       <c r="D76" s="11"/>
       <c r="E76" s="11"/>
-      <c r="F76" s="11" t="s">
+      <c r="F76" s="11"/>
+      <c r="G76" s="11"/>
+      <c r="H76" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G76" s="11"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I76" s="11"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
         <v>310</v>
       </c>
@@ -7049,12 +7240,14 @@
       <c r="C77" s="11"/>
       <c r="D77" s="11"/>
       <c r="E77" s="11"/>
-      <c r="F77" s="11" t="s">
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G77" s="11"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I77" s="11"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
         <v>312</v>
       </c>
@@ -7064,12 +7257,14 @@
       <c r="C78" s="11"/>
       <c r="D78" s="11"/>
       <c r="E78" s="11"/>
-      <c r="F78" s="11" t="s">
+      <c r="F78" s="11"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G78" s="11"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I78" s="11"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
         <v>314</v>
       </c>
@@ -7079,12 +7274,14 @@
       <c r="C79" s="11"/>
       <c r="D79" s="11"/>
       <c r="E79" s="11"/>
-      <c r="F79" s="11" t="s">
+      <c r="F79" s="11"/>
+      <c r="G79" s="11"/>
+      <c r="H79" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G79" s="11"/>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I79" s="11"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
         <v>316</v>
       </c>
@@ -7094,12 +7291,14 @@
       <c r="C80" s="11"/>
       <c r="D80" s="11"/>
       <c r="E80" s="11"/>
-      <c r="F80" s="11" t="s">
+      <c r="F80" s="11"/>
+      <c r="G80" s="11"/>
+      <c r="H80" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G80" s="11"/>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I80" s="11"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
         <v>318</v>
       </c>
@@ -7109,12 +7308,14 @@
       <c r="C81" s="11"/>
       <c r="D81" s="11"/>
       <c r="E81" s="11"/>
-      <c r="F81" s="11" t="s">
+      <c r="F81" s="11"/>
+      <c r="G81" s="11"/>
+      <c r="H81" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G81" s="11"/>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I81" s="11"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
         <v>301</v>
       </c>
@@ -7124,12 +7325,14 @@
       <c r="C82" s="11"/>
       <c r="D82" s="11"/>
       <c r="E82" s="11"/>
-      <c r="F82" s="11" t="s">
+      <c r="F82" s="11"/>
+      <c r="G82" s="11"/>
+      <c r="H82" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G82" s="11"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I82" s="11"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
         <v>304</v>
       </c>
@@ -7139,12 +7342,14 @@
       <c r="C83" s="11"/>
       <c r="D83" s="11"/>
       <c r="E83" s="11"/>
-      <c r="F83" s="11" t="s">
+      <c r="F83" s="11"/>
+      <c r="G83" s="11"/>
+      <c r="H83" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G83" s="11"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I83" s="11"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
         <v>293</v>
       </c>
@@ -7154,12 +7359,14 @@
       <c r="C84" s="11"/>
       <c r="D84" s="11"/>
       <c r="E84" s="11"/>
-      <c r="F84" s="11" t="s">
+      <c r="F84" s="11"/>
+      <c r="G84" s="11"/>
+      <c r="H84" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G84" s="11"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I84" s="11"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
         <v>296</v>
       </c>
@@ -7169,12 +7376,14 @@
       <c r="C85" s="11"/>
       <c r="D85" s="11"/>
       <c r="E85" s="11"/>
-      <c r="F85" s="11" t="s">
+      <c r="F85" s="11"/>
+      <c r="G85" s="11"/>
+      <c r="H85" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G85" s="11"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I85" s="11"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
         <v>320</v>
       </c>
@@ -7184,12 +7393,14 @@
       <c r="C86" s="11"/>
       <c r="D86" s="11"/>
       <c r="E86" s="11"/>
-      <c r="F86" s="11" t="s">
+      <c r="F86" s="11"/>
+      <c r="G86" s="11"/>
+      <c r="H86" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="G86" s="11"/>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I86" s="11"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
         <v>322</v>
       </c>
@@ -7199,12 +7410,14 @@
       <c r="C87" s="11"/>
       <c r="D87" s="11"/>
       <c r="E87" s="11"/>
-      <c r="F87" s="11" t="s">
+      <c r="F87" s="11"/>
+      <c r="G87" s="11"/>
+      <c r="H87" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="G87" s="11"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I87" s="11"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
         <v>324</v>
       </c>
@@ -7214,12 +7427,14 @@
       <c r="C88" s="11"/>
       <c r="D88" s="11"/>
       <c r="E88" s="11"/>
-      <c r="F88" s="11" t="s">
+      <c r="F88" s="11"/>
+      <c r="G88" s="11"/>
+      <c r="H88" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="G88" s="11"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I88" s="11"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
         <v>321</v>
       </c>
@@ -7229,12 +7444,14 @@
       <c r="C89" s="11"/>
       <c r="D89" s="11"/>
       <c r="E89" s="11"/>
-      <c r="F89" s="11" t="s">
+      <c r="F89" s="11"/>
+      <c r="G89" s="11"/>
+      <c r="H89" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="G89" s="11"/>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I89" s="11"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
         <v>323</v>
       </c>
@@ -7244,12 +7461,14 @@
       <c r="C90" s="11"/>
       <c r="D90" s="11"/>
       <c r="E90" s="11"/>
-      <c r="F90" s="11" t="s">
+      <c r="F90" s="11"/>
+      <c r="G90" s="11"/>
+      <c r="H90" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="G90" s="11"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I90" s="11"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
         <v>325</v>
       </c>
@@ -7259,12 +7478,14 @@
       <c r="C91" s="11"/>
       <c r="D91" s="11"/>
       <c r="E91" s="11"/>
-      <c r="F91" s="11" t="s">
+      <c r="F91" s="11"/>
+      <c r="G91" s="11"/>
+      <c r="H91" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="G91" s="11"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I91" s="11"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
         <v>326</v>
       </c>
@@ -7274,12 +7495,14 @@
       <c r="C92" s="11"/>
       <c r="D92" s="11"/>
       <c r="E92" s="11"/>
-      <c r="F92" s="11" t="s">
+      <c r="F92" s="11"/>
+      <c r="G92" s="11"/>
+      <c r="H92" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="G92" s="11"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I92" s="11"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
         <v>328</v>
       </c>
@@ -7289,12 +7512,14 @@
       <c r="C93" s="11"/>
       <c r="D93" s="11"/>
       <c r="E93" s="11"/>
-      <c r="F93" s="11" t="s">
+      <c r="F93" s="11"/>
+      <c r="G93" s="11"/>
+      <c r="H93" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="G93" s="11"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I93" s="11"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
         <v>330</v>
       </c>
@@ -7304,12 +7529,14 @@
       <c r="C94" s="11"/>
       <c r="D94" s="11"/>
       <c r="E94" s="11"/>
-      <c r="F94" s="11" t="s">
+      <c r="F94" s="11"/>
+      <c r="G94" s="11"/>
+      <c r="H94" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="G94" s="11"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I94" s="11"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
         <v>327</v>
       </c>
@@ -7319,12 +7546,14 @@
       <c r="C95" s="11"/>
       <c r="D95" s="11"/>
       <c r="E95" s="11"/>
-      <c r="F95" s="11" t="s">
+      <c r="F95" s="11"/>
+      <c r="G95" s="11"/>
+      <c r="H95" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="G95" s="11"/>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I95" s="11"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
         <v>329</v>
       </c>
@@ -7334,12 +7563,14 @@
       <c r="C96" s="11"/>
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
-      <c r="F96" s="11" t="s">
+      <c r="F96" s="11"/>
+      <c r="G96" s="11"/>
+      <c r="H96" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="G96" s="11"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I96" s="11"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
         <v>331</v>
       </c>
@@ -7349,10 +7580,188 @@
       <c r="C97" s="11"/>
       <c r="D97" s="11"/>
       <c r="E97" s="11"/>
-      <c r="F97" s="11" t="s">
+      <c r="F97" s="11"/>
+      <c r="G97" s="11"/>
+      <c r="H97" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="G97" s="11"/>
+      <c r="I97" s="11"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E98" s="11"/>
+      <c r="F98" s="11"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E99" s="11"/>
+      <c r="F99" s="11"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E100" s="11"/>
+      <c r="F100" s="11"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E101" s="11"/>
+      <c r="F101" s="11"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E102" s="11"/>
+      <c r="F102" s="11"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E103" s="11"/>
+      <c r="F103" s="11"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E104" s="11"/>
+      <c r="F104" s="11"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E105" s="11"/>
+      <c r="F105" s="11"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E106" s="11"/>
+      <c r="F106" s="11"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E107" s="11"/>
+      <c r="F107" s="11"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E108" s="11"/>
+      <c r="F108" s="11"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E109" s="11"/>
+      <c r="F109" s="11"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E110" s="11"/>
+      <c r="F110" s="11"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E111" s="11"/>
+      <c r="F111" s="11"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E112" s="11"/>
+      <c r="F112" s="11"/>
+    </row>
+    <row r="113" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E113" s="11"/>
+      <c r="F113" s="11"/>
+    </row>
+    <row r="114" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E114" s="11"/>
+      <c r="F114" s="11"/>
+    </row>
+    <row r="115" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E115" s="11"/>
+      <c r="F115" s="11"/>
+    </row>
+    <row r="116" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E116" s="11"/>
+      <c r="F116" s="11"/>
+    </row>
+    <row r="117" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E117" s="11"/>
+      <c r="F117" s="11"/>
+    </row>
+    <row r="118" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E118" s="11"/>
+      <c r="F118" s="11"/>
+    </row>
+    <row r="119" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E119" s="11"/>
+      <c r="F119" s="11"/>
+    </row>
+    <row r="120" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E120" s="11"/>
+      <c r="F120" s="11"/>
+    </row>
+    <row r="121" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E121" s="11"/>
+      <c r="F121" s="11"/>
+    </row>
+    <row r="122" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E122" s="11"/>
+      <c r="F122" s="11"/>
+    </row>
+    <row r="123" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E123" s="11"/>
+      <c r="F123" s="11"/>
+    </row>
+    <row r="124" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E124" s="11"/>
+      <c r="F124" s="11"/>
+    </row>
+    <row r="125" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E125" s="11"/>
+      <c r="F125" s="11"/>
+    </row>
+    <row r="126" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E126" s="11"/>
+      <c r="F126" s="11"/>
+    </row>
+    <row r="127" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E127" s="11"/>
+      <c r="F127" s="11"/>
+    </row>
+    <row r="128" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E128" s="11"/>
+      <c r="F128" s="11"/>
+    </row>
+    <row r="129" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E129" s="11"/>
+      <c r="F129" s="11"/>
+    </row>
+    <row r="130" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E130" s="11"/>
+      <c r="F130" s="11"/>
+    </row>
+    <row r="131" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E131" s="11"/>
+      <c r="F131" s="11"/>
+    </row>
+    <row r="132" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E132" s="11"/>
+      <c r="F132" s="11"/>
+    </row>
+    <row r="133" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E133" s="11"/>
+      <c r="F133" s="11"/>
+    </row>
+    <row r="134" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E134" s="11"/>
+      <c r="F134" s="11"/>
+    </row>
+    <row r="135" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E135" s="11"/>
+      <c r="F135" s="11"/>
+    </row>
+    <row r="136" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E136" s="11"/>
+      <c r="F136" s="11"/>
+    </row>
+    <row r="137" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E137" s="11"/>
+      <c r="F137" s="11"/>
+    </row>
+    <row r="138" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E138" s="11"/>
+      <c r="F138" s="11"/>
+    </row>
+    <row r="139" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E139" s="11"/>
+      <c r="F139" s="11"/>
+    </row>
+    <row r="140" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E140" s="11"/>
+      <c r="F140" s="11"/>
+    </row>
+    <row r="141" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E141" s="11"/>
+      <c r="F141" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Corrections to databook and framework and TB plot
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8EA89A-45C2-434C-848B-C51993A7BE08}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCCBF33-B8B5-4180-AA6B-60381F129B73}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2636,7 +2636,7 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A9" sqref="A9:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3493,8 +3493,8 @@
   <dimension ref="A1:AO41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AJ22" sqref="AJ22:AK22"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I3" sqref="I3:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5805,10 +5805,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FC8421-05BA-4BE1-A1F1-3F12A4E7E369}">
   <dimension ref="A1:I141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="E39" sqref="E39"/>
+      <selection pane="topRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6540,7 +6540,6 @@
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
       <c r="F38" s="11"/>
       <c r="G38" s="13" t="s">
         <v>448</v>
@@ -6560,9 +6559,8 @@
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
       <c r="E39" s="11">
-        <v>0.01</v>
-      </c>
-      <c r="F39" s="11"/>
+        <v>0.1</v>
+      </c>
       <c r="G39" s="13" t="s">
         <v>464</v>
       </c>
@@ -6583,7 +6581,9 @@
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
+      <c r="F40" s="11">
+        <v>0.01</v>
+      </c>
       <c r="G40" s="11" t="s">
         <v>458</v>
       </c>

</xml_diff>

<commit_message>
Control progbook comps and pars
Project method for progbook construction has been modified to exclude using junction, source and sink compartments, while only parameters marked with attribute 'is_impact' will show in the progbook.
That said, 'is_impact' is set by default to True, so the missing column in the SIR framework file should have no effect.
In terms of the TB test case, diagnosis program impacts have been established, with the exception of the tricky latent case, while treatment program impacts must still be determined.
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACCCBF33-B8B5-4180-AA6B-60381F129B73}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B0D206-BB25-4C59-AFCD-478F5354101B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Interactions" sheetId="10" r:id="rId5"/>
     <sheet name="Parameters" sheetId="9" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179017" calcMode="manual"/>
 </workbook>
 </file>
 
@@ -637,7 +637,24 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{727369DF-9454-4254-873C-A3C5C5E58366}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{B705F57E-F9D4-4723-BD44-511C9311A224}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column is for tagging a parameter as a potential program
+impact.
+Note: This tag is only enabled for a parameter by marking the
+corresponding cell 'y'.
+Anything else, including keeping the cell blank, disables the tag.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{727369DF-9454-4254-873C-A3C5C5E58366}">
       <text>
         <r>
           <rPr>
@@ -656,7 +673,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{3514B01A-966C-4E36-8CD8-B0E499FEDBF5}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{3514B01A-966C-4E36-8CD8-B0E499FEDBF5}">
       <text>
         <r>
           <rPr>
@@ -676,7 +693,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="468">
   <si>
     <t>Code Name</t>
   </si>
@@ -2077,6 +2094,9 @@
   </si>
   <si>
     <t>Maximum Value</t>
+  </si>
+  <si>
+    <t>Is Impact</t>
   </si>
 </sst>
 </file>
@@ -2531,13 +2551,13 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="25.7109375" style="3" customWidth="1"/>
+    <col min="1" max="2" width="25.73046875" style="3" customWidth="1"/>
     <col min="3" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>74</v>
       </c>
@@ -2545,7 +2565,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="7" t="s">
         <v>76</v>
       </c>
@@ -2553,7 +2573,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="7" t="s">
         <v>78</v>
       </c>
@@ -2561,7 +2581,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="7" t="s">
         <v>80</v>
       </c>
@@ -2569,7 +2589,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="7" t="s">
         <v>82</v>
       </c>
@@ -2577,7 +2597,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
         <v>84</v>
       </c>
@@ -2585,7 +2605,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
         <v>86</v>
       </c>
@@ -2593,7 +2613,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
         <v>88</v>
       </c>
@@ -2601,7 +2621,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="7" t="s">
         <v>90</v>
       </c>
@@ -2609,7 +2629,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="7" t="s">
         <v>92</v>
       </c>
@@ -2617,7 +2637,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="7" t="s">
         <v>94</v>
       </c>
@@ -2639,19 +2659,19 @@
       <selection activeCell="A9" sqref="A9:G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.73046875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.86328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.86328125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2677,7 +2697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -2700,7 +2720,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
@@ -2721,7 +2741,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
@@ -2742,7 +2762,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
@@ -2763,7 +2783,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>19</v>
       </c>
@@ -2784,7 +2804,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
@@ -2805,7 +2825,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>21</v>
       </c>
@@ -2826,7 +2846,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>100</v>
       </c>
@@ -2847,7 +2867,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>101</v>
       </c>
@@ -2868,7 +2888,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>22</v>
       </c>
@@ -2891,7 +2911,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
@@ -2914,7 +2934,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>24</v>
       </c>
@@ -2937,7 +2957,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>25</v>
       </c>
@@ -2960,7 +2980,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>26</v>
       </c>
@@ -2981,7 +3001,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>27</v>
       </c>
@@ -3004,7 +3024,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>28</v>
       </c>
@@ -3027,7 +3047,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>29</v>
       </c>
@@ -3048,7 +3068,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>30</v>
       </c>
@@ -3071,7 +3091,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>31</v>
       </c>
@@ -3094,7 +3114,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>32</v>
       </c>
@@ -3115,7 +3135,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>33</v>
       </c>
@@ -3138,7 +3158,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
         <v>34</v>
       </c>
@@ -3161,7 +3181,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>35</v>
       </c>
@@ -3184,7 +3204,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="6" t="s">
         <v>36</v>
       </c>
@@ -3205,7 +3225,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="6" t="s">
         <v>37</v>
       </c>
@@ -3228,7 +3248,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="6" t="s">
         <v>38</v>
       </c>
@@ -3251,7 +3271,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" s="6" t="s">
         <v>39</v>
       </c>
@@ -3272,7 +3292,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
         <v>40</v>
       </c>
@@ -3295,7 +3315,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="6" t="s">
         <v>41</v>
       </c>
@@ -3318,7 +3338,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="6" t="s">
         <v>42</v>
       </c>
@@ -3339,7 +3359,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="6" t="s">
         <v>43</v>
       </c>
@@ -3360,7 +3380,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="6" t="s">
         <v>46</v>
       </c>
@@ -3383,7 +3403,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
         <v>69</v>
       </c>
@@ -3407,7 +3427,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="6" t="s">
         <v>44</v>
       </c>
@@ -3430,7 +3450,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="6" t="s">
         <v>45</v>
       </c>
@@ -3453,7 +3473,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A37" s="6" t="s">
         <v>71</v>
       </c>
@@ -3492,53 +3512,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AO41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="I3" sqref="I3:I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.86328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.73046875" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.59765625" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="6.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.73046875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6.3984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.1328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.59765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.3984375" style="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5" style="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6" style="11" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7" style="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.59765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.59765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.59765625" style="11" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8" style="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.86328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.86328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.3984375" style="11" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5" style="11" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="6" style="11" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7" style="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.59765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.59765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.59765625" style="11" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8" style="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.86328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.86328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.3984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.59765625" style="11" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="3" style="11" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="4.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="4.86328125" style="11" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="8" style="11" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="5.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.59765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="5.86328125" style="11" bestFit="1" customWidth="1"/>
     <col min="38" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.45">
       <c r="B1" s="12" t="str">
         <f>Compartments!A2</f>
         <v>sus</v>
@@ -3683,7 +3703,7 @@
       <c r="AN1" s="12"/>
       <c r="AO1" s="12"/>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="str">
         <f>Compartments!A2</f>
         <v>sus</v>
@@ -3701,7 +3721,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="str">
         <f>Compartments!A3</f>
         <v>vac</v>
@@ -3716,7 +3736,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="str">
         <f>Compartments!A4</f>
         <v>lteu</v>
@@ -3737,7 +3757,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="str">
         <f>Compartments!A5</f>
         <v>ltet</v>
@@ -3755,7 +3775,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="str">
         <f>Compartments!A6</f>
         <v>ltlu</v>
@@ -3773,7 +3793,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A7" s="12" t="str">
         <f>Compartments!A7</f>
         <v>ltlt</v>
@@ -3791,7 +3811,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A8" s="12" t="str">
         <f>Compartments!A8</f>
         <v>ltr</v>
@@ -3806,7 +3826,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="str">
         <f>Compartments!A9</f>
         <v>ltex</v>
@@ -3824,7 +3844,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A10" s="12" t="str">
         <f>Compartments!A10</f>
         <v>ltlx</v>
@@ -3839,7 +3859,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A11" s="12" t="str">
         <f>Compartments!A11</f>
         <v>acj</v>
@@ -3851,7 +3871,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A12" s="12" t="str">
         <f>Compartments!A12</f>
         <v>spj</v>
@@ -3866,7 +3886,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A13" s="12" t="str">
         <f>Compartments!A13</f>
         <v>spdu</v>
@@ -3887,7 +3907,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A14" s="12" t="str">
         <f>Compartments!A14</f>
         <v>spdd</v>
@@ -3908,7 +3928,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A15" s="12" t="str">
         <f>Compartments!A15</f>
         <v>spdt</v>
@@ -3932,7 +3952,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.45">
       <c r="A16" s="12" t="str">
         <f>Compartments!A16</f>
         <v>spmu</v>
@@ -3953,7 +3973,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A17" s="12" t="str">
         <f>Compartments!A17</f>
         <v>spmd</v>
@@ -3974,7 +3994,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A18" s="12" t="str">
         <f>Compartments!A18</f>
         <v>spmt</v>
@@ -3998,7 +4018,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A19" s="12" t="str">
         <f>Compartments!A19</f>
         <v>spxu</v>
@@ -4019,7 +4039,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A20" s="12" t="str">
         <f>Compartments!A20</f>
         <v>spxd</v>
@@ -4040,7 +4060,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A21" s="12" t="str">
         <f>Compartments!A21</f>
         <v>spxt</v>
@@ -4061,7 +4081,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A22" s="12" t="str">
         <f>Compartments!A22</f>
         <v>snj</v>
@@ -4076,7 +4096,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A23" s="12" t="str">
         <f>Compartments!A23</f>
         <v>sndu</v>
@@ -4097,7 +4117,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A24" s="12" t="str">
         <f>Compartments!A24</f>
         <v>sndd</v>
@@ -4118,7 +4138,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A25" s="12" t="str">
         <f>Compartments!A25</f>
         <v>sndt</v>
@@ -4142,7 +4162,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A26" s="12" t="str">
         <f>Compartments!A26</f>
         <v>snmu</v>
@@ -4163,7 +4183,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A27" s="12" t="str">
         <f>Compartments!A27</f>
         <v>snmd</v>
@@ -4184,7 +4204,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A28" s="12" t="str">
         <f>Compartments!A28</f>
         <v>snmt</v>
@@ -4208,7 +4228,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A29" s="12" t="str">
         <f>Compartments!A29</f>
         <v>snxu</v>
@@ -4229,7 +4249,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A30" s="12" t="str">
         <f>Compartments!A30</f>
         <v>snxd</v>
@@ -4250,7 +4270,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A31" s="12" t="str">
         <f>Compartments!A31</f>
         <v>snxt</v>
@@ -4271,7 +4291,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A32" s="12" t="str">
         <f>Compartments!A32</f>
         <v>acr</v>
@@ -4286,7 +4306,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" s="12" t="s">
         <v>46</v>
       </c>
@@ -4294,7 +4314,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="12" t="s">
         <v>69</v>
       </c>
@@ -4302,31 +4322,31 @@
         <v>256</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" s="12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" s="12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" s="12"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" s="12"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" s="12"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="12"/>
     </row>
   </sheetData>
@@ -4343,21 +4363,21 @@
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.73046875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.1328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.59765625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.86328125" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.86328125" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4384,7 +4404,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
         <v>99</v>
       </c>
@@ -4403,7 +4423,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="8" t="s">
         <v>102</v>
       </c>
@@ -4422,7 +4442,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>105</v>
       </c>
@@ -4441,7 +4461,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="8" t="s">
         <v>106</v>
       </c>
@@ -4460,7 +4480,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
         <v>107</v>
       </c>
@@ -4479,7 +4499,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>116</v>
       </c>
@@ -4501,7 +4521,7 @@
       </c>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>117</v>
       </c>
@@ -4523,7 +4543,7 @@
       </c>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>118</v>
       </c>
@@ -4545,7 +4565,7 @@
       </c>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>119</v>
       </c>
@@ -4567,7 +4587,7 @@
       </c>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>120</v>
       </c>
@@ -4589,7 +4609,7 @@
       </c>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>121</v>
       </c>
@@ -4611,7 +4631,7 @@
       </c>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
         <v>248</v>
       </c>
@@ -4633,7 +4653,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="9" t="s">
         <v>122</v>
       </c>
@@ -4655,7 +4675,7 @@
       </c>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
         <v>123</v>
       </c>
@@ -4677,7 +4697,7 @@
       </c>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>124</v>
       </c>
@@ -4699,7 +4719,7 @@
       </c>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="9" t="s">
         <v>125</v>
       </c>
@@ -4721,7 +4741,7 @@
       </c>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>126</v>
       </c>
@@ -4743,7 +4763,7 @@
       </c>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>127</v>
       </c>
@@ -4765,7 +4785,7 @@
       </c>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>140</v>
       </c>
@@ -4787,7 +4807,7 @@
       </c>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
         <v>141</v>
       </c>
@@ -4809,7 +4829,7 @@
       </c>
       <c r="I21" s="11"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>147</v>
       </c>
@@ -4831,7 +4851,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="9" t="s">
         <v>143</v>
       </c>
@@ -4853,7 +4873,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="9" t="s">
         <v>144</v>
       </c>
@@ -4875,7 +4895,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="9" t="s">
         <v>146</v>
       </c>
@@ -4894,7 +4914,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="9" t="s">
         <v>142</v>
       </c>
@@ -4916,7 +4936,7 @@
       </c>
       <c r="I26" s="11"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="9" t="s">
         <v>145</v>
       </c>
@@ -4938,7 +4958,7 @@
       </c>
       <c r="I27" s="7"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="9" t="s">
         <v>157</v>
       </c>
@@ -4960,7 +4980,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
         <v>158</v>
       </c>
@@ -4982,7 +5002,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>159</v>
       </c>
@@ -5004,7 +5024,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
         <v>160</v>
       </c>
@@ -5026,7 +5046,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="9" t="s">
         <v>161</v>
       </c>
@@ -5048,7 +5068,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="9" t="s">
         <v>162</v>
       </c>
@@ -5070,7 +5090,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
         <v>169</v>
       </c>
@@ -5092,7 +5112,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
         <v>170</v>
       </c>
@@ -5114,7 +5134,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
         <v>171</v>
       </c>
@@ -5136,7 +5156,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="9" t="s">
         <v>172</v>
       </c>
@@ -5158,7 +5178,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
         <v>173</v>
       </c>
@@ -5180,7 +5200,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>174</v>
       </c>
@@ -5202,7 +5222,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>181</v>
       </c>
@@ -5224,7 +5244,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>182</v>
       </c>
@@ -5246,7 +5266,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" s="9" t="s">
         <v>183</v>
       </c>
@@ -5268,7 +5288,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" s="9" t="s">
         <v>184</v>
       </c>
@@ -5290,7 +5310,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" s="9" t="s">
         <v>185</v>
       </c>
@@ -5312,7 +5332,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="9" t="s">
         <v>186</v>
       </c>
@@ -5334,7 +5354,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" s="9" t="s">
         <v>187</v>
       </c>
@@ -5356,7 +5376,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" s="9" t="s">
         <v>188</v>
       </c>
@@ -5378,7 +5398,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="9" t="s">
         <v>189</v>
       </c>
@@ -5400,7 +5420,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="9" t="s">
         <v>199</v>
       </c>
@@ -5422,7 +5442,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="9" t="s">
         <v>200</v>
       </c>
@@ -5444,7 +5464,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="9" t="s">
         <v>201</v>
       </c>
@@ -5466,7 +5486,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="9" t="s">
         <v>202</v>
       </c>
@@ -5488,7 +5508,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" s="9" t="s">
         <v>219</v>
       </c>
@@ -5510,7 +5530,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" s="9" t="s">
         <v>220</v>
       </c>
@@ -5532,7 +5552,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" s="9" t="s">
         <v>221</v>
       </c>
@@ -5554,7 +5574,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" s="9" t="s">
         <v>222</v>
       </c>
@@ -5576,7 +5596,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" s="9" t="s">
         <v>223</v>
       </c>
@@ -5598,7 +5618,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" s="9" t="s">
         <v>224</v>
       </c>
@@ -5620,7 +5640,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" s="9" t="s">
         <v>226</v>
       </c>
@@ -5642,7 +5662,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" s="9" t="s">
         <v>227</v>
       </c>
@@ -5664,7 +5684,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" s="9" t="s">
         <v>228</v>
       </c>
@@ -5686,7 +5706,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="62" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A62" s="14" t="s">
         <v>252</v>
       </c>
@@ -5709,7 +5729,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" s="8" t="s">
         <v>244</v>
       </c>
@@ -5731,7 +5751,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" s="9" t="s">
         <v>245</v>
       </c>
@@ -5765,15 +5785,15 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1328125" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.73046875" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -5784,7 +5804,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
         <v>462</v>
       </c>
@@ -5803,28 +5823,30 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FC8421-05BA-4BE1-A1F1-3F12A4E7E369}">
-  <dimension ref="A1:I141"/>
+  <dimension ref="A1:J141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="G11" sqref="G11"/>
+      <selection pane="topRight" activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.7109375" style="10" customWidth="1"/>
-    <col min="7" max="7" width="62" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="10"/>
+    <col min="1" max="1" width="11.46484375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.59765625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.796875" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.06640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="62.06640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -5847,13 +5869,16 @@
         <v>12</v>
       </c>
       <c r="H1" s="12" t="s">
+        <v>467</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>255</v>
       </c>
@@ -5868,11 +5893,14 @@
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
       <c r="H2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="I2" s="11"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="11"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>258</v>
       </c>
@@ -5885,11 +5913,14 @@
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
       <c r="H3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="11"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="11"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>256</v>
       </c>
@@ -5904,11 +5935,14 @@
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="H4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="I4" s="11"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="11"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>257</v>
       </c>
@@ -5921,11 +5955,14 @@
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="I5" s="11"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
         <v>263</v>
       </c>
@@ -5937,12 +5974,15 @@
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="I6" s="11"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>405</v>
       </c>
@@ -5954,12 +5994,15 @@
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="I7" s="11"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
         <v>406</v>
       </c>
@@ -5971,12 +6014,15 @@
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="I8" s="11"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
         <v>407</v>
       </c>
@@ -5988,12 +6034,15 @@
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="I9" s="11"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="11"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
         <v>265</v>
       </c>
@@ -6009,12 +6058,15 @@
       <c r="G10" s="11" t="s">
         <v>405</v>
       </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H10" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="11" t="s">
         <v>267</v>
       </c>
@@ -6030,12 +6082,15 @@
       <c r="G11" s="11" t="s">
         <v>406</v>
       </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H11" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="11" t="s">
         <v>268</v>
       </c>
@@ -6051,12 +6106,15 @@
       <c r="G12" s="11" t="s">
         <v>407</v>
       </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H12" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="11" t="s">
         <v>270</v>
       </c>
@@ -6072,12 +6130,15 @@
       <c r="G13" s="11" t="s">
         <v>405</v>
       </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="11" t="s">
         <v>271</v>
       </c>
@@ -6093,12 +6154,15 @@
       <c r="G14" s="11" t="s">
         <v>406</v>
       </c>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H14" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="11" t="s">
         <v>272</v>
       </c>
@@ -6114,12 +6178,15 @@
       <c r="G15" s="11" t="s">
         <v>407</v>
       </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H15" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
         <v>412</v>
       </c>
@@ -6131,12 +6198,15 @@
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="I16" s="11"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="11"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
         <v>413</v>
       </c>
@@ -6148,12 +6218,15 @@
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
-      <c r="H17" s="13" t="s">
+      <c r="H17" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="I17" s="11"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="11"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="11" t="s">
         <v>416</v>
       </c>
@@ -6165,12 +6238,15 @@
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
-      <c r="H18" s="13" t="s">
+      <c r="H18" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="I18" s="11"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="11"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="13" t="s">
         <v>266</v>
       </c>
@@ -6186,12 +6262,15 @@
       <c r="G19" s="11" t="s">
         <v>418</v>
       </c>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H19" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="13" t="s">
         <v>273</v>
       </c>
@@ -6207,12 +6286,15 @@
       <c r="G20" s="11" t="s">
         <v>418</v>
       </c>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="13" t="s">
         <v>269</v>
       </c>
@@ -6228,12 +6310,15 @@
       <c r="G21" s="11" t="s">
         <v>419</v>
       </c>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H21" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" s="13" t="s">
         <v>275</v>
       </c>
@@ -6249,12 +6334,15 @@
       <c r="G22" s="11" t="s">
         <v>419</v>
       </c>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H22" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" s="13" t="s">
         <v>274</v>
       </c>
@@ -6270,12 +6358,15 @@
       <c r="G23" s="11" t="s">
         <v>413</v>
       </c>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H23" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="13" t="s">
         <v>276</v>
       </c>
@@ -6291,12 +6382,15 @@
       <c r="G24" s="11" t="s">
         <v>413</v>
       </c>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H24" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="13" t="s">
         <v>426</v>
       </c>
@@ -6309,11 +6403,14 @@
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
       <c r="H25" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I25" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="I25" s="11"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="11"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" s="13" t="s">
         <v>427</v>
       </c>
@@ -6326,11 +6423,14 @@
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
       <c r="H26" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I26" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="I26" s="11"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="11"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" s="13" t="s">
         <v>420</v>
       </c>
@@ -6343,11 +6443,14 @@
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="I27" s="11"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="11"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" s="13" t="s">
         <v>428</v>
       </c>
@@ -6360,11 +6463,14 @@
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
       <c r="H28" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I28" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="I28" s="11"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" s="11"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" s="17" t="s">
         <v>429</v>
       </c>
@@ -6377,11 +6483,14 @@
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
       <c r="H29" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="I29" s="11"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" s="11"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" s="17" t="s">
         <v>430</v>
       </c>
@@ -6394,11 +6503,14 @@
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
       <c r="H30" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="I30" s="11"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" s="11"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" s="13" t="s">
         <v>421</v>
       </c>
@@ -6412,12 +6524,15 @@
       <c r="G31" s="13" t="s">
         <v>449</v>
       </c>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H31" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="13" t="s">
         <v>422</v>
       </c>
@@ -6431,12 +6546,15 @@
       <c r="G32" s="13" t="s">
         <v>450</v>
       </c>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H32" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" s="13" t="s">
         <v>423</v>
       </c>
@@ -6450,12 +6568,15 @@
       <c r="G33" s="11" t="s">
         <v>453</v>
       </c>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H33" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" s="13" t="s">
         <v>424</v>
       </c>
@@ -6469,12 +6590,15 @@
       <c r="G34" s="13" t="s">
         <v>452</v>
       </c>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H34" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" s="13" t="s">
         <v>425</v>
       </c>
@@ -6488,12 +6612,15 @@
       <c r="G35" s="13" t="s">
         <v>451</v>
       </c>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H35" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" s="13" t="s">
         <v>442</v>
       </c>
@@ -6507,12 +6634,15 @@
       <c r="G36" s="11" t="s">
         <v>446</v>
       </c>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H36" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" s="13" t="s">
         <v>443</v>
       </c>
@@ -6526,12 +6656,15 @@
       <c r="G37" s="11" t="s">
         <v>447</v>
       </c>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H37" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" s="13" t="s">
         <v>456</v>
       </c>
@@ -6544,12 +6677,15 @@
       <c r="G38" s="13" t="s">
         <v>448</v>
       </c>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H38" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" s="13" t="s">
         <v>458</v>
       </c>
@@ -6564,12 +6700,15 @@
       <c r="G39" s="13" t="s">
         <v>464</v>
       </c>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H39" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" s="11" t="s">
         <v>264</v>
       </c>
@@ -6587,12 +6726,15 @@
       <c r="G40" s="11" t="s">
         <v>458</v>
       </c>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H40" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" s="11" t="s">
         <v>339</v>
       </c>
@@ -6608,12 +6750,15 @@
       <c r="G41" s="11" t="s">
         <v>460</v>
       </c>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H41" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" s="11" t="s">
         <v>346</v>
       </c>
@@ -6629,12 +6774,15 @@
       <c r="G42" s="11" t="s">
         <v>461</v>
       </c>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H42" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" s="11" t="s">
         <v>307</v>
       </c>
@@ -6649,11 +6797,14 @@
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
       <c r="H43" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I43" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="I43" s="11"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J43" s="11"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" s="13" t="s">
         <v>277</v>
       </c>
@@ -6668,11 +6819,14 @@
       <c r="F44" s="11"/>
       <c r="G44" s="11"/>
       <c r="H44" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I44" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="I44" s="11"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J44" s="11"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" s="13" t="s">
         <v>278</v>
       </c>
@@ -6687,11 +6841,14 @@
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
       <c r="H45" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I45" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="I45" s="11"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" s="11"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" s="13" t="s">
         <v>279</v>
       </c>
@@ -6706,11 +6863,14 @@
       <c r="F46" s="11"/>
       <c r="G46" s="11"/>
       <c r="H46" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I46" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="I46" s="11"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46" s="11"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" s="13" t="s">
         <v>280</v>
       </c>
@@ -6725,11 +6885,14 @@
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
       <c r="H47" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I47" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="I47" s="11"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J47" s="11"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" s="13" t="s">
         <v>281</v>
       </c>
@@ -6744,11 +6907,14 @@
       <c r="F48" s="11"/>
       <c r="G48" s="11"/>
       <c r="H48" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I48" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="I48" s="11"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J48" s="11"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A49" s="13" t="s">
         <v>282</v>
       </c>
@@ -6763,11 +6929,14 @@
       <c r="F49" s="11"/>
       <c r="G49" s="11"/>
       <c r="H49" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I49" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="I49" s="11"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J49" s="11"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50" s="13" t="s">
         <v>283</v>
       </c>
@@ -6782,11 +6951,14 @@
       <c r="F50" s="11"/>
       <c r="G50" s="11"/>
       <c r="H50" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I50" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="I50" s="11"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J50" s="11"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" s="13" t="s">
         <v>284</v>
       </c>
@@ -6801,11 +6973,14 @@
       <c r="F51" s="11"/>
       <c r="G51" s="11"/>
       <c r="H51" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I51" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="I51" s="11"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51" s="11"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52" s="13" t="s">
         <v>285</v>
       </c>
@@ -6818,11 +6993,14 @@
       <c r="F52" s="11"/>
       <c r="G52" s="11"/>
       <c r="H52" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I52" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I52" s="11"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J52" s="11"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53" s="13" t="s">
         <v>286</v>
       </c>
@@ -6835,11 +7013,14 @@
       <c r="F53" s="11"/>
       <c r="G53" s="11"/>
       <c r="H53" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I53" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I53" s="11"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J53" s="11"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" s="13" t="s">
         <v>292</v>
       </c>
@@ -6852,11 +7033,14 @@
       <c r="F54" s="11"/>
       <c r="G54" s="11"/>
       <c r="H54" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I54" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I54" s="11"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J54" s="11"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55" s="13" t="s">
         <v>309</v>
       </c>
@@ -6869,11 +7053,14 @@
       <c r="F55" s="11"/>
       <c r="G55" s="11"/>
       <c r="H55" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I55" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I55" s="11"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J55" s="11"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" s="13" t="s">
         <v>294</v>
       </c>
@@ -6886,11 +7073,14 @@
       <c r="F56" s="11"/>
       <c r="G56" s="11"/>
       <c r="H56" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I56" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I56" s="11"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J56" s="11"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57" s="13" t="s">
         <v>287</v>
       </c>
@@ -6903,11 +7093,14 @@
       <c r="F57" s="11"/>
       <c r="G57" s="11"/>
       <c r="H57" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I57" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I57" s="11"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J57" s="11"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58" s="13" t="s">
         <v>295</v>
       </c>
@@ -6920,11 +7113,14 @@
       <c r="F58" s="11"/>
       <c r="G58" s="11"/>
       <c r="H58" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I58" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I58" s="11"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J58" s="11"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59" s="13" t="s">
         <v>311</v>
       </c>
@@ -6937,11 +7133,14 @@
       <c r="F59" s="11"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I59" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I59" s="11"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J59" s="11"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60" s="13" t="s">
         <v>297</v>
       </c>
@@ -6954,11 +7153,14 @@
       <c r="F60" s="11"/>
       <c r="G60" s="11"/>
       <c r="H60" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I60" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I60" s="11"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J60" s="11"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A61" s="13" t="s">
         <v>288</v>
       </c>
@@ -6971,11 +7173,14 @@
       <c r="F61" s="11"/>
       <c r="G61" s="11"/>
       <c r="H61" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I61" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I61" s="11"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J61" s="11"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62" s="13" t="s">
         <v>298</v>
       </c>
@@ -6988,11 +7193,14 @@
       <c r="F62" s="11"/>
       <c r="G62" s="11"/>
       <c r="H62" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I62" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I62" s="11"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J62" s="11"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A63" s="13" t="s">
         <v>313</v>
       </c>
@@ -7005,11 +7213,14 @@
       <c r="F63" s="11"/>
       <c r="G63" s="11"/>
       <c r="H63" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I63" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I63" s="11"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J63" s="11"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A64" s="13" t="s">
         <v>299</v>
       </c>
@@ -7022,11 +7233,14 @@
       <c r="F64" s="11"/>
       <c r="G64" s="11"/>
       <c r="H64" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I64" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I64" s="11"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J64" s="11"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A65" s="13" t="s">
         <v>289</v>
       </c>
@@ -7039,11 +7253,14 @@
       <c r="F65" s="11"/>
       <c r="G65" s="11"/>
       <c r="H65" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I65" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I65" s="11"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J65" s="11"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A66" s="13" t="s">
         <v>300</v>
       </c>
@@ -7056,11 +7273,14 @@
       <c r="F66" s="11"/>
       <c r="G66" s="11"/>
       <c r="H66" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I66" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I66" s="11"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J66" s="11"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A67" s="13" t="s">
         <v>315</v>
       </c>
@@ -7073,11 +7293,14 @@
       <c r="F67" s="11"/>
       <c r="G67" s="11"/>
       <c r="H67" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I67" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I67" s="11"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J67" s="11"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A68" s="13" t="s">
         <v>302</v>
       </c>
@@ -7090,11 +7313,14 @@
       <c r="F68" s="11"/>
       <c r="G68" s="11"/>
       <c r="H68" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I68" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I68" s="11"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J68" s="11"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A69" s="13" t="s">
         <v>290</v>
       </c>
@@ -7107,11 +7333,14 @@
       <c r="F69" s="11"/>
       <c r="G69" s="11"/>
       <c r="H69" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I69" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I69" s="11"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J69" s="11"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A70" s="13" t="s">
         <v>303</v>
       </c>
@@ -7124,11 +7353,14 @@
       <c r="F70" s="11"/>
       <c r="G70" s="11"/>
       <c r="H70" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I70" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I70" s="11"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J70" s="11"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A71" s="13" t="s">
         <v>317</v>
       </c>
@@ -7141,11 +7373,14 @@
       <c r="F71" s="11"/>
       <c r="G71" s="11"/>
       <c r="H71" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I71" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I71" s="11"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J71" s="11"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A72" s="13" t="s">
         <v>305</v>
       </c>
@@ -7158,11 +7393,14 @@
       <c r="F72" s="11"/>
       <c r="G72" s="11"/>
       <c r="H72" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I72" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I72" s="11"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J72" s="11"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A73" s="13" t="s">
         <v>291</v>
       </c>
@@ -7175,11 +7413,14 @@
       <c r="F73" s="11"/>
       <c r="G73" s="11"/>
       <c r="H73" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I73" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I73" s="11"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J73" s="11"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A74" s="13" t="s">
         <v>306</v>
       </c>
@@ -7192,11 +7433,14 @@
       <c r="F74" s="11"/>
       <c r="G74" s="11"/>
       <c r="H74" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I74" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I74" s="11"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J74" s="11"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A75" s="13" t="s">
         <v>319</v>
       </c>
@@ -7209,11 +7453,14 @@
       <c r="F75" s="11"/>
       <c r="G75" s="11"/>
       <c r="H75" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I75" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="I75" s="11"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J75" s="11"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A76" s="13" t="s">
         <v>308</v>
       </c>
@@ -7226,11 +7473,14 @@
       <c r="F76" s="11"/>
       <c r="G76" s="11"/>
       <c r="H76" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I76" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="I76" s="11"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J76" s="11"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A77" s="13" t="s">
         <v>310</v>
       </c>
@@ -7243,11 +7493,14 @@
       <c r="F77" s="11"/>
       <c r="G77" s="11"/>
       <c r="H77" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I77" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="I77" s="11"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J77" s="11"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A78" s="13" t="s">
         <v>312</v>
       </c>
@@ -7260,11 +7513,14 @@
       <c r="F78" s="11"/>
       <c r="G78" s="11"/>
       <c r="H78" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I78" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="I78" s="11"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J78" s="11"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A79" s="13" t="s">
         <v>314</v>
       </c>
@@ -7277,11 +7533,14 @@
       <c r="F79" s="11"/>
       <c r="G79" s="11"/>
       <c r="H79" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I79" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="I79" s="11"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J79" s="11"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A80" s="13" t="s">
         <v>316</v>
       </c>
@@ -7294,11 +7553,14 @@
       <c r="F80" s="11"/>
       <c r="G80" s="11"/>
       <c r="H80" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I80" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="I80" s="11"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J80" s="11"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A81" s="13" t="s">
         <v>318</v>
       </c>
@@ -7311,11 +7573,14 @@
       <c r="F81" s="11"/>
       <c r="G81" s="11"/>
       <c r="H81" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I81" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="I81" s="11"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J81" s="11"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A82" s="13" t="s">
         <v>301</v>
       </c>
@@ -7328,11 +7593,14 @@
       <c r="F82" s="11"/>
       <c r="G82" s="11"/>
       <c r="H82" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I82" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="I82" s="11"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J82" s="11"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A83" s="13" t="s">
         <v>304</v>
       </c>
@@ -7345,11 +7613,14 @@
       <c r="F83" s="11"/>
       <c r="G83" s="11"/>
       <c r="H83" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I83" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="I83" s="11"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J83" s="11"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A84" s="13" t="s">
         <v>293</v>
       </c>
@@ -7362,11 +7633,14 @@
       <c r="F84" s="11"/>
       <c r="G84" s="11"/>
       <c r="H84" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I84" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="I84" s="11"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J84" s="11"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A85" s="13" t="s">
         <v>296</v>
       </c>
@@ -7379,11 +7653,14 @@
       <c r="F85" s="11"/>
       <c r="G85" s="11"/>
       <c r="H85" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I85" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="I85" s="11"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J85" s="11"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A86" s="13" t="s">
         <v>320</v>
       </c>
@@ -7396,11 +7673,14 @@
       <c r="F86" s="11"/>
       <c r="G86" s="11"/>
       <c r="H86" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I86" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="I86" s="11"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J86" s="11"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A87" s="13" t="s">
         <v>322</v>
       </c>
@@ -7413,11 +7693,14 @@
       <c r="F87" s="11"/>
       <c r="G87" s="11"/>
       <c r="H87" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I87" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="I87" s="11"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J87" s="11"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A88" s="13" t="s">
         <v>324</v>
       </c>
@@ -7430,11 +7713,14 @@
       <c r="F88" s="11"/>
       <c r="G88" s="11"/>
       <c r="H88" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I88" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="I88" s="11"/>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J88" s="11"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A89" s="13" t="s">
         <v>321</v>
       </c>
@@ -7447,11 +7733,14 @@
       <c r="F89" s="11"/>
       <c r="G89" s="11"/>
       <c r="H89" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I89" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="I89" s="11"/>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J89" s="11"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A90" s="13" t="s">
         <v>323</v>
       </c>
@@ -7464,11 +7753,14 @@
       <c r="F90" s="11"/>
       <c r="G90" s="11"/>
       <c r="H90" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I90" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="I90" s="11"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J90" s="11"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A91" s="13" t="s">
         <v>325</v>
       </c>
@@ -7481,11 +7773,14 @@
       <c r="F91" s="11"/>
       <c r="G91" s="11"/>
       <c r="H91" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I91" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="I91" s="11"/>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J91" s="11"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A92" s="13" t="s">
         <v>326</v>
       </c>
@@ -7498,11 +7793,14 @@
       <c r="F92" s="11"/>
       <c r="G92" s="11"/>
       <c r="H92" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I92" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="I92" s="11"/>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J92" s="11"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A93" s="13" t="s">
         <v>328</v>
       </c>
@@ -7515,11 +7813,14 @@
       <c r="F93" s="11"/>
       <c r="G93" s="11"/>
       <c r="H93" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I93" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="I93" s="11"/>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J93" s="11"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A94" s="13" t="s">
         <v>330</v>
       </c>
@@ -7532,11 +7833,14 @@
       <c r="F94" s="11"/>
       <c r="G94" s="11"/>
       <c r="H94" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I94" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="I94" s="11"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J94" s="11"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A95" s="13" t="s">
         <v>327</v>
       </c>
@@ -7549,11 +7853,14 @@
       <c r="F95" s="11"/>
       <c r="G95" s="11"/>
       <c r="H95" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I95" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="I95" s="11"/>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J95" s="11"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A96" s="13" t="s">
         <v>329</v>
       </c>
@@ -7566,11 +7873,14 @@
       <c r="F96" s="11"/>
       <c r="G96" s="11"/>
       <c r="H96" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I96" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="I96" s="11"/>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J96" s="11"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A97" s="13" t="s">
         <v>331</v>
       </c>
@@ -7583,187 +7893,195 @@
       <c r="F97" s="11"/>
       <c r="G97" s="11"/>
       <c r="H97" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I97" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="I97" s="11"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J97" s="11"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E98" s="11"/>
       <c r="F98" s="11"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E99" s="11"/>
       <c r="F99" s="11"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E100" s="11"/>
       <c r="F100" s="11"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E101" s="11"/>
       <c r="F101" s="11"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E102" s="11"/>
       <c r="F102" s="11"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E103" s="11"/>
       <c r="F103" s="11"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E104" s="11"/>
       <c r="F104" s="11"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E105" s="11"/>
       <c r="F105" s="11"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E106" s="11"/>
       <c r="F106" s="11"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E107" s="11"/>
       <c r="F107" s="11"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E108" s="11"/>
       <c r="F108" s="11"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E109" s="11"/>
       <c r="F109" s="11"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E110" s="11"/>
       <c r="F110" s="11"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E111" s="11"/>
       <c r="F111" s="11"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.45">
       <c r="E112" s="11"/>
       <c r="F112" s="11"/>
     </row>
-    <row r="113" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E113" s="11"/>
       <c r="F113" s="11"/>
     </row>
-    <row r="114" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E114" s="11"/>
       <c r="F114" s="11"/>
     </row>
-    <row r="115" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E115" s="11"/>
       <c r="F115" s="11"/>
     </row>
-    <row r="116" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E116" s="11"/>
       <c r="F116" s="11"/>
     </row>
-    <row r="117" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E117" s="11"/>
       <c r="F117" s="11"/>
     </row>
-    <row r="118" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E118" s="11"/>
       <c r="F118" s="11"/>
     </row>
-    <row r="119" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E119" s="11"/>
       <c r="F119" s="11"/>
     </row>
-    <row r="120" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E120" s="11"/>
       <c r="F120" s="11"/>
     </row>
-    <row r="121" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E121" s="11"/>
       <c r="F121" s="11"/>
     </row>
-    <row r="122" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E122" s="11"/>
       <c r="F122" s="11"/>
     </row>
-    <row r="123" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E123" s="11"/>
       <c r="F123" s="11"/>
     </row>
-    <row r="124" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E124" s="11"/>
       <c r="F124" s="11"/>
     </row>
-    <row r="125" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E125" s="11"/>
       <c r="F125" s="11"/>
     </row>
-    <row r="126" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E126" s="11"/>
       <c r="F126" s="11"/>
     </row>
-    <row r="127" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E127" s="11"/>
       <c r="F127" s="11"/>
     </row>
-    <row r="128" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E128" s="11"/>
       <c r="F128" s="11"/>
     </row>
-    <row r="129" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E129" s="11"/>
       <c r="F129" s="11"/>
     </row>
-    <row r="130" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E130" s="11"/>
       <c r="F130" s="11"/>
     </row>
-    <row r="131" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E131" s="11"/>
       <c r="F131" s="11"/>
     </row>
-    <row r="132" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E132" s="11"/>
       <c r="F132" s="11"/>
     </row>
-    <row r="133" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E133" s="11"/>
       <c r="F133" s="11"/>
     </row>
-    <row r="134" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E134" s="11"/>
       <c r="F134" s="11"/>
     </row>
-    <row r="135" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E135" s="11"/>
       <c r="F135" s="11"/>
     </row>
-    <row r="136" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E136" s="11"/>
       <c r="F136" s="11"/>
     </row>
-    <row r="137" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E137" s="11"/>
       <c r="F137" s="11"/>
     </row>
-    <row r="138" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E138" s="11"/>
       <c r="F138" s="11"/>
     </row>
-    <row r="139" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E139" s="11"/>
       <c r="F139" s="11"/>
     </row>
-    <row r="140" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E140" s="11"/>
       <c r="F140" s="11"/>
     </row>
-    <row r="141" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="5:6" x14ac:dyDescent="0.45">
       <c r="E141" s="11"/>
       <c r="F141" s="11"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H97" xr:uid="{5D10CA16-7EA3-4965-B521-FB9DA3769325}">
+      <formula1>"n,y"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Framework columns that tag calibrations
Compartments, characteristics and parameters now include a 'Can Calibrate' column to mark whether certain data can be excluded or included in calibration lists down the track.
By default, everything can be calibrated, to compensate for framework files that exclude the column entirely.
Note: No extra validation has been designed at the parsing point for this tag.
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B0D206-BB25-4C59-AFCD-478F5354101B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C5FF4F-0784-46F2-BB38-013DA9601FAF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Interactions" sheetId="10" r:id="rId5"/>
     <sheet name="Parameters" sheetId="9" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="179017" calcMode="manual"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -237,7 +237,21 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{36495753-86C4-4D54-89E3-C16AFFF3861C}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{869F18E1-69A8-42C9-BF2D-C42D4CA0C4DD}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column marks whether compartment size data can be rescaled
+during model calibration processes.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{36495753-86C4-4D54-89E3-C16AFFF3861C}">
       <text>
         <r>
           <rPr>
@@ -256,7 +270,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{B326D675-59B6-4C74-8331-BE959611E5E2}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{B326D675-59B6-4C74-8331-BE959611E5E2}">
       <text>
         <r>
           <rPr>
@@ -411,7 +425,21 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{F5D33B24-8673-47D8-A17D-383D1B97E311}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{263C29E0-F4CF-42D1-BF7B-7209668D3ED8}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column marks whether characteristic size data can be rescaled
+during model calibration processes.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{F5D33B24-8673-47D8-A17D-383D1B97E311}">
       <text>
         <r>
           <rPr>
@@ -430,7 +458,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{4BB96F35-C249-49AE-9FB6-7C63D4CCA4CC}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{4BB96F35-C249-49AE-9FB6-7C63D4CCA4CC}">
       <text>
         <r>
           <rPr>
@@ -654,7 +682,21 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{727369DF-9454-4254-873C-A3C5C5E58366}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{F3F24D97-004C-4CFA-91E0-739256AD85A9}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column marks whether parameter data can be rescaled
+during model calibration processes.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{727369DF-9454-4254-873C-A3C5C5E58366}">
       <text>
         <r>
           <rPr>
@@ -673,7 +715,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{3514B01A-966C-4E36-8CD8-B0E499FEDBF5}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{3514B01A-966C-4E36-8CD8-B0E499FEDBF5}">
       <text>
         <r>
           <rPr>
@@ -693,7 +735,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1269" uniqueCount="469">
   <si>
     <t>Code Name</t>
   </si>
@@ -2097,6 +2139,9 @@
   </si>
   <si>
     <t>Is Impact</t>
+  </si>
+  <si>
+    <t>Can Calibrate</t>
   </si>
 </sst>
 </file>
@@ -2653,10 +2698,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:G9"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2667,11 +2712,12 @@
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.3984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.86328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.86328125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2691,13 +2737,16 @@
         <v>6</v>
       </c>
       <c r="G1" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -2716,11 +2765,14 @@
       <c r="F2" s="7">
         <v>0</v>
       </c>
-      <c r="H2" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
@@ -2738,10 +2790,13 @@
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
@@ -2759,10 +2814,13 @@
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
@@ -2780,10 +2838,13 @@
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>19</v>
       </c>
@@ -2801,10 +2862,13 @@
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
@@ -2822,10 +2886,13 @@
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>21</v>
       </c>
@@ -2843,10 +2910,13 @@
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>100</v>
       </c>
@@ -2864,10 +2934,13 @@
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>101</v>
       </c>
@@ -2885,10 +2958,13 @@
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>22</v>
       </c>
@@ -2907,11 +2983,14 @@
       <c r="F11" s="7">
         <v>0</v>
       </c>
-      <c r="H11" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G11" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
@@ -2930,11 +3009,14 @@
       <c r="F12" s="7">
         <v>0</v>
       </c>
-      <c r="H12" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G12" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>24</v>
       </c>
@@ -2953,11 +3035,14 @@
       <c r="F13" s="7">
         <v>0</v>
       </c>
-      <c r="H13" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>25</v>
       </c>
@@ -2976,11 +3061,14 @@
       <c r="F14" s="7">
         <v>0</v>
       </c>
-      <c r="H14" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G14" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>26</v>
       </c>
@@ -2998,10 +3086,13 @@
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>27</v>
       </c>
@@ -3020,11 +3111,14 @@
       <c r="F16" s="7">
         <v>0</v>
       </c>
-      <c r="H16" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>28</v>
       </c>
@@ -3043,11 +3137,14 @@
       <c r="F17" s="7">
         <v>0</v>
       </c>
-      <c r="H17" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G17" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>29</v>
       </c>
@@ -3065,10 +3162,13 @@
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>30</v>
       </c>
@@ -3087,11 +3187,14 @@
       <c r="F19" s="7">
         <v>0</v>
       </c>
-      <c r="H19" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G19" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>31</v>
       </c>
@@ -3110,11 +3213,14 @@
       <c r="F20" s="7">
         <v>0</v>
       </c>
-      <c r="H20" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>32</v>
       </c>
@@ -3132,10 +3238,13 @@
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>33</v>
       </c>
@@ -3154,11 +3263,14 @@
       <c r="F22" s="7">
         <v>0</v>
       </c>
-      <c r="H22" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G22" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
         <v>34</v>
       </c>
@@ -3177,11 +3289,14 @@
       <c r="F23" s="7">
         <v>0</v>
       </c>
-      <c r="H23" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G23" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I23" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>35</v>
       </c>
@@ -3200,11 +3315,14 @@
       <c r="F24" s="7">
         <v>0</v>
       </c>
-      <c r="H24" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G24" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="6" t="s">
         <v>36</v>
       </c>
@@ -3222,10 +3340,13 @@
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="6" t="s">
         <v>37</v>
       </c>
@@ -3244,11 +3365,14 @@
       <c r="F26" s="7">
         <v>0</v>
       </c>
-      <c r="H26" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G26" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I26" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="6" t="s">
         <v>38</v>
       </c>
@@ -3267,11 +3391,14 @@
       <c r="F27" s="7">
         <v>0</v>
       </c>
-      <c r="H27" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G27" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="6" t="s">
         <v>39</v>
       </c>
@@ -3289,10 +3416,13 @@
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
         <v>40</v>
       </c>
@@ -3311,11 +3441,14 @@
       <c r="F29" s="7">
         <v>0</v>
       </c>
-      <c r="H29" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G29" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="6" t="s">
         <v>41</v>
       </c>
@@ -3334,11 +3467,14 @@
       <c r="F30" s="7">
         <v>0</v>
       </c>
-      <c r="H30" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G30" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="6" t="s">
         <v>42</v>
       </c>
@@ -3356,10 +3492,13 @@
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="6" t="s">
         <v>43</v>
       </c>
@@ -3377,10 +3516,13 @@
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="6" t="s">
         <v>46</v>
       </c>
@@ -3399,11 +3541,14 @@
       <c r="F33" s="4">
         <v>0</v>
       </c>
-      <c r="H33" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G33" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I33" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
         <v>69</v>
       </c>
@@ -3422,12 +3567,15 @@
       <c r="F34" s="4">
         <v>0</v>
       </c>
-      <c r="G34" s="11"/>
-      <c r="H34" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G34" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H34" s="11"/>
+      <c r="I34" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="6" t="s">
         <v>44</v>
       </c>
@@ -3446,11 +3594,14 @@
       <c r="F35" s="4">
         <v>0</v>
       </c>
-      <c r="H35" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G35" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I35" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="6" t="s">
         <v>45</v>
       </c>
@@ -3469,11 +3620,14 @@
       <c r="F36" s="4">
         <v>0</v>
       </c>
-      <c r="H36" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="G36" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I36" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A37" s="6" t="s">
         <v>71</v>
       </c>
@@ -3492,15 +3646,33 @@
       <c r="F37" s="4">
         <v>0</v>
       </c>
-      <c r="G37" s="11"/>
-      <c r="H37" s="7">
-        <v>-1</v>
-      </c>
+      <c r="G37" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37" s="11"/>
+      <c r="I37" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="G38" s="11"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="G39" s="11"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="G40" s="11"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="G41" s="11"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:E37" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"n,y"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G41" xr:uid="{DCB3B7DD-854D-40C7-95E9-815E0D3B9B15}">
+      <formula1>"y,n"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4357,10 +4529,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D29B4020-084C-4F00-B628-93D126F8BCA7}">
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4372,12 +4544,13 @@
     <col min="5" max="5" width="11.59765625" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.73046875" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.86328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.86328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="3"/>
+    <col min="8" max="8" width="11.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.86328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4397,14 +4570,17 @@
       <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
         <v>99</v>
       </c>
@@ -4418,12 +4594,15 @@
       <c r="G2" s="7">
         <v>0</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="8" t="s">
         <v>102</v>
       </c>
@@ -4437,12 +4616,15 @@
       <c r="G3" s="11">
         <v>0</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="7"/>
+      <c r="J3" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>105</v>
       </c>
@@ -4456,12 +4638,15 @@
       <c r="G4" s="11">
         <v>0</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="8" t="s">
         <v>106</v>
       </c>
@@ -4475,12 +4660,15 @@
       <c r="G5" s="11">
         <v>0</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
         <v>107</v>
       </c>
@@ -4494,12 +4682,15 @@
       <c r="G6" s="11">
         <v>0</v>
       </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>116</v>
       </c>
@@ -4517,11 +4708,14 @@
         <v>1</v>
       </c>
       <c r="H7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>117</v>
       </c>
@@ -4539,11 +4733,14 @@
         <v>1</v>
       </c>
       <c r="H8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>118</v>
       </c>
@@ -4561,11 +4758,14 @@
         <v>1</v>
       </c>
       <c r="H9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>119</v>
       </c>
@@ -4583,11 +4783,14 @@
         <v>1</v>
       </c>
       <c r="H10" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>120</v>
       </c>
@@ -4605,11 +4808,14 @@
         <v>1</v>
       </c>
       <c r="H11" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>121</v>
       </c>
@@ -4627,11 +4833,14 @@
         <v>1</v>
       </c>
       <c r="H12" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
         <v>248</v>
       </c>
@@ -4648,12 +4857,15 @@
       <c r="G13" s="7">
         <v>0</v>
       </c>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="9" t="s">
         <v>122</v>
       </c>
@@ -4671,11 +4883,14 @@
         <v>1</v>
       </c>
       <c r="H14" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
         <v>123</v>
       </c>
@@ -4693,11 +4908,14 @@
         <v>1</v>
       </c>
       <c r="H15" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>124</v>
       </c>
@@ -4715,11 +4933,14 @@
         <v>1</v>
       </c>
       <c r="H16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="9" t="s">
         <v>125</v>
       </c>
@@ -4737,11 +4958,14 @@
         <v>1</v>
       </c>
       <c r="H17" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>126</v>
       </c>
@@ -4759,11 +4983,14 @@
         <v>1</v>
       </c>
       <c r="H18" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>127</v>
       </c>
@@ -4781,11 +5008,14 @@
         <v>1</v>
       </c>
       <c r="H19" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="I19" s="7"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>140</v>
       </c>
@@ -4803,11 +5033,14 @@
         <v>1</v>
       </c>
       <c r="H20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="I20" s="7"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
         <v>141</v>
       </c>
@@ -4825,11 +5058,14 @@
         <v>1</v>
       </c>
       <c r="H21" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="I21" s="11"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J21" s="11"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>147</v>
       </c>
@@ -4846,12 +5082,15 @@
       <c r="G22" s="11">
         <v>0</v>
       </c>
-      <c r="H22" s="7"/>
-      <c r="I22" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H22" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="7"/>
+      <c r="J22" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" s="9" t="s">
         <v>143</v>
       </c>
@@ -4868,12 +5107,15 @@
       <c r="G23" s="11">
         <v>0</v>
       </c>
-      <c r="H23" s="7"/>
-      <c r="I23" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H23" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I23" s="7"/>
+      <c r="J23" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="9" t="s">
         <v>144</v>
       </c>
@@ -4890,12 +5132,15 @@
       <c r="G24" s="11">
         <v>0</v>
       </c>
-      <c r="H24" s="7"/>
-      <c r="I24" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H24" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="7"/>
+      <c r="J24" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="9" t="s">
         <v>146</v>
       </c>
@@ -4909,12 +5154,15 @@
       <c r="G25" s="11">
         <v>0</v>
       </c>
-      <c r="H25" s="7"/>
-      <c r="I25" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H25" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I25" s="7"/>
+      <c r="J25" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" s="9" t="s">
         <v>142</v>
       </c>
@@ -4932,11 +5180,14 @@
         <v>1</v>
       </c>
       <c r="H26" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I26" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="I26" s="11"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J26" s="11"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" s="9" t="s">
         <v>145</v>
       </c>
@@ -4954,11 +5205,14 @@
         <v>1</v>
       </c>
       <c r="H27" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="I27" s="7"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J27" s="7"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" s="9" t="s">
         <v>157</v>
       </c>
@@ -4975,12 +5229,15 @@
       <c r="G28" s="7">
         <v>0</v>
       </c>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H28" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
         <v>158</v>
       </c>
@@ -4997,12 +5254,15 @@
       <c r="G29" s="11">
         <v>0</v>
       </c>
-      <c r="H29" s="7"/>
-      <c r="I29" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H29" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29" s="7"/>
+      <c r="J29" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>159</v>
       </c>
@@ -5019,12 +5279,15 @@
       <c r="G30" s="11">
         <v>0</v>
       </c>
-      <c r="H30" s="7"/>
-      <c r="I30" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H30" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="7"/>
+      <c r="J30" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
         <v>160</v>
       </c>
@@ -5041,12 +5304,15 @@
       <c r="G31" s="11">
         <v>0</v>
       </c>
-      <c r="H31" s="7"/>
-      <c r="I31" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H31" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31" s="7"/>
+      <c r="J31" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="9" t="s">
         <v>161</v>
       </c>
@@ -5063,12 +5329,15 @@
       <c r="G32" s="11">
         <v>0</v>
       </c>
-      <c r="H32" s="7"/>
-      <c r="I32" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H32" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I32" s="7"/>
+      <c r="J32" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" s="9" t="s">
         <v>162</v>
       </c>
@@ -5085,12 +5354,15 @@
       <c r="G33" s="11">
         <v>0</v>
       </c>
-      <c r="H33" s="7"/>
-      <c r="I33" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H33" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I33" s="7"/>
+      <c r="J33" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
         <v>169</v>
       </c>
@@ -5107,12 +5379,15 @@
       <c r="G34" s="11">
         <v>0</v>
       </c>
-      <c r="H34" s="7"/>
-      <c r="I34" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H34" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" s="7"/>
+      <c r="J34" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
         <v>170</v>
       </c>
@@ -5129,12 +5404,15 @@
       <c r="G35" s="11">
         <v>0</v>
       </c>
-      <c r="H35" s="7"/>
-      <c r="I35" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H35" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I35" s="7"/>
+      <c r="J35" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
         <v>171</v>
       </c>
@@ -5151,12 +5429,15 @@
       <c r="G36" s="11">
         <v>0</v>
       </c>
-      <c r="H36" s="7"/>
-      <c r="I36" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H36" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I36" s="7"/>
+      <c r="J36" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" s="9" t="s">
         <v>172</v>
       </c>
@@ -5173,12 +5454,15 @@
       <c r="G37" s="11">
         <v>0</v>
       </c>
-      <c r="H37" s="7"/>
-      <c r="I37" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H37" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="7"/>
+      <c r="J37" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
         <v>173</v>
       </c>
@@ -5195,12 +5479,15 @@
       <c r="G38" s="11">
         <v>0</v>
       </c>
-      <c r="H38" s="7"/>
-      <c r="I38" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H38" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I38" s="7"/>
+      <c r="J38" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>174</v>
       </c>
@@ -5217,12 +5504,15 @@
       <c r="G39" s="11">
         <v>0</v>
       </c>
-      <c r="H39" s="7"/>
-      <c r="I39" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H39" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I39" s="7"/>
+      <c r="J39" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>181</v>
       </c>
@@ -5239,12 +5529,15 @@
       <c r="G40" s="11">
         <v>0</v>
       </c>
-      <c r="H40" s="7"/>
-      <c r="I40" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H40" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I40" s="7"/>
+      <c r="J40" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>182</v>
       </c>
@@ -5261,12 +5554,15 @@
       <c r="G41" s="11">
         <v>0</v>
       </c>
-      <c r="H41" s="7"/>
-      <c r="I41" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H41" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I41" s="7"/>
+      <c r="J41" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" s="9" t="s">
         <v>183</v>
       </c>
@@ -5283,12 +5579,15 @@
       <c r="G42" s="11">
         <v>0</v>
       </c>
-      <c r="H42" s="7"/>
-      <c r="I42" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H42" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I42" s="7"/>
+      <c r="J42" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" s="9" t="s">
         <v>184</v>
       </c>
@@ -5305,12 +5604,15 @@
       <c r="G43" s="11">
         <v>0</v>
       </c>
-      <c r="H43" s="7"/>
-      <c r="I43" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H43" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I43" s="7"/>
+      <c r="J43" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" s="9" t="s">
         <v>185</v>
       </c>
@@ -5327,12 +5629,15 @@
       <c r="G44" s="11">
         <v>0</v>
       </c>
-      <c r="H44" s="7"/>
-      <c r="I44" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H44" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I44" s="7"/>
+      <c r="J44" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" s="9" t="s">
         <v>186</v>
       </c>
@@ -5349,12 +5654,15 @@
       <c r="G45" s="11">
         <v>0</v>
       </c>
-      <c r="H45" s="7"/>
-      <c r="I45" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H45" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I45" s="7"/>
+      <c r="J45" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" s="9" t="s">
         <v>187</v>
       </c>
@@ -5371,12 +5679,15 @@
       <c r="G46" s="11">
         <v>0</v>
       </c>
-      <c r="H46" s="7"/>
-      <c r="I46" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H46" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I46" s="7"/>
+      <c r="J46" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" s="9" t="s">
         <v>188</v>
       </c>
@@ -5393,12 +5704,15 @@
       <c r="G47" s="11">
         <v>0</v>
       </c>
-      <c r="H47" s="7"/>
-      <c r="I47" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H47" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I47" s="7"/>
+      <c r="J47" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" s="9" t="s">
         <v>189</v>
       </c>
@@ -5415,12 +5729,15 @@
       <c r="G48" s="11">
         <v>0</v>
       </c>
-      <c r="H48" s="7"/>
-      <c r="I48" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H48" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I48" s="7"/>
+      <c r="J48" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A49" s="9" t="s">
         <v>199</v>
       </c>
@@ -5437,12 +5754,15 @@
       <c r="G49" s="11">
         <v>0</v>
       </c>
-      <c r="H49" s="7"/>
-      <c r="I49" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H49" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I49" s="7"/>
+      <c r="J49" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50" s="9" t="s">
         <v>200</v>
       </c>
@@ -5459,12 +5779,15 @@
       <c r="G50" s="11">
         <v>0</v>
       </c>
-      <c r="H50" s="7"/>
-      <c r="I50" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H50" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I50" s="7"/>
+      <c r="J50" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" s="9" t="s">
         <v>201</v>
       </c>
@@ -5481,12 +5804,15 @@
       <c r="G51" s="11">
         <v>0</v>
       </c>
-      <c r="H51" s="7"/>
-      <c r="I51" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H51" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I51" s="7"/>
+      <c r="J51" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52" s="9" t="s">
         <v>202</v>
       </c>
@@ -5503,12 +5829,15 @@
       <c r="G52" s="11">
         <v>0</v>
       </c>
-      <c r="H52" s="7"/>
-      <c r="I52" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H52" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I52" s="7"/>
+      <c r="J52" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53" s="9" t="s">
         <v>219</v>
       </c>
@@ -5525,12 +5854,15 @@
       <c r="G53" s="11">
         <v>0</v>
       </c>
-      <c r="H53" s="7"/>
-      <c r="I53" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H53" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I53" s="7"/>
+      <c r="J53" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" s="9" t="s">
         <v>220</v>
       </c>
@@ -5547,12 +5879,15 @@
       <c r="G54" s="11">
         <v>0</v>
       </c>
-      <c r="H54" s="7"/>
-      <c r="I54" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H54" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I54" s="7"/>
+      <c r="J54" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55" s="9" t="s">
         <v>221</v>
       </c>
@@ -5569,12 +5904,15 @@
       <c r="G55" s="11">
         <v>0</v>
       </c>
-      <c r="H55" s="7"/>
-      <c r="I55" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H55" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I55" s="7"/>
+      <c r="J55" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" s="9" t="s">
         <v>222</v>
       </c>
@@ -5591,12 +5929,15 @@
       <c r="G56" s="11">
         <v>0</v>
       </c>
-      <c r="H56" s="7"/>
-      <c r="I56" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H56" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I56" s="7"/>
+      <c r="J56" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57" s="9" t="s">
         <v>223</v>
       </c>
@@ -5613,12 +5954,15 @@
       <c r="G57" s="11">
         <v>0</v>
       </c>
-      <c r="H57" s="7"/>
-      <c r="I57" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H57" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I57" s="7"/>
+      <c r="J57" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58" s="9" t="s">
         <v>224</v>
       </c>
@@ -5635,12 +5979,15 @@
       <c r="G58" s="11">
         <v>0</v>
       </c>
-      <c r="H58" s="7"/>
-      <c r="I58" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H58" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I58" s="7"/>
+      <c r="J58" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59" s="9" t="s">
         <v>226</v>
       </c>
@@ -5657,12 +6004,15 @@
       <c r="G59" s="11">
         <v>0</v>
       </c>
-      <c r="H59" s="7"/>
-      <c r="I59" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H59" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I59" s="7"/>
+      <c r="J59" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60" s="9" t="s">
         <v>227</v>
       </c>
@@ -5679,12 +6029,15 @@
       <c r="G60" s="11">
         <v>0</v>
       </c>
-      <c r="H60" s="7"/>
-      <c r="I60" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H60" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I60" s="7"/>
+      <c r="J60" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A61" s="9" t="s">
         <v>228</v>
       </c>
@@ -5701,12 +6054,15 @@
       <c r="G61" s="11">
         <v>0</v>
       </c>
-      <c r="H61" s="7"/>
-      <c r="I61" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="H61" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I61" s="7"/>
+      <c r="J61" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A62" s="14" t="s">
         <v>252</v>
       </c>
@@ -5724,12 +6080,15 @@
       <c r="G62" s="11">
         <v>0</v>
       </c>
-      <c r="H62" s="11"/>
-      <c r="I62" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H62" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I62" s="11"/>
+      <c r="J62" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A63" s="8" t="s">
         <v>244</v>
       </c>
@@ -5746,12 +6105,15 @@
       <c r="G63" s="11">
         <v>0</v>
       </c>
-      <c r="H63" s="7"/>
-      <c r="I63" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H63" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I63" s="7"/>
+      <c r="J63" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A64" s="9" t="s">
         <v>245</v>
       </c>
@@ -5767,11 +6129,40 @@
       <c r="G64" s="11">
         <v>0</v>
       </c>
-      <c r="I64" s="11">
-        <v>-1</v>
-      </c>
+      <c r="H64" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J64" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="65" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="H65" s="11"/>
+    </row>
+    <row r="66" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="H66" s="11"/>
+    </row>
+    <row r="67" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="H67" s="11"/>
+    </row>
+    <row r="68" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="H68" s="11"/>
+    </row>
+    <row r="69" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="H69" s="11"/>
+    </row>
+    <row r="70" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="H70" s="11"/>
+    </row>
+    <row r="71" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="H71" s="11"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H71" xr:uid="{CE581F04-42C4-4377-AC3C-1080BAA29A3F}">
+      <formula1>"y,n"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -5823,12 +6214,12 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FC8421-05BA-4BE1-A1F1-3F12A4E7E369}">
-  <dimension ref="A1:J141"/>
+  <dimension ref="A1:K141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="G94" sqref="G94"/>
+      <selection pane="topRight" activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5841,12 +6232,13 @@
     <col min="6" max="6" width="14.06640625" style="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="62.06640625" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.1328125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.86328125" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="10"/>
+    <col min="9" max="9" width="11.46484375" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -5872,13 +6264,16 @@
         <v>467</v>
       </c>
       <c r="I1" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="11" t="s">
         <v>255</v>
       </c>
@@ -5896,11 +6291,14 @@
         <v>7</v>
       </c>
       <c r="I2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="J2" s="11"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K2" s="11"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="11" t="s">
         <v>258</v>
       </c>
@@ -5916,11 +6314,14 @@
         <v>7</v>
       </c>
       <c r="I3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="J3" s="11"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K3" s="11"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="11" t="s">
         <v>256</v>
       </c>
@@ -5938,11 +6339,14 @@
         <v>7</v>
       </c>
       <c r="I4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="J4" s="11"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K4" s="11"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="11" t="s">
         <v>257</v>
       </c>
@@ -5958,11 +6362,14 @@
         <v>7</v>
       </c>
       <c r="I5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="J5" s="11"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K5" s="11"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
         <v>263</v>
       </c>
@@ -5977,12 +6384,15 @@
       <c r="H6" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="J6" s="11"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K6" s="11"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="11" t="s">
         <v>405</v>
       </c>
@@ -5997,12 +6407,15 @@
       <c r="H7" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="J7" s="11"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K7" s="11"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
         <v>406</v>
       </c>
@@ -6017,12 +6430,15 @@
       <c r="H8" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="J8" s="11"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K8" s="11"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="11" t="s">
         <v>407</v>
       </c>
@@ -6037,12 +6453,15 @@
       <c r="H9" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="J9" s="11"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K9" s="11"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="11" t="s">
         <v>265</v>
       </c>
@@ -6061,12 +6480,15 @@
       <c r="H10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I10" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="11" t="s">
         <v>267</v>
       </c>
@@ -6085,12 +6507,15 @@
       <c r="H11" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I11" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="11" t="s">
         <v>268</v>
       </c>
@@ -6109,12 +6534,15 @@
       <c r="H12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I12" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="11" t="s">
         <v>270</v>
       </c>
@@ -6133,12 +6561,15 @@
       <c r="H13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="11" t="s">
         <v>271</v>
       </c>
@@ -6157,12 +6588,15 @@
       <c r="H14" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I14" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="11" t="s">
         <v>272</v>
       </c>
@@ -6181,12 +6615,15 @@
       <c r="H15" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I15" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
         <v>412</v>
       </c>
@@ -6201,12 +6638,15 @@
       <c r="H16" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="J16" s="11"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K16" s="11"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="11" t="s">
         <v>413</v>
       </c>
@@ -6221,12 +6661,15 @@
       <c r="H17" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I17" s="13" t="s">
+      <c r="I17" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="J17" s="11"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K17" s="11"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="11" t="s">
         <v>416</v>
       </c>
@@ -6241,12 +6684,15 @@
       <c r="H18" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="13" t="s">
+      <c r="I18" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="J18" s="11"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K18" s="11"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="13" t="s">
         <v>266</v>
       </c>
@@ -6265,12 +6711,15 @@
       <c r="H19" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I19" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="13" t="s">
         <v>273</v>
       </c>
@@ -6289,12 +6738,15 @@
       <c r="H20" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="13" t="s">
         <v>269</v>
       </c>
@@ -6313,12 +6765,15 @@
       <c r="H21" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I21" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="13" t="s">
         <v>275</v>
       </c>
@@ -6337,12 +6792,15 @@
       <c r="H22" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I22" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="13" t="s">
         <v>274</v>
       </c>
@@ -6361,12 +6819,15 @@
       <c r="H23" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I23" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="13" t="s">
         <v>276</v>
       </c>
@@ -6385,12 +6846,15 @@
       <c r="H24" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I24" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="13" t="s">
         <v>426</v>
       </c>
@@ -6406,11 +6870,14 @@
         <v>7</v>
       </c>
       <c r="I25" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J25" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="J25" s="11"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K25" s="11"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="13" t="s">
         <v>427</v>
       </c>
@@ -6426,11 +6893,14 @@
         <v>7</v>
       </c>
       <c r="I26" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J26" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="J26" s="11"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K26" s="11"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="13" t="s">
         <v>420</v>
       </c>
@@ -6446,11 +6916,14 @@
         <v>7</v>
       </c>
       <c r="I27" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="J27" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="J27" s="11"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K27" s="11"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="13" t="s">
         <v>428</v>
       </c>
@@ -6466,11 +6939,14 @@
         <v>7</v>
       </c>
       <c r="I28" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="J28" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="J28" s="11"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K28" s="11"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="17" t="s">
         <v>429</v>
       </c>
@@ -6486,11 +6962,14 @@
         <v>7</v>
       </c>
       <c r="I29" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="J29" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="J29" s="11"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K29" s="11"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="17" t="s">
         <v>430</v>
       </c>
@@ -6506,11 +6985,14 @@
         <v>7</v>
       </c>
       <c r="I30" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="J30" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="J30" s="11"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K30" s="11"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="13" t="s">
         <v>421</v>
       </c>
@@ -6527,12 +7009,15 @@
       <c r="H31" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I31" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="13" t="s">
         <v>422</v>
       </c>
@@ -6549,12 +7034,15 @@
       <c r="H32" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I32" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="13" t="s">
         <v>423</v>
       </c>
@@ -6571,12 +7059,15 @@
       <c r="H33" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I33" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="13" t="s">
         <v>424</v>
       </c>
@@ -6593,12 +7084,15 @@
       <c r="H34" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I34" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" s="13" t="s">
         <v>425</v>
       </c>
@@ -6615,12 +7109,15 @@
       <c r="H35" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I35" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="13" t="s">
         <v>442</v>
       </c>
@@ -6637,12 +7134,15 @@
       <c r="H36" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I36" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="13" t="s">
         <v>443</v>
       </c>
@@ -6659,12 +7159,15 @@
       <c r="H37" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I37" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="13" t="s">
         <v>456</v>
       </c>
@@ -6680,12 +7183,15 @@
       <c r="H38" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I38" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" s="13" t="s">
         <v>458</v>
       </c>
@@ -6703,12 +7209,15 @@
       <c r="H39" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I39" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="11" t="s">
         <v>264</v>
       </c>
@@ -6729,12 +7238,15 @@
       <c r="H40" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I40" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="11" t="s">
         <v>339</v>
       </c>
@@ -6753,12 +7265,15 @@
       <c r="H41" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I41" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" s="11" t="s">
         <v>346</v>
       </c>
@@ -6777,12 +7292,15 @@
       <c r="H42" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I42" s="11"/>
-      <c r="J42" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I42" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J42" s="11"/>
+      <c r="K42" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" s="11" t="s">
         <v>307</v>
       </c>
@@ -6800,11 +7318,14 @@
         <v>7</v>
       </c>
       <c r="I43" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J43" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="J43" s="11"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K43" s="11"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" s="13" t="s">
         <v>277</v>
       </c>
@@ -6822,11 +7343,14 @@
         <v>7</v>
       </c>
       <c r="I44" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J44" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="J44" s="11"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K44" s="11"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" s="13" t="s">
         <v>278</v>
       </c>
@@ -6844,11 +7368,14 @@
         <v>7</v>
       </c>
       <c r="I45" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J45" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="J45" s="11"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K45" s="11"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" s="13" t="s">
         <v>279</v>
       </c>
@@ -6866,11 +7393,14 @@
         <v>7</v>
       </c>
       <c r="I46" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J46" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="J46" s="11"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K46" s="11"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" s="13" t="s">
         <v>280</v>
       </c>
@@ -6888,11 +7418,14 @@
         <v>7</v>
       </c>
       <c r="I47" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J47" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="J47" s="11"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K47" s="11"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" s="13" t="s">
         <v>281</v>
       </c>
@@ -6910,11 +7443,14 @@
         <v>7</v>
       </c>
       <c r="I48" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J48" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="J48" s="11"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K48" s="11"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A49" s="13" t="s">
         <v>282</v>
       </c>
@@ -6932,11 +7468,14 @@
         <v>7</v>
       </c>
       <c r="I49" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J49" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="J49" s="11"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K49" s="11"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A50" s="13" t="s">
         <v>283</v>
       </c>
@@ -6954,11 +7493,14 @@
         <v>7</v>
       </c>
       <c r="I50" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J50" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="J50" s="11"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K50" s="11"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" s="13" t="s">
         <v>284</v>
       </c>
@@ -6976,11 +7518,14 @@
         <v>7</v>
       </c>
       <c r="I51" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J51" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="J51" s="11"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K51" s="11"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52" s="13" t="s">
         <v>285</v>
       </c>
@@ -6996,11 +7541,14 @@
         <v>73</v>
       </c>
       <c r="I52" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J52" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J52" s="11"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K52" s="11"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53" s="13" t="s">
         <v>286</v>
       </c>
@@ -7016,11 +7564,14 @@
         <v>73</v>
       </c>
       <c r="I53" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J53" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J53" s="11"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K53" s="11"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54" s="13" t="s">
         <v>292</v>
       </c>
@@ -7036,11 +7587,14 @@
         <v>73</v>
       </c>
       <c r="I54" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J54" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J54" s="11"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K54" s="11"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55" s="13" t="s">
         <v>309</v>
       </c>
@@ -7056,11 +7610,14 @@
         <v>73</v>
       </c>
       <c r="I55" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J55" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J55" s="11"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K55" s="11"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A56" s="13" t="s">
         <v>294</v>
       </c>
@@ -7076,11 +7633,14 @@
         <v>73</v>
       </c>
       <c r="I56" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J56" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J56" s="11"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K56" s="11"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57" s="13" t="s">
         <v>287</v>
       </c>
@@ -7096,11 +7656,14 @@
         <v>73</v>
       </c>
       <c r="I57" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J57" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J57" s="11"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K57" s="11"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A58" s="13" t="s">
         <v>295</v>
       </c>
@@ -7116,11 +7679,14 @@
         <v>73</v>
       </c>
       <c r="I58" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J58" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J58" s="11"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K58" s="11"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A59" s="13" t="s">
         <v>311</v>
       </c>
@@ -7136,11 +7702,14 @@
         <v>73</v>
       </c>
       <c r="I59" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J59" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J59" s="11"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K59" s="11"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A60" s="13" t="s">
         <v>297</v>
       </c>
@@ -7156,11 +7725,14 @@
         <v>73</v>
       </c>
       <c r="I60" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J60" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J60" s="11"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K60" s="11"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A61" s="13" t="s">
         <v>288</v>
       </c>
@@ -7176,11 +7748,14 @@
         <v>73</v>
       </c>
       <c r="I61" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J61" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J61" s="11"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K61" s="11"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A62" s="13" t="s">
         <v>298</v>
       </c>
@@ -7196,11 +7771,14 @@
         <v>73</v>
       </c>
       <c r="I62" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J62" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J62" s="11"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K62" s="11"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A63" s="13" t="s">
         <v>313</v>
       </c>
@@ -7216,11 +7794,14 @@
         <v>73</v>
       </c>
       <c r="I63" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J63" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J63" s="11"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K63" s="11"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A64" s="13" t="s">
         <v>299</v>
       </c>
@@ -7236,11 +7817,14 @@
         <v>73</v>
       </c>
       <c r="I64" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J64" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J64" s="11"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K64" s="11"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A65" s="13" t="s">
         <v>289</v>
       </c>
@@ -7256,11 +7840,14 @@
         <v>73</v>
       </c>
       <c r="I65" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J65" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J65" s="11"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K65" s="11"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A66" s="13" t="s">
         <v>300</v>
       </c>
@@ -7276,11 +7863,14 @@
         <v>73</v>
       </c>
       <c r="I66" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J66" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J66" s="11"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K66" s="11"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A67" s="13" t="s">
         <v>315</v>
       </c>
@@ -7296,11 +7886,14 @@
         <v>73</v>
       </c>
       <c r="I67" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J67" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J67" s="11"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K67" s="11"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A68" s="13" t="s">
         <v>302</v>
       </c>
@@ -7316,11 +7909,14 @@
         <v>73</v>
       </c>
       <c r="I68" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J68" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J68" s="11"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K68" s="11"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A69" s="13" t="s">
         <v>290</v>
       </c>
@@ -7336,11 +7932,14 @@
         <v>73</v>
       </c>
       <c r="I69" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J69" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J69" s="11"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K69" s="11"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A70" s="13" t="s">
         <v>303</v>
       </c>
@@ -7356,11 +7955,14 @@
         <v>73</v>
       </c>
       <c r="I70" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J70" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J70" s="11"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K70" s="11"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A71" s="13" t="s">
         <v>317</v>
       </c>
@@ -7376,11 +7978,14 @@
         <v>73</v>
       </c>
       <c r="I71" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J71" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J71" s="11"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K71" s="11"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A72" s="13" t="s">
         <v>305</v>
       </c>
@@ -7396,11 +8001,14 @@
         <v>73</v>
       </c>
       <c r="I72" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J72" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J72" s="11"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K72" s="11"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A73" s="13" t="s">
         <v>291</v>
       </c>
@@ -7416,11 +8024,14 @@
         <v>73</v>
       </c>
       <c r="I73" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J73" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J73" s="11"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K73" s="11"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A74" s="13" t="s">
         <v>306</v>
       </c>
@@ -7436,11 +8047,14 @@
         <v>73</v>
       </c>
       <c r="I74" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J74" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J74" s="11"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K74" s="11"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A75" s="13" t="s">
         <v>319</v>
       </c>
@@ -7456,11 +8070,14 @@
         <v>73</v>
       </c>
       <c r="I75" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J75" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="J75" s="11"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K75" s="11"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A76" s="13" t="s">
         <v>308</v>
       </c>
@@ -7476,11 +8093,14 @@
         <v>7</v>
       </c>
       <c r="I76" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J76" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="J76" s="11"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K76" s="11"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A77" s="13" t="s">
         <v>310</v>
       </c>
@@ -7496,11 +8116,14 @@
         <v>7</v>
       </c>
       <c r="I77" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J77" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="J77" s="11"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K77" s="11"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A78" s="13" t="s">
         <v>312</v>
       </c>
@@ -7516,11 +8139,14 @@
         <v>7</v>
       </c>
       <c r="I78" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J78" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="J78" s="11"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K78" s="11"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A79" s="13" t="s">
         <v>314</v>
       </c>
@@ -7536,11 +8162,14 @@
         <v>7</v>
       </c>
       <c r="I79" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J79" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="J79" s="11"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K79" s="11"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A80" s="13" t="s">
         <v>316</v>
       </c>
@@ -7556,11 +8185,14 @@
         <v>7</v>
       </c>
       <c r="I80" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J80" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="J80" s="11"/>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K80" s="11"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A81" s="13" t="s">
         <v>318</v>
       </c>
@@ -7576,11 +8208,14 @@
         <v>7</v>
       </c>
       <c r="I81" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J81" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="J81" s="11"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K81" s="11"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A82" s="13" t="s">
         <v>301</v>
       </c>
@@ -7596,11 +8231,14 @@
         <v>7</v>
       </c>
       <c r="I82" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J82" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="J82" s="11"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K82" s="11"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A83" s="13" t="s">
         <v>304</v>
       </c>
@@ -7616,11 +8254,14 @@
         <v>7</v>
       </c>
       <c r="I83" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J83" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="J83" s="11"/>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K83" s="11"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A84" s="13" t="s">
         <v>293</v>
       </c>
@@ -7636,11 +8277,14 @@
         <v>7</v>
       </c>
       <c r="I84" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J84" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="J84" s="11"/>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K84" s="11"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85" s="13" t="s">
         <v>296</v>
       </c>
@@ -7656,11 +8300,14 @@
         <v>7</v>
       </c>
       <c r="I85" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J85" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="J85" s="11"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K85" s="11"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A86" s="13" t="s">
         <v>320</v>
       </c>
@@ -7676,11 +8323,14 @@
         <v>7</v>
       </c>
       <c r="I86" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J86" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="J86" s="11"/>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K86" s="11"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A87" s="13" t="s">
         <v>322</v>
       </c>
@@ -7696,11 +8346,14 @@
         <v>7</v>
       </c>
       <c r="I87" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J87" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="J87" s="11"/>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K87" s="11"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A88" s="13" t="s">
         <v>324</v>
       </c>
@@ -7716,11 +8369,14 @@
         <v>7</v>
       </c>
       <c r="I88" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J88" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="J88" s="11"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K88" s="11"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A89" s="13" t="s">
         <v>321</v>
       </c>
@@ -7736,11 +8392,14 @@
         <v>7</v>
       </c>
       <c r="I89" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J89" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="J89" s="11"/>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K89" s="11"/>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A90" s="13" t="s">
         <v>323</v>
       </c>
@@ -7756,11 +8415,14 @@
         <v>7</v>
       </c>
       <c r="I90" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J90" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="J90" s="11"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K90" s="11"/>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A91" s="13" t="s">
         <v>325</v>
       </c>
@@ -7776,11 +8438,14 @@
         <v>7</v>
       </c>
       <c r="I91" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J91" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="J91" s="11"/>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K91" s="11"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A92" s="13" t="s">
         <v>326</v>
       </c>
@@ -7796,11 +8461,14 @@
         <v>7</v>
       </c>
       <c r="I92" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J92" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="J92" s="11"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K92" s="11"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A93" s="13" t="s">
         <v>328</v>
       </c>
@@ -7816,11 +8484,14 @@
         <v>7</v>
       </c>
       <c r="I93" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J93" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="J93" s="11"/>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K93" s="11"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A94" s="13" t="s">
         <v>330</v>
       </c>
@@ -7836,11 +8507,14 @@
         <v>7</v>
       </c>
       <c r="I94" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J94" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="J94" s="11"/>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K94" s="11"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A95" s="13" t="s">
         <v>327</v>
       </c>
@@ -7856,11 +8530,14 @@
         <v>7</v>
       </c>
       <c r="I95" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J95" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="J95" s="11"/>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K95" s="11"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A96" s="13" t="s">
         <v>329</v>
       </c>
@@ -7876,11 +8553,14 @@
         <v>7</v>
       </c>
       <c r="I96" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J96" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="J96" s="11"/>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K96" s="11"/>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A97" s="13" t="s">
         <v>331</v>
       </c>
@@ -7896,190 +8576,240 @@
         <v>7</v>
       </c>
       <c r="I97" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J97" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="J97" s="11"/>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K97" s="11"/>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E98" s="11"/>
       <c r="F98" s="11"/>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I98" s="11"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E99" s="11"/>
       <c r="F99" s="11"/>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I99" s="11"/>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E100" s="11"/>
       <c r="F100" s="11"/>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I100" s="11"/>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E101" s="11"/>
       <c r="F101" s="11"/>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I101" s="11"/>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E102" s="11"/>
       <c r="F102" s="11"/>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I102" s="11"/>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E103" s="11"/>
       <c r="F103" s="11"/>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I103" s="11"/>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E104" s="11"/>
       <c r="F104" s="11"/>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I104" s="11"/>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E105" s="11"/>
       <c r="F105" s="11"/>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I105" s="11"/>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E106" s="11"/>
       <c r="F106" s="11"/>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I106" s="11"/>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E107" s="11"/>
       <c r="F107" s="11"/>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I107" s="11"/>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E108" s="11"/>
       <c r="F108" s="11"/>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I108" s="11"/>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E109" s="11"/>
       <c r="F109" s="11"/>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I109" s="11"/>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E110" s="11"/>
       <c r="F110" s="11"/>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I110" s="11"/>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E111" s="11"/>
       <c r="F111" s="11"/>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I111" s="11"/>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.45">
       <c r="E112" s="11"/>
       <c r="F112" s="11"/>
-    </row>
-    <row r="113" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I112" s="11"/>
+    </row>
+    <row r="113" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E113" s="11"/>
       <c r="F113" s="11"/>
-    </row>
-    <row r="114" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I113" s="11"/>
+    </row>
+    <row r="114" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E114" s="11"/>
       <c r="F114" s="11"/>
-    </row>
-    <row r="115" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I114" s="11"/>
+    </row>
+    <row r="115" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E115" s="11"/>
       <c r="F115" s="11"/>
-    </row>
-    <row r="116" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I115" s="11"/>
+    </row>
+    <row r="116" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E116" s="11"/>
       <c r="F116" s="11"/>
-    </row>
-    <row r="117" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I116" s="11"/>
+    </row>
+    <row r="117" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E117" s="11"/>
       <c r="F117" s="11"/>
-    </row>
-    <row r="118" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I117" s="11"/>
+    </row>
+    <row r="118" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E118" s="11"/>
       <c r="F118" s="11"/>
-    </row>
-    <row r="119" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I118" s="11"/>
+    </row>
+    <row r="119" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E119" s="11"/>
       <c r="F119" s="11"/>
-    </row>
-    <row r="120" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I119" s="11"/>
+    </row>
+    <row r="120" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E120" s="11"/>
       <c r="F120" s="11"/>
-    </row>
-    <row r="121" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I120" s="11"/>
+    </row>
+    <row r="121" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E121" s="11"/>
       <c r="F121" s="11"/>
-    </row>
-    <row r="122" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I121" s="11"/>
+    </row>
+    <row r="122" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E122" s="11"/>
       <c r="F122" s="11"/>
-    </row>
-    <row r="123" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I122" s="11"/>
+    </row>
+    <row r="123" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E123" s="11"/>
       <c r="F123" s="11"/>
-    </row>
-    <row r="124" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I123" s="11"/>
+    </row>
+    <row r="124" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E124" s="11"/>
       <c r="F124" s="11"/>
-    </row>
-    <row r="125" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I124" s="11"/>
+    </row>
+    <row r="125" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E125" s="11"/>
       <c r="F125" s="11"/>
-    </row>
-    <row r="126" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I125" s="11"/>
+    </row>
+    <row r="126" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E126" s="11"/>
       <c r="F126" s="11"/>
-    </row>
-    <row r="127" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I126" s="11"/>
+    </row>
+    <row r="127" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E127" s="11"/>
       <c r="F127" s="11"/>
-    </row>
-    <row r="128" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I127" s="11"/>
+    </row>
+    <row r="128" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E128" s="11"/>
       <c r="F128" s="11"/>
-    </row>
-    <row r="129" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I128" s="11"/>
+    </row>
+    <row r="129" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E129" s="11"/>
       <c r="F129" s="11"/>
-    </row>
-    <row r="130" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I129" s="11"/>
+    </row>
+    <row r="130" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E130" s="11"/>
       <c r="F130" s="11"/>
-    </row>
-    <row r="131" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I130" s="11"/>
+    </row>
+    <row r="131" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E131" s="11"/>
       <c r="F131" s="11"/>
-    </row>
-    <row r="132" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I131" s="11"/>
+    </row>
+    <row r="132" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E132" s="11"/>
       <c r="F132" s="11"/>
-    </row>
-    <row r="133" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I132" s="11"/>
+    </row>
+    <row r="133" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E133" s="11"/>
       <c r="F133" s="11"/>
-    </row>
-    <row r="134" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I133" s="11"/>
+    </row>
+    <row r="134" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E134" s="11"/>
       <c r="F134" s="11"/>
-    </row>
-    <row r="135" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I134" s="11"/>
+    </row>
+    <row r="135" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E135" s="11"/>
       <c r="F135" s="11"/>
-    </row>
-    <row r="136" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I135" s="11"/>
+    </row>
+    <row r="136" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E136" s="11"/>
       <c r="F136" s="11"/>
-    </row>
-    <row r="137" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I136" s="11"/>
+    </row>
+    <row r="137" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E137" s="11"/>
       <c r="F137" s="11"/>
-    </row>
-    <row r="138" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I137" s="11"/>
+    </row>
+    <row r="138" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E138" s="11"/>
       <c r="F138" s="11"/>
-    </row>
-    <row r="139" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I138" s="11"/>
+    </row>
+    <row r="139" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E139" s="11"/>
       <c r="F139" s="11"/>
-    </row>
-    <row r="140" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I139" s="11"/>
+    </row>
+    <row r="140" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E140" s="11"/>
       <c r="F140" s="11"/>
-    </row>
-    <row r="141" spans="5:6" x14ac:dyDescent="0.45">
+      <c r="I140" s="11"/>
+    </row>
+    <row r="141" spans="5:9" x14ac:dyDescent="0.45">
       <c r="E141" s="11"/>
       <c r="F141" s="11"/>
+      <c r="I141" s="11"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H97" xr:uid="{5D10CA16-7EA3-4965-B521-FB9DA3769325}">
       <formula1>"n,y"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I141" xr:uid="{92A1E8F5-AEF7-4AE4-8A9A-A8D8ADDCA859}">
+      <formula1>"y,n"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
TB cascade stages marked and minor fix
The framework filter generator has been modified slightly to sort cascade stages properly.
The TB example framework file now includes three extra characteristics that, combined with 'acr', forms a four-stage cascade.
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C5FF4F-0784-46F2-BB38-013DA9601FAF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E39B642-2A06-419E-9E05-CDA9B838CEC2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Custom Databook Pages" sheetId="7" r:id="rId1"/>
@@ -285,6 +285,33 @@
         </r>
       </text>
     </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{F1E37F34-B070-4161-97FF-AECD5CB55541}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This optional column determines what stage of a 'cascade' this
+compartment corresponds to.
+A cascade is a specific type of compartment network where entities
+flow sequentially from the first compartment to the last.
+A cascade stage is a subset of linked compartments including the
+last in the sequence, where Stage 1 denotes all compartments.
+For instance, with three compartments A, B and C, with transition
+structure A-&gt;B-&gt;C, Stage 1 is the characteristic for (A,B,C),
+Stage 2 is the characteristic for (B,C) and Stage 3 is characteristic
+and compartment (C).
+Note: As exemplified above, only one compartment should be marked as
+a stage.
+The rest should be marked on the characteristics page.
+This value is only used for convenience in plotting and the column
+can be safely deleted for non-cascade applications.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -470,6 +497,32 @@
           <t>This column currently denotes whether a databook should request
 historical values from the user for this characteristic.
 A value of '-1' suppresses it from appearing in the databook.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{3F47B776-D969-49E3-B900-41FD43A04303}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This optional column determines what stage of a 'cascade' this
+characteristic corresponds to.
+A cascade is a specific type of compartment network where entities
+flow sequentially from the first compartment to the last.
+A cascade stage is a subset of linked compartments including the
+last in the sequence, where Stage 1 denotes all compartments.
+For instance, with three compartments A, B and C, with transition
+structure A-&gt;B-&gt;C, Stage 1 is the characteristic for (A,B,C),
+Stage 2 is the characteristic for (B,C) and Stage 3 is characteristic
+and compartment (C).
+Note: As exemplified above, one stage should be marked on the
+compartment page, with the rest marked on this page.
+This value is only used for convenience in plotting and the column
+can be safely deleted for non-cascade applications.</t>
         </r>
       </text>
     </comment>
@@ -735,7 +788,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1269" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="479">
   <si>
     <t>Code Name</t>
   </si>
@@ -2142,6 +2195,36 @@
   </si>
   <si>
     <t>Can Calibrate</t>
+  </si>
+  <si>
+    <t>Cascade Stage</t>
+  </si>
+  <si>
+    <t>Estimated number of living people that developed active TB</t>
+  </si>
+  <si>
+    <t>ac_cascade</t>
+  </si>
+  <si>
+    <t>ac_inf, acr</t>
+  </si>
+  <si>
+    <t>known_cascade</t>
+  </si>
+  <si>
+    <t>Diagnosed number of living people that developed active TB</t>
+  </si>
+  <si>
+    <t>known_inf, acr</t>
+  </si>
+  <si>
+    <t>treat_cascade</t>
+  </si>
+  <si>
+    <t>Number of living people that were treated for active TB</t>
+  </si>
+  <si>
+    <t>num_treat, acr</t>
   </si>
 </sst>
 </file>
@@ -2698,10 +2781,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G37"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2715,9 +2798,10 @@
     <col min="7" max="7" width="11.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.86328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.19921875" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2745,8 +2829,11 @@
       <c r="I1" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J1" s="12" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -2772,7 +2859,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
@@ -2796,7 +2883,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
@@ -2820,7 +2907,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
@@ -2844,7 +2931,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>19</v>
       </c>
@@ -2868,7 +2955,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
@@ -2892,7 +2979,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>21</v>
       </c>
@@ -2916,7 +3003,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>100</v>
       </c>
@@ -2940,7 +3027,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>101</v>
       </c>
@@ -2964,7 +3051,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>22</v>
       </c>
@@ -2990,7 +3077,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
@@ -3016,7 +3103,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>24</v>
       </c>
@@ -3042,7 +3129,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>25</v>
       </c>
@@ -3068,7 +3155,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>26</v>
       </c>
@@ -3092,7 +3179,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>27</v>
       </c>
@@ -3118,7 +3205,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>28</v>
       </c>
@@ -3144,7 +3231,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>29</v>
       </c>
@@ -3168,7 +3255,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>30</v>
       </c>
@@ -3194,7 +3281,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>31</v>
       </c>
@@ -3220,7 +3307,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>32</v>
       </c>
@@ -3244,7 +3331,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>33</v>
       </c>
@@ -3270,7 +3357,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
         <v>34</v>
       </c>
@@ -3296,7 +3383,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>35</v>
       </c>
@@ -3322,7 +3409,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="6" t="s">
         <v>36</v>
       </c>
@@ -3346,7 +3433,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" s="6" t="s">
         <v>37</v>
       </c>
@@ -3372,7 +3459,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" s="6" t="s">
         <v>38</v>
       </c>
@@ -3398,7 +3485,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" s="6" t="s">
         <v>39</v>
       </c>
@@ -3422,7 +3509,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
         <v>40</v>
       </c>
@@ -3448,7 +3535,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" s="6" t="s">
         <v>41</v>
       </c>
@@ -3474,7 +3561,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" s="6" t="s">
         <v>42</v>
       </c>
@@ -3498,7 +3585,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="6" t="s">
         <v>43</v>
       </c>
@@ -3521,8 +3608,11 @@
       <c r="H32" s="11" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J32" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" s="6" t="s">
         <v>46</v>
       </c>
@@ -3548,7 +3638,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
         <v>69</v>
       </c>
@@ -3574,8 +3664,9 @@
       <c r="I34" s="7">
         <v>-1</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J34" s="11"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" s="6" t="s">
         <v>44</v>
       </c>
@@ -3601,7 +3692,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" s="6" t="s">
         <v>45</v>
       </c>
@@ -3627,7 +3718,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A37" s="6" t="s">
         <v>71</v>
       </c>
@@ -3653,17 +3744,18 @@
       <c r="I37" s="7">
         <v>-1</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J37" s="11"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="G38" s="11"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="G39" s="11"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="G40" s="11"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="G41" s="11"/>
     </row>
   </sheetData>
@@ -4529,10 +4621,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D29B4020-084C-4F00-B628-93D126F8BCA7}">
-  <dimension ref="A1:J71"/>
+  <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4547,10 +4639,11 @@
     <col min="8" max="8" width="11.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.86328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="3"/>
+    <col min="11" max="11" width="12.19921875" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4579,8 +4672,11 @@
       <c r="J1" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K1" s="12" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
         <v>99</v>
       </c>
@@ -4602,7 +4698,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="8" t="s">
         <v>102</v>
       </c>
@@ -4624,7 +4720,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
         <v>105</v>
       </c>
@@ -4646,7 +4742,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="8" t="s">
         <v>106</v>
       </c>
@@ -4668,7 +4764,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
         <v>107</v>
       </c>
@@ -4690,7 +4786,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>116</v>
       </c>
@@ -4715,7 +4811,7 @@
       </c>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>117</v>
       </c>
@@ -4740,7 +4836,7 @@
       </c>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="s">
         <v>118</v>
       </c>
@@ -4765,7 +4861,7 @@
       </c>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>119</v>
       </c>
@@ -4790,7 +4886,7 @@
       </c>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>120</v>
       </c>
@@ -4815,7 +4911,7 @@
       </c>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>121</v>
       </c>
@@ -4840,7 +4936,7 @@
       </c>
       <c r="J12" s="7"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="9" t="s">
         <v>248</v>
       </c>
@@ -4865,46 +4961,48 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="14" t="s">
+        <v>473</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>474</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>475</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11">
+        <v>0</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11">
+        <v>-1</v>
+      </c>
+      <c r="K14" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A15" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B15" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C15" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D15" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7">
-        <v>1</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="J14" s="7"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A15" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>117</v>
-      </c>
       <c r="F15" s="7"/>
-      <c r="G15" s="11">
+      <c r="G15" s="7">
         <v>1</v>
       </c>
       <c r="H15" s="11" t="s">
@@ -4915,18 +5013,18 @@
       </c>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="11">
@@ -4940,18 +5038,18 @@
       </c>
       <c r="J16" s="7"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="11">
@@ -4965,18 +5063,18 @@
       </c>
       <c r="J17" s="7"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="11">
@@ -4990,18 +5088,18 @@
       </c>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="11">
@@ -5015,21 +5113,21 @@
       </c>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>151</v>
+        <v>139</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>121</v>
       </c>
       <c r="F20" s="7"/>
-      <c r="G20" s="7">
+      <c r="G20" s="11">
         <v>1</v>
       </c>
       <c r="H20" s="11" t="s">
@@ -5040,21 +5138,21 @@
       </c>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F21" s="7"/>
-      <c r="G21" s="11">
+      <c r="G21" s="7">
         <v>1</v>
       </c>
       <c r="H21" s="11" t="s">
@@ -5063,45 +5161,45 @@
       <c r="I21" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="J21" s="11"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J21" s="7"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>204</v>
+        <v>149</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>122</v>
+        <v>33</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>125</v>
+        <v>152</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I22" s="7"/>
-      <c r="J22" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I22" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="J22" s="11"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="9" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="11">
@@ -5115,18 +5213,18 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="11">
@@ -5140,15 +5238,18 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>156</v>
+        <v>124</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>127</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="11">
@@ -5162,143 +5263,142 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="9" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="11">
+        <v>0</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I26" s="7"/>
+      <c r="J26" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A27" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="F27" s="7"/>
+      <c r="G27" s="11">
         <v>1</v>
       </c>
-      <c r="H26" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I26" s="11" t="s">
+      <c r="H27" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="J26" s="11"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A27" s="9" t="s">
+      <c r="J27" s="11"/>
+    </row>
+    <row r="28" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>470</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>472</v>
+      </c>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11">
+        <v>0</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11">
+        <v>-1</v>
+      </c>
+      <c r="K28" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A29" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B29" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C29" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D29" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7">
+      <c r="F29" s="7"/>
+      <c r="G29" s="7">
         <v>1</v>
       </c>
-      <c r="H27" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I27" s="11" t="s">
+      <c r="H29" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="J27" s="7"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A28" s="9" t="s">
+      <c r="J29" s="7"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A30" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B30" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C30" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D30" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7">
+      <c r="F30" s="7"/>
+      <c r="G30" s="7">
         <v>0</v>
       </c>
-      <c r="H28" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A29" s="9" t="s">
+      <c r="H30" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A31" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B31" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C31" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D31" s="13" t="s">
         <v>28</v>
-      </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="11">
-        <v>0</v>
-      </c>
-      <c r="H29" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I29" s="7"/>
-      <c r="J29" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A30" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="F30" s="7"/>
-      <c r="G30" s="11">
-        <v>0</v>
-      </c>
-      <c r="H30" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I30" s="7"/>
-      <c r="J30" s="11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A31" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>35</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="11">
@@ -5312,18 +5412,18 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="11">
@@ -5339,16 +5439,16 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="11">
@@ -5364,16 +5464,16 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>145</v>
+        <v>37</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="11">
@@ -5389,16 +5489,16 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>145</v>
+        <v>40</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="11">
@@ -5414,13 +5514,13 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E36" s="11" t="s">
         <v>145</v>
@@ -5439,13 +5539,13 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E37" s="11" t="s">
         <v>145</v>
@@ -5464,13 +5564,13 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E38" s="11" t="s">
         <v>145</v>
@@ -5489,13 +5589,13 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E39" s="11" t="s">
         <v>145</v>
@@ -5514,15 +5614,15 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="E40" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="E40" s="11" t="s">
         <v>145</v>
       </c>
       <c r="F40" s="7"/>
@@ -5539,15 +5639,15 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="E41" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="E41" s="11" t="s">
         <v>145</v>
       </c>
       <c r="F41" s="7"/>
@@ -5564,13 +5664,13 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" s="9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="E42" s="13" t="s">
         <v>145</v>
@@ -5589,13 +5689,13 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E43" s="13" t="s">
         <v>145</v>
@@ -5614,13 +5714,13 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E44" s="13" t="s">
         <v>145</v>
@@ -5639,13 +5739,13 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" s="9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E45" s="13" t="s">
         <v>145</v>
@@ -5664,13 +5764,13 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E46" s="13" t="s">
         <v>145</v>
@@ -5689,13 +5789,13 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="E47" s="13" t="s">
         <v>145</v>
@@ -5714,13 +5814,13 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="E48" s="13" t="s">
         <v>145</v>
@@ -5737,15 +5837,15 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A49" s="9" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E49" s="13" t="s">
         <v>145</v>
@@ -5762,15 +5862,15 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A50" s="9" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E50" s="13" t="s">
         <v>145</v>
@@ -5787,15 +5887,15 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="E51" s="13" t="s">
         <v>145</v>
@@ -5812,15 +5912,15 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52" s="9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E52" s="13" t="s">
         <v>145</v>
@@ -5837,18 +5937,18 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53" s="9" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D53" s="13" t="s">
-        <v>34</v>
+        <v>144</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>145</v>
       </c>
       <c r="F53" s="7"/>
       <c r="G53" s="11">
@@ -5862,18 +5962,18 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54" s="9" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>37</v>
+        <v>142</v>
+      </c>
+      <c r="E54" s="13" t="s">
+        <v>145</v>
       </c>
       <c r="F54" s="7"/>
       <c r="G54" s="11">
@@ -5887,18 +5987,18 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55" s="9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D55" s="13" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F55" s="7"/>
       <c r="G55" s="11">
@@ -5912,18 +6012,18 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A56" s="9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="D56" s="11" t="s">
-        <v>241</v>
+        <v>230</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="F56" s="7"/>
       <c r="G56" s="11">
@@ -5937,18 +6037,18 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57" s="9" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="C57" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="D57" s="11" t="s">
-        <v>242</v>
+        <v>231</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D57" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" s="11">
@@ -5962,18 +6062,18 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A58" s="9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F58" s="7"/>
       <c r="G58" s="11">
@@ -5987,18 +6087,18 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A59" s="9" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="C59" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D59" s="13" t="s">
-        <v>36</v>
+        <v>233</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>242</v>
       </c>
       <c r="F59" s="7"/>
       <c r="G59" s="11">
@@ -6012,18 +6112,18 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A60" s="9" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="C60" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D60" s="13" t="s">
-        <v>39</v>
+        <v>234</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>240</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>243</v>
       </c>
       <c r="F60" s="7"/>
       <c r="G60" s="11">
@@ -6037,18 +6137,18 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A61" s="9" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F61" s="7"/>
       <c r="G61" s="11">
@@ -6062,44 +6162,43 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="62" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="14" t="s">
-        <v>252</v>
-      </c>
-      <c r="B62" s="14" t="s">
-        <v>253</v>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A62" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>236</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>226</v>
+        <v>29</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>254</v>
-      </c>
-      <c r="E62" s="11"/>
-      <c r="F62" s="11"/>
+        <v>39</v>
+      </c>
+      <c r="F62" s="7"/>
       <c r="G62" s="11">
         <v>0</v>
       </c>
       <c r="H62" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I62" s="11"/>
+      <c r="I62" s="7"/>
       <c r="J62" s="11">
         <v>-1</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A63" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>246</v>
-      </c>
-      <c r="C63" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="E63" s="11" t="s">
-        <v>142</v>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A63" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="F63" s="7"/>
       <c r="G63" s="11">
@@ -6113,53 +6212,132 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A64" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="B64" s="9" t="s">
-        <v>247</v>
+    <row r="64" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A64" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>253</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>252</v>
-      </c>
-      <c r="E64" s="11" t="s">
-        <v>248</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="D64" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
       <c r="G64" s="11">
         <v>0</v>
       </c>
       <c r="H64" s="11" t="s">
         <v>7</v>
       </c>
+      <c r="I64" s="11"/>
       <c r="J64" s="11">
         <v>-1</v>
       </c>
-    </row>
-    <row r="65" spans="8:8" x14ac:dyDescent="0.45">
-      <c r="H65" s="11"/>
-    </row>
-    <row r="66" spans="8:8" x14ac:dyDescent="0.45">
-      <c r="H66" s="11"/>
-    </row>
-    <row r="67" spans="8:8" x14ac:dyDescent="0.45">
-      <c r="H67" s="11"/>
-    </row>
-    <row r="68" spans="8:8" x14ac:dyDescent="0.45">
+      <c r="K64" s="11"/>
+    </row>
+    <row r="65" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A65" s="14" t="s">
+        <v>476</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>477</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>478</v>
+      </c>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11">
+        <v>0</v>
+      </c>
+      <c r="H65" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I65" s="11"/>
+      <c r="J65" s="11">
+        <v>-1</v>
+      </c>
+      <c r="K65" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A66" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="E66" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="F66" s="7"/>
+      <c r="G66" s="11">
+        <v>0</v>
+      </c>
+      <c r="H66" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I66" s="7"/>
+      <c r="J66" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A67" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C67" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="E67" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="G67" s="11">
+        <v>0</v>
+      </c>
+      <c r="H67" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J67" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
       <c r="H68" s="11"/>
     </row>
-    <row r="69" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
       <c r="H69" s="11"/>
     </row>
-    <row r="70" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
       <c r="H70" s="11"/>
     </row>
-    <row r="71" spans="8:8" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
       <c r="H71" s="11"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="H72" s="11"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="H73" s="11"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="H74" s="11"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H71" xr:uid="{CE581F04-42C4-4377-AC3C-1080BAA29A3F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H74" xr:uid="{CE581F04-42C4-4377-AC3C-1080BAA29A3F}">
       <formula1>"y,n"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6216,7 +6394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FC8421-05BA-4BE1-A1F1-3F12A4E7E369}">
   <dimension ref="A1:K141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
       <selection pane="topRight" activeCell="G27" sqref="G27"/>

</xml_diff>

<commit_message>
Framework detail columns hard-coded
Aside from comments and cross-referencing, framework files can be generated but for the transitions matrix.
Note that this refers to the maximal file set-up.
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects - Work\Optima\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E39B642-2A06-419E-9E05-CDA9B838CEC2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3428F2-6987-499C-A343-7629486D633A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Custom Databook Pages" sheetId="7" r:id="rId1"/>
@@ -2783,7 +2783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
@@ -4623,9 +4623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D29B4020-084C-4F00-B628-93D126F8BCA7}">
   <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -6394,10 +6392,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FC8421-05BA-4BE1-A1F1-3F12A4E7E369}">
   <dimension ref="A1:K141"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="G27" sqref="G27"/>
+      <selection pane="topRight" activeCell="E39" sqref="E39:F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7378,9 +7376,7 @@
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
-      <c r="E39" s="11">
-        <v>0.1</v>
-      </c>
+      <c r="E39" s="11"/>
       <c r="G39" s="13" t="s">
         <v>464</v>
       </c>
@@ -7407,9 +7403,7 @@
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
-      <c r="F40" s="11">
-        <v>0.01</v>
-      </c>
+      <c r="F40" s="11"/>
       <c r="G40" s="11" t="s">
         <v>458</v>
       </c>

</xml_diff>

<commit_message>
Add back framework max/min values to match Optima TB example
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1173843A-C0C4-4839-B1B2-32B3112A4450}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167F4E0E-18C7-4DE6-AC2C-3C8EC0C0C9EA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6392,10 +6392,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FC8421-05BA-4BE1-A1F1-3F12A4E7E369}">
   <dimension ref="A1:K141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="C3" sqref="C3"/>
+      <selection pane="topRight" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7376,7 +7376,9 @@
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
+      <c r="E39" s="11">
+        <v>0.1</v>
+      </c>
       <c r="G39" s="13" t="s">
         <v>464</v>
       </c>
@@ -7403,7 +7405,9 @@
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
+      <c r="F40" s="11">
+        <v>0.01</v>
+      </c>
       <c r="G40" s="11" t="s">
         <v>458</v>
       </c>
@@ -8985,6 +8989,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove parameter limits from framework
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167F4E0E-18C7-4DE6-AC2C-3C8EC0C0C9EA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5A7C29-D688-48A3-859C-6F2F10988DD6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6392,10 +6392,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FC8421-05BA-4BE1-A1F1-3F12A4E7E369}">
   <dimension ref="A1:K141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="E33" sqref="E33"/>
+      <selection pane="topRight" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6406,7 +6406,7 @@
     <col min="4" max="4" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="62" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="71.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" style="10" bestFit="1" customWidth="1"/>
@@ -7376,9 +7376,7 @@
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
-      <c r="E39" s="11">
-        <v>0.1</v>
-      </c>
+      <c r="E39" s="11"/>
       <c r="G39" s="13" t="s">
         <v>464</v>
       </c>
@@ -7405,9 +7403,7 @@
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
-      <c r="F40" s="11">
-        <v>0.01</v>
-      </c>
+      <c r="F40" s="11"/>
       <c r="G40" s="11" t="s">
         <v>458</v>
       </c>

</xml_diff>

<commit_message>
Cascade plotting from framework working
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F03BBA-47DA-40AB-96D1-419552006D04}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645DB66D-0252-424A-A981-E45166BA7AC9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Databook Pages" sheetId="7" r:id="rId1"/>
@@ -2257,12 +2257,6 @@
     <t>Constituents</t>
   </si>
   <si>
-    <t>main cascade</t>
-  </si>
-  <si>
-    <t>secondary cascade</t>
-  </si>
-  <si>
     <t>Plot Group</t>
   </si>
   <si>
@@ -2372,6 +2366,12 @@
   </si>
   <si>
     <t>Export</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>secondary</t>
   </si>
 </sst>
 </file>
@@ -2931,7 +2931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
@@ -2977,7 +2977,7 @@
         <v>5</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -4794,7 +4794,7 @@
         <v>5</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -5005,7 +5005,7 @@
         <v>131</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="11">
@@ -5030,7 +5030,7 @@
         <v>132</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="11">
@@ -5055,7 +5055,7 @@
         <v>133</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="11">
@@ -5080,7 +5080,7 @@
         <v>241</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7">
@@ -5131,7 +5131,7 @@
         <v>134</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7">
@@ -5156,7 +5156,7 @@
         <v>135</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="11">
@@ -5181,7 +5181,7 @@
         <v>136</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="11">
@@ -5206,7 +5206,7 @@
         <v>137</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="11">
@@ -5231,7 +5231,7 @@
         <v>138</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="11">
@@ -5256,7 +5256,7 @@
         <v>139</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="11">
@@ -5281,7 +5281,7 @@
         <v>148</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7">
@@ -5306,7 +5306,7 @@
         <v>149</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="11">
@@ -5331,7 +5331,7 @@
         <v>199</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="11">
@@ -5356,7 +5356,7 @@
         <v>200</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="11">
@@ -5381,7 +5381,7 @@
         <v>201</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="11">
@@ -5431,7 +5431,7 @@
         <v>198</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="11">
@@ -5482,7 +5482,7 @@
         <v>150</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7">
@@ -5507,7 +5507,7 @@
         <v>158</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7">
@@ -5532,7 +5532,7 @@
         <v>159</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="11">
@@ -5557,7 +5557,7 @@
         <v>160</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="11">
@@ -5582,7 +5582,7 @@
         <v>161</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="11">
@@ -5607,7 +5607,7 @@
         <v>162</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="11">
@@ -5632,7 +5632,7 @@
         <v>163</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="11">
@@ -6189,7 +6189,7 @@
         <v>224</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E55" s="7"/>
       <c r="F55" s="11">
@@ -6214,7 +6214,7 @@
         <v>225</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E56" s="7"/>
       <c r="F56" s="11">
@@ -6239,7 +6239,7 @@
         <v>226</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E57" s="7"/>
       <c r="F57" s="11">
@@ -6264,7 +6264,7 @@
         <v>227</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="E58" s="7"/>
       <c r="F58" s="11">
@@ -6289,7 +6289,7 @@
         <v>228</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="E59" s="7"/>
       <c r="F59" s="11">
@@ -6314,7 +6314,7 @@
         <v>229</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E60" s="7"/>
       <c r="F60" s="11">
@@ -6339,7 +6339,7 @@
         <v>230</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="E61" s="7"/>
       <c r="F61" s="11">
@@ -6364,7 +6364,7 @@
         <v>231</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="E62" s="7"/>
       <c r="F62" s="11">
@@ -6389,7 +6389,7 @@
         <v>232</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="E63" s="7"/>
       <c r="F63" s="11">
@@ -6414,7 +6414,7 @@
         <v>243</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D64" s="11"/>
       <c r="E64" s="11"/>
@@ -6593,10 +6593,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FC8421-05BA-4BE1-A1F1-3F12A4E7E369}">
   <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="J2" sqref="J2:J97"/>
+      <selection pane="topRight" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6644,7 +6644,7 @@
         <v>457</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="K1" s="12" t="s">
         <v>96</v>
@@ -7691,9 +7691,7 @@
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
-      <c r="E39" s="11">
-        <v>0.1</v>
-      </c>
+      <c r="E39" s="11"/>
       <c r="G39" s="13" t="s">
         <v>453</v>
       </c>
@@ -7723,9 +7721,7 @@
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
-      <c r="F40" s="11">
-        <v>0.01</v>
-      </c>
+      <c r="F40" s="11"/>
       <c r="G40" s="11" t="s">
         <v>447</v>
       </c>
@@ -9534,8 +9530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{096AAE64-6D86-4469-8C78-6B6ADE320367}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9546,7 +9542,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>506</v>
+        <v>543</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>505</v>
@@ -9587,7 +9583,7 @@
     <row r="6" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>507</v>
+        <v>544</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>505</v>
@@ -9661,7 +9657,7 @@
         <v>494</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -9675,7 +9671,7 @@
         <v>145</v>
       </c>
       <c r="F2" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9689,7 +9685,7 @@
         <v>107</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -9802,7 +9798,7 @@
         <v>488</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -9860,7 +9856,7 @@
         <v>99</v>
       </c>
       <c r="F18" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Copy default values from Gauteng
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08456FC2-B9DB-4293-8084-56888B642BF2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D6C502-8CE3-4CFD-9E2A-B03B5C9C1CCA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Databook Pages" sheetId="7" r:id="rId1"/>
@@ -2527,7 +2527,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2575,6 +2575,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
@@ -6686,17 +6690,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FC8421-05BA-4BE1-A1F1-3F12A4E7E369}">
   <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="E33" sqref="E33"/>
+      <selection pane="topRight" activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="10" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="10" bestFit="1" customWidth="1"/>
@@ -6862,7 +6866,9 @@
         <v>321</v>
       </c>
       <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
+      <c r="D6" s="13">
+        <v>0.88</v>
+      </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
@@ -6888,7 +6894,9 @@
         <v>397</v>
       </c>
       <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="D7" s="11">
+        <v>0</v>
+      </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
@@ -6914,7 +6922,9 @@
         <v>398</v>
       </c>
       <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
+      <c r="D8" s="11">
+        <v>0</v>
+      </c>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
@@ -6940,7 +6950,9 @@
         <v>399</v>
       </c>
       <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="D9" s="11">
+        <v>0</v>
+      </c>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
@@ -7146,7 +7158,9 @@
         <v>403</v>
       </c>
       <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
+      <c r="D16" s="11">
+        <v>0.2</v>
+      </c>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
@@ -7172,7 +7186,9 @@
         <v>404</v>
       </c>
       <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
+      <c r="D17" s="11">
+        <v>3.0000000000000001E-3</v>
+      </c>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
@@ -7198,7 +7214,9 @@
         <v>406</v>
       </c>
       <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
+      <c r="D18" s="11">
+        <v>0.17699999999999999</v>
+      </c>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
@@ -7404,7 +7422,9 @@
         <v>420</v>
       </c>
       <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
+      <c r="D25" s="11">
+        <v>0.5</v>
+      </c>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
@@ -7430,7 +7450,9 @@
         <v>421</v>
       </c>
       <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
+      <c r="D26" s="11">
+        <v>0.5</v>
+      </c>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
@@ -7456,7 +7478,9 @@
         <v>422</v>
       </c>
       <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
+      <c r="D27" s="11">
+        <v>1</v>
+      </c>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
@@ -7482,7 +7506,9 @@
         <v>423</v>
       </c>
       <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
+      <c r="D28" s="11">
+        <v>0.22</v>
+      </c>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
@@ -7508,7 +7534,9 @@
         <v>424</v>
       </c>
       <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
+      <c r="D29" s="11">
+        <v>1</v>
+      </c>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
@@ -7534,7 +7562,9 @@
         <v>425</v>
       </c>
       <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
+      <c r="D30" s="11">
+        <v>1</v>
+      </c>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
@@ -7756,7 +7786,7 @@
         <v>446</v>
       </c>
       <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
+      <c r="D38" s="19"/>
       <c r="F38" s="11"/>
       <c r="G38" s="13" t="s">
         <v>437</v>
@@ -7783,7 +7813,7 @@
         <v>448</v>
       </c>
       <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
+      <c r="D39" s="19"/>
       <c r="E39" s="11"/>
       <c r="G39" s="13" t="s">
         <v>453</v>
@@ -7812,7 +7842,7 @@
       <c r="C40" s="11" t="s">
         <v>400</v>
       </c>
-      <c r="D40" s="11"/>
+      <c r="D40" s="19"/>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
       <c r="G40" s="11" t="s">
@@ -7842,7 +7872,7 @@
       <c r="C41" s="11" t="s">
         <v>400</v>
       </c>
-      <c r="D41" s="11"/>
+      <c r="D41" s="19"/>
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
       <c r="G41" s="11" t="s">
@@ -7872,7 +7902,7 @@
       <c r="C42" s="11" t="s">
         <v>400</v>
       </c>
-      <c r="D42" s="11"/>
+      <c r="D42" s="19"/>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
       <c r="G42" s="11" t="s">
@@ -7902,7 +7932,7 @@
       <c r="C43" s="11" t="s">
         <v>400</v>
       </c>
-      <c r="D43" s="11"/>
+      <c r="D43" s="19"/>
       <c r="E43" s="11"/>
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
@@ -7930,7 +7960,7 @@
       <c r="C44" s="11" t="s">
         <v>443</v>
       </c>
-      <c r="D44" s="11"/>
+      <c r="D44" s="19"/>
       <c r="E44" s="11"/>
       <c r="F44" s="11"/>
       <c r="G44" s="11"/>
@@ -7958,7 +7988,7 @@
       <c r="C45" s="11" t="s">
         <v>443</v>
       </c>
-      <c r="D45" s="11"/>
+      <c r="D45" s="19"/>
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
@@ -7986,7 +8016,7 @@
       <c r="C46" s="11" t="s">
         <v>443</v>
       </c>
-      <c r="D46" s="11"/>
+      <c r="D46" s="19"/>
       <c r="E46" s="11"/>
       <c r="F46" s="11"/>
       <c r="G46" s="11"/>
@@ -8014,7 +8044,7 @@
       <c r="C47" s="11" t="s">
         <v>443</v>
       </c>
-      <c r="D47" s="11"/>
+      <c r="D47" s="19"/>
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
@@ -8042,7 +8072,7 @@
       <c r="C48" s="11" t="s">
         <v>443</v>
       </c>
-      <c r="D48" s="11"/>
+      <c r="D48" s="19"/>
       <c r="E48" s="11"/>
       <c r="F48" s="11"/>
       <c r="G48" s="11"/>
@@ -8070,7 +8100,7 @@
       <c r="C49" s="11" t="s">
         <v>443</v>
       </c>
-      <c r="D49" s="11"/>
+      <c r="D49" s="19"/>
       <c r="E49" s="11"/>
       <c r="F49" s="11"/>
       <c r="G49" s="11"/>
@@ -8098,7 +8128,7 @@
       <c r="C50" s="11" t="s">
         <v>443</v>
       </c>
-      <c r="D50" s="11"/>
+      <c r="D50" s="19"/>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
       <c r="G50" s="11"/>
@@ -8126,7 +8156,7 @@
       <c r="C51" s="11" t="s">
         <v>443</v>
       </c>
-      <c r="D51" s="11"/>
+      <c r="D51" s="19"/>
       <c r="E51" s="11"/>
       <c r="F51" s="11"/>
       <c r="G51" s="11"/>
@@ -8152,8 +8182,10 @@
         <v>348</v>
       </c>
       <c r="C52" s="11"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11"/>
+      <c r="D52" s="17">
+        <v>0.59</v>
+      </c>
+      <c r="E52" s="13"/>
       <c r="F52" s="11"/>
       <c r="G52" s="11"/>
       <c r="H52" s="11" t="s">
@@ -8178,8 +8210,10 @@
         <v>349</v>
       </c>
       <c r="C53" s="11"/>
-      <c r="D53" s="11"/>
-      <c r="E53" s="11"/>
+      <c r="D53" s="17">
+        <v>0.59</v>
+      </c>
+      <c r="E53" s="13"/>
       <c r="F53" s="11"/>
       <c r="G53" s="11"/>
       <c r="H53" s="11" t="s">
@@ -8204,8 +8238,10 @@
         <v>350</v>
       </c>
       <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="11"/>
+      <c r="D54" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="E54" s="13"/>
       <c r="F54" s="11"/>
       <c r="G54" s="11"/>
       <c r="H54" s="11" t="s">
@@ -8230,8 +8266,10 @@
         <v>351</v>
       </c>
       <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
+      <c r="D55" s="17">
+        <v>0.83</v>
+      </c>
+      <c r="E55" s="13"/>
       <c r="F55" s="11"/>
       <c r="G55" s="11"/>
       <c r="H55" s="11" t="s">
@@ -8256,8 +8294,10 @@
         <v>352</v>
       </c>
       <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11"/>
+      <c r="D56" s="17">
+        <v>0.59</v>
+      </c>
+      <c r="E56" s="13"/>
       <c r="F56" s="11"/>
       <c r="G56" s="11"/>
       <c r="H56" s="11" t="s">
@@ -8282,8 +8322,10 @@
         <v>353</v>
       </c>
       <c r="C57" s="11"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
+      <c r="D57" s="17">
+        <v>0.37</v>
+      </c>
+      <c r="E57" s="13"/>
       <c r="F57" s="11"/>
       <c r="G57" s="11"/>
       <c r="H57" s="11" t="s">
@@ -8308,8 +8350,10 @@
         <v>354</v>
       </c>
       <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
+      <c r="D58" s="17">
+        <v>0.24</v>
+      </c>
+      <c r="E58" s="13"/>
       <c r="F58" s="11"/>
       <c r="G58" s="11"/>
       <c r="H58" s="11" t="s">
@@ -8334,8 +8378,10 @@
         <v>444</v>
       </c>
       <c r="C59" s="11"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="11"/>
+      <c r="D59" s="17">
+        <v>0.52</v>
+      </c>
+      <c r="E59" s="13"/>
       <c r="F59" s="11"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11" t="s">
@@ -8360,8 +8406,10 @@
         <v>355</v>
       </c>
       <c r="C60" s="11"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11"/>
+      <c r="D60" s="17">
+        <v>0.59</v>
+      </c>
+      <c r="E60" s="13"/>
       <c r="F60" s="11"/>
       <c r="G60" s="11"/>
       <c r="H60" s="11" t="s">
@@ -8386,8 +8434,10 @@
         <v>356</v>
       </c>
       <c r="C61" s="11"/>
-      <c r="D61" s="11"/>
-      <c r="E61" s="11"/>
+      <c r="D61" s="17">
+        <v>0.37</v>
+      </c>
+      <c r="E61" s="13"/>
       <c r="F61" s="11"/>
       <c r="G61" s="11"/>
       <c r="H61" s="11" t="s">
@@ -8412,8 +8462,10 @@
         <v>357</v>
       </c>
       <c r="C62" s="11"/>
-      <c r="D62" s="11"/>
-      <c r="E62" s="11"/>
+      <c r="D62" s="17">
+        <v>0.44</v>
+      </c>
+      <c r="E62" s="13"/>
       <c r="F62" s="11"/>
       <c r="G62" s="11"/>
       <c r="H62" s="11" t="s">
@@ -8438,8 +8490,10 @@
         <v>358</v>
       </c>
       <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
-      <c r="E63" s="11"/>
+      <c r="D63" s="17">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E63" s="13"/>
       <c r="F63" s="11"/>
       <c r="G63" s="11"/>
       <c r="H63" s="11" t="s">
@@ -8464,8 +8518,10 @@
         <v>359</v>
       </c>
       <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
+      <c r="D64" s="17">
+        <v>0.59</v>
+      </c>
+      <c r="E64" s="13"/>
       <c r="F64" s="11"/>
       <c r="G64" s="11"/>
       <c r="H64" s="11" t="s">
@@ -8490,8 +8546,10 @@
         <v>360</v>
       </c>
       <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="11"/>
+      <c r="D65" s="17">
+        <v>0.59</v>
+      </c>
+      <c r="E65" s="13"/>
       <c r="F65" s="11"/>
       <c r="G65" s="11"/>
       <c r="H65" s="11" t="s">
@@ -8516,8 +8574,10 @@
         <v>361</v>
       </c>
       <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
-      <c r="E66" s="11"/>
+      <c r="D66" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="E66" s="13"/>
       <c r="F66" s="11"/>
       <c r="G66" s="11"/>
       <c r="H66" s="11" t="s">
@@ -8542,8 +8602,10 @@
         <v>362</v>
       </c>
       <c r="C67" s="11"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
+      <c r="D67" s="17">
+        <v>0.83</v>
+      </c>
+      <c r="E67" s="13"/>
       <c r="F67" s="11"/>
       <c r="G67" s="11"/>
       <c r="H67" s="11" t="s">
@@ -8568,8 +8630,10 @@
         <v>363</v>
       </c>
       <c r="C68" s="11"/>
-      <c r="D68" s="11"/>
-      <c r="E68" s="11"/>
+      <c r="D68" s="17">
+        <v>0.59</v>
+      </c>
+      <c r="E68" s="13"/>
       <c r="F68" s="11"/>
       <c r="G68" s="11"/>
       <c r="H68" s="11" t="s">
@@ -8594,8 +8658,10 @@
         <v>364</v>
       </c>
       <c r="C69" s="11"/>
-      <c r="D69" s="11"/>
-      <c r="E69" s="11"/>
+      <c r="D69" s="17">
+        <v>0.37</v>
+      </c>
+      <c r="E69" s="13"/>
       <c r="F69" s="11"/>
       <c r="G69" s="11"/>
       <c r="H69" s="11" t="s">
@@ -8620,8 +8686,10 @@
         <v>365</v>
       </c>
       <c r="C70" s="11"/>
-      <c r="D70" s="11"/>
-      <c r="E70" s="11"/>
+      <c r="D70" s="17">
+        <v>0.24</v>
+      </c>
+      <c r="E70" s="13"/>
       <c r="F70" s="11"/>
       <c r="G70" s="11"/>
       <c r="H70" s="11" t="s">
@@ -8646,8 +8714,10 @@
         <v>366</v>
       </c>
       <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
-      <c r="E71" s="11"/>
+      <c r="D71" s="17">
+        <v>0.52</v>
+      </c>
+      <c r="E71" s="13"/>
       <c r="F71" s="11"/>
       <c r="G71" s="11"/>
       <c r="H71" s="11" t="s">
@@ -8672,8 +8742,10 @@
         <v>367</v>
       </c>
       <c r="C72" s="11"/>
-      <c r="D72" s="11"/>
-      <c r="E72" s="11"/>
+      <c r="D72" s="17">
+        <v>0.59</v>
+      </c>
+      <c r="E72" s="13"/>
       <c r="F72" s="11"/>
       <c r="G72" s="11"/>
       <c r="H72" s="11" t="s">
@@ -8698,8 +8770,10 @@
         <v>368</v>
       </c>
       <c r="C73" s="11"/>
-      <c r="D73" s="11"/>
-      <c r="E73" s="11"/>
+      <c r="D73" s="17">
+        <v>0.37</v>
+      </c>
+      <c r="E73" s="13"/>
       <c r="F73" s="11"/>
       <c r="G73" s="11"/>
       <c r="H73" s="11" t="s">
@@ -8724,8 +8798,10 @@
         <v>369</v>
       </c>
       <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="11"/>
+      <c r="D74" s="17">
+        <v>0.44</v>
+      </c>
+      <c r="E74" s="13"/>
       <c r="F74" s="11"/>
       <c r="G74" s="11"/>
       <c r="H74" s="11" t="s">
@@ -8750,8 +8826,10 @@
         <v>370</v>
       </c>
       <c r="C75" s="11"/>
-      <c r="D75" s="11"/>
-      <c r="E75" s="11"/>
+      <c r="D75" s="17">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E75" s="13"/>
       <c r="F75" s="11"/>
       <c r="G75" s="11"/>
       <c r="H75" s="11" t="s">
@@ -8776,8 +8854,10 @@
         <v>371</v>
       </c>
       <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
+      <c r="D76" s="17">
+        <v>0.03</v>
+      </c>
+      <c r="E76" s="13"/>
       <c r="F76" s="11"/>
       <c r="G76" s="11"/>
       <c r="H76" s="11" t="s">
@@ -8802,8 +8882,10 @@
         <v>372</v>
       </c>
       <c r="C77" s="11"/>
-      <c r="D77" s="11"/>
-      <c r="E77" s="11"/>
+      <c r="D77" s="17">
+        <v>0.03</v>
+      </c>
+      <c r="E77" s="13"/>
       <c r="F77" s="11"/>
       <c r="G77" s="11"/>
       <c r="H77" s="11" t="s">
@@ -8828,8 +8910,10 @@
         <v>373</v>
       </c>
       <c r="C78" s="11"/>
-      <c r="D78" s="11"/>
-      <c r="E78" s="11"/>
+      <c r="D78" s="17">
+        <v>0.03</v>
+      </c>
+      <c r="E78" s="13"/>
       <c r="F78" s="11"/>
       <c r="G78" s="11"/>
       <c r="H78" s="11" t="s">
@@ -8854,8 +8938,10 @@
         <v>374</v>
       </c>
       <c r="C79" s="11"/>
-      <c r="D79" s="11"/>
-      <c r="E79" s="11"/>
+      <c r="D79" s="17">
+        <v>0.16</v>
+      </c>
+      <c r="E79" s="13"/>
       <c r="F79" s="11"/>
       <c r="G79" s="11"/>
       <c r="H79" s="11" t="s">
@@ -8880,8 +8966,10 @@
         <v>375</v>
       </c>
       <c r="C80" s="11"/>
-      <c r="D80" s="11"/>
-      <c r="E80" s="11"/>
+      <c r="D80" s="17">
+        <v>0.16</v>
+      </c>
+      <c r="E80" s="13"/>
       <c r="F80" s="11"/>
       <c r="G80" s="11"/>
       <c r="H80" s="11" t="s">
@@ -8906,8 +8994,10 @@
         <v>376</v>
       </c>
       <c r="C81" s="11"/>
-      <c r="D81" s="11"/>
-      <c r="E81" s="11"/>
+      <c r="D81" s="17">
+        <v>0.16</v>
+      </c>
+      <c r="E81" s="13"/>
       <c r="F81" s="11"/>
       <c r="G81" s="11"/>
       <c r="H81" s="11" t="s">
@@ -8932,8 +9022,7 @@
         <v>377</v>
       </c>
       <c r="C82" s="11"/>
-      <c r="D82" s="11"/>
-      <c r="E82" s="11"/>
+      <c r="D82" s="20"/>
       <c r="F82" s="11"/>
       <c r="G82" s="11"/>
       <c r="H82" s="11" t="s">
@@ -8958,7 +9047,7 @@
         <v>378</v>
       </c>
       <c r="C83" s="11"/>
-      <c r="D83" s="11"/>
+      <c r="D83" s="19"/>
       <c r="E83" s="11"/>
       <c r="F83" s="11"/>
       <c r="G83" s="11"/>
@@ -8984,7 +9073,7 @@
         <v>379</v>
       </c>
       <c r="C84" s="11"/>
-      <c r="D84" s="11"/>
+      <c r="D84" s="19"/>
       <c r="E84" s="11"/>
       <c r="F84" s="11"/>
       <c r="G84" s="11"/>
@@ -9036,7 +9125,9 @@
         <v>381</v>
       </c>
       <c r="C86" s="11"/>
-      <c r="D86" s="11"/>
+      <c r="D86" s="11">
+        <v>0.12</v>
+      </c>
       <c r="E86" s="11"/>
       <c r="F86" s="11"/>
       <c r="G86" s="11"/>
@@ -9062,7 +9153,9 @@
         <v>382</v>
       </c>
       <c r="C87" s="11"/>
-      <c r="D87" s="11"/>
+      <c r="D87" s="11">
+        <v>0.12</v>
+      </c>
       <c r="E87" s="11"/>
       <c r="F87" s="11"/>
       <c r="G87" s="11"/>
@@ -9088,7 +9181,9 @@
         <v>383</v>
       </c>
       <c r="C88" s="11"/>
-      <c r="D88" s="11"/>
+      <c r="D88" s="11">
+        <v>0.12</v>
+      </c>
       <c r="E88" s="11"/>
       <c r="F88" s="11"/>
       <c r="G88" s="11"/>
@@ -9114,7 +9209,9 @@
         <v>384</v>
       </c>
       <c r="C89" s="11"/>
-      <c r="D89" s="11"/>
+      <c r="D89" s="11">
+        <v>0.03</v>
+      </c>
       <c r="E89" s="11"/>
       <c r="F89" s="11"/>
       <c r="G89" s="11"/>
@@ -9140,7 +9237,9 @@
         <v>385</v>
       </c>
       <c r="C90" s="11"/>
-      <c r="D90" s="11"/>
+      <c r="D90" s="11">
+        <v>0.17</v>
+      </c>
       <c r="E90" s="11"/>
       <c r="F90" s="11"/>
       <c r="G90" s="11"/>
@@ -9166,7 +9265,9 @@
         <v>386</v>
       </c>
       <c r="C91" s="11"/>
-      <c r="D91" s="11"/>
+      <c r="D91" s="11">
+        <v>0.27</v>
+      </c>
       <c r="E91" s="11"/>
       <c r="F91" s="11"/>
       <c r="G91" s="11"/>
@@ -9192,7 +9293,9 @@
         <v>387</v>
       </c>
       <c r="C92" s="11"/>
-      <c r="D92" s="11"/>
+      <c r="D92" s="11">
+        <v>0.02</v>
+      </c>
       <c r="E92" s="11"/>
       <c r="F92" s="11"/>
       <c r="G92" s="11"/>
@@ -9218,7 +9321,9 @@
         <v>388</v>
       </c>
       <c r="C93" s="11"/>
-      <c r="D93" s="11"/>
+      <c r="D93" s="11">
+        <v>0.02</v>
+      </c>
       <c r="E93" s="11"/>
       <c r="F93" s="11"/>
       <c r="G93" s="11"/>
@@ -9244,7 +9349,9 @@
         <v>389</v>
       </c>
       <c r="C94" s="11"/>
-      <c r="D94" s="11"/>
+      <c r="D94" s="11">
+        <v>0.02</v>
+      </c>
       <c r="E94" s="11"/>
       <c r="F94" s="11"/>
       <c r="G94" s="11"/>
@@ -9270,7 +9377,9 @@
         <v>390</v>
       </c>
       <c r="C95" s="11"/>
-      <c r="D95" s="11"/>
+      <c r="D95" s="13">
+        <v>0.03</v>
+      </c>
       <c r="E95" s="11"/>
       <c r="F95" s="11"/>
       <c r="G95" s="11"/>
@@ -9296,7 +9405,9 @@
         <v>391</v>
       </c>
       <c r="C96" s="11"/>
-      <c r="D96" s="11"/>
+      <c r="D96" s="13">
+        <v>0.17</v>
+      </c>
       <c r="E96" s="11"/>
       <c r="F96" s="11"/>
       <c r="G96" s="11"/>
@@ -9322,7 +9433,9 @@
         <v>392</v>
       </c>
       <c r="C97" s="11"/>
-      <c r="D97" s="11"/>
+      <c r="D97" s="13">
+        <v>0.27</v>
+      </c>
       <c r="E97" s="11"/>
       <c r="F97" s="11"/>
       <c r="G97" s="11"/>
@@ -9720,7 +9833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A316BE-9EDA-47CE-ABE6-3F1E6F71A5DE}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Framework based export of plot data
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D6C502-8CE3-4CFD-9E2A-B03B5C9C1CCA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF50066-A2FA-4DC6-B010-F05A121F0B9C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Databook Pages" sheetId="7" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Cascades" sheetId="12" r:id="rId7"/>
     <sheet name="Plots" sheetId="13" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
@@ -773,7 +773,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="563">
   <si>
     <t>Code Name</t>
   </si>
@@ -2255,9 +2255,6 @@
   </si>
   <si>
     <t>:ddis</t>
-  </si>
-  <si>
-    <t>Aggregate pops</t>
   </si>
   <si>
     <t>Quantities</t>
@@ -3074,7 +3071,7 @@
         <v>5</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -4891,7 +4888,7 @@
         <v>5</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -5102,7 +5099,7 @@
         <v>131</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="11">
@@ -5127,7 +5124,7 @@
         <v>132</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="11">
@@ -5152,7 +5149,7 @@
         <v>133</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="11">
@@ -5177,7 +5174,7 @@
         <v>241</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7">
@@ -5228,7 +5225,7 @@
         <v>134</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7">
@@ -5253,7 +5250,7 @@
         <v>135</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="11">
@@ -5278,7 +5275,7 @@
         <v>136</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="11">
@@ -5303,7 +5300,7 @@
         <v>137</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="11">
@@ -5328,7 +5325,7 @@
         <v>138</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="11">
@@ -5353,7 +5350,7 @@
         <v>139</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="11">
@@ -5378,7 +5375,7 @@
         <v>148</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7">
@@ -5403,7 +5400,7 @@
         <v>149</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="11">
@@ -5428,7 +5425,7 @@
         <v>199</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="11">
@@ -5453,7 +5450,7 @@
         <v>200</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="11">
@@ -5478,7 +5475,7 @@
         <v>201</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="11">
@@ -5528,7 +5525,7 @@
         <v>198</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="11">
@@ -5579,7 +5576,7 @@
         <v>150</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7">
@@ -5604,7 +5601,7 @@
         <v>158</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7">
@@ -5629,7 +5626,7 @@
         <v>159</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="11">
@@ -5654,7 +5651,7 @@
         <v>160</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="11">
@@ -5679,7 +5676,7 @@
         <v>161</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="11">
@@ -5704,7 +5701,7 @@
         <v>162</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="11">
@@ -5729,7 +5726,7 @@
         <v>163</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="11">
@@ -6286,7 +6283,7 @@
         <v>224</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E55" s="7"/>
       <c r="F55" s="11">
@@ -6311,7 +6308,7 @@
         <v>225</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E56" s="7"/>
       <c r="F56" s="11">
@@ -6336,7 +6333,7 @@
         <v>226</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E57" s="7"/>
       <c r="F57" s="11">
@@ -6361,7 +6358,7 @@
         <v>227</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E58" s="7"/>
       <c r="F58" s="11">
@@ -6386,7 +6383,7 @@
         <v>228</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E59" s="7"/>
       <c r="F59" s="11">
@@ -6411,7 +6408,7 @@
         <v>229</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E60" s="7"/>
       <c r="F60" s="11">
@@ -6436,7 +6433,7 @@
         <v>230</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E61" s="7"/>
       <c r="F61" s="11">
@@ -6461,7 +6458,7 @@
         <v>231</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E62" s="7"/>
       <c r="F62" s="11">
@@ -6486,7 +6483,7 @@
         <v>232</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E63" s="7"/>
       <c r="F63" s="11">
@@ -6511,7 +6508,7 @@
         <v>243</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D64" s="11"/>
       <c r="E64" s="11"/>
@@ -6690,7 +6687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FC8421-05BA-4BE1-A1F1-3F12A4E7E369}">
   <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
       <selection pane="topRight" activeCell="F91" sqref="F91"/>
@@ -6741,7 +6738,7 @@
         <v>457</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="K1" s="12" t="s">
         <v>96</v>
@@ -9748,10 +9745,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -9759,7 +9756,7 @@
         <v>458</v>
       </c>
       <c r="B2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -9767,7 +9764,7 @@
         <v>462</v>
       </c>
       <c r="B3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -9775,7 +9772,7 @@
         <v>465</v>
       </c>
       <c r="B4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -9789,10 +9786,10 @@
     <row r="6" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -9800,7 +9797,7 @@
         <v>458</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -9808,7 +9805,7 @@
         <v>462</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -9816,7 +9813,7 @@
         <v>465</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -9831,10 +9828,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A316BE-9EDA-47CE-ABE6-3F1E6F71A5DE}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9843,10 +9840,9 @@
     <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="10" customWidth="1"/>
     <col min="4" max="4" width="104.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -9854,308 +9850,305 @@
         <v>1</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>494</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B2" t="s">
         <v>150</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D2" t="s">
         <v>145</v>
       </c>
-      <c r="F2" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B3" t="s">
         <v>467</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D3" t="s">
         <v>107</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3" s="10" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B4" t="s">
         <v>468</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B5" t="s">
         <v>469</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D5" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B6" t="s">
         <v>470</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D6" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B7" t="s">
         <v>471</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D7" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B8" t="s">
         <v>472</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D8" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B9" t="s">
         <v>473</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D9" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B10" t="s">
         <v>474</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D10" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B11" t="s">
         <v>475</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D11" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B12" t="s">
         <v>476</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D12" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B13" t="s">
         <v>477</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D13" t="s">
         <v>488</v>
       </c>
-      <c r="F13" s="10" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="10" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B14" t="s">
         <v>478</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D14" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B15" t="s">
         <v>479</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D15" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B16" t="s">
         <v>480</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D16" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B17" t="s">
         <v>481</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D17" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B18" t="s">
         <v>482</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D18" t="s">
         <v>99</v>
       </c>
-      <c r="F18" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B19" t="s">
         <v>483</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D19" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B20" t="s">
         <v>484</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D20" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
+        <v>561</v>
+      </c>
+      <c r="B21" t="s">
         <v>562</v>
       </c>
-      <c r="B21" t="s">
-        <v>563</v>
-      </c>
       <c r="C21" s="10" t="s">
+        <v>497</v>
+      </c>
+      <c r="D21" t="s">
         <v>498</v>
-      </c>
-      <c r="D21" t="s">
-        <v>499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename cascades, add export filtering by name
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31BA33D0-BADB-47C6-8766-83C19E48780F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC4FF8F-7C82-4052-9B80-2F1481449EB9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="16095" windowHeight="9660" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="16095" windowHeight="9660" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="14" r:id="rId1"/>
@@ -743,7 +743,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{377F5AF9-9F9B-4044-809C-788F15A68F9A}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{377F5AF9-9F9B-4044-809C-788F15A68F9A}">
       <text>
         <r>
           <rPr>
@@ -774,7 +774,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="554">
   <si>
     <t>Code Name</t>
   </si>
@@ -2261,12 +2261,6 @@
     <t>series</t>
   </si>
   <si>
-    <t>bar</t>
-  </si>
-  <si>
-    <t>['ac_prev','lt_prev','mdr_prev','xdr_prev']</t>
-  </si>
-  <si>
     <t>Constituents</t>
   </si>
   <si>
@@ -2381,75 +2375,6 @@
     <t>Export</t>
   </si>
   <si>
-    <t>main</t>
-  </si>
-  <si>
-    <t>secondary</t>
-  </si>
-  <si>
-    <t>plot1</t>
-  </si>
-  <si>
-    <t>plot2</t>
-  </si>
-  <si>
-    <t>plot3</t>
-  </si>
-  <si>
-    <t>plot4</t>
-  </si>
-  <si>
-    <t>plot5</t>
-  </si>
-  <si>
-    <t>plot6</t>
-  </si>
-  <si>
-    <t>plot7</t>
-  </si>
-  <si>
-    <t>plot8</t>
-  </si>
-  <si>
-    <t>plot9</t>
-  </si>
-  <si>
-    <t>plot10</t>
-  </si>
-  <si>
-    <t>plot11</t>
-  </si>
-  <si>
-    <t>plot12</t>
-  </si>
-  <si>
-    <t>plot13</t>
-  </si>
-  <si>
-    <t>plot14</t>
-  </si>
-  <si>
-    <t>plot15</t>
-  </si>
-  <si>
-    <t>plot16</t>
-  </si>
-  <si>
-    <t>plot17</t>
-  </si>
-  <si>
-    <t>plot18</t>
-  </si>
-  <si>
-    <t>plot19</t>
-  </si>
-  <si>
-    <t>plot20</t>
-  </si>
-  <si>
-    <t>Bar of people</t>
-  </si>
-  <si>
     <t>ac_inf,acr</t>
   </si>
   <si>
@@ -2471,19 +2396,46 @@
     <t>The Optima TB cascade</t>
   </si>
   <si>
-    <t>People with active TB</t>
-  </si>
-  <si>
-    <t>Treated for active TB</t>
-  </si>
-  <si>
-    <t>Diagnosed with active TB</t>
-  </si>
-  <si>
     <t>Non-TB deaths</t>
   </si>
   <si>
     <t>Emigration</t>
+  </si>
+  <si>
+    <t>Diagnosed</t>
+  </si>
+  <si>
+    <t>Treated</t>
+  </si>
+  <si>
+    <t>Successfully treated</t>
+  </si>
+  <si>
+    <t>Active SP-TB</t>
+  </si>
+  <si>
+    <t>Active SN-TB</t>
+  </si>
+  <si>
+    <t>SP treatment</t>
+  </si>
+  <si>
+    <t>SN treatment</t>
+  </si>
+  <si>
+    <t>spdk_inf,spmk_inf,spxk_inf</t>
+  </si>
+  <si>
+    <t>sndk_inf,snmk_inf,snxk_inf</t>
+  </si>
+  <si>
+    <t>spdt,spmt,spxt</t>
+  </si>
+  <si>
+    <t>sndt,snmt,snxt</t>
+  </si>
+  <si>
+    <t>TB treatment (including recovered)</t>
   </si>
 </sst>
 </file>
@@ -2950,18 +2902,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>561</v>
+        <v>536</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>562</v>
+        <v>537</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>563</v>
+        <v>538</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>564</v>
+        <v>539</v>
       </c>
     </row>
   </sheetData>
@@ -3082,7 +3034,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="J32" sqref="A32:J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3127,7 +3079,7 @@
         <v>5</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -4895,8 +4847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D29B4020-084C-4F00-B628-93D126F8BCA7}">
   <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4942,7 +4894,7 @@
         <v>5</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -5153,7 +5105,7 @@
         <v>131</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="11">
@@ -5178,7 +5130,7 @@
         <v>132</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="11">
@@ -5203,7 +5155,7 @@
         <v>133</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="11">
@@ -5228,7 +5180,7 @@
         <v>241</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7">
@@ -5279,7 +5231,7 @@
         <v>134</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7">
@@ -5304,7 +5256,7 @@
         <v>135</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="11">
@@ -5329,7 +5281,7 @@
         <v>136</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="11">
@@ -5354,7 +5306,7 @@
         <v>137</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="11">
@@ -5379,7 +5331,7 @@
         <v>138</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="11">
@@ -5404,7 +5356,7 @@
         <v>139</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="11">
@@ -5429,7 +5381,7 @@
         <v>148</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7">
@@ -5454,7 +5406,7 @@
         <v>149</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="11">
@@ -5479,7 +5431,7 @@
         <v>199</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="11">
@@ -5504,7 +5456,7 @@
         <v>200</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="11">
@@ -5529,7 +5481,7 @@
         <v>201</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="11">
@@ -5579,7 +5531,7 @@
         <v>198</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="11">
@@ -5630,7 +5582,7 @@
         <v>150</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7">
@@ -5655,7 +5607,7 @@
         <v>158</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7">
@@ -5680,7 +5632,7 @@
         <v>159</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="11">
@@ -5705,7 +5657,7 @@
         <v>160</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="11">
@@ -5730,7 +5682,7 @@
         <v>161</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="11">
@@ -5755,7 +5707,7 @@
         <v>162</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="11">
@@ -5780,7 +5732,7 @@
         <v>163</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="11">
@@ -6337,7 +6289,7 @@
         <v>224</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="E55" s="7"/>
       <c r="F55" s="11">
@@ -6362,7 +6314,7 @@
         <v>225</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="E56" s="7"/>
       <c r="F56" s="11">
@@ -6387,7 +6339,7 @@
         <v>226</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="E57" s="7"/>
       <c r="F57" s="11">
@@ -6412,7 +6364,7 @@
         <v>227</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="E58" s="7"/>
       <c r="F58" s="11">
@@ -6437,7 +6389,7 @@
         <v>228</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="E59" s="7"/>
       <c r="F59" s="11">
@@ -6462,7 +6414,7 @@
         <v>229</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E60" s="7"/>
       <c r="F60" s="11">
@@ -6487,7 +6439,7 @@
         <v>230</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="E61" s="7"/>
       <c r="F61" s="11">
@@ -6512,7 +6464,7 @@
         <v>231</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="E62" s="7"/>
       <c r="F62" s="11">
@@ -6537,7 +6489,7 @@
         <v>232</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="E63" s="7"/>
       <c r="F63" s="11">
@@ -6562,7 +6514,7 @@
         <v>243</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D64" s="11"/>
       <c r="E64" s="11"/>
@@ -6683,7 +6635,7 @@
     </row>
   </sheetData>
   <dataConsolidate/>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G74" xr:uid="{CE581F04-42C4-4377-AC3C-1080BAA29A3F}">
       <formula1>"y,n"</formula1>
     </dataValidation>
@@ -6741,10 +6693,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FC8421-05BA-4BE1-A1F1-3F12A4E7E369}">
   <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="B13" sqref="B13"/>
+      <selection pane="topRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6792,7 +6744,7 @@
         <v>455</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="K1" s="12" t="s">
         <v>96</v>
@@ -6834,7 +6786,7 @@
         <v>247</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>568</v>
+        <v>540</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -6888,7 +6840,7 @@
         <v>246</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>569</v>
+        <v>541</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
@@ -9785,94 +9737,146 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{096AAE64-6D86-4469-8C78-6B6ADE320367}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="55.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
+        <v>553</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>466</v>
+      </c>
+      <c r="B2" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>542</v>
+      </c>
+      <c r="B3" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>543</v>
+      </c>
+      <c r="B4" t="s">
         <v>535</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>565</v>
-      </c>
-      <c r="B2" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>567</v>
-      </c>
-      <c r="B3" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>566</v>
-      </c>
-      <c r="B4" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>544</v>
       </c>
       <c r="B5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>536</v>
+        <v>547</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>565</v>
+        <v>545</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>567</v>
+        <v>542</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>566</v>
+        <v>543</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>551</v>
+      </c>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>548</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>495</v>
+      </c>
+      <c r="E12" s="14"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>546</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="E13" s="14"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>542</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>550</v>
+      </c>
+      <c r="E14" s="14"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>543</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>552</v>
+      </c>
+      <c r="E15" s="14"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="E16" s="14"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="14"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="13"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9882,327 +9886,252 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A316BE-9EDA-47CE-ABE6-3F1E6F71A5DE}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" style="10" customWidth="1"/>
-    <col min="4" max="4" width="104.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="10" customWidth="1"/>
+    <col min="3" max="3" width="104.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>1</v>
+    <row r="1" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>536</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>493</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>492</v>
-      </c>
-      <c r="E1" s="18" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="C2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>537</v>
-      </c>
-      <c r="B2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C2" s="10" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="D2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E2" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>538</v>
-      </c>
-      <c r="B3" t="s">
-        <v>465</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>466</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="D3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>539</v>
-      </c>
-      <c r="B4" t="s">
-        <v>466</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>467</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="D4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>540</v>
-      </c>
-      <c r="B5" t="s">
-        <v>467</v>
-      </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>468</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="D5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>541</v>
-      </c>
-      <c r="B6" t="s">
-        <v>468</v>
-      </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>469</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="D6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>542</v>
-      </c>
-      <c r="B7" t="s">
-        <v>469</v>
-      </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>470</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="D7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>543</v>
-      </c>
-      <c r="B8" t="s">
-        <v>470</v>
-      </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>471</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="D8" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="B9" t="s">
-        <v>471</v>
-      </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>472</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="D9" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>545</v>
-      </c>
-      <c r="B10" t="s">
-        <v>472</v>
-      </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>473</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="D10" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>546</v>
-      </c>
-      <c r="B11" t="s">
-        <v>473</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>474</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="D11" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>547</v>
-      </c>
-      <c r="B12" t="s">
-        <v>474</v>
-      </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>475</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="D12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>548</v>
-      </c>
-      <c r="B13" t="s">
-        <v>475</v>
-      </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" t="s">
+        <v>486</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>476</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="D13" t="s">
-        <v>486</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>549</v>
-      </c>
-      <c r="B14" t="s">
-        <v>476</v>
-      </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>477</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="D14" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>550</v>
-      </c>
-      <c r="B15" t="s">
-        <v>477</v>
-      </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>478</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="D15" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>551</v>
-      </c>
-      <c r="B16" t="s">
-        <v>478</v>
-      </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>479</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="D16" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>552</v>
-      </c>
-      <c r="B17" t="s">
-        <v>479</v>
-      </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>480</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="D17" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>553</v>
-      </c>
-      <c r="B18" t="s">
-        <v>480</v>
-      </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>481</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="D18" t="s">
-        <v>99</v>
-      </c>
-      <c r="E18" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
-        <v>554</v>
-      </c>
-      <c r="B19" t="s">
-        <v>481</v>
-      </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>482</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="D19" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>555</v>
-      </c>
-      <c r="B20" t="s">
-        <v>482</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="C20" t="s">
         <v>491</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>556</v>
-      </c>
-      <c r="B21" t="s">
-        <v>557</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>495</v>
-      </c>
-      <c r="D21" t="s">
-        <v>496</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix framework to show data
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\tb-ucl-analyses\general\frameworks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romesh.abey\Desktop\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="16095" windowHeight="9660" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="468" windowWidth="16098" windowHeight="9660" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="14" r:id="rId1"/>
@@ -870,7 +870,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1868" uniqueCount="831">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1868" uniqueCount="809">
   <si>
     <t>Code Name</t>
   </si>
@@ -3290,85 +3290,19 @@
     <t>Early-LTBI (diagnosis restricted) annual probability of initiating treatment</t>
   </si>
   <si>
-    <t>{'Total population size': ['alive']}</t>
-  </si>
-  <si>
-    <t>{'Latent infections': ['lt_inf']}</t>
-  </si>
-  <si>
-    <t>{'Active TB': ['ac_inf']}</t>
-  </si>
-  <si>
-    <t>{'Active DS-TB': ['ds_inf']}</t>
-  </si>
-  <si>
-    <t>{'Active MDR-TB': ['mdr_inf']}</t>
-  </si>
-  <si>
-    <t>{'Active XDR-TB': ['xdr_inf']}</t>
-  </si>
-  <si>
-    <t>{'Smear negative active TB': ['sn_inf']}</t>
-  </si>
-  <si>
-    <t>{'Smear positive active TB': ['sp_inf']}</t>
-  </si>
-  <si>
-    <t>{'Active treatment': ['num_treat']}</t>
-  </si>
-  <si>
-    <t>{'TB-related deaths': [':ddis']}</t>
-  </si>
-  <si>
-    <t>{'Latent prevalence': ['lt_prev']}</t>
-  </si>
-  <si>
-    <t>{'Active prevalence': ['ac_prev']}</t>
-  </si>
-  <si>
-    <t>{'DR prevalence': ['dr_prev']}</t>
-  </si>
-  <si>
-    <t>{'Latent treatment': ['ltt_inf']}</t>
-  </si>
-  <si>
-    <t>{'Annual diagnosis rate': ['pd_diag']}</t>
-  </si>
-  <si>
-    <t>{'Annual diagnosis rate': ['pm_diag']}</t>
-  </si>
-  <si>
-    <t>{'Annual diagnosis rate': ['px_diag']}</t>
-  </si>
-  <si>
-    <t>{'Annual diagnosis rate': ['nd_diag']}</t>
-  </si>
-  <si>
-    <t>{'Annual diagnosis rate': ['nm_diag']}</t>
-  </si>
-  <si>
-    <t>{'Annual diagnosis rate': ['nx_diag']}</t>
-  </si>
-  <si>
-    <t>{'Annual treatment initiation': ['d_treat']}</t>
-  </si>
-  <si>
-    <t>{'Annual treatment initiation': ['m_treat']}</t>
-  </si>
-  <si>
-    <t>{'Annual treatment initiation': ['x_treat']}</t>
-  </si>
-  <si>
     <t>SP-DS number diagnosed</t>
   </si>
   <si>
-    <t>{'number diagnosed': ['spdu:spdd']}</t>
+    <t>:ddis</t>
+  </si>
+  <si>
+    <t>spdu:spdd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3972,9 +3906,9 @@
       <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="18" t="s">
         <v>343</v>
       </c>
@@ -3982,7 +3916,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="20" t="s">
         <v>345</v>
       </c>
@@ -4003,14 +3937,14 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="25.68359375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="34.26171875" style="3" customWidth="1"/>
     <col min="3" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>57</v>
       </c>
@@ -4018,7 +3952,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="7" t="s">
         <v>59</v>
       </c>
@@ -4026,7 +3960,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="11" t="s">
         <v>427</v>
       </c>
@@ -4034,7 +3968,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="11" t="s">
         <v>430</v>
       </c>
@@ -4042,7 +3976,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="7" t="s">
         <v>61</v>
       </c>
@@ -4050,7 +3984,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="7" t="s">
         <v>429</v>
       </c>
@@ -4058,7 +3992,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="11" t="s">
         <v>378</v>
       </c>
@@ -4066,7 +4000,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="11" t="s">
         <v>491</v>
       </c>
@@ -4074,7 +4008,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="7" t="s">
         <v>60</v>
       </c>
@@ -4082,7 +4016,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="7" t="s">
         <v>542</v>
       </c>
@@ -4090,23 +4024,23 @@
         <v>719</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
     </row>
@@ -4124,20 +4058,20 @@
       <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.68359375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.41796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.26171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.26171875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.68359375" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.26171875" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.15625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4167,7 +4101,7 @@
       </c>
       <c r="J1" s="18"/>
     </row>
-    <row r="2" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="32" t="s">
         <v>432</v>
       </c>
@@ -4192,7 +4126,7 @@
       </c>
       <c r="I2" s="22"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
@@ -4213,7 +4147,7 @@
       </c>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
@@ -4237,7 +4171,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
@@ -4261,7 +4195,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
@@ -4285,7 +4219,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="6" t="s">
         <v>567</v>
       </c>
@@ -4308,7 +4242,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
@@ -4332,7 +4266,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="6" t="s">
         <v>20</v>
       </c>
@@ -4356,7 +4290,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="6" t="s">
         <v>566</v>
       </c>
@@ -4379,7 +4313,7 @@
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
     </row>
-    <row r="11" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="27" t="s">
         <v>373</v>
       </c>
@@ -4404,7 +4338,7 @@
       </c>
       <c r="I11" s="22"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="6" t="s">
         <v>66</v>
       </c>
@@ -4428,7 +4362,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="6" t="s">
         <v>67</v>
       </c>
@@ -4452,7 +4386,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
@@ -4473,7 +4407,7 @@
       </c>
       <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="6" t="s">
         <v>22</v>
       </c>
@@ -4494,7 +4428,7 @@
       </c>
       <c r="G15" s="11"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="6" t="s">
         <v>23</v>
       </c>
@@ -4515,7 +4449,7 @@
       </c>
       <c r="G16" s="11"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="6" t="s">
         <v>24</v>
       </c>
@@ -4536,7 +4470,7 @@
       </c>
       <c r="G17" s="11"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="6" t="s">
         <v>25</v>
       </c>
@@ -4560,7 +4494,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="6" t="s">
         <v>565</v>
       </c>
@@ -4583,7 +4517,7 @@
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="6" t="s">
         <v>26</v>
       </c>
@@ -4604,7 +4538,7 @@
       </c>
       <c r="G20" s="11"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="6" t="s">
         <v>27</v>
       </c>
@@ -4625,7 +4559,7 @@
       </c>
       <c r="G21" s="11"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="6" t="s">
         <v>28</v>
       </c>
@@ -4649,7 +4583,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="6" t="s">
         <v>570</v>
       </c>
@@ -4672,7 +4606,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="6" t="s">
         <v>29</v>
       </c>
@@ -4693,7 +4627,7 @@
       </c>
       <c r="G24" s="11"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="6" t="s">
         <v>30</v>
       </c>
@@ -4714,7 +4648,7 @@
       </c>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="6" t="s">
         <v>31</v>
       </c>
@@ -4738,7 +4672,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="6" t="s">
         <v>572</v>
       </c>
@@ -4761,7 +4695,7 @@
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="6" t="s">
         <v>32</v>
       </c>
@@ -4782,7 +4716,7 @@
       </c>
       <c r="G28" s="11"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="6" t="s">
         <v>33</v>
       </c>
@@ -4803,7 +4737,7 @@
       </c>
       <c r="G29" s="11"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="6" t="s">
         <v>34</v>
       </c>
@@ -4824,7 +4758,7 @@
       </c>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="6" t="s">
         <v>35</v>
       </c>
@@ -4848,7 +4782,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="6" t="s">
         <v>574</v>
       </c>
@@ -4871,7 +4805,7 @@
       <c r="H32" s="11"/>
       <c r="I32" s="11"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="6" t="s">
         <v>36</v>
       </c>
@@ -4892,7 +4826,7 @@
       </c>
       <c r="G33" s="11"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="6" t="s">
         <v>37</v>
       </c>
@@ -4913,7 +4847,7 @@
       </c>
       <c r="G34" s="11"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="6" t="s">
         <v>38</v>
       </c>
@@ -4937,7 +4871,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="6" t="s">
         <v>576</v>
       </c>
@@ -4960,7 +4894,7 @@
       <c r="H36" s="11"/>
       <c r="I36" s="11"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="6" t="s">
         <v>39</v>
       </c>
@@ -4981,7 +4915,7 @@
       </c>
       <c r="G37" s="11"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="6" t="s">
         <v>40</v>
       </c>
@@ -5002,7 +4936,7 @@
       </c>
       <c r="G38" s="11"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="6" t="s">
         <v>41</v>
       </c>
@@ -5026,7 +4960,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="6" t="s">
         <v>578</v>
       </c>
@@ -5049,7 +4983,7 @@
       <c r="H40" s="11"/>
       <c r="I40" s="11"/>
     </row>
-    <row r="41" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="27" t="s">
         <v>42</v>
       </c>
@@ -5074,7 +5008,7 @@
       </c>
       <c r="I41" s="22"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="6" t="s">
         <v>45</v>
       </c>
@@ -5095,7 +5029,7 @@
       </c>
       <c r="G42" s="11"/>
     </row>
-    <row r="43" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="6" t="s">
         <v>52</v>
       </c>
@@ -5118,7 +5052,7 @@
       <c r="H43" s="11"/>
       <c r="I43" s="7"/>
     </row>
-    <row r="44" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="27" t="s">
         <v>360</v>
       </c>
@@ -5141,7 +5075,7 @@
       <c r="H44" s="22"/>
       <c r="I44" s="22"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="6" t="s">
         <v>43</v>
       </c>
@@ -5162,7 +5096,7 @@
       </c>
       <c r="G45" s="11"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="6" t="s">
         <v>44</v>
       </c>
@@ -5183,7 +5117,7 @@
       </c>
       <c r="G46" s="11"/>
     </row>
-    <row r="47" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="6" t="s">
         <v>54</v>
       </c>
@@ -5206,16 +5140,16 @@
       <c r="H47" s="11"/>
       <c r="I47" s="7"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="G48" s="11"/>
     </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G49" s="11"/>
     </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G50" s="11"/>
     </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G51" s="11"/>
     </row>
   </sheetData>
@@ -5242,59 +5176,59 @@
       <selection pane="topRight" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.26171875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.26171875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="10.83984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.68359375" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.41796875" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.15625" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.26171875" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.41796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.15625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.26171875" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.68359375" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.578125" style="11" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.5703125" style="11" customWidth="1"/>
+    <col min="16" max="16" width="11.15625" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.83984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.41796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.83984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.68359375" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.578125" style="11" customWidth="1"/>
     <col min="22" max="22" width="8" style="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.42578125" style="11" customWidth="1"/>
+    <col min="23" max="23" width="9.41796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.83984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.83984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.41796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.41796875" style="11" customWidth="1"/>
     <col min="28" max="28" width="5" style="11" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="6" style="11" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="7" style="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.42578125" style="11" customWidth="1"/>
-    <col min="33" max="33" width="6.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="7.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.41796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.41796875" style="11" customWidth="1"/>
+    <col min="33" max="33" width="6.41796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="7.41796875" style="11" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="8" style="11" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="8" style="11" customWidth="1"/>
-    <col min="37" max="37" width="5.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="6.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.42578125" style="11" customWidth="1"/>
-    <col min="41" max="41" width="11.85546875" style="11" customWidth="1"/>
+    <col min="37" max="37" width="5.83984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="6.83984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.41796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.41796875" style="11" customWidth="1"/>
+    <col min="41" max="41" width="11.83984375" style="11" customWidth="1"/>
     <col min="42" max="42" width="3" style="11" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="4.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="6.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="4.83984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="6.15625" style="22" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="8" style="11" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="5.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="9.68359375" style="11" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="5.83984375" style="11" bestFit="1" customWidth="1"/>
     <col min="48" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="32" t="s">
         <v>432</v>
       </c>
@@ -5438,7 +5372,7 @@
       <c r="AX1" s="12"/>
       <c r="AY1" s="12"/>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="32" t="s">
         <v>432</v>
       </c>
@@ -5545,7 +5479,7 @@
       <c r="AX2" s="12"/>
       <c r="AY2" s="12"/>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="12" t="s">
         <v>13</v>
       </c>
@@ -5563,7 +5497,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="12" t="s">
         <v>15</v>
       </c>
@@ -5578,7 +5512,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="12" t="s">
         <v>17</v>
       </c>
@@ -5599,7 +5533,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="12" t="s">
         <v>18</v>
       </c>
@@ -5616,7 +5550,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="21" t="s">
         <v>567</v>
       </c>
@@ -5630,7 +5564,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="12" t="s">
         <v>19</v>
       </c>
@@ -5648,7 +5582,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="12" t="s">
         <v>20</v>
       </c>
@@ -5664,7 +5598,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="21" t="s">
         <v>566</v>
       </c>
@@ -5677,7 +5611,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="12" t="s">
         <v>373</v>
       </c>
@@ -5692,7 +5626,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="12" t="s">
         <v>66</v>
       </c>
@@ -5714,7 +5648,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="12" t="s">
         <v>67</v>
       </c>
@@ -5729,7 +5663,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="12" t="s">
         <v>21</v>
       </c>
@@ -5741,7 +5675,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="12" t="s">
         <v>22</v>
       </c>
@@ -5756,7 +5690,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="12" t="s">
         <v>23</v>
       </c>
@@ -5777,7 +5711,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="12" t="s">
         <v>24</v>
       </c>
@@ -5798,7 +5732,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="12" t="s">
         <v>25</v>
       </c>
@@ -5813,7 +5747,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="21" t="s">
         <v>565</v>
       </c>
@@ -5834,7 +5768,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="12" t="s">
         <v>26</v>
       </c>
@@ -5855,7 +5789,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="12" t="s">
         <v>27</v>
       </c>
@@ -5876,7 +5810,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="12" t="s">
         <v>28</v>
       </c>
@@ -5892,7 +5826,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="21" t="s">
         <v>570</v>
       </c>
@@ -5913,7 +5847,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="12" t="s">
         <v>29</v>
       </c>
@@ -5935,7 +5869,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="12" t="s">
         <v>30</v>
       </c>
@@ -5956,7 +5890,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="12" t="s">
         <v>31</v>
       </c>
@@ -5972,7 +5906,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="21" t="s">
         <v>572</v>
       </c>
@@ -5990,7 +5924,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="12" t="s">
         <v>32</v>
       </c>
@@ -6005,7 +5939,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="12" t="s">
         <v>33</v>
       </c>
@@ -6026,7 +5960,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="12" t="s">
         <v>34</v>
       </c>
@@ -6047,7 +5981,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="12" t="s">
         <v>35</v>
       </c>
@@ -6063,7 +5997,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="21" t="s">
         <v>574</v>
       </c>
@@ -6084,7 +6018,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="12" t="s">
         <v>36</v>
       </c>
@@ -6105,7 +6039,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="12" t="s">
         <v>37</v>
       </c>
@@ -6126,7 +6060,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="12" t="s">
         <v>38</v>
       </c>
@@ -6142,7 +6076,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="21" t="s">
         <v>576</v>
       </c>
@@ -6163,7 +6097,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="37" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="12" t="s">
         <v>39</v>
       </c>
@@ -6184,7 +6118,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="12" t="s">
         <v>40</v>
       </c>
@@ -6205,7 +6139,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="39" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="12" t="s">
         <v>41</v>
       </c>
@@ -6221,7 +6155,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="40" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="21" t="s">
         <v>578</v>
       </c>
@@ -6239,7 +6173,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="41" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="12" t="s">
         <v>42</v>
       </c>
@@ -6257,7 +6191,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="42" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="12" t="s">
         <v>45</v>
       </c>
@@ -6266,7 +6200,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="43" spans="1:47" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:47" s="22" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="21" t="s">
         <v>52</v>
       </c>
@@ -6275,7 +6209,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="44" spans="1:47" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:47" s="22" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="21" t="s">
         <v>360</v>
       </c>
@@ -6290,37 +6224,37 @@
         <v>363</v>
       </c>
     </row>
-    <row r="45" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="12" t="s">
         <v>43</v>
       </c>
       <c r="B45" s="12"/>
     </row>
-    <row r="46" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="12" t="s">
         <v>44</v>
       </c>
       <c r="B46" s="12"/>
     </row>
-    <row r="47" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="12" t="s">
         <v>54</v>
       </c>
       <c r="B47" s="12"/>
     </row>
-    <row r="48" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="12"/>
       <c r="B48" s="12"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="12"/>
       <c r="B49" s="12"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="12"/>
       <c r="B50" s="12"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="12"/>
       <c r="B51" s="12"/>
     </row>
@@ -6338,21 +6272,21 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.68359375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.68359375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.41796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.68359375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.26171875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.41796875" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83984375" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -6381,7 +6315,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8" t="s">
         <v>65</v>
       </c>
@@ -6401,7 +6335,7 @@
       </c>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="8" t="s">
         <v>68</v>
       </c>
@@ -6421,7 +6355,7 @@
       </c>
       <c r="I3" s="11"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="8" t="s">
         <v>70</v>
       </c>
@@ -6441,7 +6375,7 @@
       </c>
       <c r="I4" s="11"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="8" t="s">
         <v>71</v>
       </c>
@@ -6461,7 +6395,7 @@
       </c>
       <c r="I5" s="11"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="8" t="s">
         <v>72</v>
       </c>
@@ -6481,7 +6415,7 @@
       </c>
       <c r="I6" s="11"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="9" t="s">
         <v>81</v>
       </c>
@@ -6501,7 +6435,7 @@
       </c>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="9" t="s">
         <v>82</v>
       </c>
@@ -6521,7 +6455,7 @@
       </c>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="9" t="s">
         <v>83</v>
       </c>
@@ -6541,7 +6475,7 @@
       </c>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="9" t="s">
         <v>84</v>
       </c>
@@ -6561,7 +6495,7 @@
       </c>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="9" t="s">
         <v>85</v>
       </c>
@@ -6581,7 +6515,7 @@
       </c>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="9" t="s">
         <v>86</v>
       </c>
@@ -6601,7 +6535,7 @@
       </c>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="9" t="s">
         <v>163</v>
       </c>
@@ -6619,7 +6553,7 @@
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="14" t="s">
         <v>273</v>
       </c>
@@ -6638,7 +6572,7 @@
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="9" t="s">
         <v>87</v>
       </c>
@@ -6658,7 +6592,7 @@
       </c>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="9" t="s">
         <v>88</v>
       </c>
@@ -6678,7 +6612,7 @@
       </c>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="9" t="s">
         <v>89</v>
       </c>
@@ -6698,7 +6632,7 @@
       </c>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="9" t="s">
         <v>90</v>
       </c>
@@ -6718,7 +6652,7 @@
       </c>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="9" t="s">
         <v>91</v>
       </c>
@@ -6738,7 +6672,7 @@
       </c>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="9" t="s">
         <v>92</v>
       </c>
@@ -6758,7 +6692,7 @@
       </c>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="9" t="s">
         <v>93</v>
       </c>
@@ -6778,7 +6712,7 @@
       </c>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="9" t="s">
         <v>94</v>
       </c>
@@ -6798,7 +6732,7 @@
       </c>
       <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="9" t="s">
         <v>100</v>
       </c>
@@ -6816,7 +6750,7 @@
       <c r="H23" s="7"/>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="9" t="s">
         <v>96</v>
       </c>
@@ -6834,7 +6768,7 @@
       <c r="H24" s="7"/>
       <c r="I24" s="11"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="9" t="s">
         <v>97</v>
       </c>
@@ -6852,7 +6786,7 @@
       <c r="H25" s="7"/>
       <c r="I25" s="11"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="9" t="s">
         <v>99</v>
       </c>
@@ -6870,7 +6804,7 @@
       <c r="H26" s="7"/>
       <c r="I26" s="11"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="9" t="s">
         <v>95</v>
       </c>
@@ -6890,7 +6824,7 @@
       </c>
       <c r="I27" s="11"/>
     </row>
-    <row r="28" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="14" t="s">
         <v>271</v>
       </c>
@@ -6909,7 +6843,7 @@
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="9" t="s">
         <v>98</v>
       </c>
@@ -6929,7 +6863,7 @@
       </c>
       <c r="I29" s="7"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="9" t="s">
         <v>103</v>
       </c>
@@ -6947,7 +6881,7 @@
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="9" t="s">
         <v>104</v>
       </c>
@@ -6965,7 +6899,7 @@
       <c r="H31" s="7"/>
       <c r="I31" s="11"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="9" t="s">
         <v>105</v>
       </c>
@@ -6983,7 +6917,7 @@
       <c r="H32" s="7"/>
       <c r="I32" s="11"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="9" t="s">
         <v>106</v>
       </c>
@@ -7001,7 +6935,7 @@
       <c r="H33" s="7"/>
       <c r="I33" s="11"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="9" t="s">
         <v>107</v>
       </c>
@@ -7019,7 +6953,7 @@
       <c r="H34" s="7"/>
       <c r="I34" s="11"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="9" t="s">
         <v>108</v>
       </c>
@@ -7037,7 +6971,7 @@
       <c r="H35" s="7"/>
       <c r="I35" s="11"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="9" t="s">
         <v>109</v>
       </c>
@@ -7058,7 +6992,7 @@
       <c r="H36" s="7"/>
       <c r="I36" s="11"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="9" t="s">
         <v>110</v>
       </c>
@@ -7079,7 +7013,7 @@
       <c r="H37" s="7"/>
       <c r="I37" s="11"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="9" t="s">
         <v>111</v>
       </c>
@@ -7100,7 +7034,7 @@
       <c r="H38" s="7"/>
       <c r="I38" s="11"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="9" t="s">
         <v>112</v>
       </c>
@@ -7121,7 +7055,7 @@
       <c r="H39" s="7"/>
       <c r="I39" s="11"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="9" t="s">
         <v>113</v>
       </c>
@@ -7142,7 +7076,7 @@
       <c r="H40" s="7"/>
       <c r="I40" s="11"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="9" t="s">
         <v>114</v>
       </c>
@@ -7163,7 +7097,7 @@
       <c r="H41" s="7"/>
       <c r="I41" s="11"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="9" t="s">
         <v>115</v>
       </c>
@@ -7184,7 +7118,7 @@
       <c r="H42" s="7"/>
       <c r="I42" s="11"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="9" t="s">
         <v>116</v>
       </c>
@@ -7205,7 +7139,7 @@
       <c r="H43" s="7"/>
       <c r="I43" s="11"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="9" t="s">
         <v>117</v>
       </c>
@@ -7226,7 +7160,7 @@
       <c r="H44" s="7"/>
       <c r="I44" s="11"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="9" t="s">
         <v>118</v>
       </c>
@@ -7247,7 +7181,7 @@
       <c r="H45" s="7"/>
       <c r="I45" s="11"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="9" t="s">
         <v>119</v>
       </c>
@@ -7268,7 +7202,7 @@
       <c r="H46" s="7"/>
       <c r="I46" s="11"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="9" t="s">
         <v>120</v>
       </c>
@@ -7289,7 +7223,7 @@
       <c r="H47" s="7"/>
       <c r="I47" s="11"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="9" t="s">
         <v>121</v>
       </c>
@@ -7310,7 +7244,7 @@
       <c r="H48" s="7"/>
       <c r="I48" s="11"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="9" t="s">
         <v>122</v>
       </c>
@@ -7331,7 +7265,7 @@
       <c r="H49" s="7"/>
       <c r="I49" s="11"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="9" t="s">
         <v>123</v>
       </c>
@@ -7352,7 +7286,7 @@
       <c r="H50" s="7"/>
       <c r="I50" s="11"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="9" t="s">
         <v>124</v>
       </c>
@@ -7373,7 +7307,7 @@
       <c r="H51" s="7"/>
       <c r="I51" s="11"/>
     </row>
-    <row r="52" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="14" t="s">
         <v>707</v>
       </c>
@@ -7394,7 +7328,7 @@
       <c r="H52" s="11"/>
       <c r="I52" s="11"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="9" t="s">
         <v>125</v>
       </c>
@@ -7415,7 +7349,7 @@
       <c r="H53" s="7"/>
       <c r="I53" s="11"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="9" t="s">
         <v>126</v>
       </c>
@@ -7436,7 +7370,7 @@
       <c r="H54" s="7"/>
       <c r="I54" s="11"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="9" t="s">
         <v>127</v>
       </c>
@@ -7457,7 +7391,7 @@
       <c r="H55" s="7"/>
       <c r="I55" s="11"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="9" t="s">
         <v>138</v>
       </c>
@@ -7475,7 +7409,7 @@
       <c r="H56" s="7"/>
       <c r="I56" s="11"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="9" t="s">
         <v>139</v>
       </c>
@@ -7493,7 +7427,7 @@
       <c r="H57" s="7"/>
       <c r="I57" s="11"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="9" t="s">
         <v>140</v>
       </c>
@@ -7511,7 +7445,7 @@
       <c r="H58" s="7"/>
       <c r="I58" s="11"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="9" t="s">
         <v>141</v>
       </c>
@@ -7529,7 +7463,7 @@
       <c r="H59" s="7"/>
       <c r="I59" s="11"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="9" t="s">
         <v>142</v>
       </c>
@@ -7547,7 +7481,7 @@
       <c r="H60" s="7"/>
       <c r="I60" s="11"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="9" t="s">
         <v>143</v>
       </c>
@@ -7565,7 +7499,7 @@
       <c r="H61" s="7"/>
       <c r="I61" s="11"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="9" t="s">
         <v>144</v>
       </c>
@@ -7583,7 +7517,7 @@
       <c r="H62" s="7"/>
       <c r="I62" s="11"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="9" t="s">
         <v>145</v>
       </c>
@@ -7601,7 +7535,7 @@
       <c r="H63" s="7"/>
       <c r="I63" s="11"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="9" t="s">
         <v>146</v>
       </c>
@@ -7619,7 +7553,7 @@
       <c r="H64" s="7"/>
       <c r="I64" s="11"/>
     </row>
-    <row r="65" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="14" t="s">
         <v>165</v>
       </c>
@@ -7638,7 +7572,7 @@
       <c r="H65" s="11"/>
       <c r="I65" s="11"/>
     </row>
-    <row r="66" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="14" t="s">
         <v>276</v>
       </c>
@@ -7657,7 +7591,7 @@
       <c r="H66" s="11"/>
       <c r="I66" s="11"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="8" t="s">
         <v>159</v>
       </c>
@@ -7678,7 +7612,7 @@
       <c r="H67" s="7"/>
       <c r="I67" s="11"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="9" t="s">
         <v>160</v>
       </c>
@@ -7698,25 +7632,25 @@
       <c r="G68" s="11"/>
       <c r="I68" s="11"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="G69" s="11"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="G70" s="11"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="G71" s="11"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="G72" s="11"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="G73" s="11"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="G74" s="11"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="G75" s="11"/>
     </row>
   </sheetData>
@@ -7739,15 +7673,15 @@
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.15625" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.68359375" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -7758,7 +7692,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="13" t="s">
         <v>265</v>
       </c>
@@ -7785,24 +7719,24 @@
       <selection pane="topRight" activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="63.140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.26171875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="63.15625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="11.41796875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="11.68359375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83984375" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="65.5703125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="65.578125" style="10" customWidth="1"/>
     <col min="8" max="8" width="13" style="10" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" style="60" customWidth="1"/>
+    <col min="9" max="9" width="24.68359375" style="60" customWidth="1"/>
     <col min="10" max="10" width="13" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="14.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.83984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="14.26171875" style="10" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -7837,7 +7771,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="35" t="s">
         <v>459</v>
       </c>
@@ -7860,7 +7794,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="35" t="s">
         <v>460</v>
       </c>
@@ -7883,7 +7817,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="35" t="s">
         <v>461</v>
       </c>
@@ -7909,7 +7843,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="35" t="s">
         <v>492</v>
       </c>
@@ -7935,7 +7869,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="35" t="s">
         <v>462</v>
       </c>
@@ -7960,7 +7894,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="33" t="s">
         <v>463</v>
       </c>
@@ -7985,7 +7919,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="33" t="s">
         <v>464</v>
       </c>
@@ -8010,7 +7944,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="33" t="s">
         <v>493</v>
       </c>
@@ -8035,7 +7969,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="13" t="s">
         <v>183</v>
       </c>
@@ -8060,7 +7994,7 @@
       </c>
       <c r="K10" s="11"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="13" t="s">
         <v>184</v>
       </c>
@@ -8085,7 +8019,7 @@
       </c>
       <c r="K11" s="11"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="13" t="s">
         <v>185</v>
       </c>
@@ -8110,7 +8044,7 @@
       </c>
       <c r="K12" s="11"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="13" t="s">
         <v>186</v>
       </c>
@@ -8135,7 +8069,7 @@
       </c>
       <c r="K13" s="11"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="13" t="s">
         <v>187</v>
       </c>
@@ -8160,7 +8094,7 @@
       </c>
       <c r="K14" s="11"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="13" t="s">
         <v>188</v>
       </c>
@@ -8185,7 +8119,7 @@
       </c>
       <c r="K15" s="11"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="13" t="s">
         <v>189</v>
       </c>
@@ -8210,7 +8144,7 @@
       </c>
       <c r="K16" s="11"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="13" t="s">
         <v>190</v>
       </c>
@@ -8235,7 +8169,7 @@
       </c>
       <c r="K17" s="11"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="13" t="s">
         <v>237</v>
       </c>
@@ -8258,7 +8192,7 @@
       </c>
       <c r="K18" s="11"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="13" t="s">
         <v>238</v>
       </c>
@@ -8281,7 +8215,7 @@
       </c>
       <c r="K19" s="11"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="13" t="s">
         <v>231</v>
       </c>
@@ -8306,7 +8240,7 @@
       </c>
       <c r="K20" s="11"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="13" t="s">
         <v>239</v>
       </c>
@@ -8329,7 +8263,7 @@
       </c>
       <c r="K21" s="11"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="17" t="s">
         <v>240</v>
       </c>
@@ -8352,7 +8286,7 @@
       </c>
       <c r="K22" s="11"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="17" t="s">
         <v>241</v>
       </c>
@@ -8375,7 +8309,7 @@
       </c>
       <c r="K23" s="11"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="33" t="s">
         <v>465</v>
       </c>
@@ -8402,7 +8336,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="33" t="s">
         <v>466</v>
       </c>
@@ -8429,7 +8363,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="33" t="s">
         <v>467</v>
       </c>
@@ -8456,7 +8390,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="33" t="s">
         <v>468</v>
       </c>
@@ -8483,7 +8417,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="33" t="s">
         <v>470</v>
       </c>
@@ -8510,7 +8444,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="33" t="s">
         <v>471</v>
       </c>
@@ -8537,7 +8471,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="33" t="s">
         <v>472</v>
       </c>
@@ -8564,7 +8498,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="33" t="s">
         <v>473</v>
       </c>
@@ -8591,7 +8525,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="33" t="s">
         <v>474</v>
       </c>
@@ -8618,7 +8552,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="33" t="s">
         <v>475</v>
       </c>
@@ -8645,7 +8579,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="33" t="s">
         <v>476</v>
       </c>
@@ -8672,7 +8606,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="33" t="s">
         <v>477</v>
       </c>
@@ -8699,7 +8633,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="33" t="s">
         <v>478</v>
       </c>
@@ -8726,7 +8660,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="33" t="s">
         <v>479</v>
       </c>
@@ -8753,7 +8687,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="33" t="s">
         <v>480</v>
       </c>
@@ -8780,7 +8714,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="33" t="s">
         <v>481</v>
       </c>
@@ -8807,7 +8741,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="33" t="s">
         <v>482</v>
       </c>
@@ -8834,7 +8768,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="33" t="s">
         <v>483</v>
       </c>
@@ -8861,7 +8795,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="33" t="s">
         <v>484</v>
       </c>
@@ -8888,7 +8822,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="33" t="s">
         <v>485</v>
       </c>
@@ -8915,7 +8849,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="33" t="s">
         <v>486</v>
       </c>
@@ -8942,7 +8876,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="33" t="s">
         <v>487</v>
       </c>
@@ -8969,7 +8903,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="33" t="s">
         <v>488</v>
       </c>
@@ -8996,7 +8930,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="33" t="s">
         <v>489</v>
       </c>
@@ -9023,7 +8957,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="33" t="s">
         <v>490</v>
       </c>
@@ -9050,7 +8984,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="33" t="s">
         <v>431</v>
       </c>
@@ -9077,7 +9011,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="33" t="s">
         <v>458</v>
       </c>
@@ -9104,7 +9038,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="33" t="s">
         <v>469</v>
       </c>
@@ -9131,7 +9065,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="11" t="s">
         <v>167</v>
       </c>
@@ -9156,7 +9090,7 @@
       </c>
       <c r="K52" s="11"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="11" t="s">
         <v>170</v>
       </c>
@@ -9179,7 +9113,7 @@
       </c>
       <c r="K53" s="11"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="11" t="s">
         <v>168</v>
       </c>
@@ -9206,7 +9140,7 @@
       </c>
       <c r="K54" s="11"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="11" t="s">
         <v>169</v>
       </c>
@@ -9231,7 +9165,7 @@
       </c>
       <c r="K55" s="11"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="11" t="s">
         <v>783</v>
       </c>
@@ -9254,7 +9188,7 @@
       </c>
       <c r="K56" s="11"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="11" t="s">
         <v>173</v>
       </c>
@@ -9279,7 +9213,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="11" t="s">
         <v>543</v>
       </c>
@@ -9304,7 +9238,7 @@
       </c>
       <c r="K58" s="11"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="11" t="s">
         <v>711</v>
       </c>
@@ -9329,7 +9263,7 @@
       </c>
       <c r="K59" s="11"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="11" t="s">
         <v>547</v>
       </c>
@@ -9354,7 +9288,7 @@
       </c>
       <c r="K60" s="11"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="11" t="s">
         <v>611</v>
       </c>
@@ -9379,7 +9313,7 @@
       </c>
       <c r="K61" s="11"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="11" t="s">
         <v>612</v>
       </c>
@@ -9404,7 +9338,7 @@
       </c>
       <c r="K62" s="11"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="11" t="s">
         <v>609</v>
       </c>
@@ -9428,7 +9362,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="11" t="s">
         <v>175</v>
       </c>
@@ -9452,7 +9386,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="65" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="22" t="s">
         <v>374</v>
       </c>
@@ -9476,7 +9410,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="66" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="49" t="s">
         <v>647</v>
       </c>
@@ -9500,7 +9434,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="67" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="49" t="s">
         <v>646</v>
       </c>
@@ -9524,7 +9458,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="68" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="19" t="s">
         <v>178</v>
       </c>
@@ -9548,7 +9482,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="69" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="49" t="s">
         <v>649</v>
       </c>
@@ -9572,7 +9506,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="70" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="49" t="s">
         <v>648</v>
       </c>
@@ -9596,7 +9530,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="11" t="s">
         <v>224</v>
       </c>
@@ -9621,7 +9555,7 @@
       </c>
       <c r="K71" s="11"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="11" t="s">
         <v>225</v>
       </c>
@@ -9646,7 +9580,7 @@
       </c>
       <c r="K72" s="11"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="11" t="s">
         <v>228</v>
       </c>
@@ -9671,7 +9605,7 @@
       </c>
       <c r="K73" s="11"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="13" t="s">
         <v>176</v>
       </c>
@@ -9696,7 +9630,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="13" t="s">
         <v>179</v>
       </c>
@@ -9721,7 +9655,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="13" t="s">
         <v>177</v>
       </c>
@@ -9746,7 +9680,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="13" t="s">
         <v>181</v>
       </c>
@@ -9771,7 +9705,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="13" t="s">
         <v>180</v>
       </c>
@@ -9796,7 +9730,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="13" t="s">
         <v>182</v>
       </c>
@@ -9821,7 +9755,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="13" t="s">
         <v>232</v>
       </c>
@@ -9844,7 +9778,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="13" t="s">
         <v>233</v>
       </c>
@@ -9867,7 +9801,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="13" t="s">
         <v>234</v>
       </c>
@@ -9890,7 +9824,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="13" t="s">
         <v>235</v>
       </c>
@@ -9913,7 +9847,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="13" t="s">
         <v>236</v>
       </c>
@@ -9936,7 +9870,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="13" t="s">
         <v>246</v>
       </c>
@@ -9959,7 +9893,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="13" t="s">
         <v>247</v>
       </c>
@@ -9982,7 +9916,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="13" t="s">
         <v>259</v>
       </c>
@@ -10004,7 +9938,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="13" t="s">
         <v>261</v>
       </c>
@@ -10026,7 +9960,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="11" t="s">
         <v>174</v>
       </c>
@@ -10051,7 +9985,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="11" t="s">
         <v>208</v>
       </c>
@@ -10076,7 +10010,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="11" t="s">
         <v>212</v>
       </c>
@@ -10101,7 +10035,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="11" t="s">
         <v>191</v>
       </c>
@@ -10128,7 +10062,7 @@
       </c>
       <c r="K92" s="11"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="11" t="s">
         <v>375</v>
       </c>
@@ -10153,7 +10087,7 @@
       </c>
       <c r="K93" s="11"/>
     </row>
-    <row r="94" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="26" t="s">
         <v>362</v>
       </c>
@@ -10177,7 +10111,7 @@
       </c>
       <c r="K94" s="22"/>
     </row>
-    <row r="95" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="22" t="s">
         <v>366</v>
       </c>
@@ -10201,7 +10135,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="96" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="26" t="s">
         <v>367</v>
       </c>
@@ -10225,7 +10159,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="97" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="26" t="s">
         <v>363</v>
       </c>
@@ -10248,7 +10182,7 @@
       </c>
       <c r="K97" s="22"/>
     </row>
-    <row r="98" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="22" t="s">
         <v>361</v>
       </c>
@@ -10272,7 +10206,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="99" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="35" t="s">
         <v>524</v>
       </c>
@@ -10294,7 +10228,7 @@
       </c>
       <c r="K99" s="33"/>
     </row>
-    <row r="100" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="35" t="s">
         <v>525</v>
       </c>
@@ -10316,7 +10250,7 @@
       </c>
       <c r="K100" s="33"/>
     </row>
-    <row r="101" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="35" t="s">
         <v>526</v>
       </c>
@@ -10338,7 +10272,7 @@
       </c>
       <c r="K101" s="33"/>
     </row>
-    <row r="102" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="35" t="s">
         <v>527</v>
       </c>
@@ -10360,7 +10294,7 @@
       </c>
       <c r="K102" s="33"/>
     </row>
-    <row r="103" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="35" t="s">
         <v>528</v>
       </c>
@@ -10382,7 +10316,7 @@
       </c>
       <c r="K103" s="33"/>
     </row>
-    <row r="104" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="35" t="s">
         <v>529</v>
       </c>
@@ -10404,7 +10338,7 @@
       </c>
       <c r="K104" s="33"/>
     </row>
-    <row r="105" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="41" t="s">
         <v>536</v>
       </c>
@@ -10427,7 +10361,7 @@
       </c>
       <c r="K105" s="42"/>
     </row>
-    <row r="106" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="41" t="s">
         <v>544</v>
       </c>
@@ -10452,7 +10386,7 @@
       </c>
       <c r="K106" s="42"/>
     </row>
-    <row r="107" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="41" t="s">
         <v>625</v>
       </c>
@@ -10477,7 +10411,7 @@
       </c>
       <c r="K107" s="42"/>
     </row>
-    <row r="108" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="41" t="s">
         <v>626</v>
       </c>
@@ -10502,7 +10436,7 @@
       </c>
       <c r="K108" s="42"/>
     </row>
-    <row r="109" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="41" t="s">
         <v>627</v>
       </c>
@@ -10527,7 +10461,7 @@
       </c>
       <c r="K109" s="42"/>
     </row>
-    <row r="110" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="41" t="s">
         <v>629</v>
       </c>
@@ -10552,7 +10486,7 @@
       </c>
       <c r="K110" s="42"/>
     </row>
-    <row r="111" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="41" t="s">
         <v>636</v>
       </c>
@@ -10577,7 +10511,7 @@
       </c>
       <c r="K111" s="42"/>
     </row>
-    <row r="112" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="41" t="s">
         <v>622</v>
       </c>
@@ -10601,7 +10535,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="113" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="52" t="s">
         <v>583</v>
       </c>
@@ -10625,7 +10559,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="114" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="52" t="s">
         <v>582</v>
       </c>
@@ -10649,7 +10583,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="115" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="52" t="s">
         <v>581</v>
       </c>
@@ -10673,7 +10607,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="116" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="52" t="s">
         <v>580</v>
       </c>
@@ -10697,7 +10631,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="117" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="52" t="s">
         <v>584</v>
       </c>
@@ -10721,7 +10655,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="118" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="52" t="s">
         <v>594</v>
       </c>
@@ -10745,7 +10679,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="119" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="52" t="s">
         <v>595</v>
       </c>
@@ -10769,7 +10703,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="120" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="52" t="s">
         <v>596</v>
       </c>
@@ -10793,7 +10727,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="121" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="52" t="s">
         <v>597</v>
       </c>
@@ -10817,7 +10751,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="122" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="52" t="s">
         <v>598</v>
       </c>
@@ -10841,7 +10775,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="123" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="35" t="s">
         <v>538</v>
       </c>
@@ -10864,7 +10798,7 @@
       </c>
       <c r="K123" s="33"/>
     </row>
-    <row r="124" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="35" t="s">
         <v>545</v>
       </c>
@@ -10889,7 +10823,7 @@
       </c>
       <c r="K124" s="33"/>
     </row>
-    <row r="125" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="35" t="s">
         <v>628</v>
       </c>
@@ -10914,7 +10848,7 @@
       </c>
       <c r="K125" s="33"/>
     </row>
-    <row r="126" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="35" t="s">
         <v>632</v>
       </c>
@@ -10939,7 +10873,7 @@
       </c>
       <c r="K126" s="33"/>
     </row>
-    <row r="127" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="35" t="s">
         <v>631</v>
       </c>
@@ -10964,7 +10898,7 @@
       </c>
       <c r="K127" s="33"/>
     </row>
-    <row r="128" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="35" t="s">
         <v>630</v>
       </c>
@@ -10989,7 +10923,7 @@
       </c>
       <c r="K128" s="33"/>
     </row>
-    <row r="129" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="35" t="s">
         <v>637</v>
       </c>
@@ -11014,7 +10948,7 @@
       </c>
       <c r="K129" s="33"/>
     </row>
-    <row r="130" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="35" t="s">
         <v>623</v>
       </c>
@@ -11038,7 +10972,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="131" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="52" t="s">
         <v>585</v>
       </c>
@@ -11062,7 +10996,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="132" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="52" t="s">
         <v>586</v>
       </c>
@@ -11086,7 +11020,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="133" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="52" t="s">
         <v>587</v>
       </c>
@@ -11110,7 +11044,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="134" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="52" t="s">
         <v>588</v>
       </c>
@@ -11134,7 +11068,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="135" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="52" t="s">
         <v>589</v>
       </c>
@@ -11158,7 +11092,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="136" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="52" t="s">
         <v>599</v>
       </c>
@@ -11182,7 +11116,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="137" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="52" t="s">
         <v>600</v>
       </c>
@@ -11206,7 +11140,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="138" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="52" t="s">
         <v>601</v>
       </c>
@@ -11230,7 +11164,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="139" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="52" t="s">
         <v>602</v>
       </c>
@@ -11254,7 +11188,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="140" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="52" t="s">
         <v>603</v>
       </c>
@@ -11278,7 +11212,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="141" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="43" t="s">
         <v>540</v>
       </c>
@@ -11301,7 +11235,7 @@
       </c>
       <c r="K141" s="45"/>
     </row>
-    <row r="142" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="43" t="s">
         <v>546</v>
       </c>
@@ -11326,7 +11260,7 @@
       </c>
       <c r="K142" s="45"/>
     </row>
-    <row r="143" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="43" t="s">
         <v>633</v>
       </c>
@@ -11351,7 +11285,7 @@
       </c>
       <c r="K143" s="45"/>
     </row>
-    <row r="144" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="43" t="s">
         <v>634</v>
       </c>
@@ -11376,7 +11310,7 @@
       </c>
       <c r="K144" s="45"/>
     </row>
-    <row r="145" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="43" t="s">
         <v>635</v>
       </c>
@@ -11401,7 +11335,7 @@
       </c>
       <c r="K145" s="45"/>
     </row>
-    <row r="146" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="43" t="s">
         <v>638</v>
       </c>
@@ -11426,7 +11360,7 @@
       </c>
       <c r="K146" s="45"/>
     </row>
-    <row r="147" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="43" t="s">
         <v>624</v>
       </c>
@@ -11451,7 +11385,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="148" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="52" t="s">
         <v>590</v>
       </c>
@@ -11475,7 +11409,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="149" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="52" t="s">
         <v>591</v>
       </c>
@@ -11499,7 +11433,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="150" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="52" t="s">
         <v>592</v>
       </c>
@@ -11523,7 +11457,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="151" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="52" t="s">
         <v>593</v>
       </c>
@@ -11547,7 +11481,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="152" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="52" t="s">
         <v>604</v>
       </c>
@@ -11571,7 +11505,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="153" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="52" t="s">
         <v>605</v>
       </c>
@@ -11595,7 +11529,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="154" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="52" t="s">
         <v>606</v>
       </c>
@@ -11619,7 +11553,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="155" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="52" t="s">
         <v>607</v>
       </c>
@@ -11643,7 +11577,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="13" t="s">
         <v>192</v>
       </c>
@@ -11668,7 +11602,7 @@
       </c>
       <c r="K156" s="11"/>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="13" t="s">
         <v>193</v>
       </c>
@@ -11693,7 +11627,7 @@
       </c>
       <c r="K157" s="11"/>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="13" t="s">
         <v>194</v>
       </c>
@@ -11718,7 +11652,7 @@
       </c>
       <c r="K158" s="11"/>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="13" t="s">
         <v>195</v>
       </c>
@@ -11743,7 +11677,7 @@
       </c>
       <c r="K159" s="11"/>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="13" t="s">
         <v>196</v>
       </c>
@@ -11768,7 +11702,7 @@
       </c>
       <c r="K160" s="11"/>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="13" t="s">
         <v>197</v>
       </c>
@@ -11793,7 +11727,7 @@
       </c>
       <c r="K161" s="11"/>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="13" t="s">
         <v>198</v>
       </c>
@@ -11818,7 +11752,7 @@
       </c>
       <c r="K162" s="11"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="13" t="s">
         <v>199</v>
       </c>
@@ -11843,7 +11777,7 @@
       </c>
       <c r="K163" s="11"/>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="13" t="s">
         <v>200</v>
       </c>
@@ -11868,7 +11802,7 @@
       </c>
       <c r="K164" s="11"/>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="13" t="s">
         <v>201</v>
       </c>
@@ -11893,7 +11827,7 @@
       </c>
       <c r="K165" s="11"/>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="13" t="s">
         <v>202</v>
       </c>
@@ -11918,7 +11852,7 @@
       </c>
       <c r="K166" s="11"/>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="13" t="s">
         <v>203</v>
       </c>
@@ -11943,7 +11877,7 @@
       </c>
       <c r="K167" s="11"/>
     </row>
-    <row r="168" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="33" t="s">
         <v>737</v>
       </c>
@@ -11970,7 +11904,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="169" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="33" t="s">
         <v>738</v>
       </c>
@@ -11997,7 +11931,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="170" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="33" t="s">
         <v>739</v>
       </c>
@@ -12024,7 +11958,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="171" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="33" t="s">
         <v>740</v>
       </c>
@@ -12051,7 +11985,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="172" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="33" t="s">
         <v>741</v>
       </c>
@@ -12078,7 +12012,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="173" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="33" t="s">
         <v>742</v>
       </c>
@@ -12105,7 +12039,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="174" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="33" t="s">
         <v>761</v>
       </c>
@@ -12132,7 +12066,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="175" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="33" t="s">
         <v>762</v>
       </c>
@@ -12159,7 +12093,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="176" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="33" t="s">
         <v>763</v>
       </c>
@@ -12186,7 +12120,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="177" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="33" t="s">
         <v>752</v>
       </c>
@@ -12213,7 +12147,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="178" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="33" t="s">
         <v>753</v>
       </c>
@@ -12240,7 +12174,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="179" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="33" t="s">
         <v>754</v>
       </c>
@@ -12267,7 +12201,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="180" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="33" t="s">
         <v>755</v>
       </c>
@@ -12294,7 +12228,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="181" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="33" t="s">
         <v>756</v>
       </c>
@@ -12321,7 +12255,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="182" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="33" t="s">
         <v>757</v>
       </c>
@@ -12348,17 +12282,17 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E183" s="11"/>
       <c r="F183" s="11"/>
       <c r="I183" s="59"/>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E184" s="11"/>
       <c r="F184" s="11"/>
       <c r="I184" s="59"/>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E185" s="11"/>
       <c r="F185" s="11"/>
       <c r="I185" s="59"/>
@@ -12391,13 +12325,13 @@
       <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="55.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.83984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="18" t="s">
         <v>359</v>
       </c>
@@ -12405,7 +12339,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>280</v>
       </c>
@@ -12413,7 +12347,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>348</v>
       </c>
@@ -12421,7 +12355,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>349</v>
       </c>
@@ -12429,7 +12363,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>350</v>
       </c>
@@ -12437,8 +12371,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="18" t="s">
         <v>353</v>
       </c>
@@ -12446,7 +12380,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="10" t="s">
         <v>351</v>
       </c>
@@ -12454,7 +12388,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="10" t="s">
         <v>348</v>
       </c>
@@ -12462,7 +12396,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="10" t="s">
         <v>349</v>
       </c>
@@ -12471,12 +12405,12 @@
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="18" t="s">
         <v>354</v>
       </c>
@@ -12485,7 +12419,7 @@
       </c>
       <c r="E12" s="14"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="10" t="s">
         <v>352</v>
       </c>
@@ -12494,7 +12428,7 @@
       </c>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="10" t="s">
         <v>348</v>
       </c>
@@ -12503,7 +12437,7 @@
       </c>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="10" t="s">
         <v>349</v>
       </c>
@@ -12512,18 +12446,18 @@
       </c>
       <c r="E15" s="14"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="E16" s="14"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E17" s="14"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="13"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="13"/>
     </row>
   </sheetData>
@@ -12536,18 +12470,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.15625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="10" customWidth="1"/>
-    <col min="3" max="3" width="104.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="104.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="12" t="s">
         <v>343</v>
       </c>
@@ -12561,7 +12495,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>101</v>
       </c>
@@ -12569,13 +12503,13 @@
         <v>303</v>
       </c>
       <c r="C2" t="s">
-        <v>806</v>
+        <v>98</v>
       </c>
       <c r="D2" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>279</v>
       </c>
@@ -12583,13 +12517,13 @@
         <v>303</v>
       </c>
       <c r="C3" t="s">
-        <v>807</v>
+        <v>72</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>280</v>
       </c>
@@ -12597,11 +12531,11 @@
         <v>303</v>
       </c>
       <c r="C4" t="s">
-        <v>808</v>
+        <v>95</v>
       </c>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>281</v>
       </c>
@@ -12609,11 +12543,11 @@
         <v>303</v>
       </c>
       <c r="C5" t="s">
-        <v>809</v>
+        <v>100</v>
       </c>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>282</v>
       </c>
@@ -12621,11 +12555,11 @@
         <v>303</v>
       </c>
       <c r="C6" t="s">
-        <v>810</v>
+        <v>96</v>
       </c>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>283</v>
       </c>
@@ -12633,11 +12567,11 @@
         <v>303</v>
       </c>
       <c r="C7" t="s">
-        <v>811</v>
+        <v>97</v>
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>284</v>
       </c>
@@ -12649,7 +12583,7 @@
       </c>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>285</v>
       </c>
@@ -12661,7 +12595,7 @@
       </c>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>286</v>
       </c>
@@ -12673,7 +12607,7 @@
       </c>
       <c r="G10" s="10"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>287</v>
       </c>
@@ -12681,11 +12615,11 @@
         <v>303</v>
       </c>
       <c r="C11" t="s">
-        <v>812</v>
+        <v>94</v>
       </c>
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>288</v>
       </c>
@@ -12693,11 +12627,11 @@
         <v>303</v>
       </c>
       <c r="C12" t="s">
-        <v>813</v>
+        <v>93</v>
       </c>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>289</v>
       </c>
@@ -12712,7 +12646,7 @@
       </c>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>290</v>
       </c>
@@ -12724,7 +12658,7 @@
       </c>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>291</v>
       </c>
@@ -12736,7 +12670,7 @@
       </c>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>292</v>
       </c>
@@ -12748,7 +12682,7 @@
       </c>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>293</v>
       </c>
@@ -12760,7 +12694,7 @@
       </c>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>294</v>
       </c>
@@ -12768,14 +12702,14 @@
         <v>303</v>
       </c>
       <c r="C18" t="s">
-        <v>819</v>
+        <v>65</v>
       </c>
       <c r="D18" t="s">
         <v>306</v>
       </c>
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>295</v>
       </c>
@@ -12783,11 +12717,11 @@
         <v>303</v>
       </c>
       <c r="C19" t="s">
-        <v>814</v>
+        <v>165</v>
       </c>
       <c r="G19" s="10"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>296</v>
       </c>
@@ -12795,11 +12729,11 @@
         <v>303</v>
       </c>
       <c r="C20" t="s">
-        <v>815</v>
+        <v>807</v>
       </c>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>704</v>
       </c>
@@ -12807,11 +12741,11 @@
         <v>303</v>
       </c>
       <c r="C21" t="s">
-        <v>816</v>
+        <v>115</v>
       </c>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>705</v>
       </c>
@@ -12819,11 +12753,11 @@
         <v>303</v>
       </c>
       <c r="C22" t="s">
-        <v>817</v>
+        <v>127</v>
       </c>
       <c r="G22" s="10"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>706</v>
       </c>
@@ -12831,11 +12765,11 @@
         <v>303</v>
       </c>
       <c r="C23" t="s">
-        <v>818</v>
+        <v>707</v>
       </c>
       <c r="G23" s="10"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>794</v>
       </c>
@@ -12843,11 +12777,11 @@
         <v>303</v>
       </c>
       <c r="C24" t="s">
-        <v>820</v>
+        <v>737</v>
       </c>
       <c r="G24" s="10"/>
     </row>
-    <row r="25" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="10" t="s">
         <v>795</v>
       </c>
@@ -12855,10 +12789,10 @@
         <v>303</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="10" t="s">
         <v>796</v>
       </c>
@@ -12866,10 +12800,10 @@
         <v>303</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="10" t="s">
         <v>797</v>
       </c>
@@ -12877,10 +12811,10 @@
         <v>303</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>823</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="10" t="s">
         <v>798</v>
       </c>
@@ -12888,11 +12822,11 @@
         <v>303</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>824</v>
+        <v>741</v>
       </c>
       <c r="G28" s="10"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="10" t="s">
         <v>799</v>
       </c>
@@ -12900,11 +12834,11 @@
         <v>303</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>825</v>
+        <v>742</v>
       </c>
       <c r="G29" s="10"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>800</v>
       </c>
@@ -12912,11 +12846,11 @@
         <v>303</v>
       </c>
       <c r="C30" t="s">
-        <v>826</v>
+        <v>761</v>
       </c>
       <c r="G30" s="10"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="10" t="s">
         <v>801</v>
       </c>
@@ -12924,11 +12858,11 @@
         <v>303</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>827</v>
+        <v>762</v>
       </c>
       <c r="G31" s="10"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="10" t="s">
         <v>802</v>
       </c>
@@ -12936,19 +12870,19 @@
         <v>303</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>828</v>
+        <v>763</v>
       </c>
       <c r="G32" s="10"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="10" t="s">
-        <v>829</v>
+        <v>806</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>303</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>830</v>
+        <v>808</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update TB xlsx files
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\tb-ucl-analyses\general\frameworks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romesh.abey\Desktop\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="16095" windowHeight="9660" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="468" windowWidth="16098" windowHeight="9660" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="14" r:id="rId1"/>
@@ -870,7 +870,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1868" uniqueCount="831">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1868" uniqueCount="809">
   <si>
     <t>Code Name</t>
   </si>
@@ -3290,85 +3290,19 @@
     <t>Early-LTBI (diagnosis restricted) annual probability of initiating treatment</t>
   </si>
   <si>
-    <t>{'Total population size': ['alive']}</t>
-  </si>
-  <si>
-    <t>{'Latent infections': ['lt_inf']}</t>
-  </si>
-  <si>
-    <t>{'Active TB': ['ac_inf']}</t>
-  </si>
-  <si>
-    <t>{'Active DS-TB': ['ds_inf']}</t>
-  </si>
-  <si>
-    <t>{'Active MDR-TB': ['mdr_inf']}</t>
-  </si>
-  <si>
-    <t>{'Active XDR-TB': ['xdr_inf']}</t>
-  </si>
-  <si>
-    <t>{'Smear negative active TB': ['sn_inf']}</t>
-  </si>
-  <si>
-    <t>{'Smear positive active TB': ['sp_inf']}</t>
-  </si>
-  <si>
-    <t>{'Active treatment': ['num_treat']}</t>
-  </si>
-  <si>
-    <t>{'TB-related deaths': [':ddis']}</t>
-  </si>
-  <si>
-    <t>{'Latent prevalence': ['lt_prev']}</t>
-  </si>
-  <si>
-    <t>{'Active prevalence': ['ac_prev']}</t>
-  </si>
-  <si>
-    <t>{'DR prevalence': ['dr_prev']}</t>
-  </si>
-  <si>
-    <t>{'Latent treatment': ['ltt_inf']}</t>
-  </si>
-  <si>
-    <t>{'Annual diagnosis rate': ['pd_diag']}</t>
-  </si>
-  <si>
-    <t>{'Annual diagnosis rate': ['pm_diag']}</t>
-  </si>
-  <si>
-    <t>{'Annual diagnosis rate': ['px_diag']}</t>
-  </si>
-  <si>
-    <t>{'Annual diagnosis rate': ['nd_diag']}</t>
-  </si>
-  <si>
-    <t>{'Annual diagnosis rate': ['nm_diag']}</t>
-  </si>
-  <si>
-    <t>{'Annual diagnosis rate': ['nx_diag']}</t>
-  </si>
-  <si>
-    <t>{'Annual treatment initiation': ['d_treat']}</t>
-  </si>
-  <si>
-    <t>{'Annual treatment initiation': ['m_treat']}</t>
-  </si>
-  <si>
-    <t>{'Annual treatment initiation': ['x_treat']}</t>
-  </si>
-  <si>
     <t>SP-DS number diagnosed</t>
   </si>
   <si>
-    <t>{'number diagnosed': ['spdu:spdd']}</t>
+    <t>:ddis</t>
+  </si>
+  <si>
+    <t>spdu:spdd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3972,9 +3906,9 @@
       <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="18" t="s">
         <v>343</v>
       </c>
@@ -3982,7 +3916,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="20" t="s">
         <v>345</v>
       </c>
@@ -4003,14 +3937,14 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="25.68359375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="34.26171875" style="3" customWidth="1"/>
     <col min="3" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>57</v>
       </c>
@@ -4018,7 +3952,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="7" t="s">
         <v>59</v>
       </c>
@@ -4026,7 +3960,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="11" t="s">
         <v>427</v>
       </c>
@@ -4034,7 +3968,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="11" t="s">
         <v>430</v>
       </c>
@@ -4042,7 +3976,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="7" t="s">
         <v>61</v>
       </c>
@@ -4050,7 +3984,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="7" t="s">
         <v>429</v>
       </c>
@@ -4058,7 +3992,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="11" t="s">
         <v>378</v>
       </c>
@@ -4066,7 +4000,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="11" t="s">
         <v>491</v>
       </c>
@@ -4074,7 +4008,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="7" t="s">
         <v>60</v>
       </c>
@@ -4082,7 +4016,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="7" t="s">
         <v>542</v>
       </c>
@@ -4090,23 +4024,23 @@
         <v>719</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
     </row>
@@ -4124,20 +4058,20 @@
       <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.68359375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.41796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.26171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.26171875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.68359375" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.26171875" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.15625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4167,7 +4101,7 @@
       </c>
       <c r="J1" s="18"/>
     </row>
-    <row r="2" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="32" t="s">
         <v>432</v>
       </c>
@@ -4192,7 +4126,7 @@
       </c>
       <c r="I2" s="22"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
@@ -4213,7 +4147,7 @@
       </c>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
@@ -4237,7 +4171,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
@@ -4261,7 +4195,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
@@ -4285,7 +4219,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="6" t="s">
         <v>567</v>
       </c>
@@ -4308,7 +4242,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
@@ -4332,7 +4266,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="6" t="s">
         <v>20</v>
       </c>
@@ -4356,7 +4290,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="6" t="s">
         <v>566</v>
       </c>
@@ -4379,7 +4313,7 @@
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
     </row>
-    <row r="11" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="27" t="s">
         <v>373</v>
       </c>
@@ -4404,7 +4338,7 @@
       </c>
       <c r="I11" s="22"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="6" t="s">
         <v>66</v>
       </c>
@@ -4428,7 +4362,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="6" t="s">
         <v>67</v>
       </c>
@@ -4452,7 +4386,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
@@ -4473,7 +4407,7 @@
       </c>
       <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="6" t="s">
         <v>22</v>
       </c>
@@ -4494,7 +4428,7 @@
       </c>
       <c r="G15" s="11"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="6" t="s">
         <v>23</v>
       </c>
@@ -4515,7 +4449,7 @@
       </c>
       <c r="G16" s="11"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="6" t="s">
         <v>24</v>
       </c>
@@ -4536,7 +4470,7 @@
       </c>
       <c r="G17" s="11"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="6" t="s">
         <v>25</v>
       </c>
@@ -4560,7 +4494,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="6" t="s">
         <v>565</v>
       </c>
@@ -4583,7 +4517,7 @@
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="6" t="s">
         <v>26</v>
       </c>
@@ -4604,7 +4538,7 @@
       </c>
       <c r="G20" s="11"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="6" t="s">
         <v>27</v>
       </c>
@@ -4625,7 +4559,7 @@
       </c>
       <c r="G21" s="11"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="6" t="s">
         <v>28</v>
       </c>
@@ -4649,7 +4583,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="6" t="s">
         <v>570</v>
       </c>
@@ -4672,7 +4606,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="6" t="s">
         <v>29</v>
       </c>
@@ -4693,7 +4627,7 @@
       </c>
       <c r="G24" s="11"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="6" t="s">
         <v>30</v>
       </c>
@@ -4714,7 +4648,7 @@
       </c>
       <c r="G25" s="11"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="6" t="s">
         <v>31</v>
       </c>
@@ -4738,7 +4672,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="6" t="s">
         <v>572</v>
       </c>
@@ -4761,7 +4695,7 @@
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="6" t="s">
         <v>32</v>
       </c>
@@ -4782,7 +4716,7 @@
       </c>
       <c r="G28" s="11"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="6" t="s">
         <v>33</v>
       </c>
@@ -4803,7 +4737,7 @@
       </c>
       <c r="G29" s="11"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="6" t="s">
         <v>34</v>
       </c>
@@ -4824,7 +4758,7 @@
       </c>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="6" t="s">
         <v>35</v>
       </c>
@@ -4848,7 +4782,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="6" t="s">
         <v>574</v>
       </c>
@@ -4871,7 +4805,7 @@
       <c r="H32" s="11"/>
       <c r="I32" s="11"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="6" t="s">
         <v>36</v>
       </c>
@@ -4892,7 +4826,7 @@
       </c>
       <c r="G33" s="11"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="6" t="s">
         <v>37</v>
       </c>
@@ -4913,7 +4847,7 @@
       </c>
       <c r="G34" s="11"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="6" t="s">
         <v>38</v>
       </c>
@@ -4937,7 +4871,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="6" t="s">
         <v>576</v>
       </c>
@@ -4960,7 +4894,7 @@
       <c r="H36" s="11"/>
       <c r="I36" s="11"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="6" t="s">
         <v>39</v>
       </c>
@@ -4981,7 +4915,7 @@
       </c>
       <c r="G37" s="11"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="6" t="s">
         <v>40</v>
       </c>
@@ -5002,7 +4936,7 @@
       </c>
       <c r="G38" s="11"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="6" t="s">
         <v>41</v>
       </c>
@@ -5026,7 +4960,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="6" t="s">
         <v>578</v>
       </c>
@@ -5049,7 +4983,7 @@
       <c r="H40" s="11"/>
       <c r="I40" s="11"/>
     </row>
-    <row r="41" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="27" t="s">
         <v>42</v>
       </c>
@@ -5074,7 +5008,7 @@
       </c>
       <c r="I41" s="22"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="6" t="s">
         <v>45</v>
       </c>
@@ -5095,7 +5029,7 @@
       </c>
       <c r="G42" s="11"/>
     </row>
-    <row r="43" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="6" t="s">
         <v>52</v>
       </c>
@@ -5118,7 +5052,7 @@
       <c r="H43" s="11"/>
       <c r="I43" s="7"/>
     </row>
-    <row r="44" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="27" t="s">
         <v>360</v>
       </c>
@@ -5141,7 +5075,7 @@
       <c r="H44" s="22"/>
       <c r="I44" s="22"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="6" t="s">
         <v>43</v>
       </c>
@@ -5162,7 +5096,7 @@
       </c>
       <c r="G45" s="11"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="6" t="s">
         <v>44</v>
       </c>
@@ -5183,7 +5117,7 @@
       </c>
       <c r="G46" s="11"/>
     </row>
-    <row r="47" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="6" t="s">
         <v>54</v>
       </c>
@@ -5206,16 +5140,16 @@
       <c r="H47" s="11"/>
       <c r="I47" s="7"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="G48" s="11"/>
     </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G49" s="11"/>
     </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G50" s="11"/>
     </row>
-    <row r="51" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G51" s="11"/>
     </row>
   </sheetData>
@@ -5242,59 +5176,59 @@
       <selection pane="topRight" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.26171875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.26171875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="10.83984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.68359375" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.41796875" style="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.15625" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.26171875" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.41796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.15625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.26171875" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.68359375" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.578125" style="11" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.5703125" style="11" customWidth="1"/>
+    <col min="16" max="16" width="11.15625" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.83984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.41796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.83984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.68359375" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.578125" style="11" customWidth="1"/>
     <col min="22" max="22" width="8" style="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.42578125" style="11" customWidth="1"/>
+    <col min="23" max="23" width="9.41796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.83984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.83984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.41796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.41796875" style="11" customWidth="1"/>
     <col min="28" max="28" width="5" style="11" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="6" style="11" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="7" style="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7.42578125" style="11" customWidth="1"/>
-    <col min="33" max="33" width="6.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="7.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.41796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.41796875" style="11" customWidth="1"/>
+    <col min="33" max="33" width="6.41796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="7.41796875" style="11" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="8" style="11" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="8" style="11" customWidth="1"/>
-    <col min="37" max="37" width="5.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="6.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.42578125" style="11" customWidth="1"/>
-    <col min="41" max="41" width="11.85546875" style="11" customWidth="1"/>
+    <col min="37" max="37" width="5.83984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="6.83984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.41796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.41796875" style="11" customWidth="1"/>
+    <col min="41" max="41" width="11.83984375" style="11" customWidth="1"/>
     <col min="42" max="42" width="3" style="11" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="4.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="6.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="4.83984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="6.15625" style="22" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="8" style="11" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="5.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="9.68359375" style="11" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="5.83984375" style="11" bestFit="1" customWidth="1"/>
     <col min="48" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="32" t="s">
         <v>432</v>
       </c>
@@ -5438,7 +5372,7 @@
       <c r="AX1" s="12"/>
       <c r="AY1" s="12"/>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="32" t="s">
         <v>432</v>
       </c>
@@ -5545,7 +5479,7 @@
       <c r="AX2" s="12"/>
       <c r="AY2" s="12"/>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="12" t="s">
         <v>13</v>
       </c>
@@ -5563,7 +5497,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="12" t="s">
         <v>15</v>
       </c>
@@ -5578,7 +5512,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="12" t="s">
         <v>17</v>
       </c>
@@ -5599,7 +5533,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="12" t="s">
         <v>18</v>
       </c>
@@ -5616,7 +5550,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="21" t="s">
         <v>567</v>
       </c>
@@ -5630,7 +5564,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="12" t="s">
         <v>19</v>
       </c>
@@ -5648,7 +5582,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="12" t="s">
         <v>20</v>
       </c>
@@ -5664,7 +5598,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="21" t="s">
         <v>566</v>
       </c>
@@ -5677,7 +5611,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="12" t="s">
         <v>373</v>
       </c>
@@ -5692,7 +5626,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="12" t="s">
         <v>66</v>
       </c>
@@ -5714,7 +5648,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="12" t="s">
         <v>67</v>
       </c>
@@ -5729,7 +5663,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="12" t="s">
         <v>21</v>
       </c>
@@ -5741,7 +5675,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="12" t="s">
         <v>22</v>
       </c>
@@ -5756,7 +5690,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="12" t="s">
         <v>23</v>
       </c>
@@ -5777,7 +5711,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="12" t="s">
         <v>24</v>
       </c>
@@ -5798,7 +5732,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="12" t="s">
         <v>25</v>
       </c>
@@ -5813,7 +5747,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="21" t="s">
         <v>565</v>
       </c>
@@ -5834,7 +5768,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="12" t="s">
         <v>26</v>
       </c>
@@ -5855,7 +5789,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="12" t="s">
         <v>27</v>
       </c>
@@ -5876,7 +5810,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="12" t="s">
         <v>28</v>
       </c>
@@ -5892,7 +5826,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="21" t="s">
         <v>570</v>
       </c>
@@ -5913,7 +5847,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="12" t="s">
         <v>29</v>
       </c>
@@ -5935,7 +5869,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="12" t="s">
         <v>30</v>
       </c>
@@ -5956,7 +5890,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="12" t="s">
         <v>31</v>
       </c>
@@ -5972,7 +5906,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="21" t="s">
         <v>572</v>
       </c>
@@ -5990,7 +5924,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="12" t="s">
         <v>32</v>
       </c>
@@ -6005,7 +5939,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="12" t="s">
         <v>33</v>
       </c>
@@ -6026,7 +5960,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="12" t="s">
         <v>34</v>
       </c>
@@ -6047,7 +5981,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="12" t="s">
         <v>35</v>
       </c>
@@ -6063,7 +5997,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="32" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="21" t="s">
         <v>574</v>
       </c>
@@ -6084,7 +6018,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="12" t="s">
         <v>36</v>
       </c>
@@ -6105,7 +6039,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="12" t="s">
         <v>37</v>
       </c>
@@ -6126,7 +6060,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="12" t="s">
         <v>38</v>
       </c>
@@ -6142,7 +6076,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="21" t="s">
         <v>576</v>
       </c>
@@ -6163,7 +6097,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="37" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="12" t="s">
         <v>39</v>
       </c>
@@ -6184,7 +6118,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="12" t="s">
         <v>40</v>
       </c>
@@ -6205,7 +6139,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="39" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="12" t="s">
         <v>41</v>
       </c>
@@ -6221,7 +6155,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="40" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="21" t="s">
         <v>578</v>
       </c>
@@ -6239,7 +6173,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="41" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="12" t="s">
         <v>42</v>
       </c>
@@ -6257,7 +6191,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="42" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="12" t="s">
         <v>45</v>
       </c>
@@ -6266,7 +6200,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="43" spans="1:47" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:47" s="22" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="21" t="s">
         <v>52</v>
       </c>
@@ -6275,7 +6209,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="44" spans="1:47" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:47" s="22" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="21" t="s">
         <v>360</v>
       </c>
@@ -6290,37 +6224,37 @@
         <v>363</v>
       </c>
     </row>
-    <row r="45" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="12" t="s">
         <v>43</v>
       </c>
       <c r="B45" s="12"/>
     </row>
-    <row r="46" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="12" t="s">
         <v>44</v>
       </c>
       <c r="B46" s="12"/>
     </row>
-    <row r="47" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="12" t="s">
         <v>54</v>
       </c>
       <c r="B47" s="12"/>
     </row>
-    <row r="48" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="12"/>
       <c r="B48" s="12"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="12"/>
       <c r="B49" s="12"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="12"/>
       <c r="B50" s="12"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="12"/>
       <c r="B51" s="12"/>
     </row>
@@ -6338,21 +6272,21 @@
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.68359375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.68359375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.41796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.68359375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.26171875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.41796875" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83984375" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -6381,7 +6315,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8" t="s">
         <v>65</v>
       </c>
@@ -6401,7 +6335,7 @@
       </c>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="8" t="s">
         <v>68</v>
       </c>
@@ -6421,7 +6355,7 @@
       </c>
       <c r="I3" s="11"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="8" t="s">
         <v>70</v>
       </c>
@@ -6441,7 +6375,7 @@
       </c>
       <c r="I4" s="11"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="8" t="s">
         <v>71</v>
       </c>
@@ -6461,7 +6395,7 @@
       </c>
       <c r="I5" s="11"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="8" t="s">
         <v>72</v>
       </c>
@@ -6481,7 +6415,7 @@
       </c>
       <c r="I6" s="11"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="9" t="s">
         <v>81</v>
       </c>
@@ -6501,7 +6435,7 @@
       </c>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="9" t="s">
         <v>82</v>
       </c>
@@ -6521,7 +6455,7 @@
       </c>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="9" t="s">
         <v>83</v>
       </c>
@@ -6541,7 +6475,7 @@
       </c>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="9" t="s">
         <v>84</v>
       </c>
@@ -6561,7 +6495,7 @@
       </c>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="9" t="s">
         <v>85</v>
       </c>
@@ -6581,7 +6515,7 @@
       </c>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="9" t="s">
         <v>86</v>
       </c>
@@ -6601,7 +6535,7 @@
       </c>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="9" t="s">
         <v>163</v>
       </c>
@@ -6619,7 +6553,7 @@
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="14" t="s">
         <v>273</v>
       </c>
@@ -6638,7 +6572,7 @@
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="9" t="s">
         <v>87</v>
       </c>
@@ -6658,7 +6592,7 @@
       </c>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="9" t="s">
         <v>88</v>
       </c>
@@ -6678,7 +6612,7 @@
       </c>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="9" t="s">
         <v>89</v>
       </c>
@@ -6698,7 +6632,7 @@
       </c>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="9" t="s">
         <v>90</v>
       </c>
@@ -6718,7 +6652,7 @@
       </c>
       <c r="I18" s="7"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="9" t="s">
         <v>91</v>
       </c>
@@ -6738,7 +6672,7 @@
       </c>
       <c r="I19" s="7"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="9" t="s">
         <v>92</v>
       </c>
@@ -6758,7 +6692,7 @@
       </c>
       <c r="I20" s="7"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="9" t="s">
         <v>93</v>
       </c>
@@ -6778,7 +6712,7 @@
       </c>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="9" t="s">
         <v>94</v>
       </c>
@@ -6798,7 +6732,7 @@
       </c>
       <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="9" t="s">
         <v>100</v>
       </c>
@@ -6816,7 +6750,7 @@
       <c r="H23" s="7"/>
       <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="9" t="s">
         <v>96</v>
       </c>
@@ -6834,7 +6768,7 @@
       <c r="H24" s="7"/>
       <c r="I24" s="11"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="9" t="s">
         <v>97</v>
       </c>
@@ -6852,7 +6786,7 @@
       <c r="H25" s="7"/>
       <c r="I25" s="11"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="9" t="s">
         <v>99</v>
       </c>
@@ -6870,7 +6804,7 @@
       <c r="H26" s="7"/>
       <c r="I26" s="11"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="9" t="s">
         <v>95</v>
       </c>
@@ -6890,7 +6824,7 @@
       </c>
       <c r="I27" s="11"/>
     </row>
-    <row r="28" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="14" t="s">
         <v>271</v>
       </c>
@@ -6909,7 +6843,7 @@
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="9" t="s">
         <v>98</v>
       </c>
@@ -6929,7 +6863,7 @@
       </c>
       <c r="I29" s="7"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="9" t="s">
         <v>103</v>
       </c>
@@ -6947,7 +6881,7 @@
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="9" t="s">
         <v>104</v>
       </c>
@@ -6965,7 +6899,7 @@
       <c r="H31" s="7"/>
       <c r="I31" s="11"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="9" t="s">
         <v>105</v>
       </c>
@@ -6983,7 +6917,7 @@
       <c r="H32" s="7"/>
       <c r="I32" s="11"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="9" t="s">
         <v>106</v>
       </c>
@@ -7001,7 +6935,7 @@
       <c r="H33" s="7"/>
       <c r="I33" s="11"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="9" t="s">
         <v>107</v>
       </c>
@@ -7019,7 +6953,7 @@
       <c r="H34" s="7"/>
       <c r="I34" s="11"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="9" t="s">
         <v>108</v>
       </c>
@@ -7037,7 +6971,7 @@
       <c r="H35" s="7"/>
       <c r="I35" s="11"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="9" t="s">
         <v>109</v>
       </c>
@@ -7058,7 +6992,7 @@
       <c r="H36" s="7"/>
       <c r="I36" s="11"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="9" t="s">
         <v>110</v>
       </c>
@@ -7079,7 +7013,7 @@
       <c r="H37" s="7"/>
       <c r="I37" s="11"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="9" t="s">
         <v>111</v>
       </c>
@@ -7100,7 +7034,7 @@
       <c r="H38" s="7"/>
       <c r="I38" s="11"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="9" t="s">
         <v>112</v>
       </c>
@@ -7121,7 +7055,7 @@
       <c r="H39" s="7"/>
       <c r="I39" s="11"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="9" t="s">
         <v>113</v>
       </c>
@@ -7142,7 +7076,7 @@
       <c r="H40" s="7"/>
       <c r="I40" s="11"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="9" t="s">
         <v>114</v>
       </c>
@@ -7163,7 +7097,7 @@
       <c r="H41" s="7"/>
       <c r="I41" s="11"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="9" t="s">
         <v>115</v>
       </c>
@@ -7184,7 +7118,7 @@
       <c r="H42" s="7"/>
       <c r="I42" s="11"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="9" t="s">
         <v>116</v>
       </c>
@@ -7205,7 +7139,7 @@
       <c r="H43" s="7"/>
       <c r="I43" s="11"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="9" t="s">
         <v>117</v>
       </c>
@@ -7226,7 +7160,7 @@
       <c r="H44" s="7"/>
       <c r="I44" s="11"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="9" t="s">
         <v>118</v>
       </c>
@@ -7247,7 +7181,7 @@
       <c r="H45" s="7"/>
       <c r="I45" s="11"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="9" t="s">
         <v>119</v>
       </c>
@@ -7268,7 +7202,7 @@
       <c r="H46" s="7"/>
       <c r="I46" s="11"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="9" t="s">
         <v>120</v>
       </c>
@@ -7289,7 +7223,7 @@
       <c r="H47" s="7"/>
       <c r="I47" s="11"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="9" t="s">
         <v>121</v>
       </c>
@@ -7310,7 +7244,7 @@
       <c r="H48" s="7"/>
       <c r="I48" s="11"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="9" t="s">
         <v>122</v>
       </c>
@@ -7331,7 +7265,7 @@
       <c r="H49" s="7"/>
       <c r="I49" s="11"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="9" t="s">
         <v>123</v>
       </c>
@@ -7352,7 +7286,7 @@
       <c r="H50" s="7"/>
       <c r="I50" s="11"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="9" t="s">
         <v>124</v>
       </c>
@@ -7373,7 +7307,7 @@
       <c r="H51" s="7"/>
       <c r="I51" s="11"/>
     </row>
-    <row r="52" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="14" t="s">
         <v>707</v>
       </c>
@@ -7394,7 +7328,7 @@
       <c r="H52" s="11"/>
       <c r="I52" s="11"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="9" t="s">
         <v>125</v>
       </c>
@@ -7415,7 +7349,7 @@
       <c r="H53" s="7"/>
       <c r="I53" s="11"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="9" t="s">
         <v>126</v>
       </c>
@@ -7436,7 +7370,7 @@
       <c r="H54" s="7"/>
       <c r="I54" s="11"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="9" t="s">
         <v>127</v>
       </c>
@@ -7457,7 +7391,7 @@
       <c r="H55" s="7"/>
       <c r="I55" s="11"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="9" t="s">
         <v>138</v>
       </c>
@@ -7475,7 +7409,7 @@
       <c r="H56" s="7"/>
       <c r="I56" s="11"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="9" t="s">
         <v>139</v>
       </c>
@@ -7493,7 +7427,7 @@
       <c r="H57" s="7"/>
       <c r="I57" s="11"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="9" t="s">
         <v>140</v>
       </c>
@@ -7511,7 +7445,7 @@
       <c r="H58" s="7"/>
       <c r="I58" s="11"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="9" t="s">
         <v>141</v>
       </c>
@@ -7529,7 +7463,7 @@
       <c r="H59" s="7"/>
       <c r="I59" s="11"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="9" t="s">
         <v>142</v>
       </c>
@@ -7547,7 +7481,7 @@
       <c r="H60" s="7"/>
       <c r="I60" s="11"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="9" t="s">
         <v>143</v>
       </c>
@@ -7565,7 +7499,7 @@
       <c r="H61" s="7"/>
       <c r="I61" s="11"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="9" t="s">
         <v>144</v>
       </c>
@@ -7583,7 +7517,7 @@
       <c r="H62" s="7"/>
       <c r="I62" s="11"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="9" t="s">
         <v>145</v>
       </c>
@@ -7601,7 +7535,7 @@
       <c r="H63" s="7"/>
       <c r="I63" s="11"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="9" t="s">
         <v>146</v>
       </c>
@@ -7619,7 +7553,7 @@
       <c r="H64" s="7"/>
       <c r="I64" s="11"/>
     </row>
-    <row r="65" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="14" t="s">
         <v>165</v>
       </c>
@@ -7638,7 +7572,7 @@
       <c r="H65" s="11"/>
       <c r="I65" s="11"/>
     </row>
-    <row r="66" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="14" t="s">
         <v>276</v>
       </c>
@@ -7657,7 +7591,7 @@
       <c r="H66" s="11"/>
       <c r="I66" s="11"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="8" t="s">
         <v>159</v>
       </c>
@@ -7678,7 +7612,7 @@
       <c r="H67" s="7"/>
       <c r="I67" s="11"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="9" t="s">
         <v>160</v>
       </c>
@@ -7698,25 +7632,25 @@
       <c r="G68" s="11"/>
       <c r="I68" s="11"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="G69" s="11"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="G70" s="11"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="G71" s="11"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="G72" s="11"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="G73" s="11"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="G74" s="11"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="G75" s="11"/>
     </row>
   </sheetData>
@@ -7739,15 +7673,15 @@
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.15625" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.68359375" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -7758,7 +7692,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="13" t="s">
         <v>265</v>
       </c>
@@ -7785,24 +7719,24 @@
       <selection pane="topRight" activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="63.140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.26171875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="63.15625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="11.41796875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="11.68359375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83984375" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="65.5703125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="65.578125" style="10" customWidth="1"/>
     <col min="8" max="8" width="13" style="10" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" style="60" customWidth="1"/>
+    <col min="9" max="9" width="24.68359375" style="60" customWidth="1"/>
     <col min="10" max="10" width="13" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="14.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.83984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="14.26171875" style="10" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -7837,7 +7771,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="35" t="s">
         <v>459</v>
       </c>
@@ -7860,7 +7794,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="35" t="s">
         <v>460</v>
       </c>
@@ -7883,7 +7817,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="35" t="s">
         <v>461</v>
       </c>
@@ -7909,7 +7843,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="35" t="s">
         <v>492</v>
       </c>
@@ -7935,7 +7869,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="35" t="s">
         <v>462</v>
       </c>
@@ -7960,7 +7894,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="33" t="s">
         <v>463</v>
       </c>
@@ -7985,7 +7919,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="33" t="s">
         <v>464</v>
       </c>
@@ -8010,7 +7944,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="33" t="s">
         <v>493</v>
       </c>
@@ -8035,7 +7969,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="13" t="s">
         <v>183</v>
       </c>
@@ -8060,7 +7994,7 @@
       </c>
       <c r="K10" s="11"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="13" t="s">
         <v>184</v>
       </c>
@@ -8085,7 +8019,7 @@
       </c>
       <c r="K11" s="11"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="13" t="s">
         <v>185</v>
       </c>
@@ -8110,7 +8044,7 @@
       </c>
       <c r="K12" s="11"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="13" t="s">
         <v>186</v>
       </c>
@@ -8135,7 +8069,7 @@
       </c>
       <c r="K13" s="11"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="13" t="s">
         <v>187</v>
       </c>
@@ -8160,7 +8094,7 @@
       </c>
       <c r="K14" s="11"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="13" t="s">
         <v>188</v>
       </c>
@@ -8185,7 +8119,7 @@
       </c>
       <c r="K15" s="11"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="13" t="s">
         <v>189</v>
       </c>
@@ -8210,7 +8144,7 @@
       </c>
       <c r="K16" s="11"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="13" t="s">
         <v>190</v>
       </c>
@@ -8235,7 +8169,7 @@
       </c>
       <c r="K17" s="11"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="13" t="s">
         <v>237</v>
       </c>
@@ -8258,7 +8192,7 @@
       </c>
       <c r="K18" s="11"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="13" t="s">
         <v>238</v>
       </c>
@@ -8281,7 +8215,7 @@
       </c>
       <c r="K19" s="11"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="13" t="s">
         <v>231</v>
       </c>
@@ -8306,7 +8240,7 @@
       </c>
       <c r="K20" s="11"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="13" t="s">
         <v>239</v>
       </c>
@@ -8329,7 +8263,7 @@
       </c>
       <c r="K21" s="11"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="17" t="s">
         <v>240</v>
       </c>
@@ -8352,7 +8286,7 @@
       </c>
       <c r="K22" s="11"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="17" t="s">
         <v>241</v>
       </c>
@@ -8375,7 +8309,7 @@
       </c>
       <c r="K23" s="11"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="33" t="s">
         <v>465</v>
       </c>
@@ -8402,7 +8336,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="33" t="s">
         <v>466</v>
       </c>
@@ -8429,7 +8363,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="33" t="s">
         <v>467</v>
       </c>
@@ -8456,7 +8390,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="33" t="s">
         <v>468</v>
       </c>
@@ -8483,7 +8417,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="33" t="s">
         <v>470</v>
       </c>
@@ -8510,7 +8444,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="33" t="s">
         <v>471</v>
       </c>
@@ -8537,7 +8471,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="33" t="s">
         <v>472</v>
       </c>
@@ -8564,7 +8498,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="33" t="s">
         <v>473</v>
       </c>
@@ -8591,7 +8525,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="33" t="s">
         <v>474</v>
       </c>
@@ -8618,7 +8552,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="33" t="s">
         <v>475</v>
       </c>
@@ -8645,7 +8579,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="33" t="s">
         <v>476</v>
       </c>
@@ -8672,7 +8606,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="33" t="s">
         <v>477</v>
       </c>
@@ -8699,7 +8633,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="33" t="s">
         <v>478</v>
       </c>
@@ -8726,7 +8660,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="33" t="s">
         <v>479</v>
       </c>
@@ -8753,7 +8687,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="33" t="s">
         <v>480</v>
       </c>
@@ -8780,7 +8714,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="33" t="s">
         <v>481</v>
       </c>
@@ -8807,7 +8741,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="33" t="s">
         <v>482</v>
       </c>
@@ -8834,7 +8768,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="33" t="s">
         <v>483</v>
       </c>
@@ -8861,7 +8795,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="33" t="s">
         <v>484</v>
       </c>
@@ -8888,7 +8822,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="33" t="s">
         <v>485</v>
       </c>
@@ -8915,7 +8849,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="33" t="s">
         <v>486</v>
       </c>
@@ -8942,7 +8876,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="33" t="s">
         <v>487</v>
       </c>
@@ -8969,7 +8903,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="33" t="s">
         <v>488</v>
       </c>
@@ -8996,7 +8930,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="33" t="s">
         <v>489</v>
       </c>
@@ -9023,7 +8957,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="33" t="s">
         <v>490</v>
       </c>
@@ -9050,7 +8984,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="33" t="s">
         <v>431</v>
       </c>
@@ -9077,7 +9011,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="33" t="s">
         <v>458</v>
       </c>
@@ -9104,7 +9038,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="33" t="s">
         <v>469</v>
       </c>
@@ -9131,7 +9065,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="11" t="s">
         <v>167</v>
       </c>
@@ -9156,7 +9090,7 @@
       </c>
       <c r="K52" s="11"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="11" t="s">
         <v>170</v>
       </c>
@@ -9179,7 +9113,7 @@
       </c>
       <c r="K53" s="11"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="11" t="s">
         <v>168</v>
       </c>
@@ -9206,7 +9140,7 @@
       </c>
       <c r="K54" s="11"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="11" t="s">
         <v>169</v>
       </c>
@@ -9231,7 +9165,7 @@
       </c>
       <c r="K55" s="11"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="11" t="s">
         <v>783</v>
       </c>
@@ -9254,7 +9188,7 @@
       </c>
       <c r="K56" s="11"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="11" t="s">
         <v>173</v>
       </c>
@@ -9279,7 +9213,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="11" t="s">
         <v>543</v>
       </c>
@@ -9304,7 +9238,7 @@
       </c>
       <c r="K58" s="11"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="11" t="s">
         <v>711</v>
       </c>
@@ -9329,7 +9263,7 @@
       </c>
       <c r="K59" s="11"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="11" t="s">
         <v>547</v>
       </c>
@@ -9354,7 +9288,7 @@
       </c>
       <c r="K60" s="11"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="11" t="s">
         <v>611</v>
       </c>
@@ -9379,7 +9313,7 @@
       </c>
       <c r="K61" s="11"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="11" t="s">
         <v>612</v>
       </c>
@@ -9404,7 +9338,7 @@
       </c>
       <c r="K62" s="11"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="11" t="s">
         <v>609</v>
       </c>
@@ -9428,7 +9362,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="11" t="s">
         <v>175</v>
       </c>
@@ -9452,7 +9386,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="65" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="22" t="s">
         <v>374</v>
       </c>
@@ -9476,7 +9410,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="66" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="49" t="s">
         <v>647</v>
       </c>
@@ -9500,7 +9434,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="67" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="49" t="s">
         <v>646</v>
       </c>
@@ -9524,7 +9458,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="68" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" s="48" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="19" t="s">
         <v>178</v>
       </c>
@@ -9548,7 +9482,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="69" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="49" t="s">
         <v>649</v>
       </c>
@@ -9572,7 +9506,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="70" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="49" t="s">
         <v>648</v>
       </c>
@@ -9596,7 +9530,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="11" t="s">
         <v>224</v>
       </c>
@@ -9621,7 +9555,7 @@
       </c>
       <c r="K71" s="11"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="11" t="s">
         <v>225</v>
       </c>
@@ -9646,7 +9580,7 @@
       </c>
       <c r="K72" s="11"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="11" t="s">
         <v>228</v>
       </c>
@@ -9671,7 +9605,7 @@
       </c>
       <c r="K73" s="11"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="13" t="s">
         <v>176</v>
       </c>
@@ -9696,7 +9630,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="13" t="s">
         <v>179</v>
       </c>
@@ -9721,7 +9655,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="13" t="s">
         <v>177</v>
       </c>
@@ -9746,7 +9680,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="13" t="s">
         <v>181</v>
       </c>
@@ -9771,7 +9705,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="13" t="s">
         <v>180</v>
       </c>
@@ -9796,7 +9730,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="13" t="s">
         <v>182</v>
       </c>
@@ -9821,7 +9755,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="13" t="s">
         <v>232</v>
       </c>
@@ -9844,7 +9778,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="13" t="s">
         <v>233</v>
       </c>
@@ -9867,7 +9801,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="13" t="s">
         <v>234</v>
       </c>
@@ -9890,7 +9824,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="13" t="s">
         <v>235</v>
       </c>
@@ -9913,7 +9847,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="13" t="s">
         <v>236</v>
       </c>
@@ -9936,7 +9870,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="13" t="s">
         <v>246</v>
       </c>
@@ -9959,7 +9893,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="13" t="s">
         <v>247</v>
       </c>
@@ -9982,7 +9916,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="13" t="s">
         <v>259</v>
       </c>
@@ -10004,7 +9938,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="13" t="s">
         <v>261</v>
       </c>
@@ -10026,7 +9960,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="11" t="s">
         <v>174</v>
       </c>
@@ -10051,7 +9985,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="11" t="s">
         <v>208</v>
       </c>
@@ -10076,7 +10010,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="11" t="s">
         <v>212</v>
       </c>
@@ -10101,7 +10035,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="11" t="s">
         <v>191</v>
       </c>
@@ -10128,7 +10062,7 @@
       </c>
       <c r="K92" s="11"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="11" t="s">
         <v>375</v>
       </c>
@@ -10153,7 +10087,7 @@
       </c>
       <c r="K93" s="11"/>
     </row>
-    <row r="94" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="26" t="s">
         <v>362</v>
       </c>
@@ -10177,7 +10111,7 @@
       </c>
       <c r="K94" s="22"/>
     </row>
-    <row r="95" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="22" t="s">
         <v>366</v>
       </c>
@@ -10201,7 +10135,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="96" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="26" t="s">
         <v>367</v>
       </c>
@@ -10225,7 +10159,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="97" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="26" t="s">
         <v>363</v>
       </c>
@@ -10248,7 +10182,7 @@
       </c>
       <c r="K97" s="22"/>
     </row>
-    <row r="98" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="22" t="s">
         <v>361</v>
       </c>
@@ -10272,7 +10206,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="99" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="35" t="s">
         <v>524</v>
       </c>
@@ -10294,7 +10228,7 @@
       </c>
       <c r="K99" s="33"/>
     </row>
-    <row r="100" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="35" t="s">
         <v>525</v>
       </c>
@@ -10316,7 +10250,7 @@
       </c>
       <c r="K100" s="33"/>
     </row>
-    <row r="101" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="35" t="s">
         <v>526</v>
       </c>
@@ -10338,7 +10272,7 @@
       </c>
       <c r="K101" s="33"/>
     </row>
-    <row r="102" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="35" t="s">
         <v>527</v>
       </c>
@@ -10360,7 +10294,7 @@
       </c>
       <c r="K102" s="33"/>
     </row>
-    <row r="103" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="35" t="s">
         <v>528</v>
       </c>
@@ -10382,7 +10316,7 @@
       </c>
       <c r="K103" s="33"/>
     </row>
-    <row r="104" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="35" t="s">
         <v>529</v>
       </c>
@@ -10404,7 +10338,7 @@
       </c>
       <c r="K104" s="33"/>
     </row>
-    <row r="105" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="41" t="s">
         <v>536</v>
       </c>
@@ -10427,7 +10361,7 @@
       </c>
       <c r="K105" s="42"/>
     </row>
-    <row r="106" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="41" t="s">
         <v>544</v>
       </c>
@@ -10452,7 +10386,7 @@
       </c>
       <c r="K106" s="42"/>
     </row>
-    <row r="107" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="41" t="s">
         <v>625</v>
       </c>
@@ -10477,7 +10411,7 @@
       </c>
       <c r="K107" s="42"/>
     </row>
-    <row r="108" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="41" t="s">
         <v>626</v>
       </c>
@@ -10502,7 +10436,7 @@
       </c>
       <c r="K108" s="42"/>
     </row>
-    <row r="109" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="41" t="s">
         <v>627</v>
       </c>
@@ -10527,7 +10461,7 @@
       </c>
       <c r="K109" s="42"/>
     </row>
-    <row r="110" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="41" t="s">
         <v>629</v>
       </c>
@@ -10552,7 +10486,7 @@
       </c>
       <c r="K110" s="42"/>
     </row>
-    <row r="111" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="41" t="s">
         <v>636</v>
       </c>
@@ -10577,7 +10511,7 @@
       </c>
       <c r="K111" s="42"/>
     </row>
-    <row r="112" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" s="57" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="41" t="s">
         <v>622</v>
       </c>
@@ -10601,7 +10535,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="113" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="52" t="s">
         <v>583</v>
       </c>
@@ -10625,7 +10559,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="114" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="52" t="s">
         <v>582</v>
       </c>
@@ -10649,7 +10583,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="115" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="52" t="s">
         <v>581</v>
       </c>
@@ -10673,7 +10607,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="116" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="52" t="s">
         <v>580</v>
       </c>
@@ -10697,7 +10631,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="117" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="52" t="s">
         <v>584</v>
       </c>
@@ -10721,7 +10655,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="118" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="52" t="s">
         <v>594</v>
       </c>
@@ -10745,7 +10679,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="119" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="52" t="s">
         <v>595</v>
       </c>
@@ -10769,7 +10703,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="120" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="52" t="s">
         <v>596</v>
       </c>
@@ -10793,7 +10727,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="121" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="52" t="s">
         <v>597</v>
       </c>
@@ -10817,7 +10751,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="122" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="52" t="s">
         <v>598</v>
       </c>
@@ -10841,7 +10775,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="123" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="35" t="s">
         <v>538</v>
       </c>
@@ -10864,7 +10798,7 @@
       </c>
       <c r="K123" s="33"/>
     </row>
-    <row r="124" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="35" t="s">
         <v>545</v>
       </c>
@@ -10889,7 +10823,7 @@
       </c>
       <c r="K124" s="33"/>
     </row>
-    <row r="125" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="35" t="s">
         <v>628</v>
       </c>
@@ -10914,7 +10848,7 @@
       </c>
       <c r="K125" s="33"/>
     </row>
-    <row r="126" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="35" t="s">
         <v>632</v>
       </c>
@@ -10939,7 +10873,7 @@
       </c>
       <c r="K126" s="33"/>
     </row>
-    <row r="127" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="35" t="s">
         <v>631</v>
       </c>
@@ -10964,7 +10898,7 @@
       </c>
       <c r="K127" s="33"/>
     </row>
-    <row r="128" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="35" t="s">
         <v>630</v>
       </c>
@@ -10989,7 +10923,7 @@
       </c>
       <c r="K128" s="33"/>
     </row>
-    <row r="129" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="35" t="s">
         <v>637</v>
       </c>
@@ -11014,7 +10948,7 @@
       </c>
       <c r="K129" s="33"/>
     </row>
-    <row r="130" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="35" t="s">
         <v>623</v>
       </c>
@@ -11038,7 +10972,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="131" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="52" t="s">
         <v>585</v>
       </c>
@@ -11062,7 +10996,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="132" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="52" t="s">
         <v>586</v>
       </c>
@@ -11086,7 +11020,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="133" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="52" t="s">
         <v>587</v>
       </c>
@@ -11110,7 +11044,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="134" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="52" t="s">
         <v>588</v>
       </c>
@@ -11134,7 +11068,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="135" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="52" t="s">
         <v>589</v>
       </c>
@@ -11158,7 +11092,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="136" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="52" t="s">
         <v>599</v>
       </c>
@@ -11182,7 +11116,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="137" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="52" t="s">
         <v>600</v>
       </c>
@@ -11206,7 +11140,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="138" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="52" t="s">
         <v>601</v>
       </c>
@@ -11230,7 +11164,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="139" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="52" t="s">
         <v>602</v>
       </c>
@@ -11254,7 +11188,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="140" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="52" t="s">
         <v>603</v>
       </c>
@@ -11278,7 +11212,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="141" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="43" t="s">
         <v>540</v>
       </c>
@@ -11301,7 +11235,7 @@
       </c>
       <c r="K141" s="45"/>
     </row>
-    <row r="142" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="43" t="s">
         <v>546</v>
       </c>
@@ -11326,7 +11260,7 @@
       </c>
       <c r="K142" s="45"/>
     </row>
-    <row r="143" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="43" t="s">
         <v>633</v>
       </c>
@@ -11351,7 +11285,7 @@
       </c>
       <c r="K143" s="45"/>
     </row>
-    <row r="144" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="43" t="s">
         <v>634</v>
       </c>
@@ -11376,7 +11310,7 @@
       </c>
       <c r="K144" s="45"/>
     </row>
-    <row r="145" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="43" t="s">
         <v>635</v>
       </c>
@@ -11401,7 +11335,7 @@
       </c>
       <c r="K145" s="45"/>
     </row>
-    <row r="146" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="43" t="s">
         <v>638</v>
       </c>
@@ -11426,7 +11360,7 @@
       </c>
       <c r="K146" s="45"/>
     </row>
-    <row r="147" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="43" t="s">
         <v>624</v>
       </c>
@@ -11451,7 +11385,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="148" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="52" t="s">
         <v>590</v>
       </c>
@@ -11475,7 +11409,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="149" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="52" t="s">
         <v>591</v>
       </c>
@@ -11499,7 +11433,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="150" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="52" t="s">
         <v>592</v>
       </c>
@@ -11523,7 +11457,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="151" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="52" t="s">
         <v>593</v>
       </c>
@@ -11547,7 +11481,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="152" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="52" t="s">
         <v>604</v>
       </c>
@@ -11571,7 +11505,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="153" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="52" t="s">
         <v>605</v>
       </c>
@@ -11595,7 +11529,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="154" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="52" t="s">
         <v>606</v>
       </c>
@@ -11619,7 +11553,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="155" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" s="55" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="52" t="s">
         <v>607</v>
       </c>
@@ -11643,7 +11577,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="13" t="s">
         <v>192</v>
       </c>
@@ -11668,7 +11602,7 @@
       </c>
       <c r="K156" s="11"/>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="13" t="s">
         <v>193</v>
       </c>
@@ -11693,7 +11627,7 @@
       </c>
       <c r="K157" s="11"/>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="13" t="s">
         <v>194</v>
       </c>
@@ -11718,7 +11652,7 @@
       </c>
       <c r="K158" s="11"/>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="13" t="s">
         <v>195</v>
       </c>
@@ -11743,7 +11677,7 @@
       </c>
       <c r="K159" s="11"/>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="13" t="s">
         <v>196</v>
       </c>
@@ -11768,7 +11702,7 @@
       </c>
       <c r="K160" s="11"/>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="13" t="s">
         <v>197</v>
       </c>
@@ -11793,7 +11727,7 @@
       </c>
       <c r="K161" s="11"/>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="13" t="s">
         <v>198</v>
       </c>
@@ -11818,7 +11752,7 @@
       </c>
       <c r="K162" s="11"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="13" t="s">
         <v>199</v>
       </c>
@@ -11843,7 +11777,7 @@
       </c>
       <c r="K163" s="11"/>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="13" t="s">
         <v>200</v>
       </c>
@@ -11868,7 +11802,7 @@
       </c>
       <c r="K164" s="11"/>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="13" t="s">
         <v>201</v>
       </c>
@@ -11893,7 +11827,7 @@
       </c>
       <c r="K165" s="11"/>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="13" t="s">
         <v>202</v>
       </c>
@@ -11918,7 +11852,7 @@
       </c>
       <c r="K166" s="11"/>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="13" t="s">
         <v>203</v>
       </c>
@@ -11943,7 +11877,7 @@
       </c>
       <c r="K167" s="11"/>
     </row>
-    <row r="168" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="33" t="s">
         <v>737</v>
       </c>
@@ -11970,7 +11904,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="169" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="33" t="s">
         <v>738</v>
       </c>
@@ -11997,7 +11931,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="170" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="33" t="s">
         <v>739</v>
       </c>
@@ -12024,7 +11958,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="171" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="33" t="s">
         <v>740</v>
       </c>
@@ -12051,7 +11985,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="172" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="33" t="s">
         <v>741</v>
       </c>
@@ -12078,7 +12012,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="173" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="33" t="s">
         <v>742</v>
       </c>
@@ -12105,7 +12039,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="174" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="33" t="s">
         <v>761</v>
       </c>
@@ -12132,7 +12066,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="175" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="33" t="s">
         <v>762</v>
       </c>
@@ -12159,7 +12093,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="176" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="33" t="s">
         <v>763</v>
       </c>
@@ -12186,7 +12120,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="177" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="33" t="s">
         <v>752</v>
       </c>
@@ -12213,7 +12147,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="178" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="33" t="s">
         <v>753</v>
       </c>
@@ -12240,7 +12174,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="179" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="33" t="s">
         <v>754</v>
       </c>
@@ -12267,7 +12201,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="180" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="33" t="s">
         <v>755</v>
       </c>
@@ -12294,7 +12228,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="181" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="33" t="s">
         <v>756</v>
       </c>
@@ -12321,7 +12255,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="182" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="33" t="s">
         <v>757</v>
       </c>
@@ -12348,17 +12282,17 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E183" s="11"/>
       <c r="F183" s="11"/>
       <c r="I183" s="59"/>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E184" s="11"/>
       <c r="F184" s="11"/>
       <c r="I184" s="59"/>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="E185" s="11"/>
       <c r="F185" s="11"/>
       <c r="I185" s="59"/>
@@ -12391,13 +12325,13 @@
       <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="55.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.83984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="18" t="s">
         <v>359</v>
       </c>
@@ -12405,7 +12339,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>280</v>
       </c>
@@ -12413,7 +12347,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>348</v>
       </c>
@@ -12421,7 +12355,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>349</v>
       </c>
@@ -12429,7 +12363,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>350</v>
       </c>
@@ -12437,8 +12371,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="18" t="s">
         <v>353</v>
       </c>
@@ -12446,7 +12380,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="10" t="s">
         <v>351</v>
       </c>
@@ -12454,7 +12388,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="10" t="s">
         <v>348</v>
       </c>
@@ -12462,7 +12396,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="10" t="s">
         <v>349</v>
       </c>
@@ -12471,12 +12405,12 @@
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="18" t="s">
         <v>354</v>
       </c>
@@ -12485,7 +12419,7 @@
       </c>
       <c r="E12" s="14"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="10" t="s">
         <v>352</v>
       </c>
@@ -12494,7 +12428,7 @@
       </c>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="10" t="s">
         <v>348</v>
       </c>
@@ -12503,7 +12437,7 @@
       </c>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="10" t="s">
         <v>349</v>
       </c>
@@ -12512,18 +12446,18 @@
       </c>
       <c r="E15" s="14"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="E16" s="14"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="E17" s="14"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="13"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="13"/>
     </row>
   </sheetData>
@@ -12536,18 +12470,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.15625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="10" customWidth="1"/>
-    <col min="3" max="3" width="104.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="104.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="12" t="s">
         <v>343</v>
       </c>
@@ -12561,7 +12495,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>101</v>
       </c>
@@ -12569,13 +12503,13 @@
         <v>303</v>
       </c>
       <c r="C2" t="s">
-        <v>806</v>
+        <v>98</v>
       </c>
       <c r="D2" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>279</v>
       </c>
@@ -12583,13 +12517,13 @@
         <v>303</v>
       </c>
       <c r="C3" t="s">
-        <v>807</v>
+        <v>72</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>280</v>
       </c>
@@ -12597,11 +12531,11 @@
         <v>303</v>
       </c>
       <c r="C4" t="s">
-        <v>808</v>
+        <v>95</v>
       </c>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>281</v>
       </c>
@@ -12609,11 +12543,11 @@
         <v>303</v>
       </c>
       <c r="C5" t="s">
-        <v>809</v>
+        <v>100</v>
       </c>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>282</v>
       </c>
@@ -12621,11 +12555,11 @@
         <v>303</v>
       </c>
       <c r="C6" t="s">
-        <v>810</v>
+        <v>96</v>
       </c>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>283</v>
       </c>
@@ -12633,11 +12567,11 @@
         <v>303</v>
       </c>
       <c r="C7" t="s">
-        <v>811</v>
+        <v>97</v>
       </c>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>284</v>
       </c>
@@ -12649,7 +12583,7 @@
       </c>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>285</v>
       </c>
@@ -12661,7 +12595,7 @@
       </c>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>286</v>
       </c>
@@ -12673,7 +12607,7 @@
       </c>
       <c r="G10" s="10"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>287</v>
       </c>
@@ -12681,11 +12615,11 @@
         <v>303</v>
       </c>
       <c r="C11" t="s">
-        <v>812</v>
+        <v>94</v>
       </c>
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>288</v>
       </c>
@@ -12693,11 +12627,11 @@
         <v>303</v>
       </c>
       <c r="C12" t="s">
-        <v>813</v>
+        <v>93</v>
       </c>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>289</v>
       </c>
@@ -12712,7 +12646,7 @@
       </c>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>290</v>
       </c>
@@ -12724,7 +12658,7 @@
       </c>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>291</v>
       </c>
@@ -12736,7 +12670,7 @@
       </c>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>292</v>
       </c>
@@ -12748,7 +12682,7 @@
       </c>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>293</v>
       </c>
@@ -12760,7 +12694,7 @@
       </c>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>294</v>
       </c>
@@ -12768,14 +12702,14 @@
         <v>303</v>
       </c>
       <c r="C18" t="s">
-        <v>819</v>
+        <v>65</v>
       </c>
       <c r="D18" t="s">
         <v>306</v>
       </c>
       <c r="G18" s="10"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>295</v>
       </c>
@@ -12783,11 +12717,11 @@
         <v>303</v>
       </c>
       <c r="C19" t="s">
-        <v>814</v>
+        <v>165</v>
       </c>
       <c r="G19" s="10"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>296</v>
       </c>
@@ -12795,11 +12729,11 @@
         <v>303</v>
       </c>
       <c r="C20" t="s">
-        <v>815</v>
+        <v>807</v>
       </c>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>704</v>
       </c>
@@ -12807,11 +12741,11 @@
         <v>303</v>
       </c>
       <c r="C21" t="s">
-        <v>816</v>
+        <v>115</v>
       </c>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>705</v>
       </c>
@@ -12819,11 +12753,11 @@
         <v>303</v>
       </c>
       <c r="C22" t="s">
-        <v>817</v>
+        <v>127</v>
       </c>
       <c r="G22" s="10"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>706</v>
       </c>
@@ -12831,11 +12765,11 @@
         <v>303</v>
       </c>
       <c r="C23" t="s">
-        <v>818</v>
+        <v>707</v>
       </c>
       <c r="G23" s="10"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>794</v>
       </c>
@@ -12843,11 +12777,11 @@
         <v>303</v>
       </c>
       <c r="C24" t="s">
-        <v>820</v>
+        <v>737</v>
       </c>
       <c r="G24" s="10"/>
     </row>
-    <row r="25" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="10" t="s">
         <v>795</v>
       </c>
@@ -12855,10 +12789,10 @@
         <v>303</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="10" t="s">
         <v>796</v>
       </c>
@@ -12866,10 +12800,10 @@
         <v>303</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="10" t="s">
         <v>797</v>
       </c>
@@ -12877,10 +12811,10 @@
         <v>303</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>823</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="10" t="s">
         <v>798</v>
       </c>
@@ -12888,11 +12822,11 @@
         <v>303</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>824</v>
+        <v>741</v>
       </c>
       <c r="G28" s="10"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="10" t="s">
         <v>799</v>
       </c>
@@ -12900,11 +12834,11 @@
         <v>303</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>825</v>
+        <v>742</v>
       </c>
       <c r="G29" s="10"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>800</v>
       </c>
@@ -12912,11 +12846,11 @@
         <v>303</v>
       </c>
       <c r="C30" t="s">
-        <v>826</v>
+        <v>761</v>
       </c>
       <c r="G30" s="10"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="10" t="s">
         <v>801</v>
       </c>
@@ -12924,11 +12858,11 @@
         <v>303</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>827</v>
+        <v>762</v>
       </c>
       <c r="G31" s="10"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="10" t="s">
         <v>802</v>
       </c>
@@ -12936,19 +12870,19 @@
         <v>303</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>828</v>
+        <v>763</v>
       </c>
       <c r="G32" s="10"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="10" t="s">
-        <v>829</v>
+        <v>806</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>303</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>830</v>
+        <v>808</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add missing framework units to TB
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_tb.xlsx
+++ b/tests/frameworks/framework_tb.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\tb-ucl-analyses\general\frameworks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4EC7B89-938F-4050-87FA-98FFF6E7775F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="16095" windowHeight="9660" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="16095" windowHeight="9660" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="14" r:id="rId1"/>
@@ -28,12 +29,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -54,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -77,12 +78,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -107,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -133,7 +134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -159,7 +160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -184,7 +185,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -212,7 +213,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -240,7 +241,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
       <text>
         <r>
           <rPr>
@@ -254,7 +255,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
       <text>
         <r>
           <rPr>
@@ -273,7 +274,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
       <text>
         <r>
           <rPr>
@@ -293,12 +294,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -323,7 +324,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -349,7 +350,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
       <text>
         <r>
           <rPr>
@@ -375,7 +376,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000004000000}">
       <text>
         <r>
           <rPr>
@@ -388,7 +389,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000005000000}">
       <text>
         <r>
           <rPr>
@@ -401,7 +402,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000006000000}">
       <text>
         <r>
           <rPr>
@@ -428,7 +429,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000007000000}">
       <text>
         <r>
           <rPr>
@@ -442,7 +443,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000008000000}">
       <text>
         <r>
           <rPr>
@@ -461,7 +462,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000009000000}">
       <text>
         <r>
           <rPr>
@@ -481,12 +482,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -510,7 +511,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
       <text>
         <r>
           <rPr>
@@ -535,7 +536,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000003000000}">
       <text>
         <r>
           <rPr>
@@ -553,13 +554,13 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
     <author>Rowan</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -581,7 +582,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
       <text>
         <r>
           <rPr>
@@ -604,7 +605,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000003000000}">
       <text>
         <r>
           <rPr>
@@ -617,7 +618,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000004000000}">
       <text>
         <r>
           <rPr>
@@ -630,7 +631,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000005000000}">
       <text>
         <r>
           <rPr>
@@ -643,7 +644,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000006000000}">
       <text>
         <r>
           <rPr>
@@ -656,7 +657,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000007000000}">
       <text>
         <r>
           <rPr>
@@ -669,7 +670,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000008000000}">
       <text>
         <r>
           <rPr>
@@ -686,7 +687,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000009000000}">
       <text>
         <r>
           <rPr>
@@ -700,7 +701,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -719,7 +720,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -734,7 +735,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G49" authorId="1" shapeId="0">
+    <comment ref="G49" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -758,7 +759,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B57" authorId="1" shapeId="0">
+    <comment ref="B57" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -782,7 +783,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D93" authorId="1" shapeId="0">
+    <comment ref="D93" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -811,12 +812,12 @@
 </file>
 
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
       <text>
         <r>
           <rPr>
@@ -847,7 +848,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1884" uniqueCount="805">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1886" uniqueCount="805">
   <si>
     <t>Code Name</t>
   </si>
@@ -3267,7 +3268,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3543,7 +3544,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Neutral 2" xfId="1"/>
+    <cellStyle name="Neutral 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -3664,6 +3665,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3699,6 +3717,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3874,7 +3909,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3905,7 +3940,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4134,7 +4169,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4255,7 +4290,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
@@ -5315,10 +5350,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:E47">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:E47" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"n,y"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G51">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G51" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"y,n"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5329,7 +5364,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AY51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6426,11 +6461,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="H75" sqref="H75"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8159,7 +8194,7 @@
   </sheetData>
   <dataConsolidate/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G76">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G76" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>"y,n"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8169,7 +8204,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8213,13 +8248,13 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K176"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" activeCell="B35" sqref="B35"/>
+      <selection pane="topRight" activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9817,7 +9852,9 @@
       <c r="B54" s="8" t="s">
         <v>315</v>
       </c>
-      <c r="C54" s="11"/>
+      <c r="C54" s="11" t="s">
+        <v>210</v>
+      </c>
       <c r="D54" s="11"/>
       <c r="E54" s="11">
         <v>0</v>
@@ -9871,7 +9908,9 @@
       <c r="B56" s="28" t="s">
         <v>338</v>
       </c>
-      <c r="C56" s="11"/>
+      <c r="C56" s="11" t="s">
+        <v>209</v>
+      </c>
       <c r="D56" s="11">
         <v>0</v>
       </c>
@@ -13133,10 +13172,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I174:I176">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I174:I176" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>"y,n"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H173">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H173" xr:uid="{00000000-0002-0000-0600-000001000000}">
       <formula1>"n,y"</formula1>
     </dataValidation>
   </dataValidations>
@@ -13147,7 +13186,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13288,7 +13327,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>